<commit_message>
excel update 2020-03-25 10:30 AM
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2413D9-4927-A249-9BB1-27348AC83217}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86146208-28BD-4145-9BB5-CFCE9E3E3617}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="90">
   <si>
     <t>Negative1</t>
   </si>
@@ -262,6 +262,48 @@
   </si>
   <si>
     <t>travel (Brazil)</t>
+  </si>
+  <si>
+    <t>travel (Spain, France)</t>
+  </si>
+  <si>
+    <t>travel (Dominican)</t>
+  </si>
+  <si>
+    <t>Porcupine District</t>
+  </si>
+  <si>
+    <t>Middlesex London</t>
+  </si>
+  <si>
+    <t>travel (Philippines)</t>
+  </si>
+  <si>
+    <t>travel (Mexico)</t>
+  </si>
+  <si>
+    <t>&lt;18 Male</t>
+  </si>
+  <si>
+    <t>travel (Bahamas)</t>
+  </si>
+  <si>
+    <t>Peterborough</t>
+  </si>
+  <si>
+    <t>travel (Peru)</t>
+  </si>
+  <si>
+    <t>&lt; 20 Male</t>
+  </si>
+  <si>
+    <t>travel (Egypt)</t>
+  </si>
+  <si>
+    <t>Timiskaming</t>
+  </si>
+  <si>
+    <t>travel (UK, USA)</t>
   </si>
 </sst>
 </file>
@@ -297,10 +339,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -701,6 +744,32 @@
         <v>32457</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>43915.4375</v>
+      </c>
+      <c r="B4">
+        <v>24458</v>
+      </c>
+      <c r="C4">
+        <v>10489</v>
+      </c>
+      <c r="D4">
+        <v>671</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <v>35635</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D11" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -708,10 +777,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349DD023-B549-B642-9379-4C23EAB3417F}">
-  <dimension ref="A1:F164"/>
+  <dimension ref="A1:F264"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
+      <selection activeCell="A264" sqref="A264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4004,6 +4073,2006 @@
         <v>14</v>
       </c>
     </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A165" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B165">
+        <v>589</v>
+      </c>
+      <c r="C165" t="s">
+        <v>57</v>
+      </c>
+      <c r="D165" t="s">
+        <v>45</v>
+      </c>
+      <c r="E165" t="s">
+        <v>76</v>
+      </c>
+      <c r="F165" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A166" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B166">
+        <v>590</v>
+      </c>
+      <c r="C166" t="s">
+        <v>21</v>
+      </c>
+      <c r="D166" t="s">
+        <v>17</v>
+      </c>
+      <c r="E166" t="s">
+        <v>77</v>
+      </c>
+      <c r="F166" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A167" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B167">
+        <v>591</v>
+      </c>
+      <c r="C167" t="s">
+        <v>29</v>
+      </c>
+      <c r="D167" t="s">
+        <v>25</v>
+      </c>
+      <c r="E167" t="s">
+        <v>14</v>
+      </c>
+      <c r="F167" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A168" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B168">
+        <v>592</v>
+      </c>
+      <c r="C168" t="s">
+        <v>16</v>
+      </c>
+      <c r="D168" t="s">
+        <v>24</v>
+      </c>
+      <c r="E168" t="s">
+        <v>14</v>
+      </c>
+      <c r="F168" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A169" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B169">
+        <v>593</v>
+      </c>
+      <c r="C169" t="s">
+        <v>41</v>
+      </c>
+      <c r="D169" t="s">
+        <v>24</v>
+      </c>
+      <c r="E169" t="s">
+        <v>66</v>
+      </c>
+      <c r="F169" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A170" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B170">
+        <v>594</v>
+      </c>
+      <c r="C170" t="s">
+        <v>16</v>
+      </c>
+      <c r="D170" t="s">
+        <v>35</v>
+      </c>
+      <c r="E170" t="s">
+        <v>18</v>
+      </c>
+      <c r="F170" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A171" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B171">
+        <v>595</v>
+      </c>
+      <c r="C171" t="s">
+        <v>41</v>
+      </c>
+      <c r="D171" t="s">
+        <v>24</v>
+      </c>
+      <c r="E171" t="s">
+        <v>14</v>
+      </c>
+      <c r="F171" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A172" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B172">
+        <v>596</v>
+      </c>
+      <c r="C172" t="s">
+        <v>52</v>
+      </c>
+      <c r="D172" t="s">
+        <v>78</v>
+      </c>
+      <c r="E172" t="s">
+        <v>14</v>
+      </c>
+      <c r="F172" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A173" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B173">
+        <v>597</v>
+      </c>
+      <c r="C173" t="s">
+        <v>20</v>
+      </c>
+      <c r="D173" t="s">
+        <v>78</v>
+      </c>
+      <c r="E173" t="s">
+        <v>18</v>
+      </c>
+      <c r="F173" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A174" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B174">
+        <v>598</v>
+      </c>
+      <c r="C174" t="s">
+        <v>16</v>
+      </c>
+      <c r="D174" t="s">
+        <v>48</v>
+      </c>
+      <c r="E174" t="s">
+        <v>18</v>
+      </c>
+      <c r="F174" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A175" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B175">
+        <v>599</v>
+      </c>
+      <c r="C175" t="s">
+        <v>23</v>
+      </c>
+      <c r="D175" t="s">
+        <v>25</v>
+      </c>
+      <c r="E175" t="s">
+        <v>18</v>
+      </c>
+      <c r="F175" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A176" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B176">
+        <v>600</v>
+      </c>
+      <c r="C176" t="s">
+        <v>16</v>
+      </c>
+      <c r="D176" t="s">
+        <v>25</v>
+      </c>
+      <c r="E176" t="s">
+        <v>18</v>
+      </c>
+      <c r="F176" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A177" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B177">
+        <v>601</v>
+      </c>
+      <c r="C177" t="s">
+        <v>52</v>
+      </c>
+      <c r="D177" t="s">
+        <v>25</v>
+      </c>
+      <c r="E177" t="s">
+        <v>18</v>
+      </c>
+      <c r="F177" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A178" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B178">
+        <v>602</v>
+      </c>
+      <c r="C178" t="s">
+        <v>57</v>
+      </c>
+      <c r="D178" t="s">
+        <v>78</v>
+      </c>
+      <c r="E178" t="s">
+        <v>28</v>
+      </c>
+      <c r="F178" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A179" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B179">
+        <v>603</v>
+      </c>
+      <c r="C179" t="s">
+        <v>41</v>
+      </c>
+      <c r="D179" t="s">
+        <v>70</v>
+      </c>
+      <c r="E179" t="s">
+        <v>28</v>
+      </c>
+      <c r="F179" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A180" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B180">
+        <v>604</v>
+      </c>
+      <c r="C180" t="s">
+        <v>51</v>
+      </c>
+      <c r="D180" t="s">
+        <v>79</v>
+      </c>
+      <c r="E180" t="s">
+        <v>18</v>
+      </c>
+      <c r="F180" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A181" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B181">
+        <v>605</v>
+      </c>
+      <c r="C181" t="s">
+        <v>47</v>
+      </c>
+      <c r="D181" t="s">
+        <v>79</v>
+      </c>
+      <c r="E181" t="s">
+        <v>80</v>
+      </c>
+      <c r="F181" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A182" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B182">
+        <v>606</v>
+      </c>
+      <c r="C182" t="s">
+        <v>52</v>
+      </c>
+      <c r="D182" t="s">
+        <v>46</v>
+      </c>
+      <c r="E182" t="s">
+        <v>14</v>
+      </c>
+      <c r="F182" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A183" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B183">
+        <v>607</v>
+      </c>
+      <c r="C183" t="s">
+        <v>16</v>
+      </c>
+      <c r="D183" t="s">
+        <v>35</v>
+      </c>
+      <c r="E183" t="s">
+        <v>14</v>
+      </c>
+      <c r="F183" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A184" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B184">
+        <v>608</v>
+      </c>
+      <c r="C184" t="s">
+        <v>29</v>
+      </c>
+      <c r="D184" t="s">
+        <v>46</v>
+      </c>
+      <c r="E184" t="s">
+        <v>14</v>
+      </c>
+      <c r="F184" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A185" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B185">
+        <v>609</v>
+      </c>
+      <c r="C185" t="s">
+        <v>47</v>
+      </c>
+      <c r="D185" t="s">
+        <v>46</v>
+      </c>
+      <c r="E185" t="s">
+        <v>14</v>
+      </c>
+      <c r="F185" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A186" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B186">
+        <v>610</v>
+      </c>
+      <c r="C186" t="s">
+        <v>47</v>
+      </c>
+      <c r="D186" t="s">
+        <v>46</v>
+      </c>
+      <c r="E186" t="s">
+        <v>14</v>
+      </c>
+      <c r="F186" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A187" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B187">
+        <v>611</v>
+      </c>
+      <c r="C187" t="s">
+        <v>47</v>
+      </c>
+      <c r="D187" t="s">
+        <v>35</v>
+      </c>
+      <c r="E187" t="s">
+        <v>63</v>
+      </c>
+      <c r="F187" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A188" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B188">
+        <v>612</v>
+      </c>
+      <c r="C188" t="s">
+        <v>50</v>
+      </c>
+      <c r="D188" t="s">
+        <v>38</v>
+      </c>
+      <c r="E188" t="s">
+        <v>14</v>
+      </c>
+      <c r="F188" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A189" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B189">
+        <v>613</v>
+      </c>
+      <c r="C189" t="s">
+        <v>23</v>
+      </c>
+      <c r="D189" t="s">
+        <v>70</v>
+      </c>
+      <c r="E189" t="s">
+        <v>14</v>
+      </c>
+      <c r="F189" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A190" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B190">
+        <v>614</v>
+      </c>
+      <c r="C190" t="s">
+        <v>50</v>
+      </c>
+      <c r="D190" t="s">
+        <v>65</v>
+      </c>
+      <c r="E190" t="s">
+        <v>81</v>
+      </c>
+      <c r="F190" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A191" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B191">
+        <v>615</v>
+      </c>
+      <c r="C191" t="s">
+        <v>52</v>
+      </c>
+      <c r="D191" t="s">
+        <v>22</v>
+      </c>
+      <c r="E191" t="s">
+        <v>28</v>
+      </c>
+      <c r="F191" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A192" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B192">
+        <v>616</v>
+      </c>
+      <c r="C192" t="s">
+        <v>52</v>
+      </c>
+      <c r="D192" t="s">
+        <v>13</v>
+      </c>
+      <c r="E192" t="s">
+        <v>63</v>
+      </c>
+      <c r="F192" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A193" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B193">
+        <v>617</v>
+      </c>
+      <c r="C193" t="s">
+        <v>32</v>
+      </c>
+      <c r="D193" t="s">
+        <v>65</v>
+      </c>
+      <c r="E193" t="s">
+        <v>18</v>
+      </c>
+      <c r="F193" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A194" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B194">
+        <v>618</v>
+      </c>
+      <c r="C194" t="s">
+        <v>82</v>
+      </c>
+      <c r="D194" t="s">
+        <v>65</v>
+      </c>
+      <c r="E194" t="s">
+        <v>18</v>
+      </c>
+      <c r="F194" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A195" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B195">
+        <v>619</v>
+      </c>
+      <c r="C195" t="s">
+        <v>23</v>
+      </c>
+      <c r="D195" t="s">
+        <v>65</v>
+      </c>
+      <c r="E195" t="s">
+        <v>18</v>
+      </c>
+      <c r="F195" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A196" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B196">
+        <v>620</v>
+      </c>
+      <c r="C196" t="s">
+        <v>47</v>
+      </c>
+      <c r="D196" t="s">
+        <v>22</v>
+      </c>
+      <c r="E196" t="s">
+        <v>83</v>
+      </c>
+      <c r="F196" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A197" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B197">
+        <v>621</v>
+      </c>
+      <c r="C197" t="s">
+        <v>16</v>
+      </c>
+      <c r="D197" t="s">
+        <v>25</v>
+      </c>
+      <c r="E197" t="s">
+        <v>63</v>
+      </c>
+      <c r="F197" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A198" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B198">
+        <v>622</v>
+      </c>
+      <c r="C198" t="s">
+        <v>37</v>
+      </c>
+      <c r="D198" t="s">
+        <v>25</v>
+      </c>
+      <c r="E198" t="s">
+        <v>14</v>
+      </c>
+      <c r="F198" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A199" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B199">
+        <v>623</v>
+      </c>
+      <c r="C199" t="s">
+        <v>52</v>
+      </c>
+      <c r="D199" t="s">
+        <v>25</v>
+      </c>
+      <c r="E199" t="s">
+        <v>14</v>
+      </c>
+      <c r="F199" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A200" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B200">
+        <v>624</v>
+      </c>
+      <c r="C200" t="s">
+        <v>41</v>
+      </c>
+      <c r="D200" t="s">
+        <v>25</v>
+      </c>
+      <c r="E200" t="s">
+        <v>14</v>
+      </c>
+      <c r="F200" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A201" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B201">
+        <v>625</v>
+      </c>
+      <c r="C201" t="s">
+        <v>23</v>
+      </c>
+      <c r="D201" t="s">
+        <v>25</v>
+      </c>
+      <c r="E201" t="s">
+        <v>14</v>
+      </c>
+      <c r="F201" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A202" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B202">
+        <v>626</v>
+      </c>
+      <c r="C202" t="s">
+        <v>55</v>
+      </c>
+      <c r="D202" t="s">
+        <v>25</v>
+      </c>
+      <c r="E202" t="s">
+        <v>14</v>
+      </c>
+      <c r="F202" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A203" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B203">
+        <v>627</v>
+      </c>
+      <c r="C203" t="s">
+        <v>29</v>
+      </c>
+      <c r="D203" t="s">
+        <v>71</v>
+      </c>
+      <c r="E203" t="s">
+        <v>28</v>
+      </c>
+      <c r="F203" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A204" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B204">
+        <v>628</v>
+      </c>
+      <c r="C204" t="s">
+        <v>26</v>
+      </c>
+      <c r="D204" t="s">
+        <v>25</v>
+      </c>
+      <c r="E204" t="s">
+        <v>18</v>
+      </c>
+      <c r="F204" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A205" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B205">
+        <v>629</v>
+      </c>
+      <c r="C205" t="s">
+        <v>16</v>
+      </c>
+      <c r="D205" t="s">
+        <v>25</v>
+      </c>
+      <c r="E205" t="s">
+        <v>14</v>
+      </c>
+      <c r="F205" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A206" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B206">
+        <v>630</v>
+      </c>
+      <c r="C206" t="s">
+        <v>52</v>
+      </c>
+      <c r="D206" t="s">
+        <v>17</v>
+      </c>
+      <c r="E206" t="s">
+        <v>14</v>
+      </c>
+      <c r="F206" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A207" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B207">
+        <v>631</v>
+      </c>
+      <c r="C207" t="s">
+        <v>29</v>
+      </c>
+      <c r="D207" t="s">
+        <v>25</v>
+      </c>
+      <c r="E207" t="s">
+        <v>14</v>
+      </c>
+      <c r="F207" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A208" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B208">
+        <v>632</v>
+      </c>
+      <c r="C208" t="s">
+        <v>26</v>
+      </c>
+      <c r="D208" t="s">
+        <v>25</v>
+      </c>
+      <c r="E208" t="s">
+        <v>18</v>
+      </c>
+      <c r="F208" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A209" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B209">
+        <v>633</v>
+      </c>
+      <c r="C209" t="s">
+        <v>21</v>
+      </c>
+      <c r="D209" t="s">
+        <v>24</v>
+      </c>
+      <c r="E209" t="s">
+        <v>18</v>
+      </c>
+      <c r="F209" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A210" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B210">
+        <v>634</v>
+      </c>
+      <c r="C210" t="s">
+        <v>47</v>
+      </c>
+      <c r="D210" t="s">
+        <v>84</v>
+      </c>
+      <c r="E210" t="s">
+        <v>28</v>
+      </c>
+      <c r="F210" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A211" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B211">
+        <v>635</v>
+      </c>
+      <c r="C211" t="s">
+        <v>52</v>
+      </c>
+      <c r="D211" t="s">
+        <v>24</v>
+      </c>
+      <c r="E211" t="s">
+        <v>85</v>
+      </c>
+      <c r="F211" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A212" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B212">
+        <v>636</v>
+      </c>
+      <c r="C212" t="s">
+        <v>26</v>
+      </c>
+      <c r="D212" t="s">
+        <v>25</v>
+      </c>
+      <c r="E212" t="s">
+        <v>18</v>
+      </c>
+      <c r="F212" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A213" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B213">
+        <v>637</v>
+      </c>
+      <c r="C213" t="s">
+        <v>16</v>
+      </c>
+      <c r="D213" t="s">
+        <v>25</v>
+      </c>
+      <c r="E213" t="s">
+        <v>28</v>
+      </c>
+      <c r="F213" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A214" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B214">
+        <v>638</v>
+      </c>
+      <c r="C214" t="s">
+        <v>50</v>
+      </c>
+      <c r="D214" t="s">
+        <v>17</v>
+      </c>
+      <c r="E214" t="s">
+        <v>18</v>
+      </c>
+      <c r="F214" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A215" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B215">
+        <v>639</v>
+      </c>
+      <c r="C215" t="s">
+        <v>50</v>
+      </c>
+      <c r="D215" t="s">
+        <v>17</v>
+      </c>
+      <c r="E215" t="s">
+        <v>66</v>
+      </c>
+      <c r="F215" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A216" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B216">
+        <v>640</v>
+      </c>
+      <c r="C216" t="s">
+        <v>23</v>
+      </c>
+      <c r="D216" t="s">
+        <v>17</v>
+      </c>
+      <c r="E216" t="s">
+        <v>18</v>
+      </c>
+      <c r="F216" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A217" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B217">
+        <v>641</v>
+      </c>
+      <c r="C217" t="s">
+        <v>23</v>
+      </c>
+      <c r="D217" t="s">
+        <v>35</v>
+      </c>
+      <c r="E217" t="s">
+        <v>18</v>
+      </c>
+      <c r="F217" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A218" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B218">
+        <v>642</v>
+      </c>
+      <c r="C218" t="s">
+        <v>86</v>
+      </c>
+      <c r="D218" t="s">
+        <v>25</v>
+      </c>
+      <c r="E218" t="s">
+        <v>14</v>
+      </c>
+      <c r="F218" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A219" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B219">
+        <v>643</v>
+      </c>
+      <c r="C219" t="s">
+        <v>57</v>
+      </c>
+      <c r="D219" t="s">
+        <v>25</v>
+      </c>
+      <c r="E219" t="s">
+        <v>28</v>
+      </c>
+      <c r="F219" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A220" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B220">
+        <v>644</v>
+      </c>
+      <c r="C220" t="s">
+        <v>50</v>
+      </c>
+      <c r="D220" t="s">
+        <v>24</v>
+      </c>
+      <c r="E220" t="s">
+        <v>14</v>
+      </c>
+      <c r="F220" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A221" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B221">
+        <v>645</v>
+      </c>
+      <c r="C221" t="s">
+        <v>26</v>
+      </c>
+      <c r="D221" t="s">
+        <v>65</v>
+      </c>
+      <c r="E221" t="s">
+        <v>18</v>
+      </c>
+      <c r="F221" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A222" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B222">
+        <v>646</v>
+      </c>
+      <c r="C222" t="s">
+        <v>86</v>
+      </c>
+      <c r="D222" t="s">
+        <v>24</v>
+      </c>
+      <c r="E222" t="s">
+        <v>14</v>
+      </c>
+      <c r="F222" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A223" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B223">
+        <v>647</v>
+      </c>
+      <c r="C223" t="s">
+        <v>57</v>
+      </c>
+      <c r="D223" t="s">
+        <v>24</v>
+      </c>
+      <c r="E223" t="s">
+        <v>87</v>
+      </c>
+      <c r="F223" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A224" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B224">
+        <v>648</v>
+      </c>
+      <c r="C224" t="s">
+        <v>86</v>
+      </c>
+      <c r="D224" t="s">
+        <v>24</v>
+      </c>
+      <c r="E224" t="s">
+        <v>14</v>
+      </c>
+      <c r="F224" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A225" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B225">
+        <v>649</v>
+      </c>
+      <c r="C225" t="s">
+        <v>20</v>
+      </c>
+      <c r="D225" t="s">
+        <v>25</v>
+      </c>
+      <c r="E225" t="s">
+        <v>14</v>
+      </c>
+      <c r="F225" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A226" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B226">
+        <v>650</v>
+      </c>
+      <c r="C226" t="s">
+        <v>16</v>
+      </c>
+      <c r="D226" t="s">
+        <v>88</v>
+      </c>
+      <c r="E226" t="s">
+        <v>18</v>
+      </c>
+      <c r="F226" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A227" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B227">
+        <v>651</v>
+      </c>
+      <c r="C227" t="s">
+        <v>51</v>
+      </c>
+      <c r="D227" t="s">
+        <v>25</v>
+      </c>
+      <c r="E227" t="s">
+        <v>18</v>
+      </c>
+      <c r="F227" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A228" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B228">
+        <v>652</v>
+      </c>
+      <c r="C228" t="s">
+        <v>41</v>
+      </c>
+      <c r="D228" t="s">
+        <v>84</v>
+      </c>
+      <c r="E228" t="s">
+        <v>18</v>
+      </c>
+      <c r="F228" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A229" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B229">
+        <v>653</v>
+      </c>
+      <c r="C229" t="s">
+        <v>21</v>
+      </c>
+      <c r="D229" t="s">
+        <v>24</v>
+      </c>
+      <c r="E229" t="s">
+        <v>28</v>
+      </c>
+      <c r="F229" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A230" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B230">
+        <v>654</v>
+      </c>
+      <c r="C230" t="s">
+        <v>41</v>
+      </c>
+      <c r="D230" t="s">
+        <v>24</v>
+      </c>
+      <c r="E230" t="s">
+        <v>18</v>
+      </c>
+      <c r="F230" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A231" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B231">
+        <v>655</v>
+      </c>
+      <c r="C231" t="s">
+        <v>20</v>
+      </c>
+      <c r="D231" t="s">
+        <v>24</v>
+      </c>
+      <c r="E231" t="s">
+        <v>28</v>
+      </c>
+      <c r="F231" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A232" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B232">
+        <v>656</v>
+      </c>
+      <c r="C232" t="s">
+        <v>21</v>
+      </c>
+      <c r="D232" t="s">
+        <v>24</v>
+      </c>
+      <c r="E232" t="s">
+        <v>14</v>
+      </c>
+      <c r="F232" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A233" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B233">
+        <v>657</v>
+      </c>
+      <c r="C233" t="s">
+        <v>21</v>
+      </c>
+      <c r="D233" t="s">
+        <v>25</v>
+      </c>
+      <c r="E233" t="s">
+        <v>89</v>
+      </c>
+      <c r="F233" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A234" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B234">
+        <v>658</v>
+      </c>
+      <c r="C234" t="s">
+        <v>14</v>
+      </c>
+      <c r="D234" t="s">
+        <v>14</v>
+      </c>
+      <c r="E234" t="s">
+        <v>14</v>
+      </c>
+      <c r="F234" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A235" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B235">
+        <v>659</v>
+      </c>
+      <c r="C235" t="s">
+        <v>14</v>
+      </c>
+      <c r="D235" t="s">
+        <v>14</v>
+      </c>
+      <c r="E235" t="s">
+        <v>14</v>
+      </c>
+      <c r="F235" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A236" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B236">
+        <v>660</v>
+      </c>
+      <c r="C236" t="s">
+        <v>14</v>
+      </c>
+      <c r="D236" t="s">
+        <v>14</v>
+      </c>
+      <c r="E236" t="s">
+        <v>14</v>
+      </c>
+      <c r="F236" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A237" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B237">
+        <v>661</v>
+      </c>
+      <c r="C237" t="s">
+        <v>14</v>
+      </c>
+      <c r="D237" t="s">
+        <v>14</v>
+      </c>
+      <c r="E237" t="s">
+        <v>14</v>
+      </c>
+      <c r="F237" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A238" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B238">
+        <v>662</v>
+      </c>
+      <c r="C238" t="s">
+        <v>14</v>
+      </c>
+      <c r="D238" t="s">
+        <v>14</v>
+      </c>
+      <c r="E238" t="s">
+        <v>14</v>
+      </c>
+      <c r="F238" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A239" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B239">
+        <v>663</v>
+      </c>
+      <c r="C239" t="s">
+        <v>14</v>
+      </c>
+      <c r="D239" t="s">
+        <v>14</v>
+      </c>
+      <c r="E239" t="s">
+        <v>14</v>
+      </c>
+      <c r="F239" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A240" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B240">
+        <v>664</v>
+      </c>
+      <c r="C240" t="s">
+        <v>14</v>
+      </c>
+      <c r="D240" t="s">
+        <v>14</v>
+      </c>
+      <c r="E240" t="s">
+        <v>14</v>
+      </c>
+      <c r="F240" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A241" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B241">
+        <v>665</v>
+      </c>
+      <c r="C241" t="s">
+        <v>14</v>
+      </c>
+      <c r="D241" t="s">
+        <v>14</v>
+      </c>
+      <c r="E241" t="s">
+        <v>14</v>
+      </c>
+      <c r="F241" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A242" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B242">
+        <v>666</v>
+      </c>
+      <c r="C242" t="s">
+        <v>14</v>
+      </c>
+      <c r="D242" t="s">
+        <v>14</v>
+      </c>
+      <c r="E242" t="s">
+        <v>14</v>
+      </c>
+      <c r="F242" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A243" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B243">
+        <v>667</v>
+      </c>
+      <c r="C243" t="s">
+        <v>14</v>
+      </c>
+      <c r="D243" t="s">
+        <v>14</v>
+      </c>
+      <c r="E243" t="s">
+        <v>14</v>
+      </c>
+      <c r="F243" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A244" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B244">
+        <v>668</v>
+      </c>
+      <c r="C244" t="s">
+        <v>14</v>
+      </c>
+      <c r="D244" t="s">
+        <v>14</v>
+      </c>
+      <c r="E244" t="s">
+        <v>14</v>
+      </c>
+      <c r="F244" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A245" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B245">
+        <v>669</v>
+      </c>
+      <c r="C245" t="s">
+        <v>14</v>
+      </c>
+      <c r="D245" t="s">
+        <v>14</v>
+      </c>
+      <c r="E245" t="s">
+        <v>14</v>
+      </c>
+      <c r="F245" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A246" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B246">
+        <v>670</v>
+      </c>
+      <c r="C246" t="s">
+        <v>14</v>
+      </c>
+      <c r="D246" t="s">
+        <v>14</v>
+      </c>
+      <c r="E246" t="s">
+        <v>14</v>
+      </c>
+      <c r="F246" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A247" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B247">
+        <v>671</v>
+      </c>
+      <c r="C247" t="s">
+        <v>14</v>
+      </c>
+      <c r="D247" t="s">
+        <v>14</v>
+      </c>
+      <c r="E247" t="s">
+        <v>14</v>
+      </c>
+      <c r="F247" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A248" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B248">
+        <v>672</v>
+      </c>
+      <c r="C248" t="s">
+        <v>14</v>
+      </c>
+      <c r="D248" t="s">
+        <v>14</v>
+      </c>
+      <c r="E248" t="s">
+        <v>14</v>
+      </c>
+      <c r="F248" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A249" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B249">
+        <v>673</v>
+      </c>
+      <c r="C249" t="s">
+        <v>14</v>
+      </c>
+      <c r="D249" t="s">
+        <v>14</v>
+      </c>
+      <c r="E249" t="s">
+        <v>14</v>
+      </c>
+      <c r="F249" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A250" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B250">
+        <v>674</v>
+      </c>
+      <c r="C250" t="s">
+        <v>14</v>
+      </c>
+      <c r="D250" t="s">
+        <v>14</v>
+      </c>
+      <c r="E250" t="s">
+        <v>14</v>
+      </c>
+      <c r="F250" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A251" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B251">
+        <v>675</v>
+      </c>
+      <c r="C251" t="s">
+        <v>14</v>
+      </c>
+      <c r="D251" t="s">
+        <v>14</v>
+      </c>
+      <c r="E251" t="s">
+        <v>14</v>
+      </c>
+      <c r="F251" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A252" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B252">
+        <v>676</v>
+      </c>
+      <c r="C252" t="s">
+        <v>14</v>
+      </c>
+      <c r="D252" t="s">
+        <v>14</v>
+      </c>
+      <c r="E252" t="s">
+        <v>14</v>
+      </c>
+      <c r="F252" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A253" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B253">
+        <v>677</v>
+      </c>
+      <c r="C253" t="s">
+        <v>14</v>
+      </c>
+      <c r="D253" t="s">
+        <v>14</v>
+      </c>
+      <c r="E253" t="s">
+        <v>14</v>
+      </c>
+      <c r="F253" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A254" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B254">
+        <v>678</v>
+      </c>
+      <c r="C254" t="s">
+        <v>14</v>
+      </c>
+      <c r="D254" t="s">
+        <v>14</v>
+      </c>
+      <c r="E254" t="s">
+        <v>14</v>
+      </c>
+      <c r="F254" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A255" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B255">
+        <v>679</v>
+      </c>
+      <c r="C255" t="s">
+        <v>14</v>
+      </c>
+      <c r="D255" t="s">
+        <v>14</v>
+      </c>
+      <c r="E255" t="s">
+        <v>14</v>
+      </c>
+      <c r="F255" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A256" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B256">
+        <v>680</v>
+      </c>
+      <c r="C256" t="s">
+        <v>14</v>
+      </c>
+      <c r="D256" t="s">
+        <v>14</v>
+      </c>
+      <c r="E256" t="s">
+        <v>14</v>
+      </c>
+      <c r="F256" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A257" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B257">
+        <v>681</v>
+      </c>
+      <c r="C257" t="s">
+        <v>14</v>
+      </c>
+      <c r="D257" t="s">
+        <v>14</v>
+      </c>
+      <c r="E257" t="s">
+        <v>14</v>
+      </c>
+      <c r="F257" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A258" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B258">
+        <v>682</v>
+      </c>
+      <c r="C258" t="s">
+        <v>14</v>
+      </c>
+      <c r="D258" t="s">
+        <v>14</v>
+      </c>
+      <c r="E258" t="s">
+        <v>14</v>
+      </c>
+      <c r="F258" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A259" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B259">
+        <v>683</v>
+      </c>
+      <c r="C259" t="s">
+        <v>14</v>
+      </c>
+      <c r="D259" t="s">
+        <v>14</v>
+      </c>
+      <c r="E259" t="s">
+        <v>14</v>
+      </c>
+      <c r="F259" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A260" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B260">
+        <v>684</v>
+      </c>
+      <c r="C260" t="s">
+        <v>14</v>
+      </c>
+      <c r="D260" t="s">
+        <v>14</v>
+      </c>
+      <c r="E260" t="s">
+        <v>14</v>
+      </c>
+      <c r="F260" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A261" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B261">
+        <v>685</v>
+      </c>
+      <c r="C261" t="s">
+        <v>14</v>
+      </c>
+      <c r="D261" t="s">
+        <v>14</v>
+      </c>
+      <c r="E261" t="s">
+        <v>14</v>
+      </c>
+      <c r="F261" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A262" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B262">
+        <v>686</v>
+      </c>
+      <c r="C262" t="s">
+        <v>14</v>
+      </c>
+      <c r="D262" t="s">
+        <v>14</v>
+      </c>
+      <c r="E262" t="s">
+        <v>14</v>
+      </c>
+      <c r="F262" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A263" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B263">
+        <v>687</v>
+      </c>
+      <c r="C263" t="s">
+        <v>14</v>
+      </c>
+      <c r="D263" t="s">
+        <v>14</v>
+      </c>
+      <c r="E263" t="s">
+        <v>14</v>
+      </c>
+      <c r="F263" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A264" s="2">
+        <v>43915</v>
+      </c>
+      <c r="B264">
+        <v>688</v>
+      </c>
+      <c r="C264" t="s">
+        <v>14</v>
+      </c>
+      <c r="D264" t="s">
+        <v>14</v>
+      </c>
+      <c r="E264" t="s">
+        <v>14</v>
+      </c>
+      <c r="F264" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
excel update 2020-03-25 17:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86146208-28BD-4145-9BB5-CFCE9E3E3617}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691C1B25-70F7-0046-A9C6-E00730C74DC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -661,7 +661,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -767,7 +767,31 @@
         <v>35635</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>43915.729166666664</v>
+      </c>
+      <c r="B5">
+        <v>24458</v>
+      </c>
+      <c r="C5">
+        <v>10489</v>
+      </c>
+      <c r="D5">
+        <v>667</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5">
+        <v>13</v>
+      </c>
+      <c r="G5" s="3">
+        <v>35635</v>
+      </c>
+    </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
   </sheetData>
@@ -779,7 +803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349DD023-B549-B642-9379-4C23EAB3417F}">
   <dimension ref="A1:F264"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A245" workbookViewId="0">
       <selection activeCell="A264" sqref="A264"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
excel update 2020-03-26 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691C1B25-70F7-0046-A9C6-E00730C74DC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCB8D6F-1D29-4E4D-88AC-A44B9934A5A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1065" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1745" uniqueCount="109">
   <si>
     <t>Negative1</t>
   </si>
@@ -304,6 +304,63 @@
   </si>
   <si>
     <t>travel (UK, USA)</t>
+  </si>
+  <si>
+    <t>travel (Egypt, Dubai)</t>
+  </si>
+  <si>
+    <t>travel (Germany)</t>
+  </si>
+  <si>
+    <t>travel (Denmark)</t>
+  </si>
+  <si>
+    <t>&lt; 20 Female</t>
+  </si>
+  <si>
+    <t>travel (Caribbean cruise)</t>
+  </si>
+  <si>
+    <t>travel (Cruise)</t>
+  </si>
+  <si>
+    <t>travel (Ecuador)</t>
+  </si>
+  <si>
+    <t>travel (Germany, Austria)</t>
+  </si>
+  <si>
+    <t>travel (London)</t>
+  </si>
+  <si>
+    <t>travel (Colombia)</t>
+  </si>
+  <si>
+    <t>Northwestern</t>
+  </si>
+  <si>
+    <t>travel (Dubai, Philippines)</t>
+  </si>
+  <si>
+    <t>travel (France)</t>
+  </si>
+  <si>
+    <t>20s pending</t>
+  </si>
+  <si>
+    <t>50s pending</t>
+  </si>
+  <si>
+    <t>North Bay Parry Sound</t>
+  </si>
+  <si>
+    <t>travel (Costa Rica, Spain, USA)</t>
+  </si>
+  <si>
+    <t>Oxford</t>
+  </si>
+  <si>
+    <t>Lambton</t>
   </si>
 </sst>
 </file>
@@ -658,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -717,7 +774,7 @@
       <c r="F2">
         <v>6</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>28506</v>
       </c>
     </row>
@@ -740,7 +797,7 @@
       <c r="F3">
         <v>7</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>32457</v>
       </c>
     </row>
@@ -763,7 +820,7 @@
       <c r="F4">
         <v>9</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>35635</v>
       </c>
     </row>
@@ -790,9 +847,35 @@
         <v>35635</v>
       </c>
     </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>43916.4375</v>
+      </c>
+      <c r="B6">
+        <v>26727</v>
+      </c>
+      <c r="C6">
+        <v>10965</v>
+      </c>
+      <c r="D6">
+        <v>837</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>13</v>
+      </c>
+      <c r="G6" s="3">
+        <v>38550</v>
+      </c>
+    </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E17" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -801,10 +884,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349DD023-B549-B642-9379-4C23EAB3417F}">
-  <dimension ref="A1:F264"/>
+  <dimension ref="A1:F434"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A245" workbookViewId="0">
-      <selection activeCell="A264" sqref="A264"/>
+    <sheetView tabSelected="1" topLeftCell="A391" workbookViewId="0">
+      <selection activeCell="A435" sqref="A435"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6097,6 +6180,3406 @@
         <v>14</v>
       </c>
     </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A265" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B265">
+        <v>689</v>
+      </c>
+      <c r="C265" t="s">
+        <v>41</v>
+      </c>
+      <c r="D265" t="s">
+        <v>33</v>
+      </c>
+      <c r="E265" t="s">
+        <v>63</v>
+      </c>
+      <c r="F265" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A266" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B266">
+        <v>690</v>
+      </c>
+      <c r="C266" t="s">
+        <v>37</v>
+      </c>
+      <c r="D266" t="s">
+        <v>33</v>
+      </c>
+      <c r="E266" t="s">
+        <v>90</v>
+      </c>
+      <c r="F266" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A267" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B267">
+        <v>691</v>
+      </c>
+      <c r="C267" t="s">
+        <v>29</v>
+      </c>
+      <c r="D267" t="s">
+        <v>33</v>
+      </c>
+      <c r="E267" t="s">
+        <v>14</v>
+      </c>
+      <c r="F267" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A268" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B268">
+        <v>692</v>
+      </c>
+      <c r="C268" t="s">
+        <v>41</v>
+      </c>
+      <c r="D268" t="s">
+        <v>33</v>
+      </c>
+      <c r="E268" t="s">
+        <v>63</v>
+      </c>
+      <c r="F268" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A269" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B269">
+        <v>693</v>
+      </c>
+      <c r="C269" t="s">
+        <v>29</v>
+      </c>
+      <c r="D269" t="s">
+        <v>24</v>
+      </c>
+      <c r="E269" t="s">
+        <v>18</v>
+      </c>
+      <c r="F269" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A270" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B270">
+        <v>694</v>
+      </c>
+      <c r="C270" t="s">
+        <v>37</v>
+      </c>
+      <c r="D270" t="s">
+        <v>24</v>
+      </c>
+      <c r="E270" t="s">
+        <v>91</v>
+      </c>
+      <c r="F270" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A271" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B271">
+        <v>695</v>
+      </c>
+      <c r="C271" t="s">
+        <v>41</v>
+      </c>
+      <c r="D271" t="s">
+        <v>25</v>
+      </c>
+      <c r="E271" t="s">
+        <v>14</v>
+      </c>
+      <c r="F271" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A272" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B272">
+        <v>696</v>
+      </c>
+      <c r="C272" t="s">
+        <v>50</v>
+      </c>
+      <c r="D272" t="s">
+        <v>25</v>
+      </c>
+      <c r="E272" t="s">
+        <v>14</v>
+      </c>
+      <c r="F272" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A273" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B273">
+        <v>697</v>
+      </c>
+      <c r="C273" t="s">
+        <v>50</v>
+      </c>
+      <c r="D273" t="s">
+        <v>17</v>
+      </c>
+      <c r="E273" t="s">
+        <v>92</v>
+      </c>
+      <c r="F273" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A274" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B274">
+        <v>698</v>
+      </c>
+      <c r="C274" t="s">
+        <v>93</v>
+      </c>
+      <c r="D274" t="s">
+        <v>17</v>
+      </c>
+      <c r="E274" t="s">
+        <v>18</v>
+      </c>
+      <c r="F274" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A275" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B275">
+        <v>699</v>
+      </c>
+      <c r="C275" t="s">
+        <v>29</v>
+      </c>
+      <c r="D275" t="s">
+        <v>25</v>
+      </c>
+      <c r="E275" t="s">
+        <v>66</v>
+      </c>
+      <c r="F275" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A276" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B276">
+        <v>700</v>
+      </c>
+      <c r="C276" t="s">
+        <v>16</v>
+      </c>
+      <c r="D276" t="s">
+        <v>24</v>
+      </c>
+      <c r="E276" t="s">
+        <v>14</v>
+      </c>
+      <c r="F276" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A277" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B277">
+        <v>701</v>
+      </c>
+      <c r="C277" t="s">
+        <v>16</v>
+      </c>
+      <c r="D277" t="s">
+        <v>25</v>
+      </c>
+      <c r="E277" t="s">
+        <v>14</v>
+      </c>
+      <c r="F277" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A278" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B278">
+        <v>702</v>
+      </c>
+      <c r="C278" t="s">
+        <v>21</v>
+      </c>
+      <c r="D278" t="s">
+        <v>25</v>
+      </c>
+      <c r="E278" t="s">
+        <v>14</v>
+      </c>
+      <c r="F278" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A279" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B279">
+        <v>703</v>
+      </c>
+      <c r="C279" t="s">
+        <v>41</v>
+      </c>
+      <c r="D279" t="s">
+        <v>17</v>
+      </c>
+      <c r="E279" t="s">
+        <v>28</v>
+      </c>
+      <c r="F279" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A280" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B280">
+        <v>704</v>
+      </c>
+      <c r="C280" t="s">
+        <v>26</v>
+      </c>
+      <c r="D280" t="s">
+        <v>25</v>
+      </c>
+      <c r="E280" t="s">
+        <v>28</v>
+      </c>
+      <c r="F280" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A281" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B281">
+        <v>705</v>
+      </c>
+      <c r="C281" t="s">
+        <v>52</v>
+      </c>
+      <c r="D281" t="s">
+        <v>17</v>
+      </c>
+      <c r="E281" t="s">
+        <v>18</v>
+      </c>
+      <c r="F281" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A282" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B282">
+        <v>706</v>
+      </c>
+      <c r="C282" t="s">
+        <v>16</v>
+      </c>
+      <c r="D282" t="s">
+        <v>25</v>
+      </c>
+      <c r="E282" t="s">
+        <v>18</v>
+      </c>
+      <c r="F282" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A283" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B283">
+        <v>707</v>
+      </c>
+      <c r="C283" t="s">
+        <v>86</v>
+      </c>
+      <c r="D283" t="s">
+        <v>53</v>
+      </c>
+      <c r="E283" t="s">
+        <v>18</v>
+      </c>
+      <c r="F283" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A284" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B284">
+        <v>708</v>
+      </c>
+      <c r="C284" t="s">
+        <v>16</v>
+      </c>
+      <c r="D284" t="s">
+        <v>53</v>
+      </c>
+      <c r="E284" t="s">
+        <v>18</v>
+      </c>
+      <c r="F284" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A285" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B285">
+        <v>709</v>
+      </c>
+      <c r="C285" t="s">
+        <v>52</v>
+      </c>
+      <c r="D285" t="s">
+        <v>53</v>
+      </c>
+      <c r="E285" t="s">
+        <v>14</v>
+      </c>
+      <c r="F285" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A286" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B286">
+        <v>710</v>
+      </c>
+      <c r="C286" t="s">
+        <v>16</v>
+      </c>
+      <c r="D286" t="s">
+        <v>17</v>
+      </c>
+      <c r="E286" t="s">
+        <v>28</v>
+      </c>
+      <c r="F286" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A287" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B287">
+        <v>711</v>
+      </c>
+      <c r="C287" t="s">
+        <v>47</v>
+      </c>
+      <c r="D287" t="s">
+        <v>17</v>
+      </c>
+      <c r="E287" t="s">
+        <v>14</v>
+      </c>
+      <c r="F287" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A288" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B288">
+        <v>712</v>
+      </c>
+      <c r="C288" t="s">
+        <v>37</v>
+      </c>
+      <c r="D288" t="s">
+        <v>17</v>
+      </c>
+      <c r="E288" t="s">
+        <v>14</v>
+      </c>
+      <c r="F288" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A289" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B289">
+        <v>713</v>
+      </c>
+      <c r="C289" t="s">
+        <v>29</v>
+      </c>
+      <c r="D289" t="s">
+        <v>71</v>
+      </c>
+      <c r="E289" t="s">
+        <v>94</v>
+      </c>
+      <c r="F289" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A290" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B290">
+        <v>714</v>
+      </c>
+      <c r="C290" t="s">
+        <v>23</v>
+      </c>
+      <c r="D290" t="s">
+        <v>17</v>
+      </c>
+      <c r="E290" t="s">
+        <v>28</v>
+      </c>
+      <c r="F290" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A291" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B291">
+        <v>715</v>
+      </c>
+      <c r="C291" t="s">
+        <v>23</v>
+      </c>
+      <c r="D291" t="s">
+        <v>48</v>
+      </c>
+      <c r="E291" t="s">
+        <v>14</v>
+      </c>
+      <c r="F291" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A292" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B292">
+        <v>716</v>
+      </c>
+      <c r="C292" t="s">
+        <v>26</v>
+      </c>
+      <c r="D292" t="s">
+        <v>17</v>
+      </c>
+      <c r="E292" t="s">
+        <v>18</v>
+      </c>
+      <c r="F292" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A293" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B293">
+        <v>717</v>
+      </c>
+      <c r="C293" t="s">
+        <v>47</v>
+      </c>
+      <c r="D293" t="s">
+        <v>17</v>
+      </c>
+      <c r="E293" t="s">
+        <v>18</v>
+      </c>
+      <c r="F293" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A294" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B294">
+        <v>718</v>
+      </c>
+      <c r="C294" t="s">
+        <v>20</v>
+      </c>
+      <c r="D294" t="s">
+        <v>38</v>
+      </c>
+      <c r="E294" t="s">
+        <v>28</v>
+      </c>
+      <c r="F294" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A295" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B295">
+        <v>719</v>
+      </c>
+      <c r="C295" t="s">
+        <v>20</v>
+      </c>
+      <c r="D295" t="s">
+        <v>13</v>
+      </c>
+      <c r="E295" t="s">
+        <v>18</v>
+      </c>
+      <c r="F295" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A296" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B296">
+        <v>720</v>
+      </c>
+      <c r="C296" t="s">
+        <v>21</v>
+      </c>
+      <c r="D296" t="s">
+        <v>35</v>
+      </c>
+      <c r="E296" t="s">
+        <v>28</v>
+      </c>
+      <c r="F296" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A297" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B297">
+        <v>721</v>
+      </c>
+      <c r="C297" t="s">
+        <v>41</v>
+      </c>
+      <c r="D297" t="s">
+        <v>25</v>
+      </c>
+      <c r="E297" t="s">
+        <v>14</v>
+      </c>
+      <c r="F297" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A298" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B298">
+        <v>722</v>
+      </c>
+      <c r="C298" t="s">
+        <v>41</v>
+      </c>
+      <c r="D298" t="s">
+        <v>25</v>
+      </c>
+      <c r="E298" t="s">
+        <v>14</v>
+      </c>
+      <c r="F298" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A299" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B299">
+        <v>723</v>
+      </c>
+      <c r="C299" t="s">
+        <v>52</v>
+      </c>
+      <c r="D299" t="s">
+        <v>24</v>
+      </c>
+      <c r="E299" t="s">
+        <v>14</v>
+      </c>
+      <c r="F299" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A300" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B300">
+        <v>724</v>
+      </c>
+      <c r="C300" t="s">
+        <v>20</v>
+      </c>
+      <c r="D300" t="s">
+        <v>24</v>
+      </c>
+      <c r="E300" t="s">
+        <v>43</v>
+      </c>
+      <c r="F300" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A301" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B301">
+        <v>725</v>
+      </c>
+      <c r="C301" t="s">
+        <v>23</v>
+      </c>
+      <c r="D301" t="s">
+        <v>24</v>
+      </c>
+      <c r="E301" t="s">
+        <v>28</v>
+      </c>
+      <c r="F301" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A302" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B302">
+        <v>726</v>
+      </c>
+      <c r="C302" t="s">
+        <v>93</v>
+      </c>
+      <c r="D302" t="s">
+        <v>25</v>
+      </c>
+      <c r="E302" t="s">
+        <v>14</v>
+      </c>
+      <c r="F302" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A303" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B303">
+        <v>727</v>
+      </c>
+      <c r="C303" t="s">
+        <v>37</v>
+      </c>
+      <c r="D303" t="s">
+        <v>13</v>
+      </c>
+      <c r="E303" t="s">
+        <v>87</v>
+      </c>
+      <c r="F303" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A304" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B304">
+        <v>728</v>
+      </c>
+      <c r="C304" t="s">
+        <v>52</v>
+      </c>
+      <c r="D304" t="s">
+        <v>48</v>
+      </c>
+      <c r="E304" t="s">
+        <v>28</v>
+      </c>
+      <c r="F304" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A305" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B305">
+        <v>729</v>
+      </c>
+      <c r="C305" t="s">
+        <v>20</v>
+      </c>
+      <c r="D305" t="s">
+        <v>48</v>
+      </c>
+      <c r="E305" t="s">
+        <v>95</v>
+      </c>
+      <c r="F305" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A306" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B306">
+        <v>730</v>
+      </c>
+      <c r="C306" t="s">
+        <v>51</v>
+      </c>
+      <c r="D306" t="s">
+        <v>48</v>
+      </c>
+      <c r="E306" t="s">
+        <v>18</v>
+      </c>
+      <c r="F306" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A307" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B307">
+        <v>731</v>
+      </c>
+      <c r="C307" t="s">
+        <v>16</v>
+      </c>
+      <c r="D307" t="s">
+        <v>24</v>
+      </c>
+      <c r="E307" t="s">
+        <v>18</v>
+      </c>
+      <c r="F307" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A308" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B308">
+        <v>732</v>
+      </c>
+      <c r="C308" t="s">
+        <v>26</v>
+      </c>
+      <c r="D308" t="s">
+        <v>25</v>
+      </c>
+      <c r="E308" t="s">
+        <v>96</v>
+      </c>
+      <c r="F308" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A309" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B309">
+        <v>733</v>
+      </c>
+      <c r="C309" t="s">
+        <v>20</v>
+      </c>
+      <c r="D309" t="s">
+        <v>17</v>
+      </c>
+      <c r="E309" t="s">
+        <v>97</v>
+      </c>
+      <c r="F309" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A310" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B310">
+        <v>734</v>
+      </c>
+      <c r="C310" t="s">
+        <v>41</v>
+      </c>
+      <c r="D310" t="s">
+        <v>17</v>
+      </c>
+      <c r="E310" t="s">
+        <v>98</v>
+      </c>
+      <c r="F310" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A311" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B311">
+        <v>735</v>
+      </c>
+      <c r="C311" t="s">
+        <v>26</v>
+      </c>
+      <c r="D311" t="s">
+        <v>17</v>
+      </c>
+      <c r="E311" t="s">
+        <v>64</v>
+      </c>
+      <c r="F311" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A312" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B312">
+        <v>736</v>
+      </c>
+      <c r="C312" t="s">
+        <v>50</v>
+      </c>
+      <c r="D312" t="s">
+        <v>84</v>
+      </c>
+      <c r="E312" t="s">
+        <v>99</v>
+      </c>
+      <c r="F312" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A313" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B313">
+        <v>737</v>
+      </c>
+      <c r="C313" t="s">
+        <v>50</v>
+      </c>
+      <c r="D313" t="s">
+        <v>100</v>
+      </c>
+      <c r="E313" t="s">
+        <v>99</v>
+      </c>
+      <c r="F313" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A314" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B314">
+        <v>738</v>
+      </c>
+      <c r="C314" t="s">
+        <v>52</v>
+      </c>
+      <c r="D314" t="s">
+        <v>24</v>
+      </c>
+      <c r="E314" t="s">
+        <v>101</v>
+      </c>
+      <c r="F314" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A315" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B315">
+        <v>739</v>
+      </c>
+      <c r="C315" t="s">
+        <v>26</v>
+      </c>
+      <c r="D315" t="s">
+        <v>24</v>
+      </c>
+      <c r="E315" t="s">
+        <v>14</v>
+      </c>
+      <c r="F315" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A316" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B316">
+        <v>740</v>
+      </c>
+      <c r="C316" t="s">
+        <v>23</v>
+      </c>
+      <c r="D316" t="s">
+        <v>25</v>
+      </c>
+      <c r="E316" t="s">
+        <v>102</v>
+      </c>
+      <c r="F316" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A317" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B317">
+        <v>741</v>
+      </c>
+      <c r="C317" t="s">
+        <v>23</v>
+      </c>
+      <c r="D317" t="s">
+        <v>38</v>
+      </c>
+      <c r="E317" t="s">
+        <v>18</v>
+      </c>
+      <c r="F317" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A318" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B318">
+        <v>742</v>
+      </c>
+      <c r="C318" t="s">
+        <v>23</v>
+      </c>
+      <c r="D318" t="s">
+        <v>24</v>
+      </c>
+      <c r="E318" t="s">
+        <v>18</v>
+      </c>
+      <c r="F318" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A319" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B319">
+        <v>743</v>
+      </c>
+      <c r="C319" t="s">
+        <v>51</v>
+      </c>
+      <c r="D319" t="s">
+        <v>13</v>
+      </c>
+      <c r="E319" t="s">
+        <v>18</v>
+      </c>
+      <c r="F319" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A320" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B320">
+        <v>744</v>
+      </c>
+      <c r="C320" t="s">
+        <v>57</v>
+      </c>
+      <c r="D320" t="s">
+        <v>13</v>
+      </c>
+      <c r="E320" t="s">
+        <v>87</v>
+      </c>
+      <c r="F320" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A321" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B321">
+        <v>745</v>
+      </c>
+      <c r="C321" t="s">
+        <v>86</v>
+      </c>
+      <c r="D321" t="s">
+        <v>24</v>
+      </c>
+      <c r="E321" t="s">
+        <v>102</v>
+      </c>
+      <c r="F321" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A322" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B322">
+        <v>746</v>
+      </c>
+      <c r="C322" t="s">
+        <v>16</v>
+      </c>
+      <c r="D322" t="s">
+        <v>17</v>
+      </c>
+      <c r="E322" t="s">
+        <v>18</v>
+      </c>
+      <c r="F322" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="323" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A323" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B323">
+        <v>747</v>
+      </c>
+      <c r="C323" t="s">
+        <v>52</v>
+      </c>
+      <c r="D323" t="s">
+        <v>17</v>
+      </c>
+      <c r="E323" t="s">
+        <v>14</v>
+      </c>
+      <c r="F323" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A324" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B324">
+        <v>748</v>
+      </c>
+      <c r="C324" t="s">
+        <v>26</v>
+      </c>
+      <c r="D324" t="s">
+        <v>24</v>
+      </c>
+      <c r="E324" t="s">
+        <v>14</v>
+      </c>
+      <c r="F324" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A325" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B325">
+        <v>749</v>
+      </c>
+      <c r="C325" t="s">
+        <v>103</v>
+      </c>
+      <c r="D325" t="s">
+        <v>25</v>
+      </c>
+      <c r="E325" t="s">
+        <v>14</v>
+      </c>
+      <c r="F325" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A326" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B326">
+        <v>750</v>
+      </c>
+      <c r="C326" t="s">
+        <v>27</v>
+      </c>
+      <c r="D326" t="s">
+        <v>25</v>
+      </c>
+      <c r="E326" t="s">
+        <v>18</v>
+      </c>
+      <c r="F326" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A327" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B327">
+        <v>751</v>
+      </c>
+      <c r="C327" t="s">
+        <v>16</v>
+      </c>
+      <c r="D327" t="s">
+        <v>17</v>
+      </c>
+      <c r="E327" t="s">
+        <v>18</v>
+      </c>
+      <c r="F327" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A328" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B328">
+        <v>752</v>
+      </c>
+      <c r="C328" t="s">
+        <v>21</v>
+      </c>
+      <c r="D328" t="s">
+        <v>25</v>
+      </c>
+      <c r="E328" t="s">
+        <v>18</v>
+      </c>
+      <c r="F328" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A329" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B329">
+        <v>753</v>
+      </c>
+      <c r="C329" t="s">
+        <v>21</v>
+      </c>
+      <c r="D329" t="s">
+        <v>25</v>
+      </c>
+      <c r="E329" t="s">
+        <v>18</v>
+      </c>
+      <c r="F329" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A330" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B330">
+        <v>754</v>
+      </c>
+      <c r="C330" t="s">
+        <v>16</v>
+      </c>
+      <c r="D330" t="s">
+        <v>25</v>
+      </c>
+      <c r="E330" t="s">
+        <v>18</v>
+      </c>
+      <c r="F330" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A331" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B331">
+        <v>755</v>
+      </c>
+      <c r="C331" t="s">
+        <v>20</v>
+      </c>
+      <c r="D331" t="s">
+        <v>17</v>
+      </c>
+      <c r="E331" t="s">
+        <v>18</v>
+      </c>
+      <c r="F331" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A332" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B332">
+        <v>756</v>
+      </c>
+      <c r="C332" t="s">
+        <v>20</v>
+      </c>
+      <c r="D332" t="s">
+        <v>17</v>
+      </c>
+      <c r="E332" t="s">
+        <v>18</v>
+      </c>
+      <c r="F332" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A333" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B333">
+        <v>757</v>
+      </c>
+      <c r="C333" t="s">
+        <v>20</v>
+      </c>
+      <c r="D333" t="s">
+        <v>17</v>
+      </c>
+      <c r="E333" t="s">
+        <v>14</v>
+      </c>
+      <c r="F333" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A334" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B334">
+        <v>758</v>
+      </c>
+      <c r="C334" t="s">
+        <v>21</v>
+      </c>
+      <c r="D334" t="s">
+        <v>17</v>
+      </c>
+      <c r="E334" t="s">
+        <v>18</v>
+      </c>
+      <c r="F334" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A335" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B335">
+        <v>759</v>
+      </c>
+      <c r="C335" t="s">
+        <v>41</v>
+      </c>
+      <c r="D335" t="s">
+        <v>17</v>
+      </c>
+      <c r="E335" t="s">
+        <v>18</v>
+      </c>
+      <c r="F335" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A336" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B336">
+        <v>760</v>
+      </c>
+      <c r="C336" t="s">
+        <v>51</v>
+      </c>
+      <c r="D336" t="s">
+        <v>25</v>
+      </c>
+      <c r="E336" t="s">
+        <v>14</v>
+      </c>
+      <c r="F336" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A337" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B337">
+        <v>761</v>
+      </c>
+      <c r="C337" t="s">
+        <v>41</v>
+      </c>
+      <c r="D337" t="s">
+        <v>48</v>
+      </c>
+      <c r="E337" t="s">
+        <v>14</v>
+      </c>
+      <c r="F337" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A338" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B338">
+        <v>762</v>
+      </c>
+      <c r="C338" t="s">
+        <v>12</v>
+      </c>
+      <c r="D338" t="s">
+        <v>17</v>
+      </c>
+      <c r="E338" t="s">
+        <v>14</v>
+      </c>
+      <c r="F338" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A339" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B339">
+        <v>763</v>
+      </c>
+      <c r="C339" t="s">
+        <v>23</v>
+      </c>
+      <c r="D339" t="s">
+        <v>17</v>
+      </c>
+      <c r="E339" t="s">
+        <v>18</v>
+      </c>
+      <c r="F339" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A340" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B340">
+        <v>764</v>
+      </c>
+      <c r="C340" t="s">
+        <v>37</v>
+      </c>
+      <c r="D340" t="s">
+        <v>17</v>
+      </c>
+      <c r="E340" t="s">
+        <v>18</v>
+      </c>
+      <c r="F340" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A341" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B341">
+        <v>765</v>
+      </c>
+      <c r="C341" t="s">
+        <v>16</v>
+      </c>
+      <c r="D341" t="s">
+        <v>79</v>
+      </c>
+      <c r="E341" t="s">
+        <v>18</v>
+      </c>
+      <c r="F341" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A342" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B342">
+        <v>766</v>
+      </c>
+      <c r="C342" t="s">
+        <v>47</v>
+      </c>
+      <c r="D342" t="s">
+        <v>24</v>
+      </c>
+      <c r="E342" t="s">
+        <v>14</v>
+      </c>
+      <c r="F342" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A343" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B343">
+        <v>767</v>
+      </c>
+      <c r="C343" t="s">
+        <v>57</v>
+      </c>
+      <c r="D343" t="s">
+        <v>17</v>
+      </c>
+      <c r="E343" t="s">
+        <v>18</v>
+      </c>
+      <c r="F343" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A344" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B344">
+        <v>768</v>
+      </c>
+      <c r="C344" t="s">
+        <v>23</v>
+      </c>
+      <c r="D344" t="s">
+        <v>38</v>
+      </c>
+      <c r="E344" t="s">
+        <v>18</v>
+      </c>
+      <c r="F344" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A345" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B345">
+        <v>769</v>
+      </c>
+      <c r="C345" t="s">
+        <v>41</v>
+      </c>
+      <c r="D345" t="s">
+        <v>17</v>
+      </c>
+      <c r="E345" t="s">
+        <v>74</v>
+      </c>
+      <c r="F345" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A346" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B346">
+        <v>770</v>
+      </c>
+      <c r="C346" t="s">
+        <v>26</v>
+      </c>
+      <c r="D346" t="s">
+        <v>25</v>
+      </c>
+      <c r="E346" t="s">
+        <v>18</v>
+      </c>
+      <c r="F346" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A347" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B347">
+        <v>771</v>
+      </c>
+      <c r="C347" t="s">
+        <v>50</v>
+      </c>
+      <c r="D347" t="s">
+        <v>25</v>
+      </c>
+      <c r="E347" t="s">
+        <v>74</v>
+      </c>
+      <c r="F347" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A348" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B348">
+        <v>772</v>
+      </c>
+      <c r="C348" t="s">
+        <v>26</v>
+      </c>
+      <c r="D348" t="s">
+        <v>13</v>
+      </c>
+      <c r="E348" t="s">
+        <v>18</v>
+      </c>
+      <c r="F348" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A349" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B349">
+        <v>773</v>
+      </c>
+      <c r="C349" t="s">
+        <v>26</v>
+      </c>
+      <c r="D349" t="s">
+        <v>13</v>
+      </c>
+      <c r="E349" t="s">
+        <v>18</v>
+      </c>
+      <c r="F349" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A350" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B350">
+        <v>774</v>
+      </c>
+      <c r="C350" t="s">
+        <v>37</v>
+      </c>
+      <c r="D350" t="s">
+        <v>13</v>
+      </c>
+      <c r="E350" t="s">
+        <v>18</v>
+      </c>
+      <c r="F350" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A351" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B351">
+        <v>775</v>
+      </c>
+      <c r="C351" t="s">
+        <v>52</v>
+      </c>
+      <c r="D351" t="s">
+        <v>13</v>
+      </c>
+      <c r="E351" t="s">
+        <v>18</v>
+      </c>
+      <c r="F351" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A352" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B352">
+        <v>776</v>
+      </c>
+      <c r="C352" t="s">
+        <v>52</v>
+      </c>
+      <c r="D352" t="s">
+        <v>13</v>
+      </c>
+      <c r="E352" t="s">
+        <v>18</v>
+      </c>
+      <c r="F352" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A353" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B353">
+        <v>777</v>
+      </c>
+      <c r="C353" t="s">
+        <v>37</v>
+      </c>
+      <c r="D353" t="s">
+        <v>13</v>
+      </c>
+      <c r="E353" t="s">
+        <v>18</v>
+      </c>
+      <c r="F353" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A354" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B354">
+        <v>778</v>
+      </c>
+      <c r="C354" t="s">
+        <v>37</v>
+      </c>
+      <c r="D354" t="s">
+        <v>13</v>
+      </c>
+      <c r="E354" t="s">
+        <v>18</v>
+      </c>
+      <c r="F354" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A355" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B355">
+        <v>779</v>
+      </c>
+      <c r="C355" t="s">
+        <v>37</v>
+      </c>
+      <c r="D355" t="s">
+        <v>13</v>
+      </c>
+      <c r="E355" t="s">
+        <v>18</v>
+      </c>
+      <c r="F355" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A356" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B356">
+        <v>780</v>
+      </c>
+      <c r="C356" t="s">
+        <v>29</v>
+      </c>
+      <c r="D356" t="s">
+        <v>13</v>
+      </c>
+      <c r="E356" t="s">
+        <v>18</v>
+      </c>
+      <c r="F356" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A357" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B357">
+        <v>781</v>
+      </c>
+      <c r="C357" t="s">
+        <v>29</v>
+      </c>
+      <c r="D357" t="s">
+        <v>13</v>
+      </c>
+      <c r="E357" t="s">
+        <v>18</v>
+      </c>
+      <c r="F357" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A358" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B358">
+        <v>782</v>
+      </c>
+      <c r="C358" t="s">
+        <v>55</v>
+      </c>
+      <c r="D358" t="s">
+        <v>25</v>
+      </c>
+      <c r="E358" t="s">
+        <v>14</v>
+      </c>
+      <c r="F358" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A359" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B359">
+        <v>783</v>
+      </c>
+      <c r="C359" t="s">
+        <v>104</v>
+      </c>
+      <c r="D359" t="s">
+        <v>69</v>
+      </c>
+      <c r="E359" t="s">
+        <v>18</v>
+      </c>
+      <c r="F359" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="360" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A360" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B360">
+        <v>784</v>
+      </c>
+      <c r="C360" t="s">
+        <v>21</v>
+      </c>
+      <c r="D360" t="s">
+        <v>17</v>
+      </c>
+      <c r="E360" t="s">
+        <v>18</v>
+      </c>
+      <c r="F360" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="361" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A361" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B361">
+        <v>785</v>
+      </c>
+      <c r="C361" t="s">
+        <v>52</v>
+      </c>
+      <c r="D361" t="s">
+        <v>17</v>
+      </c>
+      <c r="E361" t="s">
+        <v>14</v>
+      </c>
+      <c r="F361" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="362" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A362" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B362">
+        <v>786</v>
+      </c>
+      <c r="C362" t="s">
+        <v>23</v>
+      </c>
+      <c r="D362" t="s">
+        <v>17</v>
+      </c>
+      <c r="E362" t="s">
+        <v>18</v>
+      </c>
+      <c r="F362" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="363" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A363" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B363">
+        <v>787</v>
+      </c>
+      <c r="C363" t="s">
+        <v>26</v>
+      </c>
+      <c r="D363" t="s">
+        <v>24</v>
+      </c>
+      <c r="E363" t="s">
+        <v>18</v>
+      </c>
+      <c r="F363" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="364" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A364" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B364">
+        <v>788</v>
+      </c>
+      <c r="C364" t="s">
+        <v>37</v>
+      </c>
+      <c r="D364" t="s">
+        <v>24</v>
+      </c>
+      <c r="E364" t="s">
+        <v>28</v>
+      </c>
+      <c r="F364" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="365" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A365" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B365">
+        <v>789</v>
+      </c>
+      <c r="C365" t="s">
+        <v>37</v>
+      </c>
+      <c r="D365" t="s">
+        <v>105</v>
+      </c>
+      <c r="E365" t="s">
+        <v>87</v>
+      </c>
+      <c r="F365" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="366" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A366" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B366">
+        <v>790</v>
+      </c>
+      <c r="C366" t="s">
+        <v>21</v>
+      </c>
+      <c r="D366" t="s">
+        <v>17</v>
+      </c>
+      <c r="E366" t="s">
+        <v>102</v>
+      </c>
+      <c r="F366" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="367" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A367" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B367">
+        <v>791</v>
+      </c>
+      <c r="C367" t="s">
+        <v>86</v>
+      </c>
+      <c r="D367" t="s">
+        <v>17</v>
+      </c>
+      <c r="E367" t="s">
+        <v>18</v>
+      </c>
+      <c r="F367" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="368" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A368" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B368">
+        <v>792</v>
+      </c>
+      <c r="C368" t="s">
+        <v>29</v>
+      </c>
+      <c r="D368" t="s">
+        <v>17</v>
+      </c>
+      <c r="E368" t="s">
+        <v>18</v>
+      </c>
+      <c r="F368" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A369" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B369">
+        <v>793</v>
+      </c>
+      <c r="C369" t="s">
+        <v>52</v>
+      </c>
+      <c r="D369" t="s">
+        <v>17</v>
+      </c>
+      <c r="E369" t="s">
+        <v>18</v>
+      </c>
+      <c r="F369" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A370" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B370">
+        <v>794</v>
+      </c>
+      <c r="C370" t="s">
+        <v>50</v>
+      </c>
+      <c r="D370" t="s">
+        <v>17</v>
+      </c>
+      <c r="E370" t="s">
+        <v>18</v>
+      </c>
+      <c r="F370" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A371" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B371">
+        <v>795</v>
+      </c>
+      <c r="C371" t="s">
+        <v>26</v>
+      </c>
+      <c r="D371" t="s">
+        <v>38</v>
+      </c>
+      <c r="E371" t="s">
+        <v>58</v>
+      </c>
+      <c r="F371" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="372" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A372" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B372">
+        <v>796</v>
+      </c>
+      <c r="C372" t="s">
+        <v>50</v>
+      </c>
+      <c r="D372" t="s">
+        <v>30</v>
+      </c>
+      <c r="E372" t="s">
+        <v>18</v>
+      </c>
+      <c r="F372" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A373" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B373">
+        <v>797</v>
+      </c>
+      <c r="C373" t="s">
+        <v>60</v>
+      </c>
+      <c r="D373" t="s">
+        <v>25</v>
+      </c>
+      <c r="E373" t="s">
+        <v>14</v>
+      </c>
+      <c r="F373" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A374" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B374">
+        <v>798</v>
+      </c>
+      <c r="C374" t="s">
+        <v>50</v>
+      </c>
+      <c r="D374" t="s">
+        <v>71</v>
+      </c>
+      <c r="E374" t="s">
+        <v>106</v>
+      </c>
+      <c r="F374" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A375" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B375">
+        <v>799</v>
+      </c>
+      <c r="C375" t="s">
+        <v>51</v>
+      </c>
+      <c r="D375" t="s">
+        <v>46</v>
+      </c>
+      <c r="E375" t="s">
+        <v>14</v>
+      </c>
+      <c r="F375" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A376" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B376">
+        <v>800</v>
+      </c>
+      <c r="C376" t="s">
+        <v>50</v>
+      </c>
+      <c r="D376" t="s">
+        <v>79</v>
+      </c>
+      <c r="E376" t="s">
+        <v>14</v>
+      </c>
+      <c r="F376" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A377" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B377">
+        <v>801</v>
+      </c>
+      <c r="C377" t="s">
+        <v>16</v>
+      </c>
+      <c r="D377" t="s">
+        <v>79</v>
+      </c>
+      <c r="E377" t="s">
+        <v>18</v>
+      </c>
+      <c r="F377" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A378" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B378">
+        <v>802</v>
+      </c>
+      <c r="C378" t="s">
+        <v>26</v>
+      </c>
+      <c r="D378" t="s">
+        <v>107</v>
+      </c>
+      <c r="E378" t="s">
+        <v>18</v>
+      </c>
+      <c r="F378" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A379" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B379">
+        <v>803</v>
+      </c>
+      <c r="C379" t="s">
+        <v>26</v>
+      </c>
+      <c r="D379" t="s">
+        <v>79</v>
+      </c>
+      <c r="E379" t="s">
+        <v>28</v>
+      </c>
+      <c r="F379" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A380" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B380">
+        <v>804</v>
+      </c>
+      <c r="C380" t="s">
+        <v>16</v>
+      </c>
+      <c r="D380" t="s">
+        <v>107</v>
+      </c>
+      <c r="E380" t="s">
+        <v>18</v>
+      </c>
+      <c r="F380" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A381" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B381">
+        <v>805</v>
+      </c>
+      <c r="C381" t="s">
+        <v>12</v>
+      </c>
+      <c r="D381" t="s">
+        <v>108</v>
+      </c>
+      <c r="E381" t="s">
+        <v>14</v>
+      </c>
+      <c r="F381" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A382" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B382">
+        <v>806</v>
+      </c>
+      <c r="C382" t="s">
+        <v>37</v>
+      </c>
+      <c r="D382" t="s">
+        <v>108</v>
+      </c>
+      <c r="E382" t="s">
+        <v>14</v>
+      </c>
+      <c r="F382" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A383" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B383">
+        <v>807</v>
+      </c>
+      <c r="C383" t="s">
+        <v>47</v>
+      </c>
+      <c r="D383" t="s">
+        <v>108</v>
+      </c>
+      <c r="E383" t="s">
+        <v>14</v>
+      </c>
+      <c r="F383" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A384" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B384">
+        <v>808</v>
+      </c>
+      <c r="C384" t="s">
+        <v>57</v>
+      </c>
+      <c r="D384" t="s">
+        <v>108</v>
+      </c>
+      <c r="E384" t="s">
+        <v>18</v>
+      </c>
+      <c r="F384" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A385" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B385">
+        <v>809</v>
+      </c>
+      <c r="C385" t="s">
+        <v>12</v>
+      </c>
+      <c r="D385" t="s">
+        <v>108</v>
+      </c>
+      <c r="E385" t="s">
+        <v>14</v>
+      </c>
+      <c r="F385" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A386" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B386">
+        <v>810</v>
+      </c>
+      <c r="C386" t="s">
+        <v>47</v>
+      </c>
+      <c r="D386" t="s">
+        <v>33</v>
+      </c>
+      <c r="E386" t="s">
+        <v>18</v>
+      </c>
+      <c r="F386" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A387" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B387">
+        <v>811</v>
+      </c>
+      <c r="C387" t="s">
+        <v>37</v>
+      </c>
+      <c r="D387" t="s">
+        <v>84</v>
+      </c>
+      <c r="E387" t="s">
+        <v>18</v>
+      </c>
+      <c r="F387" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="388" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A388" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B388">
+        <v>812</v>
+      </c>
+      <c r="C388" t="s">
+        <v>52</v>
+      </c>
+      <c r="D388" t="s">
+        <v>84</v>
+      </c>
+      <c r="E388" t="s">
+        <v>18</v>
+      </c>
+      <c r="F388" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="389" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A389" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B389">
+        <v>813</v>
+      </c>
+      <c r="C389" t="s">
+        <v>14</v>
+      </c>
+      <c r="D389" t="s">
+        <v>14</v>
+      </c>
+      <c r="E389" t="s">
+        <v>14</v>
+      </c>
+      <c r="F389" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A390" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B390">
+        <v>814</v>
+      </c>
+      <c r="C390" t="s">
+        <v>14</v>
+      </c>
+      <c r="D390" t="s">
+        <v>14</v>
+      </c>
+      <c r="E390" t="s">
+        <v>14</v>
+      </c>
+      <c r="F390" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A391" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B391">
+        <v>815</v>
+      </c>
+      <c r="C391" t="s">
+        <v>14</v>
+      </c>
+      <c r="D391" t="s">
+        <v>14</v>
+      </c>
+      <c r="E391" t="s">
+        <v>14</v>
+      </c>
+      <c r="F391" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="392" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A392" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B392">
+        <v>816</v>
+      </c>
+      <c r="C392" t="s">
+        <v>14</v>
+      </c>
+      <c r="D392" t="s">
+        <v>14</v>
+      </c>
+      <c r="E392" t="s">
+        <v>14</v>
+      </c>
+      <c r="F392" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="393" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A393" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B393">
+        <v>817</v>
+      </c>
+      <c r="C393" t="s">
+        <v>14</v>
+      </c>
+      <c r="D393" t="s">
+        <v>14</v>
+      </c>
+      <c r="E393" t="s">
+        <v>14</v>
+      </c>
+      <c r="F393" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="394" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A394" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B394">
+        <v>818</v>
+      </c>
+      <c r="C394" t="s">
+        <v>14</v>
+      </c>
+      <c r="D394" t="s">
+        <v>14</v>
+      </c>
+      <c r="E394" t="s">
+        <v>14</v>
+      </c>
+      <c r="F394" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="395" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A395" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B395">
+        <v>819</v>
+      </c>
+      <c r="C395" t="s">
+        <v>14</v>
+      </c>
+      <c r="D395" t="s">
+        <v>14</v>
+      </c>
+      <c r="E395" t="s">
+        <v>14</v>
+      </c>
+      <c r="F395" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="396" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A396" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B396">
+        <v>820</v>
+      </c>
+      <c r="C396" t="s">
+        <v>14</v>
+      </c>
+      <c r="D396" t="s">
+        <v>14</v>
+      </c>
+      <c r="E396" t="s">
+        <v>14</v>
+      </c>
+      <c r="F396" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="397" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A397" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B397">
+        <v>821</v>
+      </c>
+      <c r="C397" t="s">
+        <v>14</v>
+      </c>
+      <c r="D397" t="s">
+        <v>14</v>
+      </c>
+      <c r="E397" t="s">
+        <v>14</v>
+      </c>
+      <c r="F397" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="398" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A398" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B398">
+        <v>822</v>
+      </c>
+      <c r="C398" t="s">
+        <v>14</v>
+      </c>
+      <c r="D398" t="s">
+        <v>14</v>
+      </c>
+      <c r="E398" t="s">
+        <v>14</v>
+      </c>
+      <c r="F398" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="399" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A399" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B399">
+        <v>823</v>
+      </c>
+      <c r="C399" t="s">
+        <v>14</v>
+      </c>
+      <c r="D399" t="s">
+        <v>14</v>
+      </c>
+      <c r="E399" t="s">
+        <v>14</v>
+      </c>
+      <c r="F399" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="400" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A400" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B400">
+        <v>824</v>
+      </c>
+      <c r="C400" t="s">
+        <v>14</v>
+      </c>
+      <c r="D400" t="s">
+        <v>14</v>
+      </c>
+      <c r="E400" t="s">
+        <v>14</v>
+      </c>
+      <c r="F400" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="401" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A401" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B401">
+        <v>825</v>
+      </c>
+      <c r="C401" t="s">
+        <v>14</v>
+      </c>
+      <c r="D401" t="s">
+        <v>14</v>
+      </c>
+      <c r="E401" t="s">
+        <v>14</v>
+      </c>
+      <c r="F401" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="402" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A402" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B402">
+        <v>826</v>
+      </c>
+      <c r="C402" t="s">
+        <v>14</v>
+      </c>
+      <c r="D402" t="s">
+        <v>14</v>
+      </c>
+      <c r="E402" t="s">
+        <v>14</v>
+      </c>
+      <c r="F402" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="403" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A403" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B403">
+        <v>827</v>
+      </c>
+      <c r="C403" t="s">
+        <v>14</v>
+      </c>
+      <c r="D403" t="s">
+        <v>14</v>
+      </c>
+      <c r="E403" t="s">
+        <v>14</v>
+      </c>
+      <c r="F403" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="404" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A404" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B404">
+        <v>828</v>
+      </c>
+      <c r="C404" t="s">
+        <v>14</v>
+      </c>
+      <c r="D404" t="s">
+        <v>14</v>
+      </c>
+      <c r="E404" t="s">
+        <v>14</v>
+      </c>
+      <c r="F404" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="405" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A405" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B405">
+        <v>829</v>
+      </c>
+      <c r="C405" t="s">
+        <v>14</v>
+      </c>
+      <c r="D405" t="s">
+        <v>14</v>
+      </c>
+      <c r="E405" t="s">
+        <v>14</v>
+      </c>
+      <c r="F405" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="406" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A406" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B406">
+        <v>830</v>
+      </c>
+      <c r="C406" t="s">
+        <v>14</v>
+      </c>
+      <c r="D406" t="s">
+        <v>14</v>
+      </c>
+      <c r="E406" t="s">
+        <v>14</v>
+      </c>
+      <c r="F406" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="407" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A407" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B407">
+        <v>831</v>
+      </c>
+      <c r="C407" t="s">
+        <v>14</v>
+      </c>
+      <c r="D407" t="s">
+        <v>14</v>
+      </c>
+      <c r="E407" t="s">
+        <v>14</v>
+      </c>
+      <c r="F407" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="408" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A408" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B408">
+        <v>832</v>
+      </c>
+      <c r="C408" t="s">
+        <v>14</v>
+      </c>
+      <c r="D408" t="s">
+        <v>14</v>
+      </c>
+      <c r="E408" t="s">
+        <v>14</v>
+      </c>
+      <c r="F408" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="409" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A409" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B409">
+        <v>833</v>
+      </c>
+      <c r="C409" t="s">
+        <v>14</v>
+      </c>
+      <c r="D409" t="s">
+        <v>14</v>
+      </c>
+      <c r="E409" t="s">
+        <v>14</v>
+      </c>
+      <c r="F409" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="410" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A410" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B410">
+        <v>834</v>
+      </c>
+      <c r="C410" t="s">
+        <v>14</v>
+      </c>
+      <c r="D410" t="s">
+        <v>14</v>
+      </c>
+      <c r="E410" t="s">
+        <v>14</v>
+      </c>
+      <c r="F410" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="411" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A411" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B411">
+        <v>835</v>
+      </c>
+      <c r="C411" t="s">
+        <v>14</v>
+      </c>
+      <c r="D411" t="s">
+        <v>14</v>
+      </c>
+      <c r="E411" t="s">
+        <v>14</v>
+      </c>
+      <c r="F411" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="412" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A412" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B412">
+        <v>836</v>
+      </c>
+      <c r="C412" t="s">
+        <v>14</v>
+      </c>
+      <c r="D412" t="s">
+        <v>14</v>
+      </c>
+      <c r="E412" t="s">
+        <v>14</v>
+      </c>
+      <c r="F412" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="413" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A413" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B413">
+        <v>837</v>
+      </c>
+      <c r="C413" t="s">
+        <v>14</v>
+      </c>
+      <c r="D413" t="s">
+        <v>14</v>
+      </c>
+      <c r="E413" t="s">
+        <v>14</v>
+      </c>
+      <c r="F413" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="414" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A414" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B414">
+        <v>838</v>
+      </c>
+      <c r="C414" t="s">
+        <v>14</v>
+      </c>
+      <c r="D414" t="s">
+        <v>14</v>
+      </c>
+      <c r="E414" t="s">
+        <v>14</v>
+      </c>
+      <c r="F414" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="415" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A415" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B415">
+        <v>839</v>
+      </c>
+      <c r="C415" t="s">
+        <v>14</v>
+      </c>
+      <c r="D415" t="s">
+        <v>14</v>
+      </c>
+      <c r="E415" t="s">
+        <v>14</v>
+      </c>
+      <c r="F415" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="416" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A416" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B416">
+        <v>840</v>
+      </c>
+      <c r="C416" t="s">
+        <v>14</v>
+      </c>
+      <c r="D416" t="s">
+        <v>14</v>
+      </c>
+      <c r="E416" t="s">
+        <v>14</v>
+      </c>
+      <c r="F416" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="417" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A417" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B417">
+        <v>841</v>
+      </c>
+      <c r="C417" t="s">
+        <v>14</v>
+      </c>
+      <c r="D417" t="s">
+        <v>14</v>
+      </c>
+      <c r="E417" t="s">
+        <v>14</v>
+      </c>
+      <c r="F417" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="418" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A418" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B418">
+        <v>842</v>
+      </c>
+      <c r="C418" t="s">
+        <v>14</v>
+      </c>
+      <c r="D418" t="s">
+        <v>14</v>
+      </c>
+      <c r="E418" t="s">
+        <v>14</v>
+      </c>
+      <c r="F418" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="419" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A419" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B419">
+        <v>843</v>
+      </c>
+      <c r="C419" t="s">
+        <v>14</v>
+      </c>
+      <c r="D419" t="s">
+        <v>14</v>
+      </c>
+      <c r="E419" t="s">
+        <v>14</v>
+      </c>
+      <c r="F419" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="420" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A420" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B420">
+        <v>844</v>
+      </c>
+      <c r="C420" t="s">
+        <v>14</v>
+      </c>
+      <c r="D420" t="s">
+        <v>14</v>
+      </c>
+      <c r="E420" t="s">
+        <v>14</v>
+      </c>
+      <c r="F420" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="421" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A421" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B421">
+        <v>845</v>
+      </c>
+      <c r="C421" t="s">
+        <v>14</v>
+      </c>
+      <c r="D421" t="s">
+        <v>14</v>
+      </c>
+      <c r="E421" t="s">
+        <v>14</v>
+      </c>
+      <c r="F421" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="422" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A422" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B422">
+        <v>846</v>
+      </c>
+      <c r="C422" t="s">
+        <v>14</v>
+      </c>
+      <c r="D422" t="s">
+        <v>14</v>
+      </c>
+      <c r="E422" t="s">
+        <v>14</v>
+      </c>
+      <c r="F422" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="423" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A423" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B423">
+        <v>847</v>
+      </c>
+      <c r="C423" t="s">
+        <v>14</v>
+      </c>
+      <c r="D423" t="s">
+        <v>14</v>
+      </c>
+      <c r="E423" t="s">
+        <v>14</v>
+      </c>
+      <c r="F423" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="424" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A424" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B424">
+        <v>848</v>
+      </c>
+      <c r="C424" t="s">
+        <v>14</v>
+      </c>
+      <c r="D424" t="s">
+        <v>14</v>
+      </c>
+      <c r="E424" t="s">
+        <v>14</v>
+      </c>
+      <c r="F424" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="425" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A425" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B425">
+        <v>849</v>
+      </c>
+      <c r="C425" t="s">
+        <v>14</v>
+      </c>
+      <c r="D425" t="s">
+        <v>14</v>
+      </c>
+      <c r="E425" t="s">
+        <v>14</v>
+      </c>
+      <c r="F425" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="426" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A426" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B426">
+        <v>850</v>
+      </c>
+      <c r="C426" t="s">
+        <v>14</v>
+      </c>
+      <c r="D426" t="s">
+        <v>14</v>
+      </c>
+      <c r="E426" t="s">
+        <v>14</v>
+      </c>
+      <c r="F426" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="427" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A427" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B427">
+        <v>851</v>
+      </c>
+      <c r="C427" t="s">
+        <v>14</v>
+      </c>
+      <c r="D427" t="s">
+        <v>14</v>
+      </c>
+      <c r="E427" t="s">
+        <v>14</v>
+      </c>
+      <c r="F427" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="428" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A428" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B428">
+        <v>852</v>
+      </c>
+      <c r="C428" t="s">
+        <v>14</v>
+      </c>
+      <c r="D428" t="s">
+        <v>14</v>
+      </c>
+      <c r="E428" t="s">
+        <v>14</v>
+      </c>
+      <c r="F428" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="429" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A429" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B429">
+        <v>853</v>
+      </c>
+      <c r="C429" t="s">
+        <v>14</v>
+      </c>
+      <c r="D429" t="s">
+        <v>14</v>
+      </c>
+      <c r="E429" t="s">
+        <v>14</v>
+      </c>
+      <c r="F429" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="430" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A430" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B430">
+        <v>854</v>
+      </c>
+      <c r="C430" t="s">
+        <v>14</v>
+      </c>
+      <c r="D430" t="s">
+        <v>14</v>
+      </c>
+      <c r="E430" t="s">
+        <v>14</v>
+      </c>
+      <c r="F430" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="431" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A431" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B431">
+        <v>855</v>
+      </c>
+      <c r="C431" t="s">
+        <v>14</v>
+      </c>
+      <c r="D431" t="s">
+        <v>14</v>
+      </c>
+      <c r="E431" t="s">
+        <v>14</v>
+      </c>
+      <c r="F431" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="432" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A432" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B432">
+        <v>856</v>
+      </c>
+      <c r="C432" t="s">
+        <v>14</v>
+      </c>
+      <c r="D432" t="s">
+        <v>14</v>
+      </c>
+      <c r="E432" t="s">
+        <v>14</v>
+      </c>
+      <c r="F432" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="433" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A433" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B433">
+        <v>857</v>
+      </c>
+      <c r="C433" t="s">
+        <v>14</v>
+      </c>
+      <c r="D433" t="s">
+        <v>14</v>
+      </c>
+      <c r="E433" t="s">
+        <v>14</v>
+      </c>
+      <c r="F433" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="434" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A434" s="2">
+        <v>43916</v>
+      </c>
+      <c r="B434">
+        <v>858</v>
+      </c>
+      <c r="C434" t="s">
+        <v>14</v>
+      </c>
+      <c r="D434" t="s">
+        <v>14</v>
+      </c>
+      <c r="E434" t="s">
+        <v>14</v>
+      </c>
+      <c r="F434" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
excel update 2020-03-26 17:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFCB8D6F-1D29-4E4D-88AC-A44B9934A5A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670B8EB1-15EC-5A42-90DB-1F8618C1FF7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -717,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -870,9 +870,38 @@
         <v>38550</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>43916.729166666664</v>
+      </c>
+      <c r="B7">
+        <v>26727</v>
+      </c>
+      <c r="C7">
+        <v>10965</v>
+      </c>
+      <c r="D7">
+        <v>835</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>15</v>
+      </c>
+      <c r="G7">
+        <v>38550</v>
+      </c>
+    </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D12" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D16" s="3"/>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E17" s="3"/>
@@ -886,7 +915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349DD023-B549-B642-9379-4C23EAB3417F}">
   <dimension ref="A1:F434"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A391" workbookViewId="0">
+    <sheetView topLeftCell="A389" workbookViewId="0">
       <selection activeCell="A435" sqref="A435"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
excel update 2020-03-27 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670B8EB1-15EC-5A42-90DB-1F8618C1FF7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42558F21-1202-9946-84CE-FF708C3E4065}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -715,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -732,7 +732,7 @@
     <col min="7" max="7" width="54.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -755,7 +755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43913.4375</v>
       </c>
@@ -774,11 +774,15 @@
       <c r="F2">
         <v>6</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2">
         <v>28506</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2">
+        <f>F2/SUM(B2:F2)</f>
+        <v>2.1048200378867606E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43914.4375</v>
       </c>
@@ -797,11 +801,15 @@
       <c r="F3">
         <v>7</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3">
         <v>32457</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3">
+        <f t="shared" ref="H3:H8" si="0">F3/SUM(B3:F3)</f>
+        <v>2.1566996333610624E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43915.4375</v>
       </c>
@@ -820,11 +828,15 @@
       <c r="F4">
         <v>9</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4">
         <v>35635</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>2.5256068472007858E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43915.729166666664</v>
       </c>
@@ -843,11 +855,15 @@
       <c r="F5">
         <v>13</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5">
         <v>35635</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>3.648098779290024E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43916.4375</v>
       </c>
@@ -866,11 +882,15 @@
       <c r="F6">
         <v>13</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6">
         <v>38550</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>3.3722438391699093E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43916.729166666664</v>
       </c>
@@ -892,15 +912,53 @@
       <c r="G7">
         <v>38550</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>3.8910505836575878E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>43917.4375</v>
+      </c>
+      <c r="B8">
+        <v>29967</v>
+      </c>
+      <c r="C8">
+        <v>10074</v>
+      </c>
+      <c r="D8">
+        <v>967</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>18</v>
+      </c>
+      <c r="G8">
+        <v>41032</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>4.3866062289808452E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D12" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.2">
@@ -908,6 +966,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="H2:H8" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
excel update 2020-03-28 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42558F21-1202-9946-84CE-FF708C3E4065}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBC54C7-8DF2-A147-8DCB-076F72C44AC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -715,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -732,7 +732,7 @@
     <col min="7" max="7" width="54.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -755,7 +755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43913.4375</v>
       </c>
@@ -777,12 +777,8 @@
       <c r="G2">
         <v>28506</v>
       </c>
-      <c r="H2">
-        <f>F2/SUM(B2:F2)</f>
-        <v>2.1048200378867606E-4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43914.4375</v>
       </c>
@@ -804,12 +800,8 @@
       <c r="G3">
         <v>32457</v>
       </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H8" si="0">F3/SUM(B3:F3)</f>
-        <v>2.1566996333610624E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43915.4375</v>
       </c>
@@ -831,12 +823,8 @@
       <c r="G4">
         <v>35635</v>
       </c>
-      <c r="H4">
-        <f t="shared" si="0"/>
-        <v>2.5256068472007858E-4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43915.729166666664</v>
       </c>
@@ -858,12 +846,8 @@
       <c r="G5">
         <v>35635</v>
       </c>
-      <c r="H5">
-        <f t="shared" si="0"/>
-        <v>3.648098779290024E-4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43916.4375</v>
       </c>
@@ -885,12 +869,8 @@
       <c r="G6">
         <v>38550</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="0"/>
-        <v>3.3722438391699093E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43916.729166666664</v>
       </c>
@@ -912,12 +892,8 @@
       <c r="G7">
         <v>38550</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="0"/>
-        <v>3.8910505836575878E-4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43917.4375</v>
       </c>
@@ -939,36 +915,54 @@
       <c r="G8">
         <v>41032</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="0"/>
-        <v>4.3866062289808452E-4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>43918.4375</v>
+      </c>
+      <c r="B9">
+        <v>33240</v>
+      </c>
+      <c r="C9">
+        <v>8690</v>
+      </c>
+      <c r="D9">
+        <v>1118</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>18</v>
+      </c>
+      <c r="G9">
+        <v>43072</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C11" s="3"/>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D12" s="3"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E17" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <ignoredErrors>
-    <ignoredError sqref="H2:H8" formulaRange="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
excel update 2020-03-28 17:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBC54C7-8DF2-A147-8DCB-076F72C44AC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D04B8B4-318D-684F-A083-80D263526E60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -718,7 +718,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -940,12 +940,27 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D11" s="3"/>
+      <c r="A10" s="1">
+        <v>43918.729166666664</v>
+      </c>
+      <c r="B10">
+        <v>33240</v>
+      </c>
+      <c r="C10">
+        <v>8690</v>
+      </c>
+      <c r="D10">
+        <v>1117</v>
+      </c>
+      <c r="E10">
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <v>19</v>
+      </c>
+      <c r="G10">
+        <v>43072</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D14" s="3"/>

</xml_diff>

<commit_message>
excel update 2020-03-29 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D04B8B4-318D-684F-A083-80D263526E60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF69C16B-3ABC-D741-ACB9-43FBA8A3F637}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -718,7 +718,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -962,6 +962,32 @@
         <v>43072</v>
       </c>
     </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43919.4375</v>
+      </c>
+      <c r="B11">
+        <v>40630</v>
+      </c>
+      <c r="C11">
+        <v>7203</v>
+      </c>
+      <c r="D11">
+        <v>1326</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>21</v>
+      </c>
+      <c r="G11">
+        <v>49186</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D13" s="3"/>
+    </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -972,6 +998,9 @@
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D19" s="3"/>

</xml_diff>

<commit_message>
excel update 2020-03-29 17:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF69C16B-3ABC-D741-ACB9-43FBA8A3F637}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C03FDF7-6522-FB4E-9283-680C9372C809}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -715,10 +715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -985,6 +985,29 @@
         <v>49186</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>43919.729166666664</v>
+      </c>
+      <c r="B12">
+        <v>40630</v>
+      </c>
+      <c r="C12">
+        <v>7203</v>
+      </c>
+      <c r="D12">
+        <v>1324</v>
+      </c>
+      <c r="E12">
+        <v>8</v>
+      </c>
+      <c r="F12">
+        <v>23</v>
+      </c>
+      <c r="G12">
+        <v>49186</v>
+      </c>
+    </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D13" s="3"/>
     </row>
@@ -999,11 +1022,19 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C17" s="3"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C19" s="3"/>
       <c r="D19" s="3"/>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C22" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-03-30 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA46FB5B-E4F0-3D49-A9F9-70D3FAA5EB89}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0CA5F3-71AB-3A46-82A4-05DBABACE201}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -397,10 +397,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,6 +609,184 @@
             <a:t> </a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1400"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" baseline="0"/>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1400" b="1"/>
+            <a:t>Schema change in data as of 2020/03/30 - assumptions (old field</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1400" b="1" baseline="0"/>
+            <a:t> / new field)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1400" b="1"/>
+            <a:t>:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1400" b="1" baseline="0"/>
+            <a:t>	- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1400" b="0" baseline="0"/>
+            <a:t>Positive = Number of Cases</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1400" b="0" baseline="0"/>
+            <a:t>	- Resolved = Resolved</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1400" b="0" baseline="0"/>
+            <a:t>	- Deceased = Deceased</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1400" b="0" baseline="0"/>
+            <a:t>	- Negative = Total Tested - (Number of Cases + Resolved + Deceased)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1400" b="0" baseline="0"/>
+            <a:t>	- Currently under investigation = Currently under investigation</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1400" b="0" baseline="0"/>
+            <a:t>	- Total number of patients approved for COVID-19 testing to date = Total Tested + Currently under investigation</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
         </a:p>
         <a:p>
           <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
@@ -926,7 +1105,8 @@
   <dimension ref="A1:G78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2183,7 +2363,27 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55" s="1"/>
+      <c r="A55" s="1">
+        <v>43920.4375</v>
+      </c>
+      <c r="B55">
+        <v>46301</v>
+      </c>
+      <c r="C55">
+        <v>5651</v>
+      </c>
+      <c r="D55">
+        <v>1706</v>
+      </c>
+      <c r="E55">
+        <v>431</v>
+      </c>
+      <c r="F55">
+        <v>23</v>
+      </c>
+      <c r="G55">
+        <v>54112</v>
+      </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
@@ -2193,12 +2393,16 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
+      <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
+      <c r="D60" s="3"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
@@ -2211,41 +2415,51 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D67" s="3"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D70" s="3"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="D71" s="3"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F72" s="3"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F75" s="3"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F76" s="3"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="F77" s="3"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
     </row>
   </sheetData>
@@ -10961,7 +11175,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
excel update 2020-03-31 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0CA5F3-71AB-3A46-82A4-05DBABACE201}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDFD86F-1499-6342-8A15-A6A522D4DBEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -1105,8 +1105,8 @@
   <dimension ref="A1:G78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B57" sqref="B57"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2386,7 +2386,28 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56" s="1"/>
+      <c r="A56" s="1">
+        <v>43921.4375</v>
+      </c>
+      <c r="B56">
+        <v>48562</v>
+      </c>
+      <c r="C56">
+        <v>4280</v>
+      </c>
+      <c r="D56">
+        <v>1966</v>
+      </c>
+      <c r="E56">
+        <v>534</v>
+      </c>
+      <c r="F56">
+        <v>33</v>
+      </c>
+      <c r="G56">
+        <f>51629+C53</f>
+        <v>58832</v>
+      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
@@ -2399,6 +2420,7 @@
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
       <c r="D59" s="3"/>
+      <c r="G59" s="3"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
@@ -2406,6 +2428,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
+      <c r="D61" s="3"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
@@ -2417,49 +2440,53 @@
       <c r="A64" s="1"/>
       <c r="F64" s="3"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D69" s="3"/>
+      <c r="G69" s="3"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="D70" s="3"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="D71" s="3"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
+      <c r="D72" s="3"/>
       <c r="F72" s="3"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="D73" s="3"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
       <c r="F75" s="3"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
       <c r="F76" s="3"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
       <c r="F77" s="3"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel update 2020-04-01 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDFD86F-1499-6342-8A15-A6A522D4DBEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250C8B51-E180-CA46-99EB-9689E743C777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -1105,8 +1105,8 @@
   <dimension ref="A1:G78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A67" sqref="A67"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2410,7 +2410,27 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57" s="1"/>
+      <c r="A57" s="1">
+        <v>43922.4375</v>
+      </c>
+      <c r="B57">
+        <v>51621</v>
+      </c>
+      <c r="C57">
+        <v>3135</v>
+      </c>
+      <c r="D57">
+        <v>2392</v>
+      </c>
+      <c r="E57">
+        <v>689</v>
+      </c>
+      <c r="F57">
+        <v>37</v>
+      </c>
+      <c r="G57">
+        <v>61009</v>
+      </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
@@ -2432,6 +2452,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
+      <c r="D62" s="3"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
@@ -2448,6 +2469,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
+      <c r="D68" s="3"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
@@ -2476,14 +2498,18 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
+      <c r="D75" s="3"/>
       <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
+      <c r="D76" s="3"/>
       <c r="F76" s="3"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
+      <c r="D77" s="3"/>
       <c r="F77" s="3"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
excel correction negative cases 2020-04-01
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250C8B51-E180-CA46-99EB-9689E743C777}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BA7CBC-73BD-1740-A91B-12EF785F4308}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -1102,11 +1102,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F62" sqref="F62"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2414,7 +2414,7 @@
         <v>43922.4375</v>
       </c>
       <c r="B57">
-        <v>51621</v>
+        <v>54756</v>
       </c>
       <c r="C57">
         <v>3135</v>
@@ -2463,6 +2463,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
+      <c r="D65" s="3"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D67" s="3"/>
@@ -2474,7 +2475,10 @@
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="D69" s="3"/>
-      <c r="G69" s="3"/>
+      <c r="G69" s="3">
+        <f>D78-(D65+D67+D68)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
@@ -2514,6 +2518,10 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
+      <c r="D78" s="3"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D79" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-04-02 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BA7CBC-73BD-1740-A91B-12EF785F4308}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D398CF20-2BC2-824C-80D6-7FC10C01B0B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -1105,8 +1105,8 @@
   <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2433,9 +2433,27 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58" s="1"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
+      <c r="A58" s="1">
+        <v>43923.4375</v>
+      </c>
+      <c r="B58">
+        <v>59056</v>
+      </c>
+      <c r="C58">
+        <v>2052</v>
+      </c>
+      <c r="D58">
+        <v>2793</v>
+      </c>
+      <c r="E58">
+        <v>831</v>
+      </c>
+      <c r="F58">
+        <v>53</v>
+      </c>
+      <c r="G58">
+        <v>64785</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="1"/>
@@ -2449,17 +2467,21 @@
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="D61" s="3"/>
+      <c r="G61" s="3"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="D62" s="3"/>
+      <c r="G62" s="3"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
+      <c r="D63" s="3"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
       <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
@@ -2475,10 +2497,7 @@
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="D69" s="3"/>
-      <c r="G69" s="3">
-        <f>D78-(D65+D67+D68)</f>
-        <v>0</v>
-      </c>
+      <c r="G69" s="3"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>

</xml_diff>

<commit_message>
excel update 2020-04-03 10:30 + added demo & hospitalization
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D398CF20-2BC2-824C-80D6-7FC10C01B0B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DB3980-1B98-8149-AFAD-6B629BCDA487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
-    <sheet name="Daily Summary" sheetId="2" r:id="rId2"/>
-    <sheet name="NOTES" sheetId="3" r:id="rId3"/>
+    <sheet name="Demographics" sheetId="4" r:id="rId2"/>
+    <sheet name="Daily Summary" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="NOTES" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1745" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="119">
   <si>
     <t>Negative1</t>
   </si>
@@ -362,16 +363,59 @@
   </si>
   <si>
     <t>Lambton</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>19 and under</t>
+  </si>
+  <si>
+    <t>20-39</t>
+  </si>
+  <si>
+    <t>40-59</t>
+  </si>
+  <si>
+    <t>60-79</t>
+  </si>
+  <si>
+    <t>80 and over</t>
+  </si>
+  <si>
+    <t>Number of patients hospitalized with COVID-196</t>
+  </si>
+  <si>
+    <t>Number of patients in ICU7 with COVID-19</t>
+  </si>
+  <si>
+    <t>Number of patients in ICU7 on a ventilator with COVID-19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF222222"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -397,11 +441,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1105,8 +1151,8 @@
   <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A58" sqref="A58"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2456,9 +2502,27 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59" s="1"/>
-      <c r="D59" s="3"/>
-      <c r="G59" s="3"/>
+      <c r="A59" s="1">
+        <v>43924.4375</v>
+      </c>
+      <c r="B59">
+        <v>62408</v>
+      </c>
+      <c r="C59">
+        <v>1245</v>
+      </c>
+      <c r="D59">
+        <v>3255</v>
+      </c>
+      <c r="E59">
+        <v>1023</v>
+      </c>
+      <c r="F59">
+        <v>67</v>
+      </c>
+      <c r="G59">
+        <v>67998</v>
+      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
@@ -2480,12 +2544,16 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
+      <c r="D64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
       <c r="D65" s="3"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D66" s="3"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D67" s="3"/>
@@ -2548,6 +2616,160 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
+  <dimension ref="A1:K18"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8:H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>43923.4375</v>
+      </c>
+      <c r="B2">
+        <v>1355</v>
+      </c>
+      <c r="C2">
+        <v>1421</v>
+      </c>
+      <c r="D2">
+        <v>68</v>
+      </c>
+      <c r="E2">
+        <v>826</v>
+      </c>
+      <c r="F2">
+        <v>995</v>
+      </c>
+      <c r="G2">
+        <v>716</v>
+      </c>
+      <c r="H2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>43924.4375</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1579</v>
+      </c>
+      <c r="C3" s="3">
+        <v>1657</v>
+      </c>
+      <c r="D3">
+        <v>82</v>
+      </c>
+      <c r="E3">
+        <v>945</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1178</v>
+      </c>
+      <c r="G3">
+        <v>821</v>
+      </c>
+      <c r="H3">
+        <v>226</v>
+      </c>
+      <c r="I3">
+        <v>462</v>
+      </c>
+      <c r="J3">
+        <v>194</v>
+      </c>
+      <c r="K3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G10" s="3"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G13" s="3"/>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349DD023-B549-B642-9379-4C23EAB3417F}">
   <dimension ref="A1:F434"/>
   <sheetViews>
@@ -11250,7 +11472,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{487FCA73-E0C0-7947-9245-660D3E078765}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
excel update 2020-04-04 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DB3980-1B98-8149-AFAD-6B629BCDA487}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D3C88F-6839-1443-959A-873032B4E4C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="120">
   <si>
     <t>Negative1</t>
   </si>
@@ -393,25 +393,22 @@
   </si>
   <si>
     <t>Number of patients in ICU7 on a ventilator with COVID-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF222222"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -447,7 +444,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1148,11 +1145,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:G79"/>
+  <dimension ref="A1:G81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2525,22 +2522,46 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60" s="1"/>
-      <c r="D60" s="3"/>
+      <c r="A60" s="1">
+        <v>43925.4375</v>
+      </c>
+      <c r="B60">
+        <v>66395</v>
+      </c>
+      <c r="C60">
+        <v>1336</v>
+      </c>
+      <c r="D60">
+        <v>3630</v>
+      </c>
+      <c r="E60">
+        <v>1219</v>
+      </c>
+      <c r="F60">
+        <v>94</v>
+      </c>
+      <c r="G60">
+        <v>72674</v>
+      </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
       <c r="D61" s="3"/>
-      <c r="G61" s="3"/>
+      <c r="G61" s="3" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
       <c r="D62" s="3"/>
-      <c r="G62" s="3"/>
+      <c r="G62" s="5"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
       <c r="D63" s="3"/>
+      <c r="G63" s="3"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
@@ -2557,6 +2578,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D67" s="3"/>
+      <c r="E67" s="3"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
@@ -2565,6 +2587,7 @@
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
       <c r="G69" s="3"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -2578,11 +2601,13 @@
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
       <c r="F72" s="3"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
@@ -2590,12 +2615,14 @@
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
       <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
       <c r="F75" s="3"/>
       <c r="G75" s="3"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
       <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
       <c r="F76" s="3"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
@@ -2609,6 +2636,12 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D79" s="3"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E80" s="3"/>
+    </row>
+    <row r="81" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E81" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2617,19 +2650,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8:H22"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
@@ -2693,10 +2726,10 @@
       <c r="A3" s="1">
         <v>43924.4375</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3">
         <v>1579</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3">
         <v>1657</v>
       </c>
       <c r="D3">
@@ -2705,7 +2738,7 @@
       <c r="E3">
         <v>945</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3">
         <v>1178</v>
       </c>
       <c r="G3">
@@ -2724,45 +2757,341 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>43925.4375</v>
+      </c>
+      <c r="B4">
+        <v>1755</v>
+      </c>
+      <c r="C4">
+        <v>1857</v>
+      </c>
+      <c r="D4">
+        <v>93</v>
+      </c>
+      <c r="E4">
+        <v>1025</v>
+      </c>
+      <c r="F4">
+        <v>1319</v>
+      </c>
+      <c r="G4">
+        <v>903</v>
+      </c>
+      <c r="H4">
+        <v>287</v>
+      </c>
+      <c r="I4">
+        <v>506</v>
+      </c>
+      <c r="J4">
+        <v>196</v>
+      </c>
+      <c r="K4">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
       <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
       <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="1"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
       <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-04-07 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C8A2A0-7B58-814C-95F1-100A751ECE0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6088BCB4-8428-FE48-9F0A-5C9D11677873}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="35180" yWindow="580" windowWidth="33600" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -1168,11 +1168,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:G78"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E62" sqref="E62"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2614,11 +2614,27 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63" s="1"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="G63" s="3"/>
+      <c r="A63" s="1">
+        <v>43928.4375</v>
+      </c>
+      <c r="B63">
+        <v>74683</v>
+      </c>
+      <c r="C63">
+        <v>691</v>
+      </c>
+      <c r="D63">
+        <v>4726</v>
+      </c>
+      <c r="E63">
+        <v>1802</v>
+      </c>
+      <c r="F63">
+        <v>153</v>
+      </c>
+      <c r="G63">
+        <v>82055</v>
+      </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
@@ -2627,36 +2643,26 @@
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
     </row>
-    <row r="65" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
-      <c r="D65" s="6"/>
-      <c r="E65" s="7"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="7"/>
-    </row>
-    <row r="66" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-    </row>
-    <row r="67" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="D67" s="6"/>
-      <c r="E67" s="7"/>
-      <c r="F67" s="5"/>
-    </row>
-    <row r="68" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="G65" s="3"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A66" s="1"/>
+      <c r="G66" s="3"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A67" s="1"/>
+      <c r="G67" s="3"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
-      <c r="G69" s="3"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
-      <c r="G70" s="3"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
@@ -2670,19 +2676,6 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A75" s="1"/>
-      <c r="G75" s="3"/>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A76" s="1"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A77" s="1"/>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A78" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2694,7 +2687,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H11" sqref="H10:H11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2904,17 +2897,39 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="A7" s="1">
+        <v>43928.4375</v>
+      </c>
+      <c r="B7">
+        <v>2211</v>
+      </c>
+      <c r="C7">
+        <v>2489</v>
+      </c>
+      <c r="D7">
+        <v>120</v>
+      </c>
+      <c r="E7">
+        <v>1263</v>
+      </c>
+      <c r="F7">
+        <v>1663</v>
+      </c>
+      <c r="G7">
+        <v>1168</v>
+      </c>
+      <c r="H7">
+        <v>509</v>
+      </c>
+      <c r="I7">
+        <v>614</v>
+      </c>
+      <c r="J7">
+        <v>233</v>
+      </c>
+      <c r="K7">
+        <v>187</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
@@ -2975,9 +2990,9 @@
       <c r="D12" s="3"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
@@ -2989,8 +3004,8 @@
       <c r="E13" s="5"/>
       <c r="F13" s="7"/>
       <c r="G13" s="5"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="5"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
@@ -3001,8 +3016,8 @@
       <c r="E14" s="5"/>
       <c r="F14" s="7"/>
       <c r="G14" s="5"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="5"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
@@ -3014,8 +3029,8 @@
       <c r="E15" s="5"/>
       <c r="F15" s="7"/>
       <c r="G15" s="5"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
@@ -3027,8 +3042,8 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="5"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
@@ -3039,8 +3054,8 @@
       <c r="E17" s="8"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="5"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
@@ -3052,8 +3067,8 @@
       <c r="E18" s="6"/>
       <c r="F18" s="7"/>
       <c r="G18" s="5"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="5"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
     </row>
@@ -3065,8 +3080,8 @@
       <c r="E19" s="6"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
@@ -3076,9 +3091,9 @@
       <c r="C20" s="3"/>
       <c r="E20" s="8"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
@@ -3089,9 +3104,9 @@
       <c r="D21" s="3"/>
       <c r="E21" s="6"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="5"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
@@ -3102,9 +3117,9 @@
       <c r="D22" s="3"/>
       <c r="E22" s="6"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
@@ -3114,45 +3129,45 @@
       <c r="D23" s="3"/>
       <c r="E23" s="6"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
     </row>

</xml_diff>

<commit_message>
excel update 2020-04-08 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6088BCB4-8428-FE48-9F0A-5C9D11677873}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374139E0-E066-C44A-AC22-61900A5D5F0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35180" yWindow="580" windowWidth="33600" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -855,9 +855,6 @@
           <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
         </a:p>
         <a:p>
-          <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
-        </a:p>
-        <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1400" b="1" baseline="0"/>
             <a:t>OTHER</a:t>
@@ -1171,8 +1168,8 @@
   <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2637,11 +2634,27 @@
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64" s="1"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
+      <c r="A64" s="1">
+        <v>43929.4375</v>
+      </c>
+      <c r="B64">
+        <v>77077</v>
+      </c>
+      <c r="C64">
+        <v>1102</v>
+      </c>
+      <c r="D64">
+        <v>5276</v>
+      </c>
+      <c r="E64">
+        <v>2074</v>
+      </c>
+      <c r="F64">
+        <v>174</v>
+      </c>
+      <c r="G64">
+        <v>85703</v>
+      </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="1"/>
@@ -2657,12 +2670,15 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
+      <c r="E68" s="3"/>
+      <c r="G68" s="3"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
+      <c r="E70" s="3"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
@@ -2687,7 +2703,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2932,17 +2948,39 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="A8" s="1">
+        <v>43929.4375</v>
+      </c>
+      <c r="B8">
+        <v>2433</v>
+      </c>
+      <c r="C8">
+        <v>2810</v>
+      </c>
+      <c r="D8">
+        <v>129</v>
+      </c>
+      <c r="E8">
+        <v>1369</v>
+      </c>
+      <c r="F8">
+        <v>1851</v>
+      </c>
+      <c r="G8">
+        <v>1300</v>
+      </c>
+      <c r="H8">
+        <v>624</v>
+      </c>
+      <c r="I8">
+        <v>605</v>
+      </c>
+      <c r="J8">
+        <v>246</v>
+      </c>
+      <c r="K8">
+        <v>195</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
@@ -2970,14 +3008,12 @@
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
     </row>
-    <row r="11" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="5"/>
+      <c r="F11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
@@ -2988,9 +3024,7 @@
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="8"/>
+      <c r="F12" s="3"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="3"/>
@@ -3001,9 +3035,6 @@
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="5"/>
       <c r="H13" s="7"/>
       <c r="I13" s="5"/>
       <c r="J13" s="3"/>
@@ -3013,9 +3044,7 @@
       <c r="A14" s="1"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="5"/>
+      <c r="F14" s="3"/>
       <c r="H14" s="7"/>
       <c r="I14" s="5"/>
       <c r="J14" s="3"/>
@@ -3026,9 +3055,7 @@
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="5"/>
+      <c r="F15" s="3"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="3"/>
@@ -3039,9 +3066,7 @@
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="F16" s="3"/>
       <c r="H16" s="7"/>
       <c r="I16" s="5"/>
       <c r="J16" s="3"/>
@@ -3051,9 +3076,6 @@
       <c r="A17" s="1"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
       <c r="H17" s="7"/>
       <c r="I17" s="5"/>
       <c r="J17" s="3"/>
@@ -3064,9 +3086,6 @@
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="5"/>
       <c r="H18" s="7"/>
       <c r="I18" s="5"/>
       <c r="J18" s="3"/>
@@ -3077,9 +3096,7 @@
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="F19" s="3"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="3"/>
@@ -3089,9 +3106,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="8"/>
+      <c r="F20" s="3"/>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
       <c r="J20" s="3"/>
@@ -3102,9 +3117,6 @@
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="6"/>
       <c r="H21" s="7"/>
       <c r="I21" s="5"/>
       <c r="J21" s="3"/>
@@ -3115,9 +3127,6 @@
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="6"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="3"/>
@@ -3127,9 +3136,6 @@
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="8"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="3"/>
@@ -3139,9 +3145,6 @@
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="6"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="3"/>
@@ -3151,9 +3154,6 @@
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="6"/>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="3"/>

</xml_diff>

<commit_message>
excel update 2020-04-10 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D01DC99-31BA-F642-8FC5-FA5FCAC0EB6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6C2BE2-043B-6741-9812-81C2F3A47413}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -457,7 +457,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -467,6 +467,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1167,9 +1168,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D72" sqref="D72:F89"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2680,8 +2681,27 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="1"/>
-      <c r="G66" s="3"/>
+      <c r="A66" s="1">
+        <v>43931.4375</v>
+      </c>
+      <c r="B66">
+        <v>83640</v>
+      </c>
+      <c r="C66">
+        <v>1598</v>
+      </c>
+      <c r="D66">
+        <v>6237</v>
+      </c>
+      <c r="E66">
+        <v>2574</v>
+      </c>
+      <c r="F66">
+        <v>222</v>
+      </c>
+      <c r="G66">
+        <v>94271</v>
+      </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
@@ -2697,20 +2717,14 @@
     </row>
     <row r="69" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
       <c r="F69" s="5"/>
     </row>
     <row r="70" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
-      <c r="D70" s="6"/>
-      <c r="E70" s="7"/>
       <c r="F70" s="5"/>
     </row>
     <row r="71" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
-      <c r="D71" s="6"/>
-      <c r="E71" s="5"/>
       <c r="F71" s="5"/>
       <c r="G71" s="3"/>
     </row>
@@ -2719,9 +2733,11 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
+      <c r="D73" s="9"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
+      <c r="D74" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2732,8 +2748,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3047,18 +3064,40 @@
         <v>214</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>43931.4375</v>
+      </c>
+      <c r="B10">
+        <v>2827</v>
+      </c>
+      <c r="C10">
+        <v>3373</v>
+      </c>
+      <c r="D10">
+        <v>151</v>
+      </c>
+      <c r="E10">
+        <v>1574</v>
+      </c>
+      <c r="F10">
+        <v>2159</v>
+      </c>
+      <c r="G10">
+        <v>1510</v>
+      </c>
+      <c r="H10">
+        <v>837</v>
+      </c>
+      <c r="I10">
+        <v>673</v>
+      </c>
+      <c r="J10">
+        <v>260</v>
+      </c>
+      <c r="K10">
+        <v>217</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
@@ -3112,8 +3151,6 @@
       <c r="D15" s="7"/>
       <c r="E15" s="5"/>
       <c r="F15" s="3"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
@@ -3121,11 +3158,7 @@
       <c r="A16" s="1"/>
       <c r="B16" s="3"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
       <c r="F16" s="3"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="5"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
@@ -3133,10 +3166,6 @@
       <c r="A17" s="1"/>
       <c r="B17" s="3"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="5"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="5"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
@@ -3144,10 +3173,6 @@
       <c r="A18" s="1"/>
       <c r="B18" s="3"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="5"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="5"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
     </row>
@@ -3155,11 +3180,7 @@
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="5"/>
       <c r="F19" s="3"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
@@ -3167,11 +3188,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
       <c r="F20" s="3"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
@@ -3179,10 +3196,6 @@
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
       <c r="C21" s="8"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="5"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
@@ -3190,8 +3203,6 @@
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="5"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="3"/>
@@ -3201,8 +3212,6 @@
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="5"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="3"/>
@@ -3211,49 +3220,38 @@
     <row r="24" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B24" s="3"/>
       <c r="C24" s="8"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
+      <c r="H24" s="9"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B25" s="3"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
+      <c r="H25" s="9"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
     </row>
-    <row r="26" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B26" s="3"/>
       <c r="C26" s="6"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
       <c r="F26" s="3"/>
       <c r="G26" s="6"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
+      <c r="H26" s="9"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B27" s="3"/>
       <c r="C27" s="6"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
+      <c r="H27" s="9"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B28" s="3"/>
+      <c r="D28" s="9"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>

</xml_diff>

<commit_message>
excel update 2020-04-11 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E6C2BE2-043B-6741-9812-81C2F3A47413}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E72933-6AC2-5549-A112-8075E024AE87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -399,7 +399,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000%"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -435,6 +438,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -453,11 +463,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -468,10 +479,13 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1166,11 +1180,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H80"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C69" sqref="C69"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2704,8 +2718,27 @@
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="1"/>
-      <c r="G67" s="3"/>
+      <c r="A67" s="1">
+        <v>43932.4375</v>
+      </c>
+      <c r="B67">
+        <v>86562</v>
+      </c>
+      <c r="C67">
+        <v>1517</v>
+      </c>
+      <c r="D67">
+        <v>6648</v>
+      </c>
+      <c r="E67">
+        <v>2858</v>
+      </c>
+      <c r="F67">
+        <v>253</v>
+      </c>
+      <c r="G67">
+        <v>97838</v>
+      </c>
     </row>
     <row r="68" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
@@ -2725,19 +2758,39 @@
     </row>
     <row r="71" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
+      <c r="E71" s="3"/>
       <c r="F71" s="5"/>
       <c r="G71" s="3"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="3"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="D73" s="9"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="1"/>
-      <c r="D74" s="9"/>
+      <c r="E74" s="3"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E75" s="3"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E76" s="3"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E77" s="3"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E78" s="3"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E79" s="3"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E80" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2746,11 +2799,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2758,7 +2811,7 @@
     <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -2793,7 +2846,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43923.4375</v>
       </c>
@@ -2819,7 +2872,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43924.4375</v>
       </c>
@@ -2853,8 +2906,11 @@
       <c r="K3">
         <v>140</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43925.4375</v>
       </c>
@@ -2888,8 +2944,11 @@
       <c r="K4">
         <v>152</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43926.4375</v>
       </c>
@@ -2923,8 +2982,11 @@
       <c r="K5">
         <v>154</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43927.4375</v>
       </c>
@@ -2958,8 +3020,11 @@
       <c r="K6">
         <v>160</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43928.4375</v>
       </c>
@@ -2993,8 +3058,11 @@
       <c r="K7">
         <v>187</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43929.4375</v>
       </c>
@@ -3028,8 +3096,11 @@
       <c r="K8">
         <v>195</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43930.4375</v>
       </c>
@@ -3063,8 +3134,11 @@
       <c r="K9">
         <v>214</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43931.4375</v>
       </c>
@@ -3098,19 +3172,49 @@
       <c r="K10">
         <v>217</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43932.4375</v>
+      </c>
+      <c r="B11">
+        <v>2997</v>
+      </c>
+      <c r="C11">
+        <v>3609</v>
+      </c>
+      <c r="D11">
+        <v>157</v>
+      </c>
+      <c r="E11">
+        <v>1648</v>
+      </c>
+      <c r="F11">
+        <v>2303</v>
+      </c>
+      <c r="G11">
+        <v>1615</v>
+      </c>
+      <c r="H11">
+        <v>919</v>
+      </c>
+      <c r="I11">
+        <v>691</v>
+      </c>
+      <c r="J11">
+        <v>257</v>
+      </c>
+      <c r="K11">
+        <v>215</v>
+      </c>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+    </row>
+    <row r="12" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -3121,7 +3225,7 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="3"/>
       <c r="C13" s="8"/>
@@ -3132,32 +3236,34 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
-    <row r="14" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="3"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="5"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="3"/>
       <c r="H14" s="7"/>
       <c r="I14" s="5"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="3"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="5"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="10"/>
       <c r="F15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
-    <row r="16" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="3"/>
       <c r="C16" s="5"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="10"/>
       <c r="F16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -3166,6 +3272,8 @@
       <c r="A17" s="1"/>
       <c r="B17" s="3"/>
       <c r="C17" s="5"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
@@ -3173,6 +3281,8 @@
       <c r="A18" s="1"/>
       <c r="B18" s="3"/>
       <c r="C18" s="5"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="10"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
     </row>
@@ -3180,6 +3290,8 @@
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
       <c r="C19" s="5"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="10"/>
       <c r="F19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
@@ -3188,6 +3300,8 @@
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="5"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="10"/>
       <c r="F20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -3196,6 +3310,8 @@
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
       <c r="C21" s="8"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
@@ -3203,6 +3319,8 @@
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="6"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="3"/>
@@ -3212,6 +3330,8 @@
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="C23" s="6"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="3"/>
@@ -3220,6 +3340,8 @@
     <row r="24" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B24" s="3"/>
       <c r="C24" s="8"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
       <c r="H24" s="9"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -3227,6 +3349,8 @@
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B25" s="3"/>
       <c r="C25" s="6"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
       <c r="H25" s="9"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -3234,6 +3358,8 @@
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B26" s="3"/>
       <c r="C26" s="6"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
       <c r="F26" s="3"/>
       <c r="G26" s="6"/>
       <c r="H26" s="9"/>

</xml_diff>

<commit_message>
excel update 2020-04-12 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E72933-6AC2-5549-A112-8075E024AE87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EFEC14-A2E0-574D-9EC1-6728C0CC7847}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1763" uniqueCount="121">
   <si>
     <t>Negative1</t>
   </si>
@@ -394,13 +394,19 @@
   <si>
     <t>Number of patients in ICU7 on a ventilator with COVID-19</t>
   </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Hospitalizations</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -468,7 +474,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -479,8 +485,7 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1180,11 +1185,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:H80"/>
+  <dimension ref="A1:H73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H67" sqref="H67"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E70" sqref="E70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2740,12 +2745,28 @@
         <v>97838</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="A68" s="1"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="7"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="7"/>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>43933.4375</v>
+      </c>
+      <c r="B68">
+        <v>92721</v>
+      </c>
+      <c r="C68">
+        <v>1619</v>
+      </c>
+      <c r="D68">
+        <v>7049</v>
+      </c>
+      <c r="E68">
+        <v>3121</v>
+      </c>
+      <c r="F68">
+        <v>274</v>
+      </c>
+      <c r="G68">
+        <v>104784</v>
+      </c>
       <c r="H68" s="3"/>
     </row>
     <row r="69" spans="1:8" ht="20" x14ac:dyDescent="0.2">
@@ -2756,41 +2777,14 @@
       <c r="A70" s="1"/>
       <c r="F70" s="5"/>
     </row>
-    <row r="71" spans="1:8" ht="20" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="3"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
-      <c r="D72" s="9"/>
-      <c r="E72" s="3"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
-      <c r="D73" s="9"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E74" s="3"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E75" s="3"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E76" s="3"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E77" s="3"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E78" s="3"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E79" s="3"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="E80" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2799,11 +2793,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N28"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2906,9 +2900,9 @@
       <c r="K3">
         <v>140</v>
       </c>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -2944,9 +2938,9 @@
       <c r="K4">
         <v>152</v>
       </c>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -2982,9 +2976,9 @@
       <c r="K5">
         <v>154</v>
       </c>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -3020,9 +3014,9 @@
       <c r="K6">
         <v>160</v>
       </c>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -3058,9 +3052,9 @@
       <c r="K7">
         <v>187</v>
       </c>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -3096,9 +3090,9 @@
       <c r="K8">
         <v>195</v>
       </c>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -3134,9 +3128,9 @@
       <c r="K9">
         <v>214</v>
       </c>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -3172,9 +3166,9 @@
       <c r="K10">
         <v>217</v>
       </c>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -3210,20 +3204,44 @@
       <c r="K11">
         <v>215</v>
       </c>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-    </row>
-    <row r="12" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>43933.4375</v>
+      </c>
+      <c r="B12">
+        <v>3156</v>
+      </c>
+      <c r="C12">
+        <v>3851</v>
+      </c>
+      <c r="D12">
+        <v>167</v>
+      </c>
+      <c r="E12">
+        <v>1740</v>
+      </c>
+      <c r="F12">
+        <v>2403</v>
+      </c>
+      <c r="G12">
+        <v>1705</v>
+      </c>
+      <c r="H12">
+        <v>1028</v>
+      </c>
+      <c r="I12">
+        <v>738</v>
+      </c>
+      <c r="J12">
+        <v>261</v>
+      </c>
+      <c r="K12">
+        <v>196</v>
+      </c>
     </row>
     <row r="13" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
@@ -3240,9 +3258,9 @@
       <c r="A14" s="1"/>
       <c r="B14" s="3"/>
       <c r="C14" s="5"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="3"/>
       <c r="H14" s="7"/>
       <c r="I14" s="5"/>
       <c r="J14" s="3"/>
@@ -3252,9 +3270,8 @@
       <c r="A15" s="1"/>
       <c r="B15" s="3"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="3"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
@@ -3262,9 +3279,8 @@
       <c r="A16" s="1"/>
       <c r="B16" s="3"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="3"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
@@ -3272,8 +3288,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="3"/>
       <c r="C17" s="5"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="E17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
@@ -3281,8 +3296,7 @@
       <c r="A18" s="1"/>
       <c r="B18" s="3"/>
       <c r="C18" s="5"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="10"/>
+      <c r="E18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
     </row>
@@ -3290,9 +3304,7 @@
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="3"/>
+      <c r="E19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
@@ -3300,9 +3312,7 @@
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
       <c r="C20" s="5"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="3"/>
+      <c r="E20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
@@ -3310,8 +3320,7 @@
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
       <c r="C21" s="8"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="E21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
@@ -3319,8 +3328,7 @@
       <c r="A22" s="1"/>
       <c r="B22" s="3"/>
       <c r="C22" s="6"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="E22" s="3"/>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="3"/>
@@ -3330,8 +3338,7 @@
       <c r="A23" s="1"/>
       <c r="B23" s="3"/>
       <c r="C23" s="6"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+      <c r="E23" s="3"/>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="3"/>
@@ -3340,8 +3347,7 @@
     <row r="24" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B24" s="3"/>
       <c r="C24" s="8"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
+      <c r="E24" s="3"/>
       <c r="H24" s="9"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -3349,8 +3355,7 @@
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B25" s="3"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+      <c r="E25" s="3"/>
       <c r="H25" s="9"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
@@ -3358,10 +3363,6 @@
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B26" s="3"/>
       <c r="C26" s="6"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="6"/>
       <c r="H26" s="9"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
@@ -3369,7 +3370,7 @@
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B27" s="3"/>
       <c r="C27" s="6"/>
-      <c r="F27" s="3"/>
+      <c r="E27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="9"/>
       <c r="J27" s="3"/>
@@ -3377,13 +3378,49 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B28" s="3"/>
-      <c r="D28" s="9"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+      <c r="E28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30">
+        <v>738</v>
+      </c>
+      <c r="F30" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
+        <v>117</v>
+      </c>
+      <c r="E31">
+        <v>261</v>
+      </c>
+      <c r="F31" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D32" t="s">
+        <v>118</v>
+      </c>
+      <c r="E32">
+        <v>196</v>
+      </c>
+      <c r="F32" t="s">
+        <v>119</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-04-13 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6EFEC14-A2E0-574D-9EC1-6728C0CC7847}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7F5C41-6EC5-AD4A-8271-4126C729BE68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1763" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="119">
   <si>
     <t>Negative1</t>
   </si>
@@ -394,12 +394,6 @@
   <si>
     <t>Number of patients in ICU7 on a ventilator with COVID-19</t>
   </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Hospitalizations</t>
-  </si>
 </sst>
 </file>
 
@@ -408,7 +402,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -428,21 +422,6 @@
       <color rgb="FF222222"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF222222"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -469,28 +448,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1185,11 +1160,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E70" sqref="E70"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2769,9 +2744,28 @@
       </c>
       <c r="H68" s="3"/>
     </row>
-    <row r="69" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="A69" s="1"/>
-      <c r="F69" s="5"/>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>43934.4375</v>
+      </c>
+      <c r="B69">
+        <v>97112</v>
+      </c>
+      <c r="C69">
+        <v>1534</v>
+      </c>
+      <c r="D69">
+        <v>7470</v>
+      </c>
+      <c r="E69">
+        <v>3357</v>
+      </c>
+      <c r="F69">
+        <v>291</v>
+      </c>
+      <c r="G69">
+        <v>109764</v>
+      </c>
     </row>
     <row r="70" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
@@ -2785,6 +2779,9 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
+    </row>
+    <row r="86" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G86" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2793,11 +2790,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J15" sqref="J15"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2900,9 +2897,9 @@
       <c r="K3">
         <v>140</v>
       </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -2938,9 +2935,9 @@
       <c r="K4">
         <v>152</v>
       </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -2976,9 +2973,9 @@
       <c r="K5">
         <v>154</v>
       </c>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -3014,9 +3011,9 @@
       <c r="K6">
         <v>160</v>
       </c>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -3052,9 +3049,9 @@
       <c r="K7">
         <v>187</v>
       </c>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -3090,9 +3087,9 @@
       <c r="K8">
         <v>195</v>
       </c>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="N8" s="10"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -3128,9 +3125,9 @@
       <c r="K9">
         <v>214</v>
       </c>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -3166,9 +3163,9 @@
       <c r="K10">
         <v>217</v>
       </c>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -3204,9 +3201,9 @@
       <c r="K11">
         <v>215</v>
       </c>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -3242,17 +3239,43 @@
       <c r="K12">
         <v>196</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>43934.4375</v>
+      </c>
+      <c r="B13">
+        <v>3318</v>
+      </c>
+      <c r="C13">
+        <v>4109</v>
+      </c>
+      <c r="D13">
+        <v>175</v>
+      </c>
+      <c r="E13">
+        <v>1817</v>
+      </c>
+      <c r="F13">
+        <v>2521</v>
+      </c>
+      <c r="G13">
+        <v>1797</v>
+      </c>
+      <c r="H13">
+        <v>1154</v>
+      </c>
+      <c r="I13">
+        <v>760</v>
+      </c>
+      <c r="J13">
+        <v>263</v>
+      </c>
+      <c r="K13">
+        <v>203</v>
+      </c>
+      <c r="L13" s="8"/>
     </row>
     <row r="14" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
@@ -3261,7 +3284,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="5"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="7"/>
+      <c r="H14" s="6"/>
       <c r="I14" s="5"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -3270,157 +3293,76 @@
       <c r="A15" s="1"/>
       <c r="B15" s="3"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="9"/>
+      <c r="D15" s="7"/>
       <c r="E15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
-    <row r="16" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="3"/>
+      <c r="D16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="5"/>
-      <c r="E17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
     </row>
     <row r="18" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="5"/>
-      <c r="E18" s="3"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
     </row>
-    <row r="19" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
-      <c r="C19" s="5"/>
-      <c r="E19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="H19" s="7"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
-      <c r="C20" s="5"/>
-      <c r="E20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="H20" s="7"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B21" s="3"/>
-      <c r="C21" s="8"/>
-      <c r="E21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="H21" s="7"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B22" s="3"/>
-      <c r="C22" s="6"/>
-      <c r="E22" s="3"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+      <c r="D22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="7"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B23" s="3"/>
-      <c r="C23" s="6"/>
-      <c r="E23" s="3"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B24" s="3"/>
-      <c r="C24" s="8"/>
-      <c r="E24" s="3"/>
-      <c r="H24" s="9"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="3"/>
-      <c r="C25" s="6"/>
-      <c r="E25" s="3"/>
-      <c r="H25" s="9"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B26" s="3"/>
-      <c r="C26" s="6"/>
-      <c r="H26" s="9"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="3"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B27" s="3"/>
-      <c r="C27" s="6"/>
-      <c r="E27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="9"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D29" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D30" t="s">
-        <v>116</v>
-      </c>
-      <c r="E30">
-        <v>738</v>
-      </c>
-      <c r="F30" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D31" t="s">
-        <v>117</v>
-      </c>
-      <c r="E31">
-        <v>261</v>
-      </c>
-      <c r="F31" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D32" t="s">
-        <v>118</v>
-      </c>
-      <c r="E32">
-        <v>196</v>
-      </c>
-      <c r="F32" t="s">
-        <v>119</v>
-      </c>
+      <c r="D25" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-04-14 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7F5C41-6EC5-AD4A-8271-4126C729BE68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD2FA45-9AD6-3940-84B9-BAAB147DB516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -452,14 +452,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -1163,8 +1162,8 @@
   <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A71" sqref="A71"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2767,12 +2766,32 @@
         <v>109764</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="A70" s="1"/>
-      <c r="F70" s="5"/>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>43935.4375</v>
+      </c>
+      <c r="B70">
+        <v>101227</v>
+      </c>
+      <c r="C70">
+        <v>2107</v>
+      </c>
+      <c r="D70">
+        <v>7953</v>
+      </c>
+      <c r="E70">
+        <v>3568</v>
+      </c>
+      <c r="F70">
+        <v>334</v>
+      </c>
+      <c r="G70">
+        <v>115189</v>
+      </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
+      <c r="G71" s="3"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
@@ -2790,11 +2809,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2897,9 +2916,9 @@
       <c r="K3">
         <v>140</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -2935,9 +2954,9 @@
       <c r="K4">
         <v>152</v>
       </c>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -2973,9 +2992,9 @@
       <c r="K5">
         <v>154</v>
       </c>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -3011,9 +3030,9 @@
       <c r="K6">
         <v>160</v>
       </c>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -3049,9 +3068,9 @@
       <c r="K7">
         <v>187</v>
       </c>
-      <c r="L7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -3087,9 +3106,9 @@
       <c r="K8">
         <v>195</v>
       </c>
-      <c r="L8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -3125,9 +3144,9 @@
       <c r="K9">
         <v>214</v>
       </c>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -3163,9 +3182,9 @@
       <c r="K10">
         <v>217</v>
       </c>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="8"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -3201,9 +3220,9 @@
       <c r="K11">
         <v>215</v>
       </c>
-      <c r="L11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="N11" s="8"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -3239,7 +3258,7 @@
       <c r="K12">
         <v>196</v>
       </c>
-      <c r="L12" s="8"/>
+      <c r="L12" s="7"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -3275,25 +3294,48 @@
       <c r="K13">
         <v>203</v>
       </c>
-      <c r="L13" s="8"/>
-    </row>
-    <row r="14" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="5"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
+      <c r="L13" s="7"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>43935.4375</v>
+      </c>
+      <c r="B14">
+        <v>3511</v>
+      </c>
+      <c r="C14">
+        <v>4393</v>
+      </c>
+      <c r="D14">
+        <v>182</v>
+      </c>
+      <c r="E14">
+        <v>1912</v>
+      </c>
+      <c r="F14">
+        <v>2676</v>
+      </c>
+      <c r="G14">
+        <v>1890</v>
+      </c>
+      <c r="H14">
+        <v>1287</v>
+      </c>
+      <c r="I14">
+        <v>769</v>
+      </c>
+      <c r="J14">
+        <v>255</v>
+      </c>
+      <c r="K14">
+        <v>199</v>
+      </c>
     </row>
     <row r="15" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="3"/>
       <c r="C15" s="5"/>
-      <c r="D15" s="7"/>
+      <c r="D15" s="6"/>
       <c r="E15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -3301,14 +3343,13 @@
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="3"/>
-      <c r="D17" s="3"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="3"/>
@@ -3317,6 +3358,7 @@
     <row r="18" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="3"/>
+      <c r="E18" s="3"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="3"/>
@@ -3324,30 +3366,27 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="H19" s="7"/>
+      <c r="H19" s="6"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="H20" s="7"/>
+      <c r="H20" s="6"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="H21" s="7"/>
+      <c r="E21" s="3"/>
+      <c r="H21" s="6"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="7"/>
+      <c r="E22" s="3"/>
+      <c r="H22" s="6"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
@@ -3359,10 +3398,23 @@
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E27" s="3"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E29" s="3"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-04-15 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD2FA45-9AD6-3940-84B9-BAAB147DB516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D670AF-6ED4-2245-9089-1B883876A7E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -452,14 +452,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1162,8 +1161,8 @@
   <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G75" sqref="G75"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2790,8 +2789,27 @@
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="1"/>
-      <c r="G71" s="3"/>
+      <c r="A71" s="1">
+        <v>43936.4375</v>
+      </c>
+      <c r="B71">
+        <v>110787</v>
+      </c>
+      <c r="C71">
+        <v>4429</v>
+      </c>
+      <c r="D71">
+        <v>8447</v>
+      </c>
+      <c r="E71">
+        <v>3902</v>
+      </c>
+      <c r="F71">
+        <v>385</v>
+      </c>
+      <c r="G71">
+        <v>123521</v>
+      </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
@@ -2809,11 +2827,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2916,9 +2934,9 @@
       <c r="K3">
         <v>140</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" s="7"/>
-      <c r="N3" s="7"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -2954,9 +2972,9 @@
       <c r="K4">
         <v>152</v>
       </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -2992,9 +3010,9 @@
       <c r="K5">
         <v>154</v>
       </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -3030,9 +3048,9 @@
       <c r="K6">
         <v>160</v>
       </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -3068,9 +3086,9 @@
       <c r="K7">
         <v>187</v>
       </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -3106,9 +3124,9 @@
       <c r="K8">
         <v>195</v>
       </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -3144,9 +3162,9 @@
       <c r="K9">
         <v>214</v>
       </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -3182,9 +3200,9 @@
       <c r="K10">
         <v>217</v>
       </c>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -3220,9 +3238,9 @@
       <c r="K11">
         <v>215</v>
       </c>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -3258,7 +3276,7 @@
       <c r="K12">
         <v>196</v>
       </c>
-      <c r="L12" s="7"/>
+      <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -3294,7 +3312,7 @@
       <c r="K13">
         <v>203</v>
       </c>
-      <c r="L13" s="7"/>
+      <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -3331,14 +3349,40 @@
         <v>199</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>43936.4375</v>
+      </c>
+      <c r="B15">
+        <v>3679</v>
+      </c>
+      <c r="C15">
+        <v>4720</v>
+      </c>
+      <c r="D15">
+        <v>192</v>
+      </c>
+      <c r="E15">
+        <v>1997</v>
+      </c>
+      <c r="F15">
+        <v>2794</v>
+      </c>
+      <c r="G15">
+        <v>1989</v>
+      </c>
+      <c r="H15">
+        <v>1470</v>
+      </c>
+      <c r="I15">
+        <v>795</v>
+      </c>
+      <c r="J15">
+        <v>254</v>
+      </c>
+      <c r="K15">
+        <v>188</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
@@ -3366,55 +3410,58 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
-      <c r="H19" s="6"/>
+      <c r="F19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
-      <c r="H20" s="6"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="H21" s="6"/>
+      <c r="F21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="H22" s="6"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B23" s="3"/>
-      <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E26" s="3"/>
+      <c r="F25" s="3"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F28" s="3"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="F29" s="3"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F34" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-04-16 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D670AF-6ED4-2245-9089-1B883876A7E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE3C117-F75A-AD4D-930C-DA086D5F71E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -402,7 +402,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -430,6 +430,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF222222"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -448,11 +470,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -460,8 +483,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1161,8 +1190,8 @@
   <dimension ref="A1:H86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C81" sqref="C81"/>
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2812,26 +2841,87 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="1"/>
+      <c r="A72" s="1">
+        <v>43937.4375</v>
+      </c>
+      <c r="B72">
+        <v>114515</v>
+      </c>
+      <c r="C72">
+        <v>4323</v>
+      </c>
+      <c r="D72">
+        <v>8961</v>
+      </c>
+      <c r="E72">
+        <v>4194</v>
+      </c>
+      <c r="F72">
+        <v>423</v>
+      </c>
+      <c r="G72">
+        <v>132416</v>
+      </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
     </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G74" s="3"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+    </row>
+    <row r="79" spans="1:8" ht="20" x14ac:dyDescent="0.2">
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+    </row>
+    <row r="80" spans="1:8" ht="20" x14ac:dyDescent="0.2">
+      <c r="C80" s="8"/>
+      <c r="D80" s="9"/>
+      <c r="E80" s="5"/>
+    </row>
+    <row r="81" spans="3:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+      <c r="E81" s="5"/>
+    </row>
+    <row r="82" spans="3:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C82" s="8"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="5"/>
+    </row>
+    <row r="83" spans="3:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C83" s="8"/>
+      <c r="D83" s="5"/>
+      <c r="E83" s="5"/>
+    </row>
+    <row r="84" spans="3:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C84" s="10"/>
+      <c r="D84" s="5"/>
+      <c r="E84" s="5"/>
+    </row>
+    <row r="86" spans="3:7" x14ac:dyDescent="0.2">
       <c r="G86" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C78:E78"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J17" sqref="J17"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3385,11 +3475,39 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
+      <c r="A16" s="1">
+        <v>43937.4375</v>
+      </c>
+      <c r="B16">
+        <v>3855</v>
+      </c>
+      <c r="C16">
+        <v>5046</v>
+      </c>
+      <c r="D16">
+        <v>204</v>
+      </c>
+      <c r="E16">
+        <v>2091</v>
+      </c>
+      <c r="F16">
+        <v>2929</v>
+      </c>
+      <c r="G16">
+        <v>2093</v>
+      </c>
+      <c r="H16">
+        <v>1639</v>
+      </c>
+      <c r="I16">
+        <v>807</v>
+      </c>
+      <c r="J16">
+        <v>248</v>
+      </c>
+      <c r="K16">
+        <v>200</v>
+      </c>
     </row>
     <row r="17" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
@@ -3408,60 +3526,97 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="5"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="5"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B22" s="3"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="5"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B23" s="3"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="5"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F25" s="3"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F30" s="3"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F32" s="3"/>
-    </row>
-    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F33" s="3"/>
-    </row>
-    <row r="34" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F34" s="3"/>
+    <row r="24" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="D24" s="5"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="D25" s="5"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="D26" s="10"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="D27" s="8"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="D28" s="5"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="D29" s="8"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="D30" s="10"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="D31" s="8"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="D32" s="8"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="4:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="D33" s="8"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-04-17 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE3C117-F75A-AD4D-930C-DA086D5F71E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C226D358-1310-6D47-8834-3950162D6DA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1762" uniqueCount="123">
   <si>
     <t>Negative1</t>
   </si>
@@ -393,6 +393,18 @@
   </si>
   <si>
     <t>Number of patients in ICU7 on a ventilator with COVID-19</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Number of patients hospitalized with COVID-197</t>
+  </si>
+  <si>
+    <t>Number of patients in ICU8 with COVID-19</t>
+  </si>
+  <si>
+    <t>Number of patients in ICU8 on a ventilator with COVID-19</t>
   </si>
 </sst>
 </file>
@@ -1187,11 +1199,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:H86"/>
+  <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C82" sqref="C82"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2864,10 +2876,45 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="1"/>
+      <c r="A73" s="1">
+        <v>43938.4375</v>
+      </c>
+      <c r="B73" s="11">
+        <v>122433</v>
+      </c>
+      <c r="C73" s="11">
+        <v>5993</v>
+      </c>
+      <c r="D73" s="11">
+        <v>9525</v>
+      </c>
+      <c r="E73" s="11">
+        <v>4556</v>
+      </c>
+      <c r="F73" s="11">
+        <v>478</v>
+      </c>
+      <c r="G73" s="11">
+        <v>142985</v>
+      </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G74" s="3"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C75" s="11"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="11"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
+      <c r="E76" s="11"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C77" s="11"/>
+      <c r="D77" s="3"/>
+      <c r="E77" s="11"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C78" s="11"/>
@@ -2879,38 +2926,70 @@
       <c r="D79" s="7"/>
       <c r="E79" s="7"/>
     </row>
-    <row r="80" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="C80" s="8"/>
-      <c r="D80" s="9"/>
-      <c r="E80" s="5"/>
-    </row>
-    <row r="81" spans="3:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5"/>
-    </row>
-    <row r="82" spans="3:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C82" s="8"/>
-      <c r="D82" s="9"/>
-      <c r="E82" s="5"/>
-    </row>
-    <row r="83" spans="3:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C83" s="8"/>
-      <c r="D83" s="5"/>
-      <c r="E83" s="5"/>
-    </row>
-    <row r="84" spans="3:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C84" s="10"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
-    </row>
     <row r="86" spans="3:7" x14ac:dyDescent="0.2">
       <c r="G86" s="3"/>
     </row>
+    <row r="87" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C87" s="11"/>
+      <c r="D87" s="11"/>
+      <c r="E87" s="11"/>
+    </row>
+    <row r="88" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C88" s="11"/>
+      <c r="D88" s="3"/>
+      <c r="E88" s="11"/>
+    </row>
+    <row r="89" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C89" s="11"/>
+      <c r="D89" s="3"/>
+      <c r="E89" s="11"/>
+      <c r="F89" s="3"/>
+      <c r="G89" s="3"/>
+    </row>
+    <row r="90" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C90" s="11"/>
+      <c r="D90" s="3"/>
+      <c r="E90" s="11"/>
+    </row>
+    <row r="91" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C91" s="11"/>
+      <c r="D91" s="11"/>
+      <c r="E91" s="11"/>
+    </row>
+    <row r="92" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C92" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D92" s="11">
+        <v>829</v>
+      </c>
+      <c r="E92" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="93" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C93" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D93" s="11">
+        <v>245</v>
+      </c>
+      <c r="E93" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="94" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C94" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D94" s="11">
+        <v>200</v>
+      </c>
+      <c r="E94" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C78:E78"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2920,8 +2999,8 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3509,18 +3588,47 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-      <c r="B17" s="3"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>43938.4375</v>
+      </c>
+      <c r="B17" s="11">
+        <v>4074</v>
+      </c>
+      <c r="C17" s="11">
+        <v>5380</v>
+      </c>
+      <c r="D17" s="11">
+        <v>210</v>
+      </c>
+      <c r="E17" s="11">
+        <v>2164</v>
+      </c>
+      <c r="F17" s="11">
+        <v>3067</v>
+      </c>
+      <c r="G17" s="11">
+        <v>2214</v>
+      </c>
+      <c r="H17" s="11">
+        <v>1864</v>
+      </c>
+      <c r="I17" s="11">
+        <v>829</v>
+      </c>
+      <c r="J17" s="11">
+        <v>245</v>
+      </c>
+      <c r="K17" s="11">
+        <v>200</v>
+      </c>
     </row>
     <row r="18" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="5"/>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="3"/>
@@ -3536,7 +3644,7 @@
     </row>
     <row r="20" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
-      <c r="D20" s="5"/>
+      <c r="D20" s="8"/>
       <c r="E20" s="9"/>
       <c r="F20" s="5"/>
       <c r="J20" s="3"/>
@@ -3544,33 +3652,36 @@
     </row>
     <row r="21" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B21" s="3"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="9"/>
       <c r="F21" s="5"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B22" s="3"/>
+      <c r="C22" s="8"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="9"/>
+      <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B23" s="3"/>
+      <c r="C23" s="8"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="11"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="C24" s="8"/>
       <c r="D24" s="5"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="11"/>
     </row>
     <row r="25" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="D25" s="5"/>

</xml_diff>

<commit_message>
excel update 2020-04-18 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C226D358-1310-6D47-8834-3950162D6DA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EAA568-A793-1448-9ED8-F04647CC07B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1762" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="123">
   <si>
     <t>Negative1</t>
   </si>
@@ -395,9 +395,6 @@
     <t>Number of patients in ICU7 on a ventilator with COVID-19</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Number of patients hospitalized with COVID-197</t>
   </si>
   <si>
@@ -405,6 +402,9 @@
   </si>
   <si>
     <t>Number of patients in ICU8 on a ventilator with COVID-19</t>
+  </si>
+  <si>
+    <t>Hospitalizations</t>
   </si>
 </sst>
 </file>
@@ -1202,8 +1202,8 @@
   <dimension ref="A1:H94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C85" sqref="C85"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2899,7 +2899,27 @@
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G74" s="3"/>
+      <c r="A74" s="1">
+        <v>43939.4375</v>
+      </c>
+      <c r="B74" s="11">
+        <v>131055</v>
+      </c>
+      <c r="C74" s="11">
+        <v>6833</v>
+      </c>
+      <c r="D74" s="11">
+        <v>10010</v>
+      </c>
+      <c r="E74" s="11">
+        <v>4875</v>
+      </c>
+      <c r="F74" s="11">
+        <v>514</v>
+      </c>
+      <c r="G74" s="11">
+        <v>153287</v>
+      </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C75" s="11"/>
@@ -2912,7 +2932,7 @@
       <c r="E76" s="11"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C77" s="11"/>
+      <c r="C77" s="3"/>
       <c r="D77" s="3"/>
       <c r="E77" s="11"/>
     </row>
@@ -2926,68 +2946,34 @@
       <c r="D79" s="7"/>
       <c r="E79" s="7"/>
     </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="86" spans="5:7" x14ac:dyDescent="0.2">
       <c r="G86" s="3"/>
     </row>
-    <row r="87" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C87" s="11"/>
-      <c r="D87" s="11"/>
+    <row r="87" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E87" s="11"/>
     </row>
-    <row r="88" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C88" s="11"/>
-      <c r="D88" s="3"/>
+    <row r="88" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E88" s="11"/>
     </row>
-    <row r="89" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C89" s="11"/>
-      <c r="D89" s="3"/>
+    <row r="89" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E89" s="11"/>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
     </row>
-    <row r="90" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C90" s="11"/>
-      <c r="D90" s="3"/>
+    <row r="90" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E90" s="11"/>
     </row>
-    <row r="91" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C91" s="11"/>
-      <c r="D91" s="11"/>
+    <row r="91" spans="5:7" x14ac:dyDescent="0.2">
       <c r="E91" s="11"/>
     </row>
-    <row r="92" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C92" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="D92" s="11">
-        <v>829</v>
-      </c>
-      <c r="E92" s="11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="93" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C93" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="D93" s="11">
-        <v>245</v>
-      </c>
-      <c r="E93" s="11" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="94" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C94" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="D94" s="11">
-        <v>200</v>
-      </c>
-      <c r="E94" s="11" t="s">
-        <v>119</v>
-      </c>
+    <row r="92" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E92" s="11"/>
+    </row>
+    <row r="93" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E93" s="11"/>
+    </row>
+    <row r="94" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E94" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2996,11 +2982,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K19" sqref="K19"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3103,9 +3089,18 @@
       <c r="K3">
         <v>140</v>
       </c>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
+      <c r="L3" s="6">
+        <f>I3/SUM($B3:$C3)</f>
+        <v>0.14276885043263288</v>
+      </c>
+      <c r="M3" s="6">
+        <f t="shared" ref="M3:N18" si="0">J3/SUM($B3:$C3)</f>
+        <v>5.9950556242274411E-2</v>
+      </c>
+      <c r="N3" s="6">
+        <f t="shared" si="0"/>
+        <v>4.3263288009888753E-2</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -3141,9 +3136,18 @@
       <c r="K4">
         <v>152</v>
       </c>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
+      <c r="L4" s="6">
+        <f t="shared" ref="L4:L18" si="1">I4/SUM($B4:$C4)</f>
+        <v>0.14008859357696568</v>
+      </c>
+      <c r="M4" s="6">
+        <f t="shared" si="0"/>
+        <v>5.4263565891472867E-2</v>
+      </c>
+      <c r="N4" s="6">
+        <f t="shared" si="0"/>
+        <v>4.2081949058693245E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -3179,9 +3183,18 @@
       <c r="K5">
         <v>154</v>
       </c>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
+      <c r="L5" s="6">
+        <f t="shared" si="1"/>
+        <v>0.13009950248756219</v>
+      </c>
+      <c r="M5" s="6">
+        <f t="shared" si="0"/>
+        <v>4.975124378109453E-2</v>
+      </c>
+      <c r="N5" s="6">
+        <f t="shared" si="0"/>
+        <v>3.8308457711442784E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -3217,9 +3230,18 @@
       <c r="K6">
         <v>160</v>
       </c>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
+      <c r="L6" s="6">
+        <f t="shared" si="1"/>
+        <v>0.13624797594263244</v>
+      </c>
+      <c r="M6" s="6">
+        <f t="shared" si="0"/>
+        <v>4.9965301873698818E-2</v>
+      </c>
+      <c r="N6" s="6">
+        <f t="shared" si="0"/>
+        <v>3.7011334721258386E-2</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -3255,9 +3277,18 @@
       <c r="K7">
         <v>187</v>
       </c>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
+      <c r="L7" s="6">
+        <f t="shared" si="1"/>
+        <v>0.13063829787234044</v>
+      </c>
+      <c r="M7" s="6">
+        <f t="shared" si="0"/>
+        <v>4.9574468085106384E-2</v>
+      </c>
+      <c r="N7" s="6">
+        <f t="shared" si="0"/>
+        <v>3.9787234042553195E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -3293,9 +3324,18 @@
       <c r="K8">
         <v>195</v>
       </c>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
+      <c r="L8" s="6">
+        <f t="shared" si="1"/>
+        <v>0.11539195117299256</v>
+      </c>
+      <c r="M8" s="6">
+        <f t="shared" si="0"/>
+        <v>4.6919702460423422E-2</v>
+      </c>
+      <c r="N8" s="6">
+        <f t="shared" si="0"/>
+        <v>3.7192447072286861E-2</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -3331,9 +3371,18 @@
       <c r="K9">
         <v>214</v>
       </c>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
+      <c r="L9" s="6">
+        <f t="shared" si="1"/>
+        <v>0.11041229909154437</v>
+      </c>
+      <c r="M9" s="6">
+        <f t="shared" si="0"/>
+        <v>4.6121593291404611E-2</v>
+      </c>
+      <c r="N9" s="6">
+        <f t="shared" si="0"/>
+        <v>3.7386443046820407E-2</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -3369,9 +3418,18 @@
       <c r="K10">
         <v>217</v>
       </c>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
+      <c r="L10" s="6">
+        <f t="shared" si="1"/>
+        <v>0.1085483870967742</v>
+      </c>
+      <c r="M10" s="6">
+        <f t="shared" si="0"/>
+        <v>4.1935483870967745E-2</v>
+      </c>
+      <c r="N10" s="6">
+        <f t="shared" si="0"/>
+        <v>3.5000000000000003E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -3407,9 +3465,18 @@
       <c r="K11">
         <v>215</v>
       </c>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
+      <c r="L11" s="6">
+        <f t="shared" si="1"/>
+        <v>0.10460187708144111</v>
+      </c>
+      <c r="M11" s="6">
+        <f t="shared" si="0"/>
+        <v>3.8904026642446264E-2</v>
+      </c>
+      <c r="N11" s="6">
+        <f t="shared" si="0"/>
+        <v>3.2546170148349984E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -3445,7 +3512,18 @@
       <c r="K12">
         <v>196</v>
       </c>
-      <c r="L12" s="6"/>
+      <c r="L12" s="6">
+        <f t="shared" si="1"/>
+        <v>0.10532324818039104</v>
+      </c>
+      <c r="M12" s="6">
+        <f t="shared" si="0"/>
+        <v>3.724846581989439E-2</v>
+      </c>
+      <c r="N12" s="6">
+        <f t="shared" si="0"/>
+        <v>2.7972027972027972E-2</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -3481,7 +3559,18 @@
       <c r="K13">
         <v>203</v>
       </c>
-      <c r="L13" s="6"/>
+      <c r="L13" s="6">
+        <f t="shared" si="1"/>
+        <v>0.10232933889861316</v>
+      </c>
+      <c r="M13" s="6">
+        <f t="shared" si="0"/>
+        <v>3.5411337013599033E-2</v>
+      </c>
+      <c r="N13" s="6">
+        <f t="shared" si="0"/>
+        <v>2.7332704995287466E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -3517,6 +3606,18 @@
       <c r="K14">
         <v>199</v>
       </c>
+      <c r="L14" s="6">
+        <f t="shared" si="1"/>
+        <v>9.7292510121457496E-2</v>
+      </c>
+      <c r="M14" s="6">
+        <f t="shared" si="0"/>
+        <v>3.2262145748987857E-2</v>
+      </c>
+      <c r="N14" s="6">
+        <f t="shared" si="0"/>
+        <v>2.5177125506072876E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -3552,6 +3653,18 @@
       <c r="K15">
         <v>188</v>
       </c>
+      <c r="L15" s="6">
+        <f t="shared" si="1"/>
+        <v>9.4654125491129892E-2</v>
+      </c>
+      <c r="M15" s="6">
+        <f t="shared" si="0"/>
+        <v>3.0241695439933325E-2</v>
+      </c>
+      <c r="N15" s="6">
+        <f t="shared" si="0"/>
+        <v>2.2383617097273486E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -3587,8 +3700,20 @@
       <c r="K16">
         <v>200</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16" s="6">
+        <f t="shared" si="1"/>
+        <v>9.0663970340411196E-2</v>
+      </c>
+      <c r="M16" s="6">
+        <f t="shared" si="0"/>
+        <v>2.7862037973261432E-2</v>
+      </c>
+      <c r="N16" s="6">
+        <f t="shared" si="0"/>
+        <v>2.2469385462307607E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43938.4375</v>
       </c>
@@ -3622,54 +3747,101 @@
       <c r="K17" s="11">
         <v>200</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="3"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-    </row>
-    <row r="19" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="L17" s="6">
+        <f t="shared" si="1"/>
+        <v>8.7687751216416338E-2</v>
+      </c>
+      <c r="M17" s="6">
+        <f t="shared" si="0"/>
+        <v>2.5914956632113392E-2</v>
+      </c>
+      <c r="N17" s="6">
+        <f t="shared" si="0"/>
+        <v>2.115506663845991E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>43939.4375</v>
+      </c>
+      <c r="B18" s="11">
+        <v>4277</v>
+      </c>
+      <c r="C18" s="11">
+        <v>5658</v>
+      </c>
+      <c r="D18" s="11">
+        <v>223</v>
+      </c>
+      <c r="E18" s="11">
+        <v>2269</v>
+      </c>
+      <c r="F18" s="11">
+        <v>3201</v>
+      </c>
+      <c r="G18" s="11">
+        <v>2313</v>
+      </c>
+      <c r="H18" s="11">
+        <v>1996</v>
+      </c>
+      <c r="I18" s="11">
+        <v>828</v>
+      </c>
+      <c r="J18" s="11">
+        <v>250</v>
+      </c>
+      <c r="K18" s="11">
+        <v>197</v>
+      </c>
+      <c r="L18" s="6">
+        <f t="shared" si="1"/>
+        <v>8.334172118772018E-2</v>
+      </c>
+      <c r="M18" s="6">
+        <f t="shared" si="0"/>
+        <v>2.5163563160543533E-2</v>
+      </c>
+      <c r="N18" s="6">
+        <f t="shared" si="0"/>
+        <v>1.9828887770508303E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
       <c r="D19" s="5"/>
       <c r="E19" s="9"/>
       <c r="F19" s="5"/>
+      <c r="I19" s="4"/>
       <c r="J19" s="3"/>
       <c r="K19" s="3"/>
     </row>
-    <row r="20" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
       <c r="D20" s="8"/>
       <c r="E20" s="9"/>
       <c r="F20" s="5"/>
+      <c r="I20" s="4"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B21" s="3"/>
+    <row r="21" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+      <c r="C21" s="3"/>
       <c r="D21" s="8"/>
       <c r="E21" s="9"/>
       <c r="F21" s="5"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B22" s="3"/>
-      <c r="C22" s="8"/>
+    <row r="22" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+      <c r="C22" s="3"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B23" s="3"/>
-      <c r="C23" s="8"/>
+    <row r="23" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="D23" s="5"/>
       <c r="E23" s="5"/>
       <c r="F23" s="11"/>
@@ -3677,57 +3849,94 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="C24" s="8"/>
+    <row r="24" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+      <c r="C24" s="3"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+      <c r="C25" s="3"/>
       <c r="D25" s="5"/>
       <c r="E25" s="9"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+      <c r="C26" s="3"/>
       <c r="D26" s="10"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+      <c r="C27" s="3"/>
       <c r="D27" s="8"/>
       <c r="E27" s="9"/>
       <c r="F27" s="5"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
       <c r="D28" s="5"/>
       <c r="E28" s="9"/>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+      <c r="B29" s="11"/>
+      <c r="C29" s="3"/>
       <c r="D29" s="8"/>
       <c r="E29" s="9"/>
       <c r="F29" s="5"/>
     </row>
-    <row r="30" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+      <c r="B30" s="11"/>
+      <c r="C30" s="3"/>
       <c r="D30" s="10"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+      <c r="B31" s="11"/>
+      <c r="C31" s="3"/>
       <c r="D31" s="8"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
     </row>
-    <row r="32" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+      <c r="B32" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" s="11"/>
       <c r="D32" s="8"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="4:6" ht="20" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="B33" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33" s="11">
+        <v>828</v>
+      </c>
       <c r="D33" s="8"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C34" s="11">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" s="11">
+        <v>197</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel upate 2020-04-19 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EAA568-A793-1448-9ED8-F04647CC07B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1C32AD-5651-FD4C-87A8-90A1BA120875}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1760" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="120">
   <si>
     <t>Negative1</t>
   </si>
@@ -395,16 +395,7 @@
     <t>Number of patients in ICU7 on a ventilator with COVID-19</t>
   </si>
   <si>
-    <t>Number of patients hospitalized with COVID-197</t>
-  </si>
-  <si>
-    <t>Number of patients in ICU8 with COVID-19</t>
-  </si>
-  <si>
-    <t>Number of patients in ICU8 on a ventilator with COVID-19</t>
-  </si>
-  <si>
-    <t>Hospitalizations</t>
+    <t>Resolved2</t>
   </si>
 </sst>
 </file>
@@ -414,7 +405,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -430,12 +421,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color rgb="FF222222"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -448,21 +433,6 @@
       <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF222222"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -482,27 +452,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1199,11 +1164,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:H94"/>
+  <dimension ref="A1:H91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2879,22 +2844,22 @@
       <c r="A73" s="1">
         <v>43938.4375</v>
       </c>
-      <c r="B73" s="11">
+      <c r="B73" s="7">
         <v>122433</v>
       </c>
-      <c r="C73" s="11">
+      <c r="C73" s="7">
         <v>5993</v>
       </c>
-      <c r="D73" s="11">
+      <c r="D73" s="7">
         <v>9525</v>
       </c>
-      <c r="E73" s="11">
+      <c r="E73" s="7">
         <v>4556</v>
       </c>
-      <c r="F73" s="11">
+      <c r="F73" s="7">
         <v>478</v>
       </c>
-      <c r="G73" s="11">
+      <c r="G73" s="7">
         <v>142985</v>
       </c>
     </row>
@@ -2902,78 +2867,83 @@
       <c r="A74" s="1">
         <v>43939.4375</v>
       </c>
-      <c r="B74" s="11">
+      <c r="B74" s="7">
         <v>131055</v>
       </c>
-      <c r="C74" s="11">
+      <c r="C74" s="7">
         <v>6833</v>
       </c>
-      <c r="D74" s="11">
+      <c r="D74" s="7">
         <v>10010</v>
       </c>
-      <c r="E74" s="11">
+      <c r="E74" s="7">
         <v>4875</v>
       </c>
-      <c r="F74" s="11">
+      <c r="F74" s="7">
         <v>514</v>
       </c>
-      <c r="G74" s="11">
+      <c r="G74" s="7">
         <v>153287</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C75" s="11"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="11"/>
+      <c r="A75" s="1">
+        <v>43940.4375</v>
+      </c>
+      <c r="B75" s="7">
+        <v>139757</v>
+      </c>
+      <c r="C75" s="7">
+        <v>5736</v>
+      </c>
+      <c r="D75" s="7">
+        <v>10578</v>
+      </c>
+      <c r="E75" s="7">
+        <v>5209</v>
+      </c>
+      <c r="F75" s="7">
+        <v>553</v>
+      </c>
+      <c r="G75" s="7">
+        <v>161833</v>
+      </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C76" s="11"/>
-      <c r="D76" s="11"/>
-      <c r="E76" s="11"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
-      <c r="E77" s="11"/>
+      <c r="E77" s="7"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C78" s="11"/>
-      <c r="D78" s="11"/>
-      <c r="E78" s="11"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
     </row>
     <row r="79" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="C79" s="7"/>
-      <c r="D79" s="7"/>
-      <c r="E79" s="7"/>
-    </row>
-    <row r="86" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="C79" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D79" s="8">
+        <v>5209</v>
+      </c>
+      <c r="E79" s="6">
+        <v>49.2</v>
+      </c>
+    </row>
+    <row r="86" spans="6:7" x14ac:dyDescent="0.2">
       <c r="G86" s="3"/>
     </row>
-    <row r="87" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E87" s="11"/>
-    </row>
-    <row r="88" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E88" s="11"/>
-    </row>
-    <row r="89" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E89" s="11"/>
+    <row r="89" spans="6:7" x14ac:dyDescent="0.2">
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
     </row>
-    <row r="90" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E90" s="11"/>
-    </row>
-    <row r="91" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E91" s="11"/>
-    </row>
-    <row r="92" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E92" s="11"/>
-    </row>
-    <row r="93" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E93" s="11"/>
-    </row>
-    <row r="94" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E94" s="11"/>
+    <row r="91" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="F91" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2986,7 +2956,7 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3089,18 +3059,9 @@
       <c r="K3">
         <v>140</v>
       </c>
-      <c r="L3" s="6">
-        <f>I3/SUM($B3:$C3)</f>
-        <v>0.14276885043263288</v>
-      </c>
-      <c r="M3" s="6">
-        <f t="shared" ref="M3:N18" si="0">J3/SUM($B3:$C3)</f>
-        <v>5.9950556242274411E-2</v>
-      </c>
-      <c r="N3" s="6">
-        <f t="shared" si="0"/>
-        <v>4.3263288009888753E-2</v>
-      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -3136,18 +3097,9 @@
       <c r="K4">
         <v>152</v>
       </c>
-      <c r="L4" s="6">
-        <f t="shared" ref="L4:L18" si="1">I4/SUM($B4:$C4)</f>
-        <v>0.14008859357696568</v>
-      </c>
-      <c r="M4" s="6">
-        <f t="shared" si="0"/>
-        <v>5.4263565891472867E-2</v>
-      </c>
-      <c r="N4" s="6">
-        <f t="shared" si="0"/>
-        <v>4.2081949058693245E-2</v>
-      </c>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -3183,18 +3135,9 @@
       <c r="K5">
         <v>154</v>
       </c>
-      <c r="L5" s="6">
-        <f t="shared" si="1"/>
-        <v>0.13009950248756219</v>
-      </c>
-      <c r="M5" s="6">
-        <f t="shared" si="0"/>
-        <v>4.975124378109453E-2</v>
-      </c>
-      <c r="N5" s="6">
-        <f t="shared" si="0"/>
-        <v>3.8308457711442784E-2</v>
-      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -3230,18 +3173,9 @@
       <c r="K6">
         <v>160</v>
       </c>
-      <c r="L6" s="6">
-        <f t="shared" si="1"/>
-        <v>0.13624797594263244</v>
-      </c>
-      <c r="M6" s="6">
-        <f t="shared" si="0"/>
-        <v>4.9965301873698818E-2</v>
-      </c>
-      <c r="N6" s="6">
-        <f t="shared" si="0"/>
-        <v>3.7011334721258386E-2</v>
-      </c>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -3277,18 +3211,9 @@
       <c r="K7">
         <v>187</v>
       </c>
-      <c r="L7" s="6">
-        <f t="shared" si="1"/>
-        <v>0.13063829787234044</v>
-      </c>
-      <c r="M7" s="6">
-        <f t="shared" si="0"/>
-        <v>4.9574468085106384E-2</v>
-      </c>
-      <c r="N7" s="6">
-        <f t="shared" si="0"/>
-        <v>3.9787234042553195E-2</v>
-      </c>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -3324,18 +3249,9 @@
       <c r="K8">
         <v>195</v>
       </c>
-      <c r="L8" s="6">
-        <f t="shared" si="1"/>
-        <v>0.11539195117299256</v>
-      </c>
-      <c r="M8" s="6">
-        <f t="shared" si="0"/>
-        <v>4.6919702460423422E-2</v>
-      </c>
-      <c r="N8" s="6">
-        <f t="shared" si="0"/>
-        <v>3.7192447072286861E-2</v>
-      </c>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -3371,18 +3287,9 @@
       <c r="K9">
         <v>214</v>
       </c>
-      <c r="L9" s="6">
-        <f t="shared" si="1"/>
-        <v>0.11041229909154437</v>
-      </c>
-      <c r="M9" s="6">
-        <f t="shared" si="0"/>
-        <v>4.6121593291404611E-2</v>
-      </c>
-      <c r="N9" s="6">
-        <f t="shared" si="0"/>
-        <v>3.7386443046820407E-2</v>
-      </c>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -3418,18 +3325,9 @@
       <c r="K10">
         <v>217</v>
       </c>
-      <c r="L10" s="6">
-        <f t="shared" si="1"/>
-        <v>0.1085483870967742</v>
-      </c>
-      <c r="M10" s="6">
-        <f t="shared" si="0"/>
-        <v>4.1935483870967745E-2</v>
-      </c>
-      <c r="N10" s="6">
-        <f t="shared" si="0"/>
-        <v>3.5000000000000003E-2</v>
-      </c>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -3465,18 +3363,9 @@
       <c r="K11">
         <v>215</v>
       </c>
-      <c r="L11" s="6">
-        <f t="shared" si="1"/>
-        <v>0.10460187708144111</v>
-      </c>
-      <c r="M11" s="6">
-        <f t="shared" si="0"/>
-        <v>3.8904026642446264E-2</v>
-      </c>
-      <c r="N11" s="6">
-        <f t="shared" si="0"/>
-        <v>3.2546170148349984E-2</v>
-      </c>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -3512,18 +3401,9 @@
       <c r="K12">
         <v>196</v>
       </c>
-      <c r="L12" s="6">
-        <f t="shared" si="1"/>
-        <v>0.10532324818039104</v>
-      </c>
-      <c r="M12" s="6">
-        <f t="shared" si="0"/>
-        <v>3.724846581989439E-2</v>
-      </c>
-      <c r="N12" s="6">
-        <f t="shared" si="0"/>
-        <v>2.7972027972027972E-2</v>
-      </c>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -3559,18 +3439,9 @@
       <c r="K13">
         <v>203</v>
       </c>
-      <c r="L13" s="6">
-        <f t="shared" si="1"/>
-        <v>0.10232933889861316</v>
-      </c>
-      <c r="M13" s="6">
-        <f t="shared" si="0"/>
-        <v>3.5411337013599033E-2</v>
-      </c>
-      <c r="N13" s="6">
-        <f t="shared" si="0"/>
-        <v>2.7332704995287466E-2</v>
-      </c>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -3606,18 +3477,9 @@
       <c r="K14">
         <v>199</v>
       </c>
-      <c r="L14" s="6">
-        <f t="shared" si="1"/>
-        <v>9.7292510121457496E-2</v>
-      </c>
-      <c r="M14" s="6">
-        <f t="shared" si="0"/>
-        <v>3.2262145748987857E-2</v>
-      </c>
-      <c r="N14" s="6">
-        <f t="shared" si="0"/>
-        <v>2.5177125506072876E-2</v>
-      </c>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -3653,18 +3515,9 @@
       <c r="K15">
         <v>188</v>
       </c>
-      <c r="L15" s="6">
-        <f t="shared" si="1"/>
-        <v>9.4654125491129892E-2</v>
-      </c>
-      <c r="M15" s="6">
-        <f t="shared" si="0"/>
-        <v>3.0241695439933325E-2</v>
-      </c>
-      <c r="N15" s="6">
-        <f t="shared" si="0"/>
-        <v>2.2383617097273486E-2</v>
-      </c>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -3700,243 +3553,203 @@
       <c r="K16">
         <v>200</v>
       </c>
-      <c r="L16" s="6">
-        <f t="shared" si="1"/>
-        <v>9.0663970340411196E-2</v>
-      </c>
-      <c r="M16" s="6">
-        <f t="shared" si="0"/>
-        <v>2.7862037973261432E-2</v>
-      </c>
-      <c r="N16" s="6">
-        <f t="shared" si="0"/>
-        <v>2.2469385462307607E-2</v>
-      </c>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43938.4375</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17" s="7">
         <v>4074</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="7">
         <v>5380</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="7">
         <v>210</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="7">
         <v>2164</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="7">
         <v>3067</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="7">
         <v>2214</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="7">
         <v>1864</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="7">
         <v>829</v>
       </c>
-      <c r="J17" s="11">
+      <c r="J17" s="7">
         <v>245</v>
       </c>
-      <c r="K17" s="11">
+      <c r="K17" s="7">
         <v>200</v>
       </c>
-      <c r="L17" s="6">
-        <f t="shared" si="1"/>
-        <v>8.7687751216416338E-2</v>
-      </c>
-      <c r="M17" s="6">
-        <f t="shared" si="0"/>
-        <v>2.5914956632113392E-2</v>
-      </c>
-      <c r="N17" s="6">
-        <f t="shared" si="0"/>
-        <v>2.115506663845991E-2</v>
-      </c>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43939.4375</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18" s="7">
         <v>4277</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="7">
         <v>5658</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="7">
         <v>223</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="7">
         <v>2269</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="7">
         <v>3201</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="7">
         <v>2313</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="7">
         <v>1996</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I18" s="7">
         <v>828</v>
       </c>
-      <c r="J18" s="11">
+      <c r="J18" s="7">
         <v>250</v>
       </c>
-      <c r="K18" s="11">
+      <c r="K18" s="7">
         <v>197</v>
       </c>
-      <c r="L18" s="6">
-        <f t="shared" si="1"/>
-        <v>8.334172118772018E-2</v>
-      </c>
-      <c r="M18" s="6">
-        <f t="shared" si="0"/>
-        <v>2.5163563160543533E-2</v>
-      </c>
-      <c r="N18" s="6">
-        <f t="shared" si="0"/>
-        <v>1.9828887770508303E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="B19" s="3"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="5"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-    </row>
-    <row r="20" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>43940.4375</v>
+      </c>
+      <c r="B19" s="7">
+        <v>4495</v>
+      </c>
+      <c r="C19" s="7">
+        <v>5996</v>
+      </c>
+      <c r="D19" s="7">
+        <v>235</v>
+      </c>
+      <c r="E19" s="7">
+        <v>2408</v>
+      </c>
+      <c r="F19" s="7">
+        <v>3354</v>
+      </c>
+      <c r="G19" s="7">
+        <v>2437</v>
+      </c>
+      <c r="H19" s="7">
+        <v>2135</v>
+      </c>
+      <c r="I19" s="7">
+        <v>809</v>
+      </c>
+      <c r="J19" s="7">
+        <v>247</v>
+      </c>
+      <c r="K19" s="7">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="5"/>
+      <c r="E20" s="3"/>
       <c r="I20" s="4"/>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C21" s="3"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="5"/>
+      <c r="E21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C22" s="3"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="11"/>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="E23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C24" s="3"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="11"/>
-    </row>
-    <row r="25" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C25" s="3"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="5"/>
-    </row>
-    <row r="26" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+      <c r="E25" s="3"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C26" s="3"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-    </row>
-    <row r="27" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+      <c r="E26" s="3"/>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C27" s="3"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="5"/>
+      <c r="F27" s="7"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="5"/>
-    </row>
-    <row r="29" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="B29" s="11"/>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B29" s="7"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="5"/>
-    </row>
-    <row r="30" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="B30" s="11"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B30" s="7"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-    </row>
-    <row r="31" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="B31" s="11"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B31" s="7"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-    </row>
-    <row r="32" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="B32" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-    </row>
-    <row r="33" spans="2:6" ht="20" x14ac:dyDescent="0.2">
-      <c r="B33" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="C33" s="11">
-        <v>828</v>
-      </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B34" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="C34" s="11">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B35" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C35" s="11">
-        <v>197</v>
-      </c>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-04-20 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1C32AD-5651-FD4C-87A8-90A1BA120875}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DBA684-4612-A54E-B424-30E5335C53A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1756" uniqueCount="119">
   <si>
     <t>Negative1</t>
   </si>
@@ -393,9 +393,6 @@
   </si>
   <si>
     <t>Number of patients in ICU7 on a ventilator with COVID-19</t>
-  </si>
-  <si>
-    <t>Resolved2</t>
   </si>
 </sst>
 </file>
@@ -1167,8 +1164,8 @@
   <dimension ref="A1:H91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A85" sqref="A85"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2910,9 +2907,27 @@
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C76" s="7"/>
-      <c r="D76" s="7"/>
-      <c r="E76" s="7"/>
+      <c r="A76" s="1">
+        <v>43941.4375</v>
+      </c>
+      <c r="B76" s="7">
+        <v>147557</v>
+      </c>
+      <c r="C76" s="7">
+        <v>3799</v>
+      </c>
+      <c r="D76" s="7">
+        <v>11184</v>
+      </c>
+      <c r="E76" s="7">
+        <v>5515</v>
+      </c>
+      <c r="F76" s="7">
+        <v>584</v>
+      </c>
+      <c r="G76" s="7">
+        <v>168639</v>
+      </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C77" s="3"/>
@@ -2925,15 +2940,9 @@
       <c r="E78" s="7"/>
     </row>
     <row r="79" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="C79" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D79" s="8">
-        <v>5209</v>
-      </c>
-      <c r="E79" s="6">
-        <v>49.2</v>
-      </c>
+      <c r="C79" s="6"/>
+      <c r="D79" s="8"/>
+      <c r="E79" s="6"/>
     </row>
     <row r="86" spans="6:7" x14ac:dyDescent="0.2">
       <c r="G86" s="3"/>
@@ -2955,8 +2964,8 @@
   <dimension ref="A1:N35"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3669,11 +3678,39 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="3"/>
+      <c r="A20" s="1">
+        <v>43941.4375</v>
+      </c>
+      <c r="B20" s="7">
+        <v>4728</v>
+      </c>
+      <c r="C20" s="7">
+        <v>6354</v>
+      </c>
+      <c r="D20" s="7">
+        <v>248</v>
+      </c>
+      <c r="E20" s="7">
+        <v>2525</v>
+      </c>
+      <c r="F20" s="7">
+        <v>3502</v>
+      </c>
+      <c r="G20" s="7">
+        <v>2580</v>
+      </c>
+      <c r="H20" s="7">
+        <v>2312</v>
+      </c>
+      <c r="I20" s="7">
+        <v>802</v>
+      </c>
+      <c r="J20" s="7">
+        <v>247</v>
+      </c>
+      <c r="K20" s="7">
+        <v>193</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C21" s="3"/>
@@ -3682,74 +3719,70 @@
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C24" s="3"/>
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
       <c r="F27" s="7"/>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
+      <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B29" s="7"/>
-      <c r="C29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B30" s="7"/>
-      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B31" s="7"/>
-      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
       <c r="F31" s="7"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
+      <c r="D32" s="3"/>
       <c r="F32" s="7"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-04-21 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DBA684-4612-A54E-B424-30E5335C53A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08938E30-5C4E-D843-8DE5-9BE096E81A63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -453,7 +453,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -462,7 +462,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1161,11 +1160,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:H91"/>
+  <dimension ref="A1:H99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C73" sqref="C73"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2930,9 +2929,27 @@
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="7"/>
+      <c r="A77" s="1">
+        <v>43942.4375</v>
+      </c>
+      <c r="B77">
+        <v>156007</v>
+      </c>
+      <c r="C77" s="7">
+        <v>5546</v>
+      </c>
+      <c r="D77" s="7">
+        <v>11735</v>
+      </c>
+      <c r="E77" s="7">
+        <v>5806</v>
+      </c>
+      <c r="F77" s="7">
+        <v>622</v>
+      </c>
+      <c r="G77">
+        <v>179716</v>
+      </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C78" s="3"/>
@@ -2941,18 +2958,40 @@
     </row>
     <row r="79" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="C79" s="6"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="6"/>
-    </row>
-    <row r="86" spans="6:7" x14ac:dyDescent="0.2">
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+    </row>
+    <row r="81" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+    </row>
+    <row r="82" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
+    </row>
+    <row r="83" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+    </row>
+    <row r="86" spans="4:7" x14ac:dyDescent="0.2">
       <c r="G86" s="3"/>
     </row>
-    <row r="89" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F89" s="3"/>
+    <row r="89" spans="4:7" x14ac:dyDescent="0.2">
       <c r="G89" s="3"/>
     </row>
-    <row r="91" spans="6:7" x14ac:dyDescent="0.2">
-      <c r="F91" s="3"/>
+    <row r="99" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D99" s="7"/>
+      <c r="E99" s="7"/>
+      <c r="F99" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2961,11 +3000,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3713,10 +3752,39 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="3"/>
+      <c r="A21" s="1">
+        <v>43942.4375</v>
+      </c>
+      <c r="B21" s="7">
+        <v>4955</v>
+      </c>
+      <c r="C21" s="7">
+        <v>6663</v>
+      </c>
+      <c r="D21" s="7">
+        <v>260</v>
+      </c>
+      <c r="E21" s="7">
+        <v>2657</v>
+      </c>
+      <c r="F21" s="7">
+        <v>3665</v>
+      </c>
+      <c r="G21" s="7">
+        <v>2687</v>
+      </c>
+      <c r="H21" s="7">
+        <v>2457</v>
+      </c>
+      <c r="I21" s="7">
+        <v>859</v>
+      </c>
+      <c r="J21" s="7">
+        <v>250</v>
+      </c>
+      <c r="K21" s="7">
+        <v>194</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D22" s="3"/>
@@ -3724,65 +3792,91 @@
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="E24" s="3"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
       <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D27" s="3"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B28" s="7"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
       <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B29" s="7"/>
-      <c r="E29" s="3"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B30" s="7"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B31" s="7"/>
-      <c r="D31" s="3"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
       <c r="F31" s="7"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B32" s="7"/>
-      <c r="D32" s="3"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
       <c r="F32" s="7"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" s="7"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" s="7"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-04-22 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08938E30-5C4E-D843-8DE5-9BE096E81A63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFBBD2B-F989-CB45-B41C-559656161773}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -453,7 +453,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -462,6 +462,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1163,8 +1164,8 @@
   <dimension ref="A1:H99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C91" sqref="C91"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C85" sqref="C85:D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2952,9 +2953,27 @@
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C78" s="3"/>
-      <c r="D78" s="7"/>
-      <c r="E78" s="7"/>
+      <c r="A78" s="1">
+        <v>43943.4375</v>
+      </c>
+      <c r="B78" s="7">
+        <v>165406</v>
+      </c>
+      <c r="C78" s="7">
+        <v>6845</v>
+      </c>
+      <c r="D78" s="7">
+        <v>12245</v>
+      </c>
+      <c r="E78" s="7">
+        <v>6221</v>
+      </c>
+      <c r="F78" s="7">
+        <v>659</v>
+      </c>
+      <c r="G78" s="7">
+        <v>191376</v>
+      </c>
     </row>
     <row r="79" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="C79" s="6"/>
@@ -2963,7 +2982,7 @@
       <c r="F79" s="7"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D80" s="7"/>
+      <c r="D80" s="3"/>
       <c r="E80" s="7"/>
       <c r="F80" s="7"/>
     </row>
@@ -2973,7 +2992,7 @@
       <c r="F81" s="7"/>
     </row>
     <row r="82" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D82" s="7"/>
+      <c r="D82" s="3"/>
       <c r="E82" s="7"/>
       <c r="F82" s="7"/>
     </row>
@@ -2988,8 +3007,10 @@
     <row r="89" spans="4:7" x14ac:dyDescent="0.2">
       <c r="G89" s="3"/>
     </row>
-    <row r="99" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D99" s="7"/>
+    <row r="93" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="F93" s="3"/>
+    </row>
+    <row r="99" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E99" s="7"/>
       <c r="F99" s="7"/>
     </row>
@@ -3000,11 +3021,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N37"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3145,7 +3166,7 @@
       <c r="K4">
         <v>152</v>
       </c>
-      <c r="L4" s="5"/>
+      <c r="L4" s="8"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
     </row>
@@ -3183,7 +3204,7 @@
       <c r="K5">
         <v>154</v>
       </c>
-      <c r="L5" s="5"/>
+      <c r="L5" s="8"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
     </row>
@@ -3221,7 +3242,7 @@
       <c r="K6">
         <v>160</v>
       </c>
-      <c r="L6" s="5"/>
+      <c r="L6" s="8"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
     </row>
@@ -3259,7 +3280,7 @@
       <c r="K7">
         <v>187</v>
       </c>
-      <c r="L7" s="5"/>
+      <c r="L7" s="8"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
     </row>
@@ -3297,7 +3318,7 @@
       <c r="K8">
         <v>195</v>
       </c>
-      <c r="L8" s="5"/>
+      <c r="L8" s="8"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
     </row>
@@ -3335,7 +3356,7 @@
       <c r="K9">
         <v>214</v>
       </c>
-      <c r="L9" s="5"/>
+      <c r="L9" s="8"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
     </row>
@@ -3373,7 +3394,7 @@
       <c r="K10">
         <v>217</v>
       </c>
-      <c r="L10" s="5"/>
+      <c r="L10" s="8"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
@@ -3411,7 +3432,7 @@
       <c r="K11">
         <v>215</v>
       </c>
-      <c r="L11" s="5"/>
+      <c r="L11" s="8"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
     </row>
@@ -3449,7 +3470,7 @@
       <c r="K12">
         <v>196</v>
       </c>
-      <c r="L12" s="5"/>
+      <c r="L12" s="8"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
     </row>
@@ -3487,7 +3508,7 @@
       <c r="K13">
         <v>203</v>
       </c>
-      <c r="L13" s="5"/>
+      <c r="L13" s="8"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
     </row>
@@ -3525,7 +3546,7 @@
       <c r="K14">
         <v>199</v>
       </c>
-      <c r="L14" s="5"/>
+      <c r="L14" s="8"/>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
     </row>
@@ -3563,7 +3584,7 @@
       <c r="K15">
         <v>188</v>
       </c>
-      <c r="L15" s="5"/>
+      <c r="L15" s="8"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
     </row>
@@ -3601,7 +3622,7 @@
       <c r="K16">
         <v>200</v>
       </c>
-      <c r="L16" s="5"/>
+      <c r="L16" s="8"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
     </row>
@@ -3639,7 +3660,7 @@
       <c r="K17" s="7">
         <v>200</v>
       </c>
-      <c r="L17" s="5"/>
+      <c r="L17" s="8"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
     </row>
@@ -3677,7 +3698,7 @@
       <c r="K18" s="7">
         <v>197</v>
       </c>
-      <c r="L18" s="5"/>
+      <c r="L18" s="8"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
     </row>
@@ -3715,6 +3736,7 @@
       <c r="K19" s="7">
         <v>196</v>
       </c>
+      <c r="L19" s="8"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -3750,6 +3772,7 @@
       <c r="K20" s="7">
         <v>193</v>
       </c>
+      <c r="L20" s="8"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -3785,11 +3808,43 @@
       <c r="K21" s="7">
         <v>194</v>
       </c>
+      <c r="L21" s="8"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="3"/>
+      <c r="A22" s="1">
+        <v>43943.4375</v>
+      </c>
+      <c r="B22" s="7">
+        <v>5169</v>
+      </c>
+      <c r="C22" s="7">
+        <v>6952</v>
+      </c>
+      <c r="D22" s="7">
+        <v>270</v>
+      </c>
+      <c r="E22" s="7">
+        <v>2781</v>
+      </c>
+      <c r="F22" s="7">
+        <v>3798</v>
+      </c>
+      <c r="G22" s="7">
+        <v>2778</v>
+      </c>
+      <c r="H22" s="7">
+        <v>2609</v>
+      </c>
+      <c r="I22" s="7">
+        <v>878</v>
+      </c>
+      <c r="J22" s="7">
+        <v>243</v>
+      </c>
+      <c r="K22" s="7">
+        <v>192</v>
+      </c>
+      <c r="L22" s="8"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D23" s="7"/>
@@ -3800,83 +3855,67 @@
       <c r="K23" s="3"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
+      <c r="E24" s="3"/>
       <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
+      <c r="E25" s="3"/>
       <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
       <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
+      <c r="E27" s="3"/>
       <c r="F27" s="7"/>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
+      <c r="E28" s="3"/>
       <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
+      <c r="E29" s="3"/>
       <c r="F29" s="7"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
+      <c r="E30" s="3"/>
       <c r="F30" s="7"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
       <c r="F31" s="7"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
+      <c r="E32" s="3"/>
       <c r="F32" s="7"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
+      <c r="E33" s="3"/>
       <c r="F33" s="7"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
+      <c r="E34" s="3"/>
       <c r="F34" s="7"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
       <c r="F35" s="7"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
       <c r="F36" s="7"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
       <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E38" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-04-23 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAFBBD2B-F989-CB45-B41C-559656161773}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAA4E3E-24E8-CB43-8C9A-8C5995CB3A27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -402,7 +402,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -423,13 +423,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -453,14 +446,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -1163,9 +1155,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
   <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C85" sqref="C85:D99"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D96" sqref="C85:D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2841,22 +2833,22 @@
       <c r="A73" s="1">
         <v>43938.4375</v>
       </c>
-      <c r="B73" s="7">
+      <c r="B73" s="6">
         <v>122433</v>
       </c>
-      <c r="C73" s="7">
+      <c r="C73" s="6">
         <v>5993</v>
       </c>
-      <c r="D73" s="7">
+      <c r="D73" s="6">
         <v>9525</v>
       </c>
-      <c r="E73" s="7">
+      <c r="E73" s="6">
         <v>4556</v>
       </c>
-      <c r="F73" s="7">
+      <c r="F73" s="6">
         <v>478</v>
       </c>
-      <c r="G73" s="7">
+      <c r="G73" s="6">
         <v>142985</v>
       </c>
     </row>
@@ -2864,22 +2856,22 @@
       <c r="A74" s="1">
         <v>43939.4375</v>
       </c>
-      <c r="B74" s="7">
+      <c r="B74" s="6">
         <v>131055</v>
       </c>
-      <c r="C74" s="7">
+      <c r="C74" s="6">
         <v>6833</v>
       </c>
-      <c r="D74" s="7">
+      <c r="D74" s="6">
         <v>10010</v>
       </c>
-      <c r="E74" s="7">
+      <c r="E74" s="6">
         <v>4875</v>
       </c>
-      <c r="F74" s="7">
+      <c r="F74" s="6">
         <v>514</v>
       </c>
-      <c r="G74" s="7">
+      <c r="G74" s="6">
         <v>153287</v>
       </c>
     </row>
@@ -2887,22 +2879,22 @@
       <c r="A75" s="1">
         <v>43940.4375</v>
       </c>
-      <c r="B75" s="7">
+      <c r="B75" s="6">
         <v>139757</v>
       </c>
-      <c r="C75" s="7">
+      <c r="C75" s="6">
         <v>5736</v>
       </c>
-      <c r="D75" s="7">
+      <c r="D75" s="6">
         <v>10578</v>
       </c>
-      <c r="E75" s="7">
+      <c r="E75" s="6">
         <v>5209</v>
       </c>
-      <c r="F75" s="7">
+      <c r="F75" s="6">
         <v>553</v>
       </c>
-      <c r="G75" s="7">
+      <c r="G75" s="6">
         <v>161833</v>
       </c>
     </row>
@@ -2910,22 +2902,22 @@
       <c r="A76" s="1">
         <v>43941.4375</v>
       </c>
-      <c r="B76" s="7">
+      <c r="B76" s="6">
         <v>147557</v>
       </c>
-      <c r="C76" s="7">
+      <c r="C76" s="6">
         <v>3799</v>
       </c>
-      <c r="D76" s="7">
+      <c r="D76" s="6">
         <v>11184</v>
       </c>
-      <c r="E76" s="7">
+      <c r="E76" s="6">
         <v>5515</v>
       </c>
-      <c r="F76" s="7">
+      <c r="F76" s="6">
         <v>584</v>
       </c>
-      <c r="G76" s="7">
+      <c r="G76" s="6">
         <v>168639</v>
       </c>
     </row>
@@ -2936,16 +2928,16 @@
       <c r="B77">
         <v>156007</v>
       </c>
-      <c r="C77" s="7">
+      <c r="C77" s="6">
         <v>5546</v>
       </c>
-      <c r="D77" s="7">
+      <c r="D77" s="6">
         <v>11735</v>
       </c>
-      <c r="E77" s="7">
+      <c r="E77" s="6">
         <v>5806</v>
       </c>
-      <c r="F77" s="7">
+      <c r="F77" s="6">
         <v>622</v>
       </c>
       <c r="G77">
@@ -2956,50 +2948,67 @@
       <c r="A78" s="1">
         <v>43943.4375</v>
       </c>
-      <c r="B78" s="7">
+      <c r="B78" s="6">
         <v>165406</v>
       </c>
-      <c r="C78" s="7">
+      <c r="C78" s="6">
         <v>6845</v>
       </c>
-      <c r="D78" s="7">
+      <c r="D78" s="6">
         <v>12245</v>
       </c>
-      <c r="E78" s="7">
+      <c r="E78" s="6">
         <v>6221</v>
       </c>
-      <c r="F78" s="7">
+      <c r="F78" s="6">
         <v>659</v>
       </c>
-      <c r="G78" s="7">
+      <c r="G78" s="6">
         <v>191376</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="C79" s="6"/>
-      <c r="D79" s="7"/>
-      <c r="E79" s="7"/>
-      <c r="F79" s="7"/>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>43944.4375</v>
+      </c>
+      <c r="B79" s="6">
+        <v>174473</v>
+      </c>
+      <c r="C79" s="6">
+        <v>6757</v>
+      </c>
+      <c r="D79" s="6">
+        <v>12879</v>
+      </c>
+      <c r="E79" s="6">
+        <v>6680</v>
+      </c>
+      <c r="F79" s="6">
+        <v>713</v>
+      </c>
+      <c r="G79" s="6">
+        <v>201502</v>
+      </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D80" s="3"/>
-      <c r="E80" s="7"/>
-      <c r="F80" s="7"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
     </row>
     <row r="81" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D81" s="7"/>
-      <c r="E81" s="7"/>
-      <c r="F81" s="7"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
     </row>
     <row r="82" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D82" s="3"/>
-      <c r="E82" s="7"/>
-      <c r="F82" s="7"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
     </row>
     <row r="83" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D83" s="7"/>
-      <c r="E83" s="7"/>
-      <c r="F83" s="7"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
     </row>
     <row r="86" spans="4:7" x14ac:dyDescent="0.2">
       <c r="G86" s="3"/>
@@ -3010,9 +3019,12 @@
     <row r="93" spans="4:7" x14ac:dyDescent="0.2">
       <c r="F93" s="3"/>
     </row>
+    <row r="94" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="F94" s="3"/>
+    </row>
     <row r="99" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E99" s="7"/>
-      <c r="F99" s="7"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3023,9 +3035,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3166,7 +3178,7 @@
       <c r="K4">
         <v>152</v>
       </c>
-      <c r="L4" s="8"/>
+      <c r="L4" s="7"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
     </row>
@@ -3204,7 +3216,7 @@
       <c r="K5">
         <v>154</v>
       </c>
-      <c r="L5" s="8"/>
+      <c r="L5" s="7"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
     </row>
@@ -3242,7 +3254,7 @@
       <c r="K6">
         <v>160</v>
       </c>
-      <c r="L6" s="8"/>
+      <c r="L6" s="7"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
     </row>
@@ -3280,7 +3292,7 @@
       <c r="K7">
         <v>187</v>
       </c>
-      <c r="L7" s="8"/>
+      <c r="L7" s="7"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
     </row>
@@ -3318,7 +3330,7 @@
       <c r="K8">
         <v>195</v>
       </c>
-      <c r="L8" s="8"/>
+      <c r="L8" s="7"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
     </row>
@@ -3356,7 +3368,7 @@
       <c r="K9">
         <v>214</v>
       </c>
-      <c r="L9" s="8"/>
+      <c r="L9" s="7"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
     </row>
@@ -3394,7 +3406,7 @@
       <c r="K10">
         <v>217</v>
       </c>
-      <c r="L10" s="8"/>
+      <c r="L10" s="7"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
@@ -3432,7 +3444,7 @@
       <c r="K11">
         <v>215</v>
       </c>
-      <c r="L11" s="8"/>
+      <c r="L11" s="7"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
     </row>
@@ -3470,7 +3482,7 @@
       <c r="K12">
         <v>196</v>
       </c>
-      <c r="L12" s="8"/>
+      <c r="L12" s="7"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
     </row>
@@ -3508,7 +3520,7 @@
       <c r="K13">
         <v>203</v>
       </c>
-      <c r="L13" s="8"/>
+      <c r="L13" s="7"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
     </row>
@@ -3546,7 +3558,7 @@
       <c r="K14">
         <v>199</v>
       </c>
-      <c r="L14" s="8"/>
+      <c r="L14" s="7"/>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
     </row>
@@ -3584,7 +3596,7 @@
       <c r="K15">
         <v>188</v>
       </c>
-      <c r="L15" s="8"/>
+      <c r="L15" s="7"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
     </row>
@@ -3622,7 +3634,7 @@
       <c r="K16">
         <v>200</v>
       </c>
-      <c r="L16" s="8"/>
+      <c r="L16" s="7"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
     </row>
@@ -3630,37 +3642,37 @@
       <c r="A17" s="1">
         <v>43938.4375</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>4074</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6">
         <v>5380</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>210</v>
       </c>
-      <c r="E17" s="7">
+      <c r="E17" s="6">
         <v>2164</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <v>3067</v>
       </c>
-      <c r="G17" s="7">
+      <c r="G17" s="6">
         <v>2214</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="6">
         <v>1864</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="6">
         <v>829</v>
       </c>
-      <c r="J17" s="7">
+      <c r="J17" s="6">
         <v>245</v>
       </c>
-      <c r="K17" s="7">
+      <c r="K17" s="6">
         <v>200</v>
       </c>
-      <c r="L17" s="8"/>
+      <c r="L17" s="7"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
     </row>
@@ -3668,37 +3680,37 @@
       <c r="A18" s="1">
         <v>43939.4375</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <v>4277</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6">
         <v>5658</v>
       </c>
-      <c r="D18" s="7">
+      <c r="D18" s="6">
         <v>223</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="6">
         <v>2269</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="6">
         <v>3201</v>
       </c>
-      <c r="G18" s="7">
+      <c r="G18" s="6">
         <v>2313</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="6">
         <v>1996</v>
       </c>
-      <c r="I18" s="7">
+      <c r="I18" s="6">
         <v>828</v>
       </c>
-      <c r="J18" s="7">
+      <c r="J18" s="6">
         <v>250</v>
       </c>
-      <c r="K18" s="7">
+      <c r="K18" s="6">
         <v>197</v>
       </c>
-      <c r="L18" s="8"/>
+      <c r="L18" s="7"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
     </row>
@@ -3706,216 +3718,249 @@
       <c r="A19" s="1">
         <v>43940.4375</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <v>4495</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <v>5996</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <v>235</v>
       </c>
-      <c r="E19" s="7">
+      <c r="E19" s="6">
         <v>2408</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <v>3354</v>
       </c>
-      <c r="G19" s="7">
+      <c r="G19" s="6">
         <v>2437</v>
       </c>
-      <c r="H19" s="7">
+      <c r="H19" s="6">
         <v>2135</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="6">
         <v>809</v>
       </c>
-      <c r="J19" s="7">
+      <c r="J19" s="6">
         <v>247</v>
       </c>
-      <c r="K19" s="7">
+      <c r="K19" s="6">
         <v>196</v>
       </c>
-      <c r="L19" s="8"/>
+      <c r="L19" s="7"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43941.4375</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="6">
         <v>4728</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6">
         <v>6354</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="6">
         <v>248</v>
       </c>
-      <c r="E20" s="7">
+      <c r="E20" s="6">
         <v>2525</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="6">
         <v>3502</v>
       </c>
-      <c r="G20" s="7">
+      <c r="G20" s="6">
         <v>2580</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="6">
         <v>2312</v>
       </c>
-      <c r="I20" s="7">
+      <c r="I20" s="6">
         <v>802</v>
       </c>
-      <c r="J20" s="7">
+      <c r="J20" s="6">
         <v>247</v>
       </c>
-      <c r="K20" s="7">
+      <c r="K20" s="6">
         <v>193</v>
       </c>
-      <c r="L20" s="8"/>
+      <c r="L20" s="7"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43942.4375</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <v>4955</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6">
         <v>6663</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>260</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E21" s="6">
         <v>2657</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <v>3665</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G21" s="6">
         <v>2687</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H21" s="6">
         <v>2457</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="6">
         <v>859</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J21" s="6">
         <v>250</v>
       </c>
-      <c r="K21" s="7">
+      <c r="K21" s="6">
         <v>194</v>
       </c>
-      <c r="L21" s="8"/>
+      <c r="L21" s="7"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43943.4375</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="6">
         <v>5169</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6">
         <v>6952</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="6">
         <v>270</v>
       </c>
-      <c r="E22" s="7">
+      <c r="E22" s="6">
         <v>2781</v>
       </c>
-      <c r="F22" s="7">
+      <c r="F22" s="6">
         <v>3798</v>
       </c>
-      <c r="G22" s="7">
+      <c r="G22" s="6">
         <v>2778</v>
       </c>
-      <c r="H22" s="7">
+      <c r="H22" s="6">
         <v>2609</v>
       </c>
-      <c r="I22" s="7">
+      <c r="I22" s="6">
         <v>878</v>
       </c>
-      <c r="J22" s="7">
+      <c r="J22" s="6">
         <v>243</v>
       </c>
-      <c r="K22" s="7">
+      <c r="K22" s="6">
         <v>192</v>
       </c>
-      <c r="L22" s="8"/>
+      <c r="L22" s="7"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
+      <c r="A23" s="1">
+        <v>43944.4375</v>
+      </c>
+      <c r="B23" s="6">
+        <v>5408</v>
+      </c>
+      <c r="C23" s="6">
+        <v>7342</v>
+      </c>
+      <c r="D23" s="6">
+        <v>284</v>
+      </c>
+      <c r="E23" s="6">
+        <v>2914</v>
+      </c>
+      <c r="F23" s="6">
+        <v>3945</v>
+      </c>
+      <c r="G23" s="6">
+        <v>2909</v>
+      </c>
+      <c r="H23" s="6">
+        <v>2816</v>
+      </c>
+      <c r="I23" s="6">
+        <v>887</v>
+      </c>
+      <c r="J23" s="6">
+        <v>233</v>
+      </c>
+      <c r="K23" s="6">
+        <v>185</v>
+      </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E24" s="3"/>
-      <c r="F24" s="7"/>
+      <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E25" s="3"/>
-      <c r="F25" s="7"/>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="F26" s="7"/>
+      <c r="D26" s="3"/>
+      <c r="F26" s="6"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="D27" s="3"/>
       <c r="E27" s="3"/>
-      <c r="F27" s="7"/>
+      <c r="F27" s="6"/>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B28" s="7"/>
+      <c r="B28" s="6"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="7"/>
+      <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B29" s="7"/>
+      <c r="B29" s="6"/>
+      <c r="D29" s="3"/>
       <c r="E29" s="3"/>
-      <c r="F29" s="7"/>
+      <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B30" s="7"/>
+      <c r="B30" s="6"/>
+      <c r="D30" s="3"/>
       <c r="E30" s="3"/>
-      <c r="F30" s="7"/>
+      <c r="F30" s="6"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B31" s="7"/>
-      <c r="F31" s="7"/>
+      <c r="B31" s="6"/>
+      <c r="D31" s="3"/>
+      <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B32" s="7"/>
+      <c r="B32" s="6"/>
+      <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="7"/>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B33" s="7"/>
+      <c r="B33" s="6"/>
       <c r="E33" s="3"/>
-      <c r="F33" s="7"/>
+      <c r="F33" s="6"/>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B34" s="7"/>
+      <c r="B34" s="6"/>
       <c r="E34" s="3"/>
-      <c r="F34" s="7"/>
+      <c r="F34" s="6"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B35" s="7"/>
-      <c r="F35" s="7"/>
+      <c r="B35" s="6"/>
+      <c r="F35" s="6"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F36" s="7"/>
+      <c r="F36" s="6"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F37" s="7"/>
+      <c r="F37" s="6"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E38" s="7"/>
+      <c r="E38" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-04-24 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAA4E3E-24E8-CB43-8C9A-8C5995CB3A27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05936818-6800-5640-BA95-5D2FC041E87C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -402,7 +402,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -420,6 +420,27 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF222222"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF222222"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -442,11 +463,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -455,8 +477,13 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1153,11 +1180,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:H99"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D96" sqref="C85:D96"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2991,40 +3018,38 @@
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D80" s="3"/>
-      <c r="E80" s="6"/>
-      <c r="F80" s="6"/>
+      <c r="A80" s="1">
+        <v>43945.4375</v>
+      </c>
+      <c r="B80" s="6">
+        <v>185671</v>
+      </c>
+      <c r="C80" s="6">
+        <v>5414</v>
+      </c>
+      <c r="D80" s="6">
+        <v>13519</v>
+      </c>
+      <c r="E80" s="6">
+        <v>7087</v>
+      </c>
+      <c r="F80" s="6">
+        <v>763</v>
+      </c>
+      <c r="G80" s="6">
+        <v>212454</v>
+      </c>
     </row>
     <row r="81" spans="4:7" x14ac:dyDescent="0.2">
       <c r="D81" s="6"/>
       <c r="E81" s="6"/>
       <c r="F81" s="6"/>
     </row>
-    <row r="82" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D82" s="3"/>
-      <c r="E82" s="6"/>
-      <c r="F82" s="6"/>
-    </row>
-    <row r="83" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D83" s="6"/>
-      <c r="E83" s="6"/>
-      <c r="F83" s="6"/>
-    </row>
     <row r="86" spans="4:7" x14ac:dyDescent="0.2">
       <c r="G86" s="3"/>
     </row>
     <row r="89" spans="4:7" x14ac:dyDescent="0.2">
       <c r="G89" s="3"/>
-    </row>
-    <row r="93" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="F93" s="3"/>
-    </row>
-    <row r="94" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="F94" s="3"/>
-    </row>
-    <row r="99" spans="5:6" x14ac:dyDescent="0.2">
-      <c r="E99" s="6"/>
-      <c r="F99" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3033,11 +3058,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G33" sqref="G33"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3894,73 +3919,158 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="E24" s="3"/>
-      <c r="F24" s="6"/>
+      <c r="A24" s="1">
+        <v>43945.4375</v>
+      </c>
+      <c r="B24" s="6">
+        <v>5640</v>
+      </c>
+      <c r="C24" s="6">
+        <v>7737</v>
+      </c>
+      <c r="D24" s="6">
+        <v>292</v>
+      </c>
+      <c r="E24" s="6">
+        <v>3052</v>
+      </c>
+      <c r="F24" s="6">
+        <v>4108</v>
+      </c>
+      <c r="G24" s="6">
+        <v>3029</v>
+      </c>
+      <c r="H24" s="6">
+        <v>3029</v>
+      </c>
+      <c r="I24" s="6">
+        <v>910</v>
+      </c>
+      <c r="J24" s="6">
+        <v>243</v>
+      </c>
+      <c r="K24" s="6">
+        <v>193</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E25" s="3"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D26" s="3"/>
+    <row r="26" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="8"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+    <row r="27" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+      <c r="C27" s="8"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
       <c r="F27" s="6"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B28" s="6"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="6"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C28" s="9"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B29" s="6"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="6"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C29" s="9"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B30" s="6"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C30" s="11"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B31" s="6"/>
-      <c r="D31" s="3"/>
-      <c r="F31" s="6"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C31" s="8"/>
+      <c r="D31" s="10"/>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B32" s="6"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="6"/>
-    </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C32" s="8"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="33" spans="2:6" ht="20" x14ac:dyDescent="0.2">
       <c r="B33" s="6"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="2:6" ht="20" x14ac:dyDescent="0.2">
       <c r="B34" s="6"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="6"/>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="C34" s="8"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" spans="2:6" ht="20" x14ac:dyDescent="0.2">
       <c r="B35" s="6"/>
-      <c r="F35" s="6"/>
-    </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F36" s="6"/>
-    </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="F37" s="6"/>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E38" s="6"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="C36" s="8"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="C37" s="8"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="8"/>
+      <c r="F37" s="3"/>
+    </row>
+    <row r="38" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="C38" s="11"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="3"/>
+    </row>
+    <row r="39" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="C39" s="9"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="3"/>
+    </row>
+    <row r="40" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="C40" s="9"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="C41" s="9"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="8"/>
+    </row>
+    <row r="42" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="C42" s="11"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="8"/>
+    </row>
+    <row r="43" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="C43" s="9"/>
+      <c r="D43" s="8"/>
+      <c r="E43" s="8"/>
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="C44" s="9"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+    </row>
+    <row r="45" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="C45" s="9"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-04-25 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05936818-6800-5640-BA95-5D2FC041E87C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19424FFC-1DEA-3941-ADBF-F514D9517348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="34940" yWindow="840" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -1182,9 +1182,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
   <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C82" sqref="C82"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3040,15 +3040,56 @@
         <v>212454</v>
       </c>
     </row>
-    <row r="81" spans="4:7" x14ac:dyDescent="0.2">
-      <c r="D81" s="6"/>
-      <c r="E81" s="6"/>
-      <c r="F81" s="6"/>
-    </row>
-    <row r="86" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>43946.4375</v>
+      </c>
+      <c r="B81" s="6">
+        <v>195303</v>
+      </c>
+      <c r="C81" s="6">
+        <v>8171</v>
+      </c>
+      <c r="D81" s="6">
+        <v>13995</v>
+      </c>
+      <c r="E81" s="6">
+        <v>7509</v>
+      </c>
+      <c r="F81" s="6">
+        <v>811</v>
+      </c>
+      <c r="G81" s="6">
+        <v>225789</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C82" s="9"/>
+      <c r="D82" s="10"/>
+      <c r="E82" s="8"/>
+    </row>
+    <row r="83" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C83" s="8"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="8"/>
+    </row>
+    <row r="84" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C84" s="9"/>
+      <c r="D84" s="10"/>
+      <c r="E84" s="8"/>
+    </row>
+    <row r="85" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C85" s="9"/>
+      <c r="D85" s="8"/>
+      <c r="E85" s="8"/>
+    </row>
+    <row r="86" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C86" s="11"/>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8"/>
       <c r="G86" s="3"/>
     </row>
-    <row r="89" spans="4:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G89" s="3"/>
     </row>
   </sheetData>
@@ -3060,14 +3101,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
@@ -3954,102 +3995,121 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="E25" s="3"/>
-      <c r="F25" s="6"/>
+      <c r="A25" s="1">
+        <v>43946.4375</v>
+      </c>
+      <c r="B25" s="6">
+        <v>5827</v>
+      </c>
+      <c r="C25" s="6">
+        <v>8030</v>
+      </c>
+      <c r="D25" s="6">
+        <v>309</v>
+      </c>
+      <c r="E25" s="6">
+        <v>3179</v>
+      </c>
+      <c r="F25" s="6">
+        <v>4276</v>
+      </c>
+      <c r="G25" s="6">
+        <v>3108</v>
+      </c>
+      <c r="H25" s="6">
+        <v>3114</v>
+      </c>
+      <c r="I25" s="6">
+        <v>925</v>
+      </c>
+      <c r="J25" s="6">
+        <v>245</v>
+      </c>
+      <c r="K25" s="6">
+        <v>195</v>
+      </c>
     </row>
     <row r="26" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="C26" s="9"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="8"/>
       <c r="F26" s="6"/>
     </row>
     <row r="27" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="C27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="10"/>
       <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
       <c r="F27" s="6"/>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="B28" s="6"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
     </row>
     <row r="29" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="B29" s="6"/>
-      <c r="C29" s="9"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="10"/>
       <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
     </row>
     <row r="30" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="B30" s="6"/>
-      <c r="C30" s="11"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="10"/>
       <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
     </row>
     <row r="31" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="B31" s="6"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="8"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="10"/>
+      <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="B32" s="6"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="10"/>
+      <c r="D32" s="8"/>
     </row>
     <row r="33" spans="2:6" ht="20" x14ac:dyDescent="0.2">
-      <c r="B33" s="6"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
     </row>
     <row r="34" spans="2:6" ht="20" x14ac:dyDescent="0.2">
-      <c r="B34" s="6"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="8"/>
+      <c r="B34" s="9"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="3"/>
     </row>
     <row r="35" spans="2:6" ht="20" x14ac:dyDescent="0.2">
-      <c r="B35" s="6"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="8"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="8"/>
     </row>
     <row r="36" spans="2:6" ht="20" x14ac:dyDescent="0.2">
-      <c r="C36" s="8"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="8"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="8"/>
     </row>
     <row r="37" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="B37" s="11"/>
       <c r="C37" s="8"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="8"/>
+      <c r="D37" s="8"/>
       <c r="F37" s="3"/>
     </row>
     <row r="38" spans="2:6" ht="20" x14ac:dyDescent="0.2">
-      <c r="C38" s="11"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="8"/>
       <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
       <c r="F38" s="3"/>
     </row>
     <row r="39" spans="2:6" ht="20" x14ac:dyDescent="0.2">
-      <c r="C39" s="9"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="8"/>
+      <c r="B39" s="9"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="8"/>
       <c r="F39" s="3"/>
     </row>
     <row r="40" spans="2:6" ht="20" x14ac:dyDescent="0.2">
-      <c r="C40" s="9"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="8"/>
-    </row>
-    <row r="41" spans="2:6" ht="20" x14ac:dyDescent="0.2">
-      <c r="C41" s="9"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="8"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
     </row>
     <row r="42" spans="2:6" ht="20" x14ac:dyDescent="0.2">
       <c r="C42" s="11"/>

</xml_diff>

<commit_message>
excel update 2020-04-26 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19424FFC-1DEA-3941-ADBF-F514D9517348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DF420F-5624-D645-B07D-4709AE5CFA63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34940" yWindow="840" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -1182,9 +1182,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
   <dimension ref="A1:H89"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B83" sqref="B83"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1198,7 +1198,7 @@
     <col min="7" max="7" width="54.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43872.645833333336</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43873.645833333336</v>
       </c>
@@ -1266,8 +1266,9 @@
       <c r="G3">
         <v>313</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43874.645833333336</v>
       </c>
@@ -1289,8 +1290,9 @@
       <c r="G4">
         <v>340</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43875.645833333336</v>
       </c>
@@ -1312,8 +1314,9 @@
       <c r="G5">
         <v>364</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43875.645833333336</v>
       </c>
@@ -1335,8 +1338,9 @@
       <c r="G6">
         <v>364</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43875.645833333336</v>
       </c>
@@ -1358,8 +1362,9 @@
       <c r="G7">
         <v>364</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43878.645833333336</v>
       </c>
@@ -1381,8 +1386,9 @@
       <c r="G8">
         <v>402</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43879.645833333336</v>
       </c>
@@ -1404,8 +1410,9 @@
       <c r="G9">
         <v>421</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43880.645833333336</v>
       </c>
@@ -1427,8 +1434,9 @@
       <c r="G10">
         <v>456</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43881.645833333336</v>
       </c>
@@ -1450,8 +1458,9 @@
       <c r="G11">
         <v>479</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43882.645833333336</v>
       </c>
@@ -1473,8 +1482,9 @@
       <c r="G12">
         <v>498</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43882.645833333336</v>
       </c>
@@ -1496,8 +1506,9 @@
       <c r="G13">
         <v>498</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43882.645833333336</v>
       </c>
@@ -1519,8 +1530,9 @@
       <c r="G14">
         <v>498</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43885.645833333336</v>
       </c>
@@ -1542,8 +1554,9 @@
       <c r="G15">
         <v>553</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43886.645833333336</v>
       </c>
@@ -1565,8 +1578,9 @@
       <c r="G16">
         <v>593</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43887.645833333336</v>
       </c>
@@ -1588,8 +1602,9 @@
       <c r="G17">
         <v>629</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43888.645833333336</v>
       </c>
@@ -1611,8 +1626,9 @@
       <c r="G18">
         <v>699</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43888.645833333336</v>
       </c>
@@ -1634,8 +1650,9 @@
       <c r="G19">
         <v>699</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43889.645833333336</v>
       </c>
@@ -1657,8 +1674,9 @@
       <c r="G20">
         <v>768</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43889.645833333336</v>
       </c>
@@ -1680,8 +1698,9 @@
       <c r="G21">
         <v>768</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43892.645833333336</v>
       </c>
@@ -1703,8 +1722,9 @@
       <c r="G22">
         <v>1005</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43893.645833333336</v>
       </c>
@@ -1726,8 +1746,9 @@
       <c r="G23">
         <v>1126</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43894.645833333336</v>
       </c>
@@ -1749,8 +1770,9 @@
       <c r="G24">
         <v>1338</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43895.645833333336</v>
       </c>
@@ -1772,8 +1794,9 @@
       <c r="G25">
         <v>1566</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43896.645833333336</v>
       </c>
@@ -1795,8 +1818,9 @@
       <c r="G26">
         <v>1763</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43897.604166666664</v>
       </c>
@@ -1818,8 +1842,9 @@
       <c r="G27">
         <v>1982</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43897.645833333336</v>
       </c>
@@ -1841,8 +1866,9 @@
       <c r="G28">
         <v>1982</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43899.604166666664</v>
       </c>
@@ -1864,8 +1890,9 @@
       <c r="G29">
         <v>2403</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43900.604166666664</v>
       </c>
@@ -1887,8 +1914,9 @@
       <c r="G30">
         <v>2747</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>43900.604166666664</v>
       </c>
@@ -1910,8 +1938,9 @@
       <c r="G31">
         <v>2747</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>43901.604166666664</v>
       </c>
@@ -1933,8 +1962,9 @@
       <c r="G32">
         <v>3395</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43902.604166666664</v>
       </c>
@@ -1956,8 +1986,9 @@
       <c r="G33">
         <v>4185</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43903.604166666664</v>
       </c>
@@ -1979,8 +2010,9 @@
       <c r="G34">
         <v>5129</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>43904.895833333336</v>
       </c>
@@ -2002,8 +2034,9 @@
       <c r="G35">
         <v>6648</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>43905.895833333336</v>
       </c>
@@ -2025,8 +2058,9 @@
       <c r="G36">
         <v>8465</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>43906.895833333336</v>
       </c>
@@ -2048,8 +2082,9 @@
       <c r="G37">
         <v>10178</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>43907.895833333336</v>
       </c>
@@ -2071,8 +2106,9 @@
       <c r="G38">
         <v>11171</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>43909.604166666664</v>
       </c>
@@ -2094,8 +2130,9 @@
       <c r="G39">
         <v>16650</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>43909.895833333336</v>
       </c>
@@ -2117,8 +2154,9 @@
       <c r="G40">
         <v>16650</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>43911.604166666664</v>
       </c>
@@ -2140,8 +2178,9 @@
       <c r="G41">
         <v>23384</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>43911.895833333336</v>
       </c>
@@ -2163,8 +2202,9 @@
       <c r="G42">
         <v>23384</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>43912.895833333336</v>
       </c>
@@ -2186,8 +2226,9 @@
       <c r="G43">
         <v>26420</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43913.4375</v>
       </c>
@@ -2209,8 +2250,9 @@
       <c r="G44">
         <v>28506</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43914.4375</v>
       </c>
@@ -2232,8 +2274,9 @@
       <c r="G45">
         <v>32457</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>43915.4375</v>
       </c>
@@ -2255,8 +2298,9 @@
       <c r="G46">
         <v>35635</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>43915.729166666664</v>
       </c>
@@ -2278,8 +2322,9 @@
       <c r="G47">
         <v>35635</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>43916.4375</v>
       </c>
@@ -2301,8 +2346,9 @@
       <c r="G48">
         <v>38550</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>43916.729166666664</v>
       </c>
@@ -2324,8 +2370,9 @@
       <c r="G49">
         <v>38550</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>43917.4375</v>
       </c>
@@ -2347,8 +2394,9 @@
       <c r="G50">
         <v>41032</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>43918.4375</v>
       </c>
@@ -2370,8 +2418,9 @@
       <c r="G51">
         <v>43072</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H51" s="6"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>43918.729166666664</v>
       </c>
@@ -2393,8 +2442,9 @@
       <c r="G52">
         <v>43072</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H52" s="6"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>43919.4375</v>
       </c>
@@ -2416,8 +2466,9 @@
       <c r="G53">
         <v>49186</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H53" s="6"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>43919.729166666664</v>
       </c>
@@ -2439,8 +2490,9 @@
       <c r="G54">
         <v>49186</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H54" s="6"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>43920.4375</v>
       </c>
@@ -2462,8 +2514,9 @@
       <c r="G55">
         <v>54112</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H55" s="6"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>43921.4375</v>
       </c>
@@ -2486,8 +2539,9 @@
         <f>51629+C53</f>
         <v>58832</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H56" s="6"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>43922.4375</v>
       </c>
@@ -2509,8 +2563,9 @@
       <c r="G57">
         <v>61009</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H57" s="6"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>43923.4375</v>
       </c>
@@ -2532,8 +2587,9 @@
       <c r="G58">
         <v>64785</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H58" s="6"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>43924.4375</v>
       </c>
@@ -2555,8 +2611,9 @@
       <c r="G59">
         <v>67998</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H59" s="6"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>43925.4375</v>
       </c>
@@ -2578,8 +2635,9 @@
       <c r="G60">
         <v>72674</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H60" s="6"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>43926.4375</v>
       </c>
@@ -2601,8 +2659,9 @@
       <c r="G61">
         <v>76027</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H61" s="6"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>43927.4375</v>
       </c>
@@ -2624,8 +2683,9 @@
       <c r="G62">
         <v>79125</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H62" s="6"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>43928.4375</v>
       </c>
@@ -2647,8 +2707,9 @@
       <c r="G63">
         <v>82055</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H63" s="6"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>43929.4375</v>
       </c>
@@ -2670,6 +2731,7 @@
       <c r="G64">
         <v>85703</v>
       </c>
+      <c r="H64" s="6"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
@@ -2693,6 +2755,7 @@
       <c r="G65">
         <v>89906</v>
       </c>
+      <c r="H65" s="6"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
@@ -2716,6 +2779,7 @@
       <c r="G66">
         <v>94271</v>
       </c>
+      <c r="H66" s="6"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
@@ -2739,6 +2803,7 @@
       <c r="G67">
         <v>97838</v>
       </c>
+      <c r="H67" s="6"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
@@ -2762,7 +2827,7 @@
       <c r="G68">
         <v>104784</v>
       </c>
-      <c r="H68" s="3"/>
+      <c r="H68" s="6"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
@@ -2786,6 +2851,7 @@
       <c r="G69">
         <v>109764</v>
       </c>
+      <c r="H69" s="6"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
@@ -2809,6 +2875,7 @@
       <c r="G70">
         <v>115189</v>
       </c>
+      <c r="H70" s="6"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
@@ -2832,6 +2899,7 @@
       <c r="G71">
         <v>123521</v>
       </c>
+      <c r="H71" s="6"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
@@ -2855,6 +2923,7 @@
       <c r="G72">
         <v>132416</v>
       </c>
+      <c r="H72" s="6"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
@@ -2878,6 +2947,7 @@
       <c r="G73" s="6">
         <v>142985</v>
       </c>
+      <c r="H73" s="6"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
@@ -2901,6 +2971,7 @@
       <c r="G74" s="6">
         <v>153287</v>
       </c>
+      <c r="H74" s="6"/>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
@@ -2924,6 +2995,7 @@
       <c r="G75" s="6">
         <v>161833</v>
       </c>
+      <c r="H75" s="6"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
@@ -2947,6 +3019,7 @@
       <c r="G76" s="6">
         <v>168639</v>
       </c>
+      <c r="H76" s="6"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
@@ -2970,6 +3043,7 @@
       <c r="G77">
         <v>179716</v>
       </c>
+      <c r="H77" s="6"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
@@ -2993,6 +3067,7 @@
       <c r="G78" s="6">
         <v>191376</v>
       </c>
+      <c r="H78" s="6"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
@@ -3016,6 +3091,7 @@
       <c r="G79" s="6">
         <v>201502</v>
       </c>
+      <c r="H79" s="6"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
@@ -3039,8 +3115,9 @@
       <c r="G80" s="6">
         <v>212454</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H80" s="6"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>43946.4375</v>
       </c>
@@ -3062,34 +3139,54 @@
       <c r="G81" s="6">
         <v>225789</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C82" s="9"/>
-      <c r="D82" s="10"/>
-      <c r="E82" s="8"/>
-    </row>
-    <row r="83" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="H81" s="6"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>43947.4375</v>
+      </c>
+      <c r="B82" s="6">
+        <v>206371</v>
+      </c>
+      <c r="C82" s="6">
+        <v>7417</v>
+      </c>
+      <c r="D82" s="6">
+        <v>14432</v>
+      </c>
+      <c r="E82" s="6">
+        <v>8000</v>
+      </c>
+      <c r="F82" s="6">
+        <v>835</v>
+      </c>
+      <c r="G82" s="6">
+        <v>237055</v>
+      </c>
+      <c r="H82" s="6"/>
+    </row>
+    <row r="83" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
+      <c r="D83" s="10"/>
       <c r="E83" s="8"/>
     </row>
-    <row r="84" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="C84" s="9"/>
       <c r="D84" s="10"/>
       <c r="E84" s="8"/>
     </row>
-    <row r="85" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="C85" s="9"/>
-      <c r="D85" s="8"/>
+      <c r="D85" s="10"/>
       <c r="E85" s="8"/>
     </row>
-    <row r="86" spans="1:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:8" ht="20" x14ac:dyDescent="0.2">
       <c r="C86" s="11"/>
       <c r="D86" s="8"/>
       <c r="E86" s="8"/>
       <c r="G86" s="3"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G89" s="3"/>
     </row>
   </sheetData>
@@ -3101,9 +3198,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4029,105 +4126,122 @@
         <v>195</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="B26" s="8"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="8"/>
-      <c r="F26" s="6"/>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>43947.4375</v>
+      </c>
+      <c r="B26" s="6">
+        <v>6005</v>
+      </c>
+      <c r="C26" s="6">
+        <v>8290</v>
+      </c>
+      <c r="D26" s="6">
+        <v>320</v>
+      </c>
+      <c r="E26" s="6">
+        <v>3292</v>
+      </c>
+      <c r="F26" s="6">
+        <v>4391</v>
+      </c>
+      <c r="G26" s="6">
+        <v>3207</v>
+      </c>
+      <c r="H26" s="6">
+        <v>3213</v>
+      </c>
+      <c r="I26" s="6">
+        <v>938</v>
+      </c>
+      <c r="J26" s="6">
+        <v>252</v>
+      </c>
+      <c r="K26" s="6">
+        <v>195</v>
+      </c>
     </row>
     <row r="27" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B27" s="8"/>
       <c r="C27" s="10"/>
-      <c r="D27" s="8"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
+      <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B29" s="8"/>
       <c r="C29" s="10"/>
-      <c r="D29" s="8"/>
+      <c r="E29" s="3"/>
     </row>
     <row r="30" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B30" s="8"/>
       <c r="C30" s="10"/>
-      <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B31" s="8"/>
       <c r="C31" s="10"/>
-      <c r="D31" s="8"/>
+      <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B32" s="8"/>
       <c r="C32" s="10"/>
-      <c r="D32" s="8"/>
-    </row>
-    <row r="33" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="B33" s="11"/>
       <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-    </row>
-    <row r="34" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="B34" s="9"/>
       <c r="C34" s="10"/>
-      <c r="D34" s="8"/>
       <c r="E34" s="3"/>
     </row>
-    <row r="35" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="B35" s="9"/>
       <c r="C35" s="10"/>
-      <c r="D35" s="8"/>
-    </row>
-    <row r="36" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="B36" s="9"/>
       <c r="C36" s="10"/>
-      <c r="D36" s="8"/>
-    </row>
-    <row r="37" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="B37" s="11"/>
       <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="F37" s="3"/>
-    </row>
-    <row r="38" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="E37" s="3"/>
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="B38" s="9"/>
       <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="B39" s="9"/>
       <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="F39" s="3"/>
-    </row>
-    <row r="40" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="B40" s="9"/>
       <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-    </row>
-    <row r="42" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="C42" s="11"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-    </row>
-    <row r="43" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="C43" s="9"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="C44" s="9"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
     </row>
-    <row r="45" spans="2:6" ht="20" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="C45" s="9"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>

</xml_diff>

<commit_message>
excel update 2020-04-27 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0DF420F-5624-D645-B07D-4709AE5CFA63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CD25D6-CE0B-9E40-994C-1F669BE72FF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -468,7 +468,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -481,6 +481,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1180,11 +1182,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:H89"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3165,29 +3167,89 @@
       </c>
       <c r="H82" s="6"/>
     </row>
-    <row r="83" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="C83" s="8"/>
-      <c r="D83" s="10"/>
-      <c r="E83" s="8"/>
-    </row>
-    <row r="84" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="C84" s="9"/>
-      <c r="D84" s="10"/>
-      <c r="E84" s="8"/>
-    </row>
-    <row r="85" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="C85" s="9"/>
-      <c r="D85" s="10"/>
-      <c r="E85" s="8"/>
-    </row>
-    <row r="86" spans="1:8" ht="20" x14ac:dyDescent="0.2">
-      <c r="C86" s="11"/>
-      <c r="D86" s="8"/>
-      <c r="E86" s="8"/>
-      <c r="G86" s="3"/>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>43948.4375</v>
+      </c>
+      <c r="B83" s="6">
+        <v>217915</v>
+      </c>
+      <c r="C83" s="6">
+        <v>5001</v>
+      </c>
+      <c r="D83" s="6">
+        <v>14856</v>
+      </c>
+      <c r="E83" s="6">
+        <v>8525</v>
+      </c>
+      <c r="F83" s="6">
+        <v>892</v>
+      </c>
+      <c r="G83" s="6">
+        <v>247189</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="6"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="6"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="6"/>
+      <c r="B86" s="6"/>
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D87" s="3"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G89" s="3"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D90" s="3"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D91" s="3"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D93" s="3"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D94" s="3"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D95" s="3"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D96" s="3"/>
+    </row>
+    <row r="98" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D98" s="3"/>
+      <c r="F98" s="3"/>
+    </row>
+    <row r="99" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D99" s="3"/>
+    </row>
+    <row r="100" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D100" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3196,11 +3258,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N45"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H30" sqref="H30"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4161,9 +4223,40 @@
         <v>195</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="B27" s="8"/>
-      <c r="C27" s="10"/>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>43948.4375</v>
+      </c>
+      <c r="B27" s="6">
+        <v>6168</v>
+      </c>
+      <c r="C27" s="6">
+        <v>8548</v>
+      </c>
+      <c r="D27" s="6">
+        <v>326</v>
+      </c>
+      <c r="E27" s="6">
+        <v>3398</v>
+      </c>
+      <c r="F27" s="6">
+        <v>4504</v>
+      </c>
+      <c r="G27" s="6">
+        <v>3302</v>
+      </c>
+      <c r="H27" s="6">
+        <v>3318</v>
+      </c>
+      <c r="I27" s="6">
+        <v>945</v>
+      </c>
+      <c r="J27" s="6">
+        <v>241</v>
+      </c>
+      <c r="K27" s="6">
+        <v>191</v>
+      </c>
     </row>
     <row r="28" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B28" s="8"/>
@@ -4173,78 +4266,125 @@
     <row r="29" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B29" s="8"/>
       <c r="C29" s="10"/>
+      <c r="D29" s="6"/>
       <c r="E29" s="3"/>
     </row>
     <row r="30" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B30" s="8"/>
       <c r="C30" s="10"/>
+      <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B31" s="8"/>
       <c r="C31" s="10"/>
+      <c r="D31" s="6"/>
       <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B32" s="8"/>
       <c r="C32" s="10"/>
+      <c r="D32" s="6"/>
       <c r="E32" s="3"/>
     </row>
     <row r="33" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="B33" s="11"/>
-      <c r="C33" s="8"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="6"/>
       <c r="E33" s="3"/>
     </row>
     <row r="34" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="B34" s="9"/>
       <c r="C34" s="10"/>
+      <c r="D34" s="6"/>
       <c r="E34" s="3"/>
     </row>
     <row r="35" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="B35" s="9"/>
       <c r="C35" s="10"/>
+      <c r="D35" s="6"/>
     </row>
     <row r="36" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="B36" s="9"/>
       <c r="C36" s="10"/>
+      <c r="D36" s="6"/>
       <c r="E36" s="3"/>
     </row>
     <row r="37" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="B37" s="11"/>
-      <c r="C37" s="8"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="6"/>
       <c r="E37" s="3"/>
       <c r="G37" s="3"/>
     </row>
     <row r="38" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="B38" s="9"/>
       <c r="C38" s="8"/>
+      <c r="D38" s="6"/>
       <c r="E38" s="3"/>
     </row>
     <row r="39" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="B39" s="9"/>
-      <c r="C39" s="8"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="6"/>
     </row>
     <row r="40" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="B40" s="9"/>
-      <c r="C40" s="8"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="6"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B41" s="6"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="6"/>
     </row>
     <row r="42" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C42" s="11"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="6"/>
     </row>
     <row r="43" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="B43" s="6"/>
       <c r="C43" s="9"/>
       <c r="D43" s="8"/>
       <c r="E43" s="8"/>
       <c r="F43" s="6"/>
     </row>
     <row r="44" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C44" s="9"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="13"/>
       <c r="D44" s="8"/>
       <c r="E44" s="8"/>
     </row>
     <row r="45" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C45" s="9"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="13"/>
       <c r="D45" s="8"/>
       <c r="E45" s="8"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B46" s="6"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="6"/>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-04-28 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CD25D6-CE0B-9E40-994C-1F669BE72FF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3B4417-AFDC-5D4B-AF78-82DB252636BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -468,7 +468,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -479,10 +479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1182,11 +1179,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:H100"/>
+  <dimension ref="A1:H89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3191,13 +3188,27 @@
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="6"/>
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
-      <c r="D84" s="6"/>
-      <c r="E84" s="6"/>
-      <c r="F84" s="6"/>
-      <c r="G84" s="6"/>
+      <c r="A84" s="1">
+        <v>43949.4375</v>
+      </c>
+      <c r="B84" s="6">
+        <v>227744</v>
+      </c>
+      <c r="C84" s="6">
+        <v>6282</v>
+      </c>
+      <c r="D84" s="6">
+        <v>15381</v>
+      </c>
+      <c r="E84" s="6">
+        <v>8964</v>
+      </c>
+      <c r="F84" s="6">
+        <v>951</v>
+      </c>
+      <c r="G84" s="6">
+        <v>259322</v>
+      </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="6"/>
@@ -3211,45 +3222,10 @@
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="6"/>
       <c r="B86" s="6"/>
-      <c r="C86" s="6"/>
-      <c r="D86" s="6"/>
-      <c r="E86" s="6"/>
-      <c r="F86" s="6"/>
       <c r="G86" s="6"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D87" s="3"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G89" s="3"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D90" s="3"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D91" s="3"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D93" s="3"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D94" s="3"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D95" s="3"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D96" s="3"/>
-    </row>
-    <row r="98" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D98" s="3"/>
-      <c r="F98" s="3"/>
-    </row>
-    <row r="99" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D99" s="3"/>
-    </row>
-    <row r="100" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D100" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3262,7 +3238,7 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomLeft" activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4258,123 +4234,121 @@
         <v>191</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="E28" s="3"/>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>43949.4375</v>
+      </c>
+      <c r="B28" s="6">
+        <v>6392</v>
+      </c>
+      <c r="C28" s="6">
+        <v>8848</v>
+      </c>
+      <c r="D28" s="6">
+        <v>346</v>
+      </c>
+      <c r="E28" s="6">
+        <v>3521</v>
+      </c>
+      <c r="F28" s="6">
+        <v>4644</v>
+      </c>
+      <c r="G28" s="6">
+        <v>3420</v>
+      </c>
+      <c r="H28" s="6">
+        <v>3443</v>
+      </c>
+      <c r="I28" s="6">
+        <v>957</v>
+      </c>
+      <c r="J28" s="6">
+        <v>239</v>
+      </c>
+      <c r="K28" s="6">
+        <v>187</v>
+      </c>
     </row>
     <row r="29" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B29" s="8"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="3"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B30" s="8"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="6"/>
+      <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B31" s="8"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="3"/>
+      <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B32" s="8"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="3"/>
     </row>
     <row r="33" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="B33" s="11"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="B33" s="10"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="9"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="3"/>
-    </row>
-    <row r="35" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35" s="9"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="6"/>
-    </row>
-    <row r="36" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B36" s="9"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="3"/>
+      <c r="D36" s="3"/>
     </row>
     <row r="37" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="B37" s="11"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="3"/>
+      <c r="B37" s="10"/>
+      <c r="D37" s="3"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B38" s="9"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="3"/>
-    </row>
-    <row r="39" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B39" s="9"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="6"/>
-    </row>
-    <row r="40" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B40" s="9"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="6"/>
+      <c r="D40" s="3"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B41" s="6"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="6"/>
-    </row>
-    <row r="42" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="D41" s="3"/>
+      <c r="F41" s="3"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B42" s="6"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="6"/>
-    </row>
-    <row r="43" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B43" s="6"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="6"/>
-    </row>
-    <row r="44" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="D43" s="3"/>
+      <c r="F43" s="3"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B44" s="6"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-    </row>
-    <row r="45" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B45" s="6"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B46" s="6"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="6"/>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" s="6"/>

</xml_diff>

<commit_message>
excel update 2020-04-29 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3B4417-AFDC-5D4B-AF78-82DB252636BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D309A6FB-73F2-2947-9688-24A3A97D99DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -1182,8 +1182,8 @@
   <dimension ref="A1:H89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C92" sqref="C92"/>
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3211,13 +3211,27 @@
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="6"/>
-      <c r="B85" s="6"/>
-      <c r="C85" s="6"/>
-      <c r="D85" s="6"/>
-      <c r="E85" s="6"/>
-      <c r="F85" s="6"/>
-      <c r="G85" s="6"/>
+      <c r="A85" s="1">
+        <v>43950.4375</v>
+      </c>
+      <c r="B85" s="6">
+        <v>238258</v>
+      </c>
+      <c r="C85" s="6">
+        <v>9530</v>
+      </c>
+      <c r="D85" s="6">
+        <v>15728</v>
+      </c>
+      <c r="E85" s="6">
+        <v>9612</v>
+      </c>
+      <c r="F85" s="6">
+        <v>996</v>
+      </c>
+      <c r="G85" s="6">
+        <v>274124</v>
+      </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="6"/>
@@ -3238,7 +3252,7 @@
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I33" sqref="I33"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4269,12 +4283,40 @@
         <v>187</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="B29" s="8"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>43950.4375</v>
+      </c>
+      <c r="B29" s="6">
+        <v>6546</v>
+      </c>
+      <c r="C29" s="6">
+        <v>9041</v>
+      </c>
+      <c r="D29" s="6">
+        <v>363</v>
+      </c>
+      <c r="E29" s="6">
+        <v>3583</v>
+      </c>
+      <c r="F29" s="6">
+        <v>4725</v>
+      </c>
+      <c r="G29" s="6">
+        <v>3486</v>
+      </c>
+      <c r="H29" s="6">
+        <v>3564</v>
+      </c>
+      <c r="I29" s="6">
+        <v>977</v>
+      </c>
+      <c r="J29" s="6">
+        <v>235</v>
+      </c>
+      <c r="K29" s="6">
+        <v>186</v>
+      </c>
     </row>
     <row r="30" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B30" s="8"/>
@@ -4282,18 +4324,16 @@
     </row>
     <row r="31" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B31" s="8"/>
-      <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B32" s="8"/>
+      <c r="D32" s="3"/>
     </row>
     <row r="33" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="B33" s="10"/>
-      <c r="D33" s="3"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="9"/>
-      <c r="D34" s="3"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35" s="9"/>
@@ -4305,7 +4345,6 @@
     </row>
     <row r="37" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="B37" s="10"/>
-      <c r="D37" s="3"/>
       <c r="G37" s="3"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
@@ -4323,11 +4362,9 @@
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B41" s="6"/>
       <c r="D41" s="3"/>
-      <c r="F41" s="3"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B42" s="6"/>
-      <c r="D42" s="3"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B43" s="6"/>
@@ -4340,6 +4377,7 @@
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B45" s="6"/>
+      <c r="D45" s="3"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B46" s="6"/>
@@ -4352,8 +4390,6 @@
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" s="6"/>

</xml_diff>

<commit_message>
excel update 2020-04-30 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D309A6FB-73F2-2947-9688-24A3A97D99DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED7972C-B112-3141-A84F-C8253A2A8287}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="19380" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="19380" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -402,7 +402,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -430,21 +430,6 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF222222"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -463,12 +448,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -478,11 +462,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1179,11 +1160,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:H89"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A85" sqref="A85"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C93" sqref="C93:D107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3234,12 +3215,42 @@
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="6"/>
-      <c r="B86" s="6"/>
-      <c r="G86" s="6"/>
+      <c r="A86" s="1">
+        <v>43951.4375</v>
+      </c>
+      <c r="B86" s="6">
+        <v>250048</v>
+      </c>
+      <c r="C86" s="6">
+        <v>11859</v>
+      </c>
+      <c r="D86" s="6">
+        <v>16187</v>
+      </c>
+      <c r="E86" s="6">
+        <v>10205</v>
+      </c>
+      <c r="F86" s="6">
+        <v>1082</v>
+      </c>
+      <c r="G86" s="6">
+        <v>289381</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D88" s="3"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G89" s="3"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D90" s="3"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D91" s="3"/>
+    </row>
+    <row r="101" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F101" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3250,9 +3261,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4318,69 +4329,90 @@
         <v>186</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="B30" s="8"/>
-      <c r="D30" s="3"/>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>43951.4375</v>
+      </c>
+      <c r="B30" s="6">
+        <v>6754</v>
+      </c>
+      <c r="C30" s="6">
+        <v>9280</v>
+      </c>
+      <c r="D30" s="6">
+        <v>371</v>
+      </c>
+      <c r="E30" s="6">
+        <v>3693</v>
+      </c>
+      <c r="F30" s="6">
+        <v>4871</v>
+      </c>
+      <c r="G30" s="6">
+        <v>3581</v>
+      </c>
+      <c r="H30" s="6">
+        <v>3664</v>
+      </c>
+      <c r="I30" s="6">
+        <v>999</v>
+      </c>
+      <c r="J30" s="6">
+        <v>233</v>
+      </c>
+      <c r="K30" s="6">
+        <v>181</v>
+      </c>
     </row>
     <row r="31" spans="1:14" ht="20" x14ac:dyDescent="0.2">
       <c r="B31" s="8"/>
     </row>
-    <row r="32" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="B32" s="8"/>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C32" s="3"/>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="B33" s="10"/>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B34" s="9"/>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C33" s="3"/>
     </row>
     <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B35" s="9"/>
+      <c r="C35" s="3"/>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B36" s="9"/>
+      <c r="C36" s="3"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="B37" s="10"/>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C37" s="3"/>
       <c r="G37" s="3"/>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B38" s="9"/>
+      <c r="C38" s="3"/>
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B39" s="9"/>
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B40" s="9"/>
+      <c r="C40" s="3"/>
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B41" s="6"/>
+      <c r="C41" s="3"/>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B42" s="6"/>
+      <c r="C42" s="3"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B43" s="6"/>
       <c r="D43" s="3"/>
       <c r="F43" s="3"/>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B44" s="6"/>
       <c r="D44" s="3"/>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B45" s="6"/>
       <c r="D45" s="3"/>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B46" s="6"/>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B47" s="6"/>

</xml_diff>

<commit_message>
excel update 2020-05-01 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED7972C-B112-3141-A84F-C8253A2A8287}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA5375D-D0B1-F141-895C-2772566ED877}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="19380" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -402,7 +402,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -430,6 +430,21 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF222222"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -448,11 +463,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -462,8 +478,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1160,11 +1180,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:H87"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C93" sqref="C93:D107"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3237,20 +3257,28 @@
         <v>289381</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D88" s="3"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="G89" s="3"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D90" s="3"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="D91" s="3"/>
-    </row>
-    <row r="101" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F101" s="3"/>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>43952.4375</v>
+      </c>
+      <c r="B87" s="6">
+        <v>265500</v>
+      </c>
+      <c r="C87" s="6">
+        <v>11975</v>
+      </c>
+      <c r="D87" s="6">
+        <v>16608</v>
+      </c>
+      <c r="E87" s="6">
+        <v>10825</v>
+      </c>
+      <c r="F87" s="6">
+        <v>1121</v>
+      </c>
+      <c r="G87" s="6">
+        <v>306029</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3259,11 +3287,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4364,69 +4392,151 @@
         <v>181</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="20" x14ac:dyDescent="0.2">
-      <c r="B31" s="8"/>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>43952.4375</v>
+      </c>
+      <c r="B31" s="6">
+        <v>6917</v>
+      </c>
+      <c r="C31" s="6">
+        <v>9538</v>
+      </c>
+      <c r="D31" s="6">
+        <v>384</v>
+      </c>
+      <c r="E31" s="6">
+        <v>3786</v>
+      </c>
+      <c r="F31" s="6">
+        <v>5004</v>
+      </c>
+      <c r="G31" s="6">
+        <v>3673</v>
+      </c>
+      <c r="H31" s="6">
+        <v>3753</v>
+      </c>
+      <c r="I31" s="6">
+        <v>1017</v>
+      </c>
+      <c r="J31" s="6">
+        <v>225</v>
+      </c>
+      <c r="K31" s="6">
+        <v>175</v>
+      </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="C32" s="3"/>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C33" s="3"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C37" s="3"/>
-      <c r="G37" s="3"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C42" s="3"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D43" s="3"/>
-      <c r="F43" s="3"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D45" s="3"/>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C33" s="9"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="8"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+    </row>
+    <row r="35" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C35" s="9"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C36" s="9"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C37" s="11"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+    </row>
+    <row r="38" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C38" s="8"/>
+      <c r="D38" s="10"/>
+      <c r="E38" s="8"/>
+    </row>
+    <row r="39" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C39" s="8"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="8"/>
+    </row>
+    <row r="40" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C40" s="8"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C41" s="8"/>
+      <c r="D41" s="10"/>
+      <c r="E41" s="8"/>
+    </row>
+    <row r="42" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C42" s="8"/>
+      <c r="D42" s="10"/>
+      <c r="E42" s="8"/>
+    </row>
+    <row r="43" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C43" s="8"/>
+      <c r="D43" s="10"/>
+      <c r="E43" s="8"/>
+    </row>
+    <row r="44" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C44" s="8"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="8"/>
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C45" s="11"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="3"/>
+    </row>
+    <row r="46" spans="2:7" ht="20" x14ac:dyDescent="0.2">
+      <c r="C46" s="9"/>
+      <c r="D46" s="10"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="B47" s="6"/>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C47" s="9"/>
+      <c r="D47" s="10"/>
+      <c r="E47" s="8"/>
+    </row>
+    <row r="48" spans="2:7" ht="20" x14ac:dyDescent="0.2">
       <c r="B48" s="6"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C48" s="9"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="8"/>
+    </row>
+    <row r="49" spans="2:5" ht="20" x14ac:dyDescent="0.2">
       <c r="B49" s="6"/>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C49" s="11"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+    </row>
+    <row r="50" spans="2:5" ht="20" x14ac:dyDescent="0.2">
       <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+    </row>
+    <row r="51" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="C51" s="9"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+    </row>
+    <row r="52" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="C52" s="9"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-02 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA5375D-D0B1-F141-895C-2772566ED877}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EE6FB3-13EE-FD40-8AA0-ADDD6C64E5B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="19380" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -402,7 +402,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -420,27 +420,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF222222"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF222222"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -463,27 +442,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1180,11 +1152,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:H87"/>
+  <dimension ref="A1:J88"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C99" sqref="C99"/>
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C90" sqref="C90:F109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1266,7 +1238,7 @@
       <c r="G3">
         <v>313</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -1290,7 +1262,7 @@
       <c r="G4">
         <v>340</v>
       </c>
-      <c r="H4" s="6"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -1314,7 +1286,7 @@
       <c r="G5">
         <v>364</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -1338,7 +1310,7 @@
       <c r="G6">
         <v>364</v>
       </c>
-      <c r="H6" s="6"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -1362,7 +1334,7 @@
       <c r="G7">
         <v>364</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -1386,7 +1358,7 @@
       <c r="G8">
         <v>402</v>
       </c>
-      <c r="H8" s="6"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -1410,7 +1382,7 @@
       <c r="G9">
         <v>421</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -1434,7 +1406,7 @@
       <c r="G10">
         <v>456</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -1458,7 +1430,7 @@
       <c r="G11">
         <v>479</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -1482,7 +1454,7 @@
       <c r="G12">
         <v>498</v>
       </c>
-      <c r="H12" s="6"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -1506,7 +1478,7 @@
       <c r="G13">
         <v>498</v>
       </c>
-      <c r="H13" s="6"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -1530,7 +1502,7 @@
       <c r="G14">
         <v>498</v>
       </c>
-      <c r="H14" s="6"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -1554,7 +1526,7 @@
       <c r="G15">
         <v>553</v>
       </c>
-      <c r="H15" s="6"/>
+      <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -1578,7 +1550,7 @@
       <c r="G16">
         <v>593</v>
       </c>
-      <c r="H16" s="6"/>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -1602,7 +1574,7 @@
       <c r="G17">
         <v>629</v>
       </c>
-      <c r="H17" s="6"/>
+      <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -1626,7 +1598,7 @@
       <c r="G18">
         <v>699</v>
       </c>
-      <c r="H18" s="6"/>
+      <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -1650,7 +1622,7 @@
       <c r="G19">
         <v>699</v>
       </c>
-      <c r="H19" s="6"/>
+      <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -1674,7 +1646,7 @@
       <c r="G20">
         <v>768</v>
       </c>
-      <c r="H20" s="6"/>
+      <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -1698,7 +1670,7 @@
       <c r="G21">
         <v>768</v>
       </c>
-      <c r="H21" s="6"/>
+      <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
@@ -1722,7 +1694,7 @@
       <c r="G22">
         <v>1005</v>
       </c>
-      <c r="H22" s="6"/>
+      <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
@@ -1746,7 +1718,7 @@
       <c r="G23">
         <v>1126</v>
       </c>
-      <c r="H23" s="6"/>
+      <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
@@ -1770,7 +1742,7 @@
       <c r="G24">
         <v>1338</v>
       </c>
-      <c r="H24" s="6"/>
+      <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
@@ -1794,7 +1766,7 @@
       <c r="G25">
         <v>1566</v>
       </c>
-      <c r="H25" s="6"/>
+      <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
@@ -1818,7 +1790,7 @@
       <c r="G26">
         <v>1763</v>
       </c>
-      <c r="H26" s="6"/>
+      <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
@@ -1842,7 +1814,7 @@
       <c r="G27">
         <v>1982</v>
       </c>
-      <c r="H27" s="6"/>
+      <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
@@ -1866,7 +1838,7 @@
       <c r="G28">
         <v>1982</v>
       </c>
-      <c r="H28" s="6"/>
+      <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
@@ -1890,7 +1862,7 @@
       <c r="G29">
         <v>2403</v>
       </c>
-      <c r="H29" s="6"/>
+      <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
@@ -1914,7 +1886,7 @@
       <c r="G30">
         <v>2747</v>
       </c>
-      <c r="H30" s="6"/>
+      <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
@@ -1938,7 +1910,7 @@
       <c r="G31">
         <v>2747</v>
       </c>
-      <c r="H31" s="6"/>
+      <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
@@ -1962,7 +1934,7 @@
       <c r="G32">
         <v>3395</v>
       </c>
-      <c r="H32" s="6"/>
+      <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
@@ -1986,7 +1958,7 @@
       <c r="G33">
         <v>4185</v>
       </c>
-      <c r="H33" s="6"/>
+      <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
@@ -2010,7 +1982,7 @@
       <c r="G34">
         <v>5129</v>
       </c>
-      <c r="H34" s="6"/>
+      <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
@@ -2034,7 +2006,7 @@
       <c r="G35">
         <v>6648</v>
       </c>
-      <c r="H35" s="6"/>
+      <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
@@ -2058,7 +2030,7 @@
       <c r="G36">
         <v>8465</v>
       </c>
-      <c r="H36" s="6"/>
+      <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
@@ -2082,7 +2054,7 @@
       <c r="G37">
         <v>10178</v>
       </c>
-      <c r="H37" s="6"/>
+      <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
@@ -2106,7 +2078,7 @@
       <c r="G38">
         <v>11171</v>
       </c>
-      <c r="H38" s="6"/>
+      <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
@@ -2130,7 +2102,7 @@
       <c r="G39">
         <v>16650</v>
       </c>
-      <c r="H39" s="6"/>
+      <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
@@ -2154,7 +2126,7 @@
       <c r="G40">
         <v>16650</v>
       </c>
-      <c r="H40" s="6"/>
+      <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
@@ -2178,7 +2150,7 @@
       <c r="G41">
         <v>23384</v>
       </c>
-      <c r="H41" s="6"/>
+      <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
@@ -2202,7 +2174,7 @@
       <c r="G42">
         <v>23384</v>
       </c>
-      <c r="H42" s="6"/>
+      <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
@@ -2226,7 +2198,7 @@
       <c r="G43">
         <v>26420</v>
       </c>
-      <c r="H43" s="6"/>
+      <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
@@ -2250,7 +2222,7 @@
       <c r="G44">
         <v>28506</v>
       </c>
-      <c r="H44" s="6"/>
+      <c r="H44" s="5"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
@@ -2274,7 +2246,7 @@
       <c r="G45">
         <v>32457</v>
       </c>
-      <c r="H45" s="6"/>
+      <c r="H45" s="5"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
@@ -2298,7 +2270,7 @@
       <c r="G46">
         <v>35635</v>
       </c>
-      <c r="H46" s="6"/>
+      <c r="H46" s="5"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
@@ -2322,7 +2294,7 @@
       <c r="G47">
         <v>35635</v>
       </c>
-      <c r="H47" s="6"/>
+      <c r="H47" s="5"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
@@ -2346,9 +2318,9 @@
       <c r="G48">
         <v>38550</v>
       </c>
-      <c r="H48" s="6"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H48" s="5"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>43916.729166666664</v>
       </c>
@@ -2370,9 +2342,9 @@
       <c r="G49">
         <v>38550</v>
       </c>
-      <c r="H49" s="6"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H49" s="5"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>43917.4375</v>
       </c>
@@ -2394,9 +2366,9 @@
       <c r="G50">
         <v>41032</v>
       </c>
-      <c r="H50" s="6"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H50" s="5"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>43918.4375</v>
       </c>
@@ -2418,9 +2390,9 @@
       <c r="G51">
         <v>43072</v>
       </c>
-      <c r="H51" s="6"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H51" s="5"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>43918.729166666664</v>
       </c>
@@ -2442,9 +2414,9 @@
       <c r="G52">
         <v>43072</v>
       </c>
-      <c r="H52" s="6"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H52" s="5"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>43919.4375</v>
       </c>
@@ -2466,9 +2438,9 @@
       <c r="G53">
         <v>49186</v>
       </c>
-      <c r="H53" s="6"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H53" s="5"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>43919.729166666664</v>
       </c>
@@ -2490,9 +2462,9 @@
       <c r="G54">
         <v>49186</v>
       </c>
-      <c r="H54" s="6"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H54" s="5"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>43920.4375</v>
       </c>
@@ -2514,9 +2486,9 @@
       <c r="G55">
         <v>54112</v>
       </c>
-      <c r="H55" s="6"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H55" s="5"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>43921.4375</v>
       </c>
@@ -2539,9 +2511,20 @@
         <f>51629+C53</f>
         <v>58832</v>
       </c>
-      <c r="H56" s="6"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H56" s="5">
+        <f>D56-D55</f>
+        <v>260</v>
+      </c>
+      <c r="I56">
+        <f>SUM(B56,D56:F56)</f>
+        <v>51095</v>
+      </c>
+      <c r="J56">
+        <f>H56/I56</f>
+        <v>5.0885605245131619E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>43922.4375</v>
       </c>
@@ -2563,9 +2546,10 @@
       <c r="G57">
         <v>61009</v>
       </c>
-      <c r="H57" s="6"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>43923.4375</v>
       </c>
@@ -2587,9 +2571,10 @@
       <c r="G58">
         <v>64785</v>
       </c>
-      <c r="H58" s="6"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>43924.4375</v>
       </c>
@@ -2611,9 +2596,10 @@
       <c r="G59">
         <v>67998</v>
       </c>
-      <c r="H59" s="6"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>43925.4375</v>
       </c>
@@ -2635,9 +2621,10 @@
       <c r="G60">
         <v>72674</v>
       </c>
-      <c r="H60" s="6"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>43926.4375</v>
       </c>
@@ -2659,9 +2646,10 @@
       <c r="G61">
         <v>76027</v>
       </c>
-      <c r="H61" s="6"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>43927.4375</v>
       </c>
@@ -2683,9 +2671,10 @@
       <c r="G62">
         <v>79125</v>
       </c>
-      <c r="H62" s="6"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>43928.4375</v>
       </c>
@@ -2707,9 +2696,10 @@
       <c r="G63">
         <v>82055</v>
       </c>
-      <c r="H63" s="6"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>43929.4375</v>
       </c>
@@ -2731,9 +2721,10 @@
       <c r="G64">
         <v>85703</v>
       </c>
-      <c r="H64" s="6"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>43930.4375</v>
       </c>
@@ -2755,9 +2746,10 @@
       <c r="G65">
         <v>89906</v>
       </c>
-      <c r="H65" s="6"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>43931.4375</v>
       </c>
@@ -2779,9 +2771,10 @@
       <c r="G66">
         <v>94271</v>
       </c>
-      <c r="H66" s="6"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>43932.4375</v>
       </c>
@@ -2803,9 +2796,10 @@
       <c r="G67">
         <v>97838</v>
       </c>
-      <c r="H67" s="6"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>43933.4375</v>
       </c>
@@ -2827,9 +2821,10 @@
       <c r="G68">
         <v>104784</v>
       </c>
-      <c r="H68" s="6"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>43934.4375</v>
       </c>
@@ -2851,9 +2846,10 @@
       <c r="G69">
         <v>109764</v>
       </c>
-      <c r="H69" s="6"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>43935.4375</v>
       </c>
@@ -2875,9 +2871,10 @@
       <c r="G70">
         <v>115189</v>
       </c>
-      <c r="H70" s="6"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>43936.4375</v>
       </c>
@@ -2899,9 +2896,10 @@
       <c r="G71">
         <v>123521</v>
       </c>
-      <c r="H71" s="6"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>43937.4375</v>
       </c>
@@ -2923,361 +2921,405 @@
       <c r="G72">
         <v>132416</v>
       </c>
-      <c r="H72" s="6"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H72" s="5"/>
+      <c r="I72" s="5"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>43938.4375</v>
       </c>
-      <c r="B73" s="6">
+      <c r="B73" s="5">
         <v>122433</v>
       </c>
-      <c r="C73" s="6">
+      <c r="C73" s="5">
         <v>5993</v>
       </c>
-      <c r="D73" s="6">
+      <c r="D73" s="5">
         <v>9525</v>
       </c>
-      <c r="E73" s="6">
+      <c r="E73" s="5">
         <v>4556</v>
       </c>
-      <c r="F73" s="6">
+      <c r="F73" s="5">
         <v>478</v>
       </c>
-      <c r="G73" s="6">
+      <c r="G73" s="5">
         <v>142985</v>
       </c>
-      <c r="H73" s="6"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H73" s="5"/>
+      <c r="I73" s="5"/>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>43939.4375</v>
       </c>
-      <c r="B74" s="6">
+      <c r="B74" s="5">
         <v>131055</v>
       </c>
-      <c r="C74" s="6">
+      <c r="C74" s="5">
         <v>6833</v>
       </c>
-      <c r="D74" s="6">
+      <c r="D74" s="5">
         <v>10010</v>
       </c>
-      <c r="E74" s="6">
+      <c r="E74" s="5">
         <v>4875</v>
       </c>
-      <c r="F74" s="6">
+      <c r="F74" s="5">
         <v>514</v>
       </c>
-      <c r="G74" s="6">
+      <c r="G74" s="5">
         <v>153287</v>
       </c>
-      <c r="H74" s="6"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>43940.4375</v>
       </c>
-      <c r="B75" s="6">
+      <c r="B75" s="5">
         <v>139757</v>
       </c>
-      <c r="C75" s="6">
+      <c r="C75" s="5">
         <v>5736</v>
       </c>
-      <c r="D75" s="6">
+      <c r="D75" s="5">
         <v>10578</v>
       </c>
-      <c r="E75" s="6">
+      <c r="E75" s="5">
         <v>5209</v>
       </c>
-      <c r="F75" s="6">
+      <c r="F75" s="5">
         <v>553</v>
       </c>
-      <c r="G75" s="6">
+      <c r="G75" s="5">
         <v>161833</v>
       </c>
-      <c r="H75" s="6"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>43941.4375</v>
       </c>
-      <c r="B76" s="6">
+      <c r="B76" s="5">
         <v>147557</v>
       </c>
-      <c r="C76" s="6">
+      <c r="C76" s="5">
         <v>3799</v>
       </c>
-      <c r="D76" s="6">
+      <c r="D76" s="5">
         <v>11184</v>
       </c>
-      <c r="E76" s="6">
+      <c r="E76" s="5">
         <v>5515</v>
       </c>
-      <c r="F76" s="6">
+      <c r="F76" s="5">
         <v>584</v>
       </c>
-      <c r="G76" s="6">
+      <c r="G76" s="5">
         <v>168639</v>
       </c>
-      <c r="H76" s="6"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H76" s="5"/>
+      <c r="I76" s="5"/>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>43942.4375</v>
       </c>
       <c r="B77">
         <v>156007</v>
       </c>
-      <c r="C77" s="6">
+      <c r="C77" s="5">
         <v>5546</v>
       </c>
-      <c r="D77" s="6">
+      <c r="D77" s="5">
         <v>11735</v>
       </c>
-      <c r="E77" s="6">
+      <c r="E77" s="5">
         <v>5806</v>
       </c>
-      <c r="F77" s="6">
+      <c r="F77" s="5">
         <v>622</v>
       </c>
       <c r="G77">
         <v>179716</v>
       </c>
-      <c r="H77" s="6"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H77" s="5"/>
+      <c r="I77" s="5"/>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>43943.4375</v>
       </c>
-      <c r="B78" s="6">
+      <c r="B78" s="5">
         <v>165406</v>
       </c>
-      <c r="C78" s="6">
+      <c r="C78" s="5">
         <v>6845</v>
       </c>
-      <c r="D78" s="6">
+      <c r="D78" s="5">
         <v>12245</v>
       </c>
-      <c r="E78" s="6">
+      <c r="E78" s="5">
         <v>6221</v>
       </c>
-      <c r="F78" s="6">
+      <c r="F78" s="5">
         <v>659</v>
       </c>
-      <c r="G78" s="6">
+      <c r="G78" s="5">
         <v>191376</v>
       </c>
-      <c r="H78" s="6"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H78" s="5"/>
+      <c r="I78" s="5"/>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>43944.4375</v>
       </c>
-      <c r="B79" s="6">
+      <c r="B79" s="5">
         <v>174473</v>
       </c>
-      <c r="C79" s="6">
+      <c r="C79" s="5">
         <v>6757</v>
       </c>
-      <c r="D79" s="6">
+      <c r="D79" s="5">
         <v>12879</v>
       </c>
-      <c r="E79" s="6">
+      <c r="E79" s="5">
         <v>6680</v>
       </c>
-      <c r="F79" s="6">
+      <c r="F79" s="5">
         <v>713</v>
       </c>
-      <c r="G79" s="6">
+      <c r="G79" s="5">
         <v>201502</v>
       </c>
-      <c r="H79" s="6"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H79" s="5"/>
+      <c r="I79" s="5"/>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>43945.4375</v>
       </c>
-      <c r="B80" s="6">
+      <c r="B80" s="5">
         <v>185671</v>
       </c>
-      <c r="C80" s="6">
+      <c r="C80" s="5">
         <v>5414</v>
       </c>
-      <c r="D80" s="6">
+      <c r="D80" s="5">
         <v>13519</v>
       </c>
-      <c r="E80" s="6">
+      <c r="E80" s="5">
         <v>7087</v>
       </c>
-      <c r="F80" s="6">
+      <c r="F80" s="5">
         <v>763</v>
       </c>
-      <c r="G80" s="6">
+      <c r="G80" s="5">
         <v>212454</v>
       </c>
-      <c r="H80" s="6"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H80" s="5"/>
+      <c r="I80" s="5"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>43946.4375</v>
       </c>
-      <c r="B81" s="6">
+      <c r="B81" s="5">
         <v>195303</v>
       </c>
-      <c r="C81" s="6">
+      <c r="C81" s="5">
         <v>8171</v>
       </c>
-      <c r="D81" s="6">
+      <c r="D81" s="5">
         <v>13995</v>
       </c>
-      <c r="E81" s="6">
+      <c r="E81" s="5">
         <v>7509</v>
       </c>
-      <c r="F81" s="6">
+      <c r="F81" s="5">
         <v>811</v>
       </c>
-      <c r="G81" s="6">
+      <c r="G81" s="5">
         <v>225789</v>
       </c>
-      <c r="H81" s="6"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H81" s="5"/>
+      <c r="I81" s="5"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>43947.4375</v>
       </c>
-      <c r="B82" s="6">
+      <c r="B82" s="5">
         <v>206371</v>
       </c>
-      <c r="C82" s="6">
+      <c r="C82" s="5">
         <v>7417</v>
       </c>
-      <c r="D82" s="6">
+      <c r="D82" s="5">
         <v>14432</v>
       </c>
-      <c r="E82" s="6">
+      <c r="E82" s="5">
         <v>8000</v>
       </c>
-      <c r="F82" s="6">
+      <c r="F82" s="5">
         <v>835</v>
       </c>
-      <c r="G82" s="6">
+      <c r="G82" s="5">
         <v>237055</v>
       </c>
-      <c r="H82" s="6"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H82" s="5"/>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>43948.4375</v>
       </c>
-      <c r="B83" s="6">
+      <c r="B83" s="5">
         <v>217915</v>
       </c>
-      <c r="C83" s="6">
+      <c r="C83" s="5">
         <v>5001</v>
       </c>
-      <c r="D83" s="6">
+      <c r="D83" s="5">
         <v>14856</v>
       </c>
-      <c r="E83" s="6">
+      <c r="E83" s="5">
         <v>8525</v>
       </c>
-      <c r="F83" s="6">
+      <c r="F83" s="5">
         <v>892</v>
       </c>
-      <c r="G83" s="6">
+      <c r="G83" s="5">
         <v>247189</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H83" s="5"/>
+      <c r="I83" s="5"/>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>43949.4375</v>
       </c>
-      <c r="B84" s="6">
+      <c r="B84" s="5">
         <v>227744</v>
       </c>
-      <c r="C84" s="6">
+      <c r="C84" s="5">
         <v>6282</v>
       </c>
-      <c r="D84" s="6">
+      <c r="D84" s="5">
         <v>15381</v>
       </c>
-      <c r="E84" s="6">
+      <c r="E84" s="5">
         <v>8964</v>
       </c>
-      <c r="F84" s="6">
+      <c r="F84" s="5">
         <v>951</v>
       </c>
-      <c r="G84" s="6">
+      <c r="G84" s="5">
         <v>259322</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H84" s="5"/>
+      <c r="I84" s="5"/>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>43950.4375</v>
       </c>
-      <c r="B85" s="6">
+      <c r="B85" s="5">
         <v>238258</v>
       </c>
-      <c r="C85" s="6">
+      <c r="C85" s="5">
         <v>9530</v>
       </c>
-      <c r="D85" s="6">
+      <c r="D85" s="5">
         <v>15728</v>
       </c>
-      <c r="E85" s="6">
+      <c r="E85" s="5">
         <v>9612</v>
       </c>
-      <c r="F85" s="6">
+      <c r="F85" s="5">
         <v>996</v>
       </c>
-      <c r="G85" s="6">
+      <c r="G85" s="5">
         <v>274124</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H85" s="5"/>
+      <c r="I85" s="5"/>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>43951.4375</v>
       </c>
-      <c r="B86" s="6">
+      <c r="B86" s="5">
         <v>250048</v>
       </c>
-      <c r="C86" s="6">
+      <c r="C86" s="5">
         <v>11859</v>
       </c>
-      <c r="D86" s="6">
+      <c r="D86" s="5">
         <v>16187</v>
       </c>
-      <c r="E86" s="6">
+      <c r="E86" s="5">
         <v>10205</v>
       </c>
-      <c r="F86" s="6">
+      <c r="F86" s="5">
         <v>1082</v>
       </c>
-      <c r="G86" s="6">
+      <c r="G86" s="5">
         <v>289381</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H86" s="5"/>
+      <c r="I86" s="5"/>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>43952.4375</v>
       </c>
-      <c r="B87" s="6">
+      <c r="B87" s="5">
         <v>265500</v>
       </c>
-      <c r="C87" s="6">
+      <c r="C87" s="5">
         <v>11975</v>
       </c>
-      <c r="D87" s="6">
+      <c r="D87" s="5">
         <v>16608</v>
       </c>
-      <c r="E87" s="6">
+      <c r="E87" s="5">
         <v>10825</v>
       </c>
-      <c r="F87" s="6">
+      <c r="F87" s="5">
         <v>1121</v>
       </c>
-      <c r="G87" s="6">
+      <c r="G87" s="5">
         <v>306029</v>
+      </c>
+      <c r="H87" s="5"/>
+      <c r="I87" s="5"/>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>43953.4375</v>
+      </c>
+      <c r="B88" s="5">
+        <v>280674</v>
+      </c>
+      <c r="C88" s="5">
+        <v>12829</v>
+      </c>
+      <c r="D88" s="5">
+        <v>17119</v>
+      </c>
+      <c r="E88" s="5">
+        <v>11390</v>
+      </c>
+      <c r="F88" s="5">
+        <v>1176</v>
+      </c>
+      <c r="G88" s="5">
+        <v>323188</v>
       </c>
     </row>
   </sheetData>
@@ -3287,11 +3329,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3300,7 +3342,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
@@ -3394,9 +3436,9 @@
       <c r="K3">
         <v>140</v>
       </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -3432,9 +3474,9 @@
       <c r="K4">
         <v>152</v>
       </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -3470,9 +3512,9 @@
       <c r="K5">
         <v>154</v>
       </c>
-      <c r="L5" s="7"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -3508,9 +3550,9 @@
       <c r="K6">
         <v>160</v>
       </c>
-      <c r="L6" s="7"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -3546,9 +3588,9 @@
       <c r="K7">
         <v>187</v>
       </c>
-      <c r="L7" s="7"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -3584,9 +3626,9 @@
       <c r="K8">
         <v>195</v>
       </c>
-      <c r="L8" s="7"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -3622,9 +3664,9 @@
       <c r="K9">
         <v>214</v>
       </c>
-      <c r="L9" s="7"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -3660,9 +3702,9 @@
       <c r="K10">
         <v>217</v>
       </c>
-      <c r="L10" s="7"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -3698,9 +3740,9 @@
       <c r="K11">
         <v>215</v>
       </c>
-      <c r="L11" s="7"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -3736,9 +3778,9 @@
       <c r="K12">
         <v>196</v>
       </c>
-      <c r="L12" s="7"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -3774,9 +3816,9 @@
       <c r="K13">
         <v>203</v>
       </c>
-      <c r="L13" s="7"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -3812,9 +3854,9 @@
       <c r="K14">
         <v>199</v>
       </c>
-      <c r="L14" s="7"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -3850,9 +3892,9 @@
       <c r="K15">
         <v>188</v>
       </c>
-      <c r="L15" s="7"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -3888,262 +3930,262 @@
       <c r="K16">
         <v>200</v>
       </c>
-      <c r="L16" s="7"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43938.4375</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <v>4074</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>5380</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>210</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>2164</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <v>3067</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <v>2214</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <v>1864</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="5">
         <v>829</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J17" s="5">
         <v>245</v>
       </c>
-      <c r="K17" s="6">
+      <c r="K17" s="5">
         <v>200</v>
       </c>
-      <c r="L17" s="7"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43939.4375</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>4277</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>5658</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <v>223</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>2269</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <v>3201</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="5">
         <v>2313</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="5">
         <v>1996</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="5">
         <v>828</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J18" s="5">
         <v>250</v>
       </c>
-      <c r="K18" s="6">
+      <c r="K18" s="5">
         <v>197</v>
       </c>
-      <c r="L18" s="7"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43940.4375</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <v>4495</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>5996</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <v>235</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>2408</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="5">
         <v>3354</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="5">
         <v>2437</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="5">
         <v>2135</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="5">
         <v>809</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="5">
         <v>247</v>
       </c>
-      <c r="K19" s="6">
+      <c r="K19" s="5">
         <v>196</v>
       </c>
-      <c r="L19" s="7"/>
+      <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43941.4375</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <v>4728</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>6354</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <v>248</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>2525</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="5">
         <v>3502</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="5">
         <v>2580</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="5">
         <v>2312</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20" s="5">
         <v>802</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J20" s="5">
         <v>247</v>
       </c>
-      <c r="K20" s="6">
+      <c r="K20" s="5">
         <v>193</v>
       </c>
-      <c r="L20" s="7"/>
+      <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43942.4375</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>4955</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>6663</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <v>260</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>2657</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="5">
         <v>3665</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="5">
         <v>2687</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="5">
         <v>2457</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="5">
         <v>859</v>
       </c>
-      <c r="J21" s="6">
+      <c r="J21" s="5">
         <v>250</v>
       </c>
-      <c r="K21" s="6">
+      <c r="K21" s="5">
         <v>194</v>
       </c>
-      <c r="L21" s="7"/>
+      <c r="L21" s="6"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43943.4375</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <v>5169</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>6952</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <v>270</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <v>2781</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="5">
         <v>3798</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="5">
         <v>2778</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="5">
         <v>2609</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="5">
         <v>878</v>
       </c>
-      <c r="J22" s="6">
+      <c r="J22" s="5">
         <v>243</v>
       </c>
-      <c r="K22" s="6">
+      <c r="K22" s="5">
         <v>192</v>
       </c>
-      <c r="L22" s="7"/>
+      <c r="L22" s="6"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43944.4375</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <v>5408</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="5">
         <v>7342</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <v>284</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="5">
         <v>2914</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="5">
         <v>3945</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="5">
         <v>2909</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="5">
         <v>2816</v>
       </c>
-      <c r="I23" s="6">
+      <c r="I23" s="5">
         <v>887</v>
       </c>
-      <c r="J23" s="6">
+      <c r="J23" s="5">
         <v>233</v>
       </c>
-      <c r="K23" s="6">
+      <c r="K23" s="5">
         <v>185</v>
       </c>
     </row>
@@ -4151,34 +4193,34 @@
       <c r="A24" s="1">
         <v>43945.4375</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <v>5640</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="5">
         <v>7737</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <v>292</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="5">
         <v>3052</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="5">
         <v>4108</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="5">
         <v>3029</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H24" s="5">
         <v>3029</v>
       </c>
-      <c r="I24" s="6">
+      <c r="I24" s="5">
         <v>910</v>
       </c>
-      <c r="J24" s="6">
+      <c r="J24" s="5">
         <v>243</v>
       </c>
-      <c r="K24" s="6">
+      <c r="K24" s="5">
         <v>193</v>
       </c>
     </row>
@@ -4186,34 +4228,34 @@
       <c r="A25" s="1">
         <v>43946.4375</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <v>5827</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5">
         <v>8030</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <v>309</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="5">
         <v>3179</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="5">
         <v>4276</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="5">
         <v>3108</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="5">
         <v>3114</v>
       </c>
-      <c r="I25" s="6">
+      <c r="I25" s="5">
         <v>925</v>
       </c>
-      <c r="J25" s="6">
+      <c r="J25" s="5">
         <v>245</v>
       </c>
-      <c r="K25" s="6">
+      <c r="K25" s="5">
         <v>195</v>
       </c>
     </row>
@@ -4221,34 +4263,34 @@
       <c r="A26" s="1">
         <v>43947.4375</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <v>6005</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="5">
         <v>8290</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="5">
         <v>320</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="5">
         <v>3292</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="5">
         <v>4391</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="5">
         <v>3207</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H26" s="5">
         <v>3213</v>
       </c>
-      <c r="I26" s="6">
+      <c r="I26" s="5">
         <v>938</v>
       </c>
-      <c r="J26" s="6">
+      <c r="J26" s="5">
         <v>252</v>
       </c>
-      <c r="K26" s="6">
+      <c r="K26" s="5">
         <v>195</v>
       </c>
     </row>
@@ -4256,34 +4298,34 @@
       <c r="A27" s="1">
         <v>43948.4375</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="5">
         <v>6168</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="5">
         <v>8548</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <v>326</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="5">
         <v>3398</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="5">
         <v>4504</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="5">
         <v>3302</v>
       </c>
-      <c r="H27" s="6">
+      <c r="H27" s="5">
         <v>3318</v>
       </c>
-      <c r="I27" s="6">
+      <c r="I27" s="5">
         <v>945</v>
       </c>
-      <c r="J27" s="6">
+      <c r="J27" s="5">
         <v>241</v>
       </c>
-      <c r="K27" s="6">
+      <c r="K27" s="5">
         <v>191</v>
       </c>
     </row>
@@ -4291,34 +4333,34 @@
       <c r="A28" s="1">
         <v>43949.4375</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="5">
         <v>6392</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="5">
         <v>8848</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="5">
         <v>346</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="5">
         <v>3521</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="5">
         <v>4644</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G28" s="5">
         <v>3420</v>
       </c>
-      <c r="H28" s="6">
+      <c r="H28" s="5">
         <v>3443</v>
       </c>
-      <c r="I28" s="6">
+      <c r="I28" s="5">
         <v>957</v>
       </c>
-      <c r="J28" s="6">
+      <c r="J28" s="5">
         <v>239</v>
       </c>
-      <c r="K28" s="6">
+      <c r="K28" s="5">
         <v>187</v>
       </c>
     </row>
@@ -4326,34 +4368,34 @@
       <c r="A29" s="1">
         <v>43950.4375</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="5">
         <v>6546</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="5">
         <v>9041</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="5">
         <v>363</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="5">
         <v>3583</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="5">
         <v>4725</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="5">
         <v>3486</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H29" s="5">
         <v>3564</v>
       </c>
-      <c r="I29" s="6">
+      <c r="I29" s="5">
         <v>977</v>
       </c>
-      <c r="J29" s="6">
+      <c r="J29" s="5">
         <v>235</v>
       </c>
-      <c r="K29" s="6">
+      <c r="K29" s="5">
         <v>186</v>
       </c>
     </row>
@@ -4361,34 +4403,34 @@
       <c r="A30" s="1">
         <v>43951.4375</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="5">
         <v>6754</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="5">
         <v>9280</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="5">
         <v>371</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="5">
         <v>3693</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="5">
         <v>4871</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G30" s="5">
         <v>3581</v>
       </c>
-      <c r="H30" s="6">
+      <c r="H30" s="5">
         <v>3664</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I30" s="5">
         <v>999</v>
       </c>
-      <c r="J30" s="6">
+      <c r="J30" s="5">
         <v>233</v>
       </c>
-      <c r="K30" s="6">
+      <c r="K30" s="5">
         <v>181</v>
       </c>
     </row>
@@ -4396,147 +4438,71 @@
       <c r="A31" s="1">
         <v>43952.4375</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="5">
         <v>6917</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="5">
         <v>9538</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <v>384</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="5">
         <v>3786</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="5">
         <v>5004</v>
       </c>
-      <c r="G31" s="6">
+      <c r="G31" s="5">
         <v>3673</v>
       </c>
-      <c r="H31" s="6">
+      <c r="H31" s="5">
         <v>3753</v>
       </c>
-      <c r="I31" s="6">
+      <c r="I31" s="5">
         <v>1017</v>
       </c>
-      <c r="J31" s="6">
+      <c r="J31" s="5">
         <v>225</v>
       </c>
-      <c r="K31" s="6">
+      <c r="K31" s="5">
         <v>175</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C33" s="9"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="8"/>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-    </row>
-    <row r="35" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C35" s="9"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="8"/>
-    </row>
-    <row r="36" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C36" s="9"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="8"/>
-    </row>
-    <row r="37" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C37" s="11"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-    </row>
-    <row r="38" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C38" s="8"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="8"/>
-    </row>
-    <row r="39" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C39" s="8"/>
-      <c r="D39" s="10"/>
-      <c r="E39" s="8"/>
-    </row>
-    <row r="40" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-    </row>
-    <row r="41" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C41" s="8"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="8"/>
-    </row>
-    <row r="42" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C42" s="8"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="8"/>
-    </row>
-    <row r="43" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C43" s="8"/>
-      <c r="D43" s="10"/>
-      <c r="E43" s="8"/>
-    </row>
-    <row r="44" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C44" s="8"/>
-      <c r="D44" s="10"/>
-      <c r="E44" s="8"/>
-      <c r="G44" s="3"/>
-    </row>
-    <row r="45" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C45" s="11"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="3"/>
-    </row>
-    <row r="46" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="C46" s="9"/>
-      <c r="D46" s="10"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="B47" s="6"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="8"/>
-    </row>
-    <row r="48" spans="2:7" ht="20" x14ac:dyDescent="0.2">
-      <c r="B48" s="6"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="8"/>
-    </row>
-    <row r="49" spans="2:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="B49" s="6"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
-    </row>
-    <row r="50" spans="2:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="B50" s="6"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-    </row>
-    <row r="51" spans="2:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="C51" s="9"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-    </row>
-    <row r="52" spans="2:5" ht="20" x14ac:dyDescent="0.2">
-      <c r="C52" s="9"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
+      <c r="A32" s="1">
+        <v>43953.4375</v>
+      </c>
+      <c r="B32" s="5">
+        <v>7113</v>
+      </c>
+      <c r="C32" s="5">
+        <v>9845</v>
+      </c>
+      <c r="D32" s="5">
+        <v>405</v>
+      </c>
+      <c r="E32" s="5">
+        <v>3918</v>
+      </c>
+      <c r="F32" s="5">
+        <v>5169</v>
+      </c>
+      <c r="G32" s="5">
+        <v>3776</v>
+      </c>
+      <c r="H32" s="5">
+        <v>3842</v>
+      </c>
+      <c r="I32" s="5">
+        <v>977</v>
+      </c>
+      <c r="J32" s="5">
+        <v>221</v>
+      </c>
+      <c r="K32" s="5">
+        <v>154</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-03 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EE6FB3-13EE-FD40-8AA0-ADDD6C64E5B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80886EBD-DDE0-B843-8089-AEB544F0C668}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -402,7 +402,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -420,6 +420,27 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF222222"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF222222"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -442,20 +463,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1152,11 +1180,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:J88"/>
+  <dimension ref="A1:J94"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C90" sqref="C90:F109"/>
+      <selection pane="bottomLeft" activeCell="C95" sqref="C95:F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1238,7 +1266,7 @@
       <c r="G3">
         <v>313</v>
       </c>
-      <c r="H3" s="5"/>
+      <c r="H3" s="6"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -1262,7 +1290,7 @@
       <c r="G4">
         <v>340</v>
       </c>
-      <c r="H4" s="5"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -1286,7 +1314,7 @@
       <c r="G5">
         <v>364</v>
       </c>
-      <c r="H5" s="5"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -1310,7 +1338,7 @@
       <c r="G6">
         <v>364</v>
       </c>
-      <c r="H6" s="5"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -1334,7 +1362,7 @@
       <c r="G7">
         <v>364</v>
       </c>
-      <c r="H7" s="5"/>
+      <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -1358,7 +1386,7 @@
       <c r="G8">
         <v>402</v>
       </c>
-      <c r="H8" s="5"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -1382,7 +1410,7 @@
       <c r="G9">
         <v>421</v>
       </c>
-      <c r="H9" s="5"/>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -1406,7 +1434,7 @@
       <c r="G10">
         <v>456</v>
       </c>
-      <c r="H10" s="5"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -1430,7 +1458,7 @@
       <c r="G11">
         <v>479</v>
       </c>
-      <c r="H11" s="5"/>
+      <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -1454,7 +1482,7 @@
       <c r="G12">
         <v>498</v>
       </c>
-      <c r="H12" s="5"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -1478,7 +1506,7 @@
       <c r="G13">
         <v>498</v>
       </c>
-      <c r="H13" s="5"/>
+      <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -1502,7 +1530,7 @@
       <c r="G14">
         <v>498</v>
       </c>
-      <c r="H14" s="5"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -1526,7 +1554,7 @@
       <c r="G15">
         <v>553</v>
       </c>
-      <c r="H15" s="5"/>
+      <c r="H15" s="6"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -1550,7 +1578,7 @@
       <c r="G16">
         <v>593</v>
       </c>
-      <c r="H16" s="5"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -1574,7 +1602,7 @@
       <c r="G17">
         <v>629</v>
       </c>
-      <c r="H17" s="5"/>
+      <c r="H17" s="6"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -1598,7 +1626,7 @@
       <c r="G18">
         <v>699</v>
       </c>
-      <c r="H18" s="5"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -1622,7 +1650,7 @@
       <c r="G19">
         <v>699</v>
       </c>
-      <c r="H19" s="5"/>
+      <c r="H19" s="6"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -1646,7 +1674,7 @@
       <c r="G20">
         <v>768</v>
       </c>
-      <c r="H20" s="5"/>
+      <c r="H20" s="6"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -1670,7 +1698,7 @@
       <c r="G21">
         <v>768</v>
       </c>
-      <c r="H21" s="5"/>
+      <c r="H21" s="6"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
@@ -1694,7 +1722,7 @@
       <c r="G22">
         <v>1005</v>
       </c>
-      <c r="H22" s="5"/>
+      <c r="H22" s="6"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
@@ -1718,7 +1746,7 @@
       <c r="G23">
         <v>1126</v>
       </c>
-      <c r="H23" s="5"/>
+      <c r="H23" s="6"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
@@ -1742,7 +1770,7 @@
       <c r="G24">
         <v>1338</v>
       </c>
-      <c r="H24" s="5"/>
+      <c r="H24" s="6"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
@@ -1766,7 +1794,7 @@
       <c r="G25">
         <v>1566</v>
       </c>
-      <c r="H25" s="5"/>
+      <c r="H25" s="6"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
@@ -1790,7 +1818,7 @@
       <c r="G26">
         <v>1763</v>
       </c>
-      <c r="H26" s="5"/>
+      <c r="H26" s="6"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
@@ -1814,7 +1842,7 @@
       <c r="G27">
         <v>1982</v>
       </c>
-      <c r="H27" s="5"/>
+      <c r="H27" s="6"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
@@ -1838,7 +1866,7 @@
       <c r="G28">
         <v>1982</v>
       </c>
-      <c r="H28" s="5"/>
+      <c r="H28" s="6"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
@@ -1862,7 +1890,7 @@
       <c r="G29">
         <v>2403</v>
       </c>
-      <c r="H29" s="5"/>
+      <c r="H29" s="6"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
@@ -1886,7 +1914,7 @@
       <c r="G30">
         <v>2747</v>
       </c>
-      <c r="H30" s="5"/>
+      <c r="H30" s="6"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
@@ -1910,7 +1938,7 @@
       <c r="G31">
         <v>2747</v>
       </c>
-      <c r="H31" s="5"/>
+      <c r="H31" s="6"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
@@ -1934,7 +1962,7 @@
       <c r="G32">
         <v>3395</v>
       </c>
-      <c r="H32" s="5"/>
+      <c r="H32" s="6"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
@@ -1958,7 +1986,7 @@
       <c r="G33">
         <v>4185</v>
       </c>
-      <c r="H33" s="5"/>
+      <c r="H33" s="6"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
@@ -1982,7 +2010,7 @@
       <c r="G34">
         <v>5129</v>
       </c>
-      <c r="H34" s="5"/>
+      <c r="H34" s="6"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
@@ -2006,7 +2034,7 @@
       <c r="G35">
         <v>6648</v>
       </c>
-      <c r="H35" s="5"/>
+      <c r="H35" s="6"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
@@ -2030,7 +2058,7 @@
       <c r="G36">
         <v>8465</v>
       </c>
-      <c r="H36" s="5"/>
+      <c r="H36" s="6"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
@@ -2054,7 +2082,7 @@
       <c r="G37">
         <v>10178</v>
       </c>
-      <c r="H37" s="5"/>
+      <c r="H37" s="6"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
@@ -2078,7 +2106,7 @@
       <c r="G38">
         <v>11171</v>
       </c>
-      <c r="H38" s="5"/>
+      <c r="H38" s="6"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
@@ -2102,7 +2130,7 @@
       <c r="G39">
         <v>16650</v>
       </c>
-      <c r="H39" s="5"/>
+      <c r="H39" s="6"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
@@ -2126,7 +2154,7 @@
       <c r="G40">
         <v>16650</v>
       </c>
-      <c r="H40" s="5"/>
+      <c r="H40" s="6"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
@@ -2150,7 +2178,7 @@
       <c r="G41">
         <v>23384</v>
       </c>
-      <c r="H41" s="5"/>
+      <c r="H41" s="6"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
@@ -2174,7 +2202,7 @@
       <c r="G42">
         <v>23384</v>
       </c>
-      <c r="H42" s="5"/>
+      <c r="H42" s="6"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
@@ -2198,7 +2226,7 @@
       <c r="G43">
         <v>26420</v>
       </c>
-      <c r="H43" s="5"/>
+      <c r="H43" s="6"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
@@ -2222,7 +2250,7 @@
       <c r="G44">
         <v>28506</v>
       </c>
-      <c r="H44" s="5"/>
+      <c r="H44" s="6"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
@@ -2246,7 +2274,7 @@
       <c r="G45">
         <v>32457</v>
       </c>
-      <c r="H45" s="5"/>
+      <c r="H45" s="6"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
@@ -2270,7 +2298,7 @@
       <c r="G46">
         <v>35635</v>
       </c>
-      <c r="H46" s="5"/>
+      <c r="H46" s="6"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
@@ -2294,7 +2322,7 @@
       <c r="G47">
         <v>35635</v>
       </c>
-      <c r="H47" s="5"/>
+      <c r="H47" s="6"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
@@ -2318,7 +2346,7 @@
       <c r="G48">
         <v>38550</v>
       </c>
-      <c r="H48" s="5"/>
+      <c r="H48" s="6"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
@@ -2342,7 +2370,7 @@
       <c r="G49">
         <v>38550</v>
       </c>
-      <c r="H49" s="5"/>
+      <c r="H49" s="6"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
@@ -2366,7 +2394,7 @@
       <c r="G50">
         <v>41032</v>
       </c>
-      <c r="H50" s="5"/>
+      <c r="H50" s="6"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
@@ -2390,7 +2418,7 @@
       <c r="G51">
         <v>43072</v>
       </c>
-      <c r="H51" s="5"/>
+      <c r="H51" s="6"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
@@ -2414,7 +2442,7 @@
       <c r="G52">
         <v>43072</v>
       </c>
-      <c r="H52" s="5"/>
+      <c r="H52" s="6"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
@@ -2438,7 +2466,7 @@
       <c r="G53">
         <v>49186</v>
       </c>
-      <c r="H53" s="5"/>
+      <c r="H53" s="6"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
@@ -2462,7 +2490,7 @@
       <c r="G54">
         <v>49186</v>
       </c>
-      <c r="H54" s="5"/>
+      <c r="H54" s="6"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
@@ -2486,7 +2514,7 @@
       <c r="G55">
         <v>54112</v>
       </c>
-      <c r="H55" s="5"/>
+      <c r="H55" s="6"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
@@ -2511,7 +2539,7 @@
         <f>51629+C53</f>
         <v>58832</v>
       </c>
-      <c r="H56" s="5">
+      <c r="H56" s="6">
         <f>D56-D55</f>
         <v>260</v>
       </c>
@@ -2546,8 +2574,8 @@
       <c r="G57">
         <v>61009</v>
       </c>
-      <c r="H57" s="5"/>
-      <c r="I57" s="5"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
@@ -2571,8 +2599,8 @@
       <c r="G58">
         <v>64785</v>
       </c>
-      <c r="H58" s="5"/>
-      <c r="I58" s="5"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
@@ -2596,8 +2624,8 @@
       <c r="G59">
         <v>67998</v>
       </c>
-      <c r="H59" s="5"/>
-      <c r="I59" s="5"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
@@ -2621,8 +2649,8 @@
       <c r="G60">
         <v>72674</v>
       </c>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
@@ -2646,8 +2674,8 @@
       <c r="G61">
         <v>76027</v>
       </c>
-      <c r="H61" s="5"/>
-      <c r="I61" s="5"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
@@ -2671,8 +2699,8 @@
       <c r="G62">
         <v>79125</v>
       </c>
-      <c r="H62" s="5"/>
-      <c r="I62" s="5"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
@@ -2696,8 +2724,8 @@
       <c r="G63">
         <v>82055</v>
       </c>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
@@ -2721,8 +2749,8 @@
       <c r="G64">
         <v>85703</v>
       </c>
-      <c r="H64" s="5"/>
-      <c r="I64" s="5"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
@@ -2746,8 +2774,8 @@
       <c r="G65">
         <v>89906</v>
       </c>
-      <c r="H65" s="5"/>
-      <c r="I65" s="5"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
@@ -2771,8 +2799,8 @@
       <c r="G66">
         <v>94271</v>
       </c>
-      <c r="H66" s="5"/>
-      <c r="I66" s="5"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
@@ -2796,8 +2824,8 @@
       <c r="G67">
         <v>97838</v>
       </c>
-      <c r="H67" s="5"/>
-      <c r="I67" s="5"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
@@ -2821,8 +2849,8 @@
       <c r="G68">
         <v>104784</v>
       </c>
-      <c r="H68" s="5"/>
-      <c r="I68" s="5"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
@@ -2846,8 +2874,8 @@
       <c r="G69">
         <v>109764</v>
       </c>
-      <c r="H69" s="5"/>
-      <c r="I69" s="5"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
@@ -2871,8 +2899,8 @@
       <c r="G70">
         <v>115189</v>
       </c>
-      <c r="H70" s="5"/>
-      <c r="I70" s="5"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
@@ -2896,8 +2924,8 @@
       <c r="G71">
         <v>123521</v>
       </c>
-      <c r="H71" s="5"/>
-      <c r="I71" s="5"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
@@ -2921,108 +2949,108 @@
       <c r="G72">
         <v>132416</v>
       </c>
-      <c r="H72" s="5"/>
-      <c r="I72" s="5"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>43938.4375</v>
       </c>
-      <c r="B73" s="5">
+      <c r="B73" s="6">
         <v>122433</v>
       </c>
-      <c r="C73" s="5">
+      <c r="C73" s="6">
         <v>5993</v>
       </c>
-      <c r="D73" s="5">
+      <c r="D73" s="6">
         <v>9525</v>
       </c>
-      <c r="E73" s="5">
+      <c r="E73" s="6">
         <v>4556</v>
       </c>
-      <c r="F73" s="5">
+      <c r="F73" s="6">
         <v>478</v>
       </c>
-      <c r="G73" s="5">
+      <c r="G73" s="6">
         <v>142985</v>
       </c>
-      <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>43939.4375</v>
       </c>
-      <c r="B74" s="5">
+      <c r="B74" s="6">
         <v>131055</v>
       </c>
-      <c r="C74" s="5">
+      <c r="C74" s="6">
         <v>6833</v>
       </c>
-      <c r="D74" s="5">
+      <c r="D74" s="6">
         <v>10010</v>
       </c>
-      <c r="E74" s="5">
+      <c r="E74" s="6">
         <v>4875</v>
       </c>
-      <c r="F74" s="5">
+      <c r="F74" s="6">
         <v>514</v>
       </c>
-      <c r="G74" s="5">
+      <c r="G74" s="6">
         <v>153287</v>
       </c>
-      <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>43940.4375</v>
       </c>
-      <c r="B75" s="5">
+      <c r="B75" s="6">
         <v>139757</v>
       </c>
-      <c r="C75" s="5">
+      <c r="C75" s="6">
         <v>5736</v>
       </c>
-      <c r="D75" s="5">
+      <c r="D75" s="6">
         <v>10578</v>
       </c>
-      <c r="E75" s="5">
+      <c r="E75" s="6">
         <v>5209</v>
       </c>
-      <c r="F75" s="5">
+      <c r="F75" s="6">
         <v>553</v>
       </c>
-      <c r="G75" s="5">
+      <c r="G75" s="6">
         <v>161833</v>
       </c>
-      <c r="H75" s="5"/>
-      <c r="I75" s="5"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>43941.4375</v>
       </c>
-      <c r="B76" s="5">
+      <c r="B76" s="6">
         <v>147557</v>
       </c>
-      <c r="C76" s="5">
+      <c r="C76" s="6">
         <v>3799</v>
       </c>
-      <c r="D76" s="5">
+      <c r="D76" s="6">
         <v>11184</v>
       </c>
-      <c r="E76" s="5">
+      <c r="E76" s="6">
         <v>5515</v>
       </c>
-      <c r="F76" s="5">
+      <c r="F76" s="6">
         <v>584</v>
       </c>
-      <c r="G76" s="5">
+      <c r="G76" s="6">
         <v>168639</v>
       </c>
-      <c r="H76" s="5"/>
-      <c r="I76" s="5"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
@@ -3031,296 +3059,339 @@
       <c r="B77">
         <v>156007</v>
       </c>
-      <c r="C77" s="5">
+      <c r="C77" s="6">
         <v>5546</v>
       </c>
-      <c r="D77" s="5">
+      <c r="D77" s="6">
         <v>11735</v>
       </c>
-      <c r="E77" s="5">
+      <c r="E77" s="6">
         <v>5806</v>
       </c>
-      <c r="F77" s="5">
+      <c r="F77" s="6">
         <v>622</v>
       </c>
       <c r="G77">
         <v>179716</v>
       </c>
-      <c r="H77" s="5"/>
-      <c r="I77" s="5"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>43943.4375</v>
       </c>
-      <c r="B78" s="5">
+      <c r="B78" s="6">
         <v>165406</v>
       </c>
-      <c r="C78" s="5">
+      <c r="C78" s="6">
         <v>6845</v>
       </c>
-      <c r="D78" s="5">
+      <c r="D78" s="6">
         <v>12245</v>
       </c>
-      <c r="E78" s="5">
+      <c r="E78" s="6">
         <v>6221</v>
       </c>
-      <c r="F78" s="5">
+      <c r="F78" s="6">
         <v>659</v>
       </c>
-      <c r="G78" s="5">
+      <c r="G78" s="6">
         <v>191376</v>
       </c>
-      <c r="H78" s="5"/>
-      <c r="I78" s="5"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>43944.4375</v>
       </c>
-      <c r="B79" s="5">
+      <c r="B79" s="6">
         <v>174473</v>
       </c>
-      <c r="C79" s="5">
+      <c r="C79" s="6">
         <v>6757</v>
       </c>
-      <c r="D79" s="5">
+      <c r="D79" s="6">
         <v>12879</v>
       </c>
-      <c r="E79" s="5">
+      <c r="E79" s="6">
         <v>6680</v>
       </c>
-      <c r="F79" s="5">
+      <c r="F79" s="6">
         <v>713</v>
       </c>
-      <c r="G79" s="5">
+      <c r="G79" s="6">
         <v>201502</v>
       </c>
-      <c r="H79" s="5"/>
-      <c r="I79" s="5"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>43945.4375</v>
       </c>
-      <c r="B80" s="5">
+      <c r="B80" s="6">
         <v>185671</v>
       </c>
-      <c r="C80" s="5">
+      <c r="C80" s="6">
         <v>5414</v>
       </c>
-      <c r="D80" s="5">
+      <c r="D80" s="6">
         <v>13519</v>
       </c>
-      <c r="E80" s="5">
+      <c r="E80" s="6">
         <v>7087</v>
       </c>
-      <c r="F80" s="5">
+      <c r="F80" s="6">
         <v>763</v>
       </c>
-      <c r="G80" s="5">
+      <c r="G80" s="6">
         <v>212454</v>
       </c>
-      <c r="H80" s="5"/>
-      <c r="I80" s="5"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>43946.4375</v>
       </c>
-      <c r="B81" s="5">
+      <c r="B81" s="6">
         <v>195303</v>
       </c>
-      <c r="C81" s="5">
+      <c r="C81" s="6">
         <v>8171</v>
       </c>
-      <c r="D81" s="5">
+      <c r="D81" s="6">
         <v>13995</v>
       </c>
-      <c r="E81" s="5">
+      <c r="E81" s="6">
         <v>7509</v>
       </c>
-      <c r="F81" s="5">
+      <c r="F81" s="6">
         <v>811</v>
       </c>
-      <c r="G81" s="5">
+      <c r="G81" s="6">
         <v>225789</v>
       </c>
-      <c r="H81" s="5"/>
-      <c r="I81" s="5"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>43947.4375</v>
       </c>
-      <c r="B82" s="5">
+      <c r="B82" s="6">
         <v>206371</v>
       </c>
-      <c r="C82" s="5">
+      <c r="C82" s="6">
         <v>7417</v>
       </c>
-      <c r="D82" s="5">
+      <c r="D82" s="6">
         <v>14432</v>
       </c>
-      <c r="E82" s="5">
+      <c r="E82" s="6">
         <v>8000</v>
       </c>
-      <c r="F82" s="5">
+      <c r="F82" s="6">
         <v>835</v>
       </c>
-      <c r="G82" s="5">
+      <c r="G82" s="6">
         <v>237055</v>
       </c>
-      <c r="H82" s="5"/>
-      <c r="I82" s="5"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>43948.4375</v>
       </c>
-      <c r="B83" s="5">
+      <c r="B83" s="6">
         <v>217915</v>
       </c>
-      <c r="C83" s="5">
+      <c r="C83" s="6">
         <v>5001</v>
       </c>
-      <c r="D83" s="5">
+      <c r="D83" s="6">
         <v>14856</v>
       </c>
-      <c r="E83" s="5">
+      <c r="E83" s="6">
         <v>8525</v>
       </c>
-      <c r="F83" s="5">
+      <c r="F83" s="6">
         <v>892</v>
       </c>
-      <c r="G83" s="5">
+      <c r="G83" s="6">
         <v>247189</v>
       </c>
-      <c r="H83" s="5"/>
-      <c r="I83" s="5"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>43949.4375</v>
       </c>
-      <c r="B84" s="5">
+      <c r="B84" s="6">
         <v>227744</v>
       </c>
-      <c r="C84" s="5">
+      <c r="C84" s="6">
         <v>6282</v>
       </c>
-      <c r="D84" s="5">
+      <c r="D84" s="6">
         <v>15381</v>
       </c>
-      <c r="E84" s="5">
+      <c r="E84" s="6">
         <v>8964</v>
       </c>
-      <c r="F84" s="5">
+      <c r="F84" s="6">
         <v>951</v>
       </c>
-      <c r="G84" s="5">
+      <c r="G84" s="6">
         <v>259322</v>
       </c>
-      <c r="H84" s="5"/>
-      <c r="I84" s="5"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>43950.4375</v>
       </c>
-      <c r="B85" s="5">
+      <c r="B85" s="6">
         <v>238258</v>
       </c>
-      <c r="C85" s="5">
+      <c r="C85" s="6">
         <v>9530</v>
       </c>
-      <c r="D85" s="5">
+      <c r="D85" s="6">
         <v>15728</v>
       </c>
-      <c r="E85" s="5">
+      <c r="E85" s="6">
         <v>9612</v>
       </c>
-      <c r="F85" s="5">
+      <c r="F85" s="6">
         <v>996</v>
       </c>
-      <c r="G85" s="5">
+      <c r="G85" s="6">
         <v>274124</v>
       </c>
-      <c r="H85" s="5"/>
-      <c r="I85" s="5"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>43951.4375</v>
       </c>
-      <c r="B86" s="5">
+      <c r="B86" s="6">
         <v>250048</v>
       </c>
-      <c r="C86" s="5">
+      <c r="C86" s="6">
         <v>11859</v>
       </c>
-      <c r="D86" s="5">
+      <c r="D86" s="6">
         <v>16187</v>
       </c>
-      <c r="E86" s="5">
+      <c r="E86" s="6">
         <v>10205</v>
       </c>
-      <c r="F86" s="5">
+      <c r="F86" s="6">
         <v>1082</v>
       </c>
-      <c r="G86" s="5">
+      <c r="G86" s="6">
         <v>289381</v>
       </c>
-      <c r="H86" s="5"/>
-      <c r="I86" s="5"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>43952.4375</v>
       </c>
-      <c r="B87" s="5">
+      <c r="B87" s="6">
         <v>265500</v>
       </c>
-      <c r="C87" s="5">
+      <c r="C87" s="6">
         <v>11975</v>
       </c>
-      <c r="D87" s="5">
+      <c r="D87" s="6">
         <v>16608</v>
       </c>
-      <c r="E87" s="5">
+      <c r="E87" s="6">
         <v>10825</v>
       </c>
-      <c r="F87" s="5">
+      <c r="F87" s="6">
         <v>1121</v>
       </c>
-      <c r="G87" s="5">
+      <c r="G87" s="6">
         <v>306029</v>
       </c>
-      <c r="H87" s="5"/>
-      <c r="I87" s="5"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>43953.4375</v>
       </c>
-      <c r="B88" s="5">
+      <c r="B88" s="6">
         <v>280674</v>
       </c>
-      <c r="C88" s="5">
+      <c r="C88" s="6">
         <v>12829</v>
       </c>
-      <c r="D88" s="5">
+      <c r="D88" s="6">
         <v>17119</v>
       </c>
-      <c r="E88" s="5">
+      <c r="E88" s="6">
         <v>11390</v>
       </c>
-      <c r="F88" s="5">
+      <c r="F88" s="6">
         <v>1176</v>
       </c>
-      <c r="G88" s="5">
+      <c r="G88" s="6">
         <v>323188</v>
       </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>43954.4375</v>
+      </c>
+      <c r="B89" s="6">
+        <v>296731</v>
+      </c>
+      <c r="C89" s="6">
+        <v>9785</v>
+      </c>
+      <c r="D89" s="6">
+        <v>17553</v>
+      </c>
+      <c r="E89" s="6">
+        <v>12005</v>
+      </c>
+      <c r="F89" s="6">
+        <v>1216</v>
+      </c>
+      <c r="G89" s="6">
+        <v>337290</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="20" x14ac:dyDescent="0.2">
+      <c r="C91" s="9"/>
+      <c r="D91" s="10"/>
+      <c r="E91" s="8"/>
+    </row>
+    <row r="92" spans="1:9" ht="20" x14ac:dyDescent="0.2">
+      <c r="C92" s="8"/>
+      <c r="D92" s="8"/>
+      <c r="E92" s="8"/>
+    </row>
+    <row r="93" spans="1:9" ht="20" x14ac:dyDescent="0.2">
+      <c r="C93" s="9"/>
+      <c r="D93" s="10"/>
+      <c r="E93" s="8"/>
+    </row>
+    <row r="94" spans="1:9" ht="20" x14ac:dyDescent="0.2">
+      <c r="C94" s="9"/>
+      <c r="D94" s="10"/>
+      <c r="E94" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3329,11 +3400,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3342,7 +3413,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
@@ -3436,9 +3507,9 @@
       <c r="K3">
         <v>140</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -3474,9 +3545,9 @@
       <c r="K4">
         <v>152</v>
       </c>
-      <c r="L4" s="6"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -3512,9 +3583,9 @@
       <c r="K5">
         <v>154</v>
       </c>
-      <c r="L5" s="6"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -3550,9 +3621,9 @@
       <c r="K6">
         <v>160</v>
       </c>
-      <c r="L6" s="6"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -3588,9 +3659,9 @@
       <c r="K7">
         <v>187</v>
       </c>
-      <c r="L7" s="6"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -3626,9 +3697,9 @@
       <c r="K8">
         <v>195</v>
       </c>
-      <c r="L8" s="6"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -3664,9 +3735,9 @@
       <c r="K9">
         <v>214</v>
       </c>
-      <c r="L9" s="6"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -3702,9 +3773,9 @@
       <c r="K10">
         <v>217</v>
       </c>
-      <c r="L10" s="6"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -3740,9 +3811,9 @@
       <c r="K11">
         <v>215</v>
       </c>
-      <c r="L11" s="6"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -3778,9 +3849,9 @@
       <c r="K12">
         <v>196</v>
       </c>
-      <c r="L12" s="6"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -3816,9 +3887,9 @@
       <c r="K13">
         <v>203</v>
       </c>
-      <c r="L13" s="6"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -3854,9 +3925,9 @@
       <c r="K14">
         <v>199</v>
       </c>
-      <c r="L14" s="6"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -3892,9 +3963,9 @@
       <c r="K15">
         <v>188</v>
       </c>
-      <c r="L15" s="6"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -3930,262 +4001,262 @@
       <c r="K16">
         <v>200</v>
       </c>
-      <c r="L16" s="6"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43938.4375</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="6">
         <v>4074</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="6">
         <v>5380</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="6">
         <v>210</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="6">
         <v>2164</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="6">
         <v>3067</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="6">
         <v>2214</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="6">
         <v>1864</v>
       </c>
-      <c r="I17" s="5">
+      <c r="I17" s="6">
         <v>829</v>
       </c>
-      <c r="J17" s="5">
+      <c r="J17" s="6">
         <v>245</v>
       </c>
-      <c r="K17" s="5">
+      <c r="K17" s="6">
         <v>200</v>
       </c>
-      <c r="L17" s="6"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43939.4375</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="6">
         <v>4277</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="6">
         <v>5658</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="6">
         <v>223</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="6">
         <v>2269</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="6">
         <v>3201</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="6">
         <v>2313</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H18" s="6">
         <v>1996</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I18" s="6">
         <v>828</v>
       </c>
-      <c r="J18" s="5">
+      <c r="J18" s="6">
         <v>250</v>
       </c>
-      <c r="K18" s="5">
+      <c r="K18" s="6">
         <v>197</v>
       </c>
-      <c r="L18" s="6"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43940.4375</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="6">
         <v>4495</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="6">
         <v>5996</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="6">
         <v>235</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="6">
         <v>2408</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="6">
         <v>3354</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="6">
         <v>2437</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19" s="6">
         <v>2135</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I19" s="6">
         <v>809</v>
       </c>
-      <c r="J19" s="5">
+      <c r="J19" s="6">
         <v>247</v>
       </c>
-      <c r="K19" s="5">
+      <c r="K19" s="6">
         <v>196</v>
       </c>
-      <c r="L19" s="6"/>
+      <c r="L19" s="7"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43941.4375</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="6">
         <v>4728</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="6">
         <v>6354</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="6">
         <v>248</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="6">
         <v>2525</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="6">
         <v>3502</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="6">
         <v>2580</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="6">
         <v>2312</v>
       </c>
-      <c r="I20" s="5">
+      <c r="I20" s="6">
         <v>802</v>
       </c>
-      <c r="J20" s="5">
+      <c r="J20" s="6">
         <v>247</v>
       </c>
-      <c r="K20" s="5">
+      <c r="K20" s="6">
         <v>193</v>
       </c>
-      <c r="L20" s="6"/>
+      <c r="L20" s="7"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43942.4375</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="6">
         <v>4955</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="6">
         <v>6663</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="6">
         <v>260</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="6">
         <v>2657</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="6">
         <v>3665</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="6">
         <v>2687</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="6">
         <v>2457</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I21" s="6">
         <v>859</v>
       </c>
-      <c r="J21" s="5">
+      <c r="J21" s="6">
         <v>250</v>
       </c>
-      <c r="K21" s="5">
+      <c r="K21" s="6">
         <v>194</v>
       </c>
-      <c r="L21" s="6"/>
+      <c r="L21" s="7"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43943.4375</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="6">
         <v>5169</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="6">
         <v>6952</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="6">
         <v>270</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="6">
         <v>2781</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="6">
         <v>3798</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="6">
         <v>2778</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="6">
         <v>2609</v>
       </c>
-      <c r="I22" s="5">
+      <c r="I22" s="6">
         <v>878</v>
       </c>
-      <c r="J22" s="5">
+      <c r="J22" s="6">
         <v>243</v>
       </c>
-      <c r="K22" s="5">
+      <c r="K22" s="6">
         <v>192</v>
       </c>
-      <c r="L22" s="6"/>
+      <c r="L22" s="7"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43944.4375</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="6">
         <v>5408</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="6">
         <v>7342</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="6">
         <v>284</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="6">
         <v>2914</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="6">
         <v>3945</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="6">
         <v>2909</v>
       </c>
-      <c r="H23" s="5">
+      <c r="H23" s="6">
         <v>2816</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I23" s="6">
         <v>887</v>
       </c>
-      <c r="J23" s="5">
+      <c r="J23" s="6">
         <v>233</v>
       </c>
-      <c r="K23" s="5">
+      <c r="K23" s="6">
         <v>185</v>
       </c>
     </row>
@@ -4193,34 +4264,34 @@
       <c r="A24" s="1">
         <v>43945.4375</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="6">
         <v>5640</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="6">
         <v>7737</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="6">
         <v>292</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="6">
         <v>3052</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="6">
         <v>4108</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="6">
         <v>3029</v>
       </c>
-      <c r="H24" s="5">
+      <c r="H24" s="6">
         <v>3029</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I24" s="6">
         <v>910</v>
       </c>
-      <c r="J24" s="5">
+      <c r="J24" s="6">
         <v>243</v>
       </c>
-      <c r="K24" s="5">
+      <c r="K24" s="6">
         <v>193</v>
       </c>
     </row>
@@ -4228,34 +4299,34 @@
       <c r="A25" s="1">
         <v>43946.4375</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="6">
         <v>5827</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="6">
         <v>8030</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="6">
         <v>309</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="6">
         <v>3179</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="6">
         <v>4276</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="6">
         <v>3108</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H25" s="6">
         <v>3114</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I25" s="6">
         <v>925</v>
       </c>
-      <c r="J25" s="5">
+      <c r="J25" s="6">
         <v>245</v>
       </c>
-      <c r="K25" s="5">
+      <c r="K25" s="6">
         <v>195</v>
       </c>
     </row>
@@ -4263,34 +4334,34 @@
       <c r="A26" s="1">
         <v>43947.4375</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="6">
         <v>6005</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="6">
         <v>8290</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="6">
         <v>320</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="6">
         <v>3292</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="6">
         <v>4391</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="6">
         <v>3207</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H26" s="6">
         <v>3213</v>
       </c>
-      <c r="I26" s="5">
+      <c r="I26" s="6">
         <v>938</v>
       </c>
-      <c r="J26" s="5">
+      <c r="J26" s="6">
         <v>252</v>
       </c>
-      <c r="K26" s="5">
+      <c r="K26" s="6">
         <v>195</v>
       </c>
     </row>
@@ -4298,34 +4369,34 @@
       <c r="A27" s="1">
         <v>43948.4375</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="6">
         <v>6168</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="6">
         <v>8548</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="6">
         <v>326</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="6">
         <v>3398</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F27" s="6">
         <v>4504</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="6">
         <v>3302</v>
       </c>
-      <c r="H27" s="5">
+      <c r="H27" s="6">
         <v>3318</v>
       </c>
-      <c r="I27" s="5">
+      <c r="I27" s="6">
         <v>945</v>
       </c>
-      <c r="J27" s="5">
+      <c r="J27" s="6">
         <v>241</v>
       </c>
-      <c r="K27" s="5">
+      <c r="K27" s="6">
         <v>191</v>
       </c>
     </row>
@@ -4333,34 +4404,34 @@
       <c r="A28" s="1">
         <v>43949.4375</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="6">
         <v>6392</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="6">
         <v>8848</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="6">
         <v>346</v>
       </c>
-      <c r="E28" s="5">
+      <c r="E28" s="6">
         <v>3521</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F28" s="6">
         <v>4644</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="6">
         <v>3420</v>
       </c>
-      <c r="H28" s="5">
+      <c r="H28" s="6">
         <v>3443</v>
       </c>
-      <c r="I28" s="5">
+      <c r="I28" s="6">
         <v>957</v>
       </c>
-      <c r="J28" s="5">
+      <c r="J28" s="6">
         <v>239</v>
       </c>
-      <c r="K28" s="5">
+      <c r="K28" s="6">
         <v>187</v>
       </c>
     </row>
@@ -4368,34 +4439,34 @@
       <c r="A29" s="1">
         <v>43950.4375</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="6">
         <v>6546</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="6">
         <v>9041</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="6">
         <v>363</v>
       </c>
-      <c r="E29" s="5">
+      <c r="E29" s="6">
         <v>3583</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29" s="6">
         <v>4725</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="6">
         <v>3486</v>
       </c>
-      <c r="H29" s="5">
+      <c r="H29" s="6">
         <v>3564</v>
       </c>
-      <c r="I29" s="5">
+      <c r="I29" s="6">
         <v>977</v>
       </c>
-      <c r="J29" s="5">
+      <c r="J29" s="6">
         <v>235</v>
       </c>
-      <c r="K29" s="5">
+      <c r="K29" s="6">
         <v>186</v>
       </c>
     </row>
@@ -4403,34 +4474,34 @@
       <c r="A30" s="1">
         <v>43951.4375</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="6">
         <v>6754</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="6">
         <v>9280</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="6">
         <v>371</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="6">
         <v>3693</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F30" s="6">
         <v>4871</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G30" s="6">
         <v>3581</v>
       </c>
-      <c r="H30" s="5">
+      <c r="H30" s="6">
         <v>3664</v>
       </c>
-      <c r="I30" s="5">
+      <c r="I30" s="6">
         <v>999</v>
       </c>
-      <c r="J30" s="5">
+      <c r="J30" s="6">
         <v>233</v>
       </c>
-      <c r="K30" s="5">
+      <c r="K30" s="6">
         <v>181</v>
       </c>
     </row>
@@ -4438,34 +4509,34 @@
       <c r="A31" s="1">
         <v>43952.4375</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="6">
         <v>6917</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="6">
         <v>9538</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="6">
         <v>384</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="6">
         <v>3786</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F31" s="6">
         <v>5004</v>
       </c>
-      <c r="G31" s="5">
+      <c r="G31" s="6">
         <v>3673</v>
       </c>
-      <c r="H31" s="5">
+      <c r="H31" s="6">
         <v>3753</v>
       </c>
-      <c r="I31" s="5">
+      <c r="I31" s="6">
         <v>1017</v>
       </c>
-      <c r="J31" s="5">
+      <c r="J31" s="6">
         <v>225</v>
       </c>
-      <c r="K31" s="5">
+      <c r="K31" s="6">
         <v>175</v>
       </c>
     </row>
@@ -4473,36 +4544,152 @@
       <c r="A32" s="1">
         <v>43953.4375</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="6">
         <v>7113</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="6">
         <v>9845</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="6">
         <v>405</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="6">
         <v>3918</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F32" s="6">
         <v>5169</v>
       </c>
-      <c r="G32" s="5">
+      <c r="G32" s="6">
         <v>3776</v>
       </c>
-      <c r="H32" s="5">
+      <c r="H32" s="6">
         <v>3842</v>
       </c>
-      <c r="I32" s="5">
+      <c r="I32" s="6">
         <v>977</v>
       </c>
-      <c r="J32" s="5">
+      <c r="J32" s="6">
         <v>221</v>
       </c>
-      <c r="K32" s="5">
+      <c r="K32" s="6">
         <v>154</v>
       </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>43954.4375</v>
+      </c>
+      <c r="B33" s="6">
+        <v>7284</v>
+      </c>
+      <c r="C33" s="6">
+        <v>10112</v>
+      </c>
+      <c r="D33" s="6">
+        <v>416</v>
+      </c>
+      <c r="E33" s="6">
+        <v>4041</v>
+      </c>
+      <c r="F33" s="6">
+        <v>5290</v>
+      </c>
+      <c r="G33" s="6">
+        <v>3865</v>
+      </c>
+      <c r="H33" s="6">
+        <v>3932</v>
+      </c>
+      <c r="I33" s="6">
+        <v>1010</v>
+      </c>
+      <c r="J33" s="6">
+        <v>232</v>
+      </c>
+      <c r="K33" s="6">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B35" s="11"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B36" s="8"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B37" s="8"/>
+      <c r="C37" s="10"/>
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B39" s="8"/>
+      <c r="C39" s="10"/>
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B40" s="8"/>
+      <c r="C40" s="10"/>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B41" s="8"/>
+      <c r="C41" s="10"/>
+      <c r="D41" s="8"/>
+    </row>
+    <row r="42" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B42" s="8"/>
+      <c r="C42" s="10"/>
+      <c r="D42" s="8"/>
+    </row>
+    <row r="43" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B43" s="11"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
+    </row>
+    <row r="44" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B44" s="9"/>
+      <c r="C44" s="10"/>
+      <c r="D44" s="8"/>
+    </row>
+    <row r="45" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B45" s="9"/>
+      <c r="C45" s="10"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B46" s="9"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="8"/>
+    </row>
+    <row r="47" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B47" s="11"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B48" s="9"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="8"/>
+    </row>
+    <row r="49" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="B49" s="9"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+    </row>
+    <row r="50" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+      <c r="B50" s="9"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-04 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80886EBD-DDE0-B843-8089-AEB544F0C668}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F34EDB-7AFA-7241-B5F1-D092779FE430}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -468,7 +468,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -479,7 +479,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -1180,11 +1179,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:J94"/>
+  <dimension ref="A1:I90"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C95" sqref="C95:F110"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2348,7 +2347,7 @@
       </c>
       <c r="H48" s="6"/>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>43916.729166666664</v>
       </c>
@@ -2372,7 +2371,7 @@
       </c>
       <c r="H49" s="6"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>43917.4375</v>
       </c>
@@ -2396,7 +2395,7 @@
       </c>
       <c r="H50" s="6"/>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>43918.4375</v>
       </c>
@@ -2420,7 +2419,7 @@
       </c>
       <c r="H51" s="6"/>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>43918.729166666664</v>
       </c>
@@ -2444,7 +2443,7 @@
       </c>
       <c r="H52" s="6"/>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>43919.4375</v>
       </c>
@@ -2468,7 +2467,7 @@
       </c>
       <c r="H53" s="6"/>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>43919.729166666664</v>
       </c>
@@ -2492,7 +2491,7 @@
       </c>
       <c r="H54" s="6"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>43920.4375</v>
       </c>
@@ -2516,7 +2515,7 @@
       </c>
       <c r="H55" s="6"/>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>43921.4375</v>
       </c>
@@ -2539,20 +2538,9 @@
         <f>51629+C53</f>
         <v>58832</v>
       </c>
-      <c r="H56" s="6">
-        <f>D56-D55</f>
-        <v>260</v>
-      </c>
-      <c r="I56">
-        <f>SUM(B56,D56:F56)</f>
-        <v>51095</v>
-      </c>
-      <c r="J56">
-        <f>H56/I56</f>
-        <v>5.0885605245131619E-3</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H56" s="6"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>43922.4375</v>
       </c>
@@ -2577,7 +2565,7 @@
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>43923.4375</v>
       </c>
@@ -2602,7 +2590,7 @@
       <c r="H58" s="6"/>
       <c r="I58" s="6"/>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>43924.4375</v>
       </c>
@@ -2627,7 +2615,7 @@
       <c r="H59" s="6"/>
       <c r="I59" s="6"/>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>43925.4375</v>
       </c>
@@ -2652,7 +2640,7 @@
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>43926.4375</v>
       </c>
@@ -2677,7 +2665,7 @@
       <c r="H61" s="6"/>
       <c r="I61" s="6"/>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>43927.4375</v>
       </c>
@@ -2702,7 +2690,7 @@
       <c r="H62" s="6"/>
       <c r="I62" s="6"/>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>43928.4375</v>
       </c>
@@ -2727,7 +2715,7 @@
       <c r="H63" s="6"/>
       <c r="I63" s="6"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>43929.4375</v>
       </c>
@@ -3373,25 +3361,28 @@
         <v>337290</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="20" x14ac:dyDescent="0.2">
-      <c r="C91" s="9"/>
-      <c r="D91" s="10"/>
-      <c r="E91" s="8"/>
-    </row>
-    <row r="92" spans="1:9" ht="20" x14ac:dyDescent="0.2">
-      <c r="C92" s="8"/>
-      <c r="D92" s="8"/>
-      <c r="E92" s="8"/>
-    </row>
-    <row r="93" spans="1:9" ht="20" x14ac:dyDescent="0.2">
-      <c r="C93" s="9"/>
-      <c r="D93" s="10"/>
-      <c r="E93" s="8"/>
-    </row>
-    <row r="94" spans="1:9" ht="20" x14ac:dyDescent="0.2">
-      <c r="C94" s="9"/>
-      <c r="D94" s="10"/>
-      <c r="E94" s="8"/>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>43955.4375</v>
+      </c>
+      <c r="B90" s="6">
+        <v>310332</v>
+      </c>
+      <c r="C90" s="6">
+        <v>6265</v>
+      </c>
+      <c r="D90" s="6">
+        <v>17923</v>
+      </c>
+      <c r="E90" s="6">
+        <v>12505</v>
+      </c>
+      <c r="F90" s="6">
+        <v>1300</v>
+      </c>
+      <c r="G90" s="6">
+        <v>348325</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3402,9 +3393,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4610,86 +4601,97 @@
         <v>174</v>
       </c>
     </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>43955.4375</v>
+      </c>
+      <c r="B34" s="6">
+        <v>7453</v>
+      </c>
+      <c r="C34" s="6">
+        <v>10312</v>
+      </c>
+      <c r="D34" s="6">
+        <v>431</v>
+      </c>
+      <c r="E34" s="6">
+        <v>4156</v>
+      </c>
+      <c r="F34" s="6">
+        <v>5403</v>
+      </c>
+      <c r="G34" s="6">
+        <v>3939</v>
+      </c>
+      <c r="H34" s="6">
+        <v>3984</v>
+      </c>
+      <c r="I34" s="6">
+        <v>984</v>
+      </c>
+      <c r="J34" s="6">
+        <v>225</v>
+      </c>
+      <c r="K34" s="6">
+        <v>175</v>
+      </c>
+    </row>
     <row r="35" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B35" s="11"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
+      <c r="B35" s="10"/>
+      <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B36" s="8"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="8"/>
+      <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B37" s="8"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
+      <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B39" s="8"/>
-      <c r="C39" s="10"/>
-      <c r="D39" s="8"/>
+      <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B40" s="8"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="8"/>
+      <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B41" s="8"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="8"/>
+      <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B42" s="8"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="8"/>
     </row>
     <row r="43" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B43" s="11"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-    </row>
-    <row r="44" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B43" s="10"/>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B44" s="9"/>
-      <c r="C44" s="10"/>
-      <c r="D44" s="8"/>
-    </row>
-    <row r="45" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="D44" s="3"/>
+      <c r="F44" s="3"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B45" s="9"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="3"/>
-    </row>
-    <row r="46" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B46" s="9"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="8"/>
     </row>
     <row r="47" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B47" s="11"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-    </row>
-    <row r="48" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B47" s="10"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B48" s="9"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="8"/>
-    </row>
-    <row r="49" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B49" s="9"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-    </row>
-    <row r="50" spans="2:4" ht="20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B50" s="9"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-05 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F34EDB-7AFA-7241-B5F1-D092779FE430}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A372787F-D2F5-D644-9334-7F8C55866A69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -402,7 +402,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -430,21 +430,6 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF222222"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -463,12 +448,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -478,11 +462,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1179,11 +1160,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I90"/>
+  <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A91" sqref="A91"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C96" sqref="C96:F112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3337,6 +3318,7 @@
       <c r="G88" s="6">
         <v>323188</v>
       </c>
+      <c r="H88" s="6"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
@@ -3360,6 +3342,7 @@
       <c r="G89" s="6">
         <v>337290</v>
       </c>
+      <c r="H89" s="6"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
@@ -3383,6 +3366,39 @@
       <c r="G90" s="6">
         <v>348325</v>
       </c>
+      <c r="H90" s="6"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>43956.4375</v>
+      </c>
+      <c r="B91" s="6">
+        <v>320264</v>
+      </c>
+      <c r="C91" s="6">
+        <v>6023</v>
+      </c>
+      <c r="D91" s="6">
+        <v>18310</v>
+      </c>
+      <c r="E91" s="6">
+        <v>12779</v>
+      </c>
+      <c r="F91" s="6">
+        <v>1361</v>
+      </c>
+      <c r="G91" s="6">
+        <v>358737</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D92" s="3"/>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D94" s="3"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D95" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3393,9 +3409,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4636,62 +4652,76 @@
         <v>175</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B35" s="10"/>
-      <c r="D35" s="3"/>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>43956.4375</v>
+      </c>
+      <c r="B35" s="6">
+        <v>7629</v>
+      </c>
+      <c r="C35" s="6">
+        <v>10521</v>
+      </c>
+      <c r="D35" s="6">
+        <v>451</v>
+      </c>
+      <c r="E35" s="6">
+        <v>4257</v>
+      </c>
+      <c r="F35" s="6">
+        <v>5528</v>
+      </c>
+      <c r="G35" s="6">
+        <v>4012</v>
+      </c>
+      <c r="H35" s="6">
+        <v>4051</v>
+      </c>
+      <c r="I35" s="6">
+        <v>1043</v>
+      </c>
+      <c r="J35" s="6">
+        <v>223</v>
+      </c>
+      <c r="K35" s="6">
+        <v>166</v>
+      </c>
     </row>
     <row r="36" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B36" s="8"/>
       <c r="D36" s="3"/>
     </row>
-    <row r="37" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B37" s="8"/>
-    </row>
-    <row r="38" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B38" s="8"/>
-      <c r="D38" s="3"/>
-    </row>
-    <row r="39" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B39" s="8"/>
-      <c r="D39" s="3"/>
-    </row>
-    <row r="40" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B40" s="8"/>
-      <c r="D40" s="3"/>
-    </row>
-    <row r="41" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B41" s="8"/>
-      <c r="D41" s="3"/>
-    </row>
-    <row r="42" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B42" s="8"/>
-    </row>
-    <row r="43" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B43" s="10"/>
-      <c r="D43" s="3"/>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C39" s="3"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C43" s="3"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B44" s="9"/>
-      <c r="D44" s="3"/>
+      <c r="C44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B45" s="9"/>
-    </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B46" s="9"/>
-    </row>
-    <row r="47" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B47" s="10"/>
+      <c r="C46" s="3"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C47" s="3"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B48" s="9"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B49" s="9"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B50" s="9"/>
+      <c r="C48" s="3"/>
+      <c r="E48" s="3"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C50" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-06 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A372787F-D2F5-D644-9334-7F8C55866A69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F78533F-74A1-5146-9F47-7AAC9CDFFF32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -402,7 +402,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -423,12 +423,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF222222"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -452,7 +446,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -461,7 +455,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1160,11 +1153,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I96"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C96" sqref="C96:F112"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C104" sqref="C104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3392,13 +3385,40 @@
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D92" s="3"/>
+      <c r="A92" s="1">
+        <v>43957.4375</v>
+      </c>
+      <c r="B92" s="6">
+        <v>332302</v>
+      </c>
+      <c r="C92" s="6">
+        <v>8790</v>
+      </c>
+      <c r="D92" s="6">
+        <v>18722</v>
+      </c>
+      <c r="E92" s="6">
+        <v>13222</v>
+      </c>
+      <c r="F92" s="6">
+        <v>1429</v>
+      </c>
+      <c r="G92" s="6">
+        <v>374465</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C93" s="6"/>
+      <c r="D93" s="3"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D94" s="3"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D95" s="3"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D96" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3407,11 +3427,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A36" sqref="A36"/>
+      <selection pane="bottomLeft" activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4687,41 +4707,68 @@
         <v>166</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B36" s="8"/>
-      <c r="D36" s="3"/>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>43957.4375</v>
+      </c>
+      <c r="B36" s="6">
+        <v>7824</v>
+      </c>
+      <c r="C36" s="6">
+        <v>10732</v>
+      </c>
+      <c r="D36" s="6">
+        <v>473</v>
+      </c>
+      <c r="E36" s="6">
+        <v>4379</v>
+      </c>
+      <c r="F36" s="6">
+        <v>5652</v>
+      </c>
+      <c r="G36" s="6">
+        <v>4089</v>
+      </c>
+      <c r="H36" s="6">
+        <v>4116</v>
+      </c>
+      <c r="I36" s="6">
+        <v>1032</v>
+      </c>
+      <c r="J36" s="6">
+        <v>219</v>
+      </c>
+      <c r="K36" s="6">
+        <v>174</v>
+      </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C44" s="3"/>
-      <c r="F44" s="3"/>
+      <c r="D44" s="3"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="F47" s="3"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C48" s="3"/>
-      <c r="E48" s="3"/>
-    </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C50" s="3"/>
+      <c r="D48" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-07 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F78533F-74A1-5146-9F47-7AAC9CDFFF32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3495E247-F12E-B54C-B719-C76881EEC6E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -1153,11 +1153,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I96"/>
+  <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C104" sqref="C104"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C100" sqref="C100:F114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3408,8 +3408,27 @@
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C93" s="6"/>
-      <c r="D93" s="3"/>
+      <c r="A93" s="1">
+        <v>43958.4375</v>
+      </c>
+      <c r="B93" s="6">
+        <v>346687</v>
+      </c>
+      <c r="C93" s="6">
+        <v>13012</v>
+      </c>
+      <c r="D93" s="6">
+        <v>19121</v>
+      </c>
+      <c r="E93" s="6">
+        <v>13569</v>
+      </c>
+      <c r="F93" s="6">
+        <v>1477</v>
+      </c>
+      <c r="G93" s="6">
+        <v>393866</v>
+      </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D94" s="3"/>
@@ -3419,6 +3438,12 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D96" s="3"/>
+    </row>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D97" s="3"/>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D98" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3427,11 +3452,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J40" sqref="J40"/>
+      <selection pane="bottomLeft" activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4742,14 +4767,49 @@
         <v>174</v>
       </c>
     </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>43958.4375</v>
+      </c>
+      <c r="B37" s="6">
+        <v>8004</v>
+      </c>
+      <c r="C37" s="6">
+        <v>10954</v>
+      </c>
+      <c r="D37" s="6">
+        <v>485</v>
+      </c>
+      <c r="E37" s="6">
+        <v>4478</v>
+      </c>
+      <c r="F37" s="6">
+        <v>5788</v>
+      </c>
+      <c r="G37" s="6">
+        <v>4176</v>
+      </c>
+      <c r="H37" s="6">
+        <v>4182</v>
+      </c>
+      <c r="I37" s="6">
+        <v>1033</v>
+      </c>
+      <c r="J37" s="6">
+        <v>220</v>
+      </c>
+      <c r="K37" s="6">
+        <v>155</v>
+      </c>
+    </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D39" s="3"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D41" s="3"/>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D40" s="3"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D42" s="3"/>
@@ -4760,8 +4820,8 @@
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D44" s="3"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D46" s="3"/>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D45" s="3"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D47" s="3"/>
@@ -4769,6 +4829,9 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D49" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-08 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3495E247-F12E-B54C-B719-C76881EEC6E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA308A0-C60B-C242-8CAD-4F00F8B14726}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -1153,11 +1153,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C100" sqref="C100:F114"/>
+      <selection pane="bottomLeft" activeCell="C98" sqref="C98:F115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3431,7 +3431,27 @@
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D94" s="3"/>
+      <c r="A94" s="1">
+        <v>43959.4375</v>
+      </c>
+      <c r="B94" s="6">
+        <v>362021</v>
+      </c>
+      <c r="C94" s="6">
+        <v>14641</v>
+      </c>
+      <c r="D94" s="6">
+        <v>19598</v>
+      </c>
+      <c r="E94" s="6">
+        <v>13990</v>
+      </c>
+      <c r="F94" s="6">
+        <v>1540</v>
+      </c>
+      <c r="G94" s="6">
+        <v>411790</v>
+      </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D95" s="3"/>
@@ -3441,9 +3461,6 @@
     </row>
     <row r="97" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D97" s="3"/>
-    </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D98" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3452,11 +3469,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J41" sqref="J41"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4803,7 +4820,39 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D38" s="3"/>
+      <c r="A38" s="1">
+        <v>43959.4375</v>
+      </c>
+      <c r="B38" s="6">
+        <v>8213</v>
+      </c>
+      <c r="C38" s="6">
+        <v>11222</v>
+      </c>
+      <c r="D38" s="6">
+        <v>504</v>
+      </c>
+      <c r="E38" s="6">
+        <v>4602</v>
+      </c>
+      <c r="F38" s="6">
+        <v>5972</v>
+      </c>
+      <c r="G38" s="6">
+        <v>4254</v>
+      </c>
+      <c r="H38" s="6">
+        <v>4254</v>
+      </c>
+      <c r="I38" s="6">
+        <v>1028</v>
+      </c>
+      <c r="J38" s="6">
+        <v>213</v>
+      </c>
+      <c r="K38" s="6">
+        <v>166</v>
+      </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D39" s="3"/>
@@ -4817,21 +4866,27 @@
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D44" s="3"/>
-    </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D45" s="3"/>
     </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D46" s="3"/>
+    </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D47" s="3"/>
-      <c r="F47" s="3"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D49" s="3"/>
+    <row r="50" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D50" s="3"/>
+      <c r="F50" s="3"/>
+    </row>
+    <row r="51" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D52" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-09 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA308A0-C60B-C242-8CAD-4F00F8B14726}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5150409A-4A49-F24F-B2E2-B9D4AA242385}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -1153,11 +1153,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I97"/>
+  <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C98" sqref="C98:F115"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3454,13 +3454,36 @@
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D95" s="3"/>
+      <c r="A95" s="1">
+        <v>43960.4375</v>
+      </c>
+      <c r="B95" s="6">
+        <v>380450</v>
+      </c>
+      <c r="C95" s="6">
+        <v>15307</v>
+      </c>
+      <c r="D95" s="6">
+        <v>19944</v>
+      </c>
+      <c r="E95" s="6">
+        <v>14383</v>
+      </c>
+      <c r="F95" s="6">
+        <v>1599</v>
+      </c>
+      <c r="G95" s="6">
+        <v>431683</v>
+      </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="D96" s="3"/>
     </row>
     <row r="97" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D97" s="3"/>
+    </row>
+    <row r="98" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D98" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3469,11 +3492,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J42" sqref="J42"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4855,38 +4878,74 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D39" s="3"/>
+      <c r="A39" s="1">
+        <v>43960.4375</v>
+      </c>
+      <c r="B39" s="6">
+        <v>8382</v>
+      </c>
+      <c r="C39" s="6">
+        <v>11407</v>
+      </c>
+      <c r="D39" s="6">
+        <v>516</v>
+      </c>
+      <c r="E39" s="6">
+        <v>4692</v>
+      </c>
+      <c r="F39" s="6">
+        <v>6079</v>
+      </c>
+      <c r="G39" s="6">
+        <v>4310</v>
+      </c>
+      <c r="H39" s="6">
+        <v>4333</v>
+      </c>
+      <c r="I39" s="6">
+        <v>1016</v>
+      </c>
+      <c r="J39" s="6">
+        <v>203</v>
+      </c>
+      <c r="K39" s="6">
+        <v>158</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D40" s="3"/>
+      <c r="C40" s="3"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D42" s="3"/>
+      <c r="C42" s="3"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D43" s="3"/>
+      <c r="C43" s="3"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D45" s="3"/>
+      <c r="C45" s="3"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D46" s="3"/>
+      <c r="C46" s="3"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D47" s="3"/>
+      <c r="C47" s="3"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D48" s="3"/>
-    </row>
-    <row r="50" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D50" s="3"/>
+      <c r="C48" s="3"/>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C50" s="3"/>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D51" s="3"/>
-    </row>
-    <row r="52" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D52" s="3"/>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C51" s="3"/>
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C52" s="3"/>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C54" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-10 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5150409A-4A49-F24F-B2E2-B9D4AA242385}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D37BB96-451E-D14E-BF05-3F3E62D795BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -1153,11 +1153,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B97" sqref="B97"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C100" sqref="C100:F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3477,13 +3477,36 @@
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D96" s="3"/>
+      <c r="A96" s="1">
+        <v>43961.4375</v>
+      </c>
+      <c r="B96" s="6">
+        <v>397350</v>
+      </c>
+      <c r="C96" s="6">
+        <v>14816</v>
+      </c>
+      <c r="D96" s="6">
+        <v>20238</v>
+      </c>
+      <c r="E96" s="6">
+        <v>14772</v>
+      </c>
+      <c r="F96" s="6">
+        <v>1634</v>
+      </c>
+      <c r="G96" s="6">
+        <v>448810</v>
+      </c>
     </row>
     <row r="97" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D97" s="3"/>
     </row>
     <row r="98" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D98" s="3"/>
+    </row>
+    <row r="99" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D99" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3494,9 +3517,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J43" sqref="J43"/>
+      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4913,39 +4936,70 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C40" s="3"/>
+      <c r="A40" s="1">
+        <v>43961.4375</v>
+      </c>
+      <c r="B40" s="6">
+        <v>8494</v>
+      </c>
+      <c r="C40" s="6">
+        <v>11582</v>
+      </c>
+      <c r="D40" s="6">
+        <v>524</v>
+      </c>
+      <c r="E40" s="6">
+        <v>4762</v>
+      </c>
+      <c r="F40" s="6">
+        <v>6187</v>
+      </c>
+      <c r="G40" s="6">
+        <v>4364</v>
+      </c>
+      <c r="H40" s="6">
+        <v>4390</v>
+      </c>
+      <c r="I40" s="6">
+        <v>961</v>
+      </c>
+      <c r="J40" s="6">
+        <v>195</v>
+      </c>
+      <c r="K40" s="6">
+        <v>140</v>
+      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C42" s="3"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C43" s="3"/>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C45" s="3"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C46" s="3"/>
+      <c r="D45" s="3"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C48" s="3"/>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C50" s="3"/>
-      <c r="F50" s="3"/>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C51" s="3"/>
-      <c r="E51" s="3"/>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C52" s="3"/>
-    </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C54" s="3"/>
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D50" s="3"/>
+    </row>
+    <row r="52" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D52" s="3"/>
+      <c r="F52" s="3"/>
+    </row>
+    <row r="53" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D54" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-11 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D37BB96-451E-D14E-BF05-3F3E62D795BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7771D8A-1906-CA4C-8F0F-AD8324F9CFAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -1153,11 +1153,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I99"/>
+  <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C100" sqref="C100:F117"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F105" sqref="F105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3499,14 +3499,31 @@
         <v>448810</v>
       </c>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D97" s="3"/>
-    </row>
-    <row r="98" spans="4:4" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>43962.4375</v>
+      </c>
+      <c r="B97" s="6">
+        <v>410618</v>
+      </c>
+      <c r="C97" s="6">
+        <v>9018</v>
+      </c>
+      <c r="D97" s="6">
+        <v>20546</v>
+      </c>
+      <c r="E97" s="6">
+        <v>15131</v>
+      </c>
+      <c r="F97" s="6">
+        <v>1669</v>
+      </c>
+      <c r="G97" s="6">
+        <v>456982</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D98" s="3"/>
-    </row>
-    <row r="99" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D99" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3515,11 +3532,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N54"/>
+  <dimension ref="A1:N56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4970,36 +4987,78 @@
         <v>140</v>
       </c>
     </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>43962.4375</v>
+      </c>
+      <c r="B41" s="6">
+        <v>8615</v>
+      </c>
+      <c r="C41" s="6">
+        <v>11768</v>
+      </c>
+      <c r="D41" s="6">
+        <v>538</v>
+      </c>
+      <c r="E41" s="6">
+        <v>4857</v>
+      </c>
+      <c r="F41" s="6">
+        <v>6287</v>
+      </c>
+      <c r="G41" s="6">
+        <v>4411</v>
+      </c>
+      <c r="H41" s="6">
+        <v>4439</v>
+      </c>
+      <c r="I41" s="6">
+        <v>1027</v>
+      </c>
+      <c r="J41" s="6">
+        <v>194</v>
+      </c>
+      <c r="K41" s="6">
+        <v>147</v>
+      </c>
+    </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D42" s="3"/>
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C43" s="3"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D44" s="3"/>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D45" s="3"/>
+      <c r="C44" s="3"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C46" s="3"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D47" s="3"/>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D48" s="3"/>
-    </row>
-    <row r="49" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D49" s="3"/>
-    </row>
-    <row r="50" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D50" s="3"/>
-    </row>
-    <row r="52" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D52" s="3"/>
+      <c r="C47" s="3"/>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C50" s="3"/>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C52" s="3"/>
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D53" s="3"/>
-    </row>
-    <row r="54" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D54" s="3"/>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C54" s="3"/>
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C56" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-12 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7771D8A-1906-CA4C-8F0F-AD8324F9CFAD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35B4FBE-1D32-E642-8FB0-FFD8BC187D46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -446,7 +446,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -454,7 +454,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1155,9 +1154,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
   <dimension ref="A1:I98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F105" sqref="F105"/>
+      <selection pane="bottomLeft" activeCell="C100" sqref="C100:F120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3523,7 +3522,27 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D98" s="3"/>
+      <c r="A98" s="1">
+        <v>43963.4375</v>
+      </c>
+      <c r="B98" s="6">
+        <v>421898</v>
+      </c>
+      <c r="C98" s="6">
+        <v>10811</v>
+      </c>
+      <c r="D98" s="6">
+        <v>20907</v>
+      </c>
+      <c r="E98" s="6">
+        <v>15391</v>
+      </c>
+      <c r="F98" s="6">
+        <v>1725</v>
+      </c>
+      <c r="G98" s="6">
+        <v>470732</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3532,11 +3551,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N56"/>
+  <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3677,7 +3696,7 @@
       <c r="K4">
         <v>152</v>
       </c>
-      <c r="L4" s="7"/>
+      <c r="L4" s="5"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
     </row>
@@ -3715,7 +3734,7 @@
       <c r="K5">
         <v>154</v>
       </c>
-      <c r="L5" s="7"/>
+      <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
     </row>
@@ -3753,7 +3772,7 @@
       <c r="K6">
         <v>160</v>
       </c>
-      <c r="L6" s="7"/>
+      <c r="L6" s="5"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
     </row>
@@ -3791,7 +3810,7 @@
       <c r="K7">
         <v>187</v>
       </c>
-      <c r="L7" s="7"/>
+      <c r="L7" s="5"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
     </row>
@@ -3829,7 +3848,7 @@
       <c r="K8">
         <v>195</v>
       </c>
-      <c r="L8" s="7"/>
+      <c r="L8" s="5"/>
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
     </row>
@@ -3867,7 +3886,7 @@
       <c r="K9">
         <v>214</v>
       </c>
-      <c r="L9" s="7"/>
+      <c r="L9" s="5"/>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
     </row>
@@ -3905,7 +3924,7 @@
       <c r="K10">
         <v>217</v>
       </c>
-      <c r="L10" s="7"/>
+      <c r="L10" s="5"/>
       <c r="M10" s="5"/>
       <c r="N10" s="5"/>
     </row>
@@ -3943,7 +3962,7 @@
       <c r="K11">
         <v>215</v>
       </c>
-      <c r="L11" s="7"/>
+      <c r="L11" s="5"/>
       <c r="M11" s="5"/>
       <c r="N11" s="5"/>
     </row>
@@ -3981,7 +4000,7 @@
       <c r="K12">
         <v>196</v>
       </c>
-      <c r="L12" s="7"/>
+      <c r="L12" s="5"/>
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
     </row>
@@ -4019,7 +4038,7 @@
       <c r="K13">
         <v>203</v>
       </c>
-      <c r="L13" s="7"/>
+      <c r="L13" s="5"/>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
     </row>
@@ -4057,7 +4076,7 @@
       <c r="K14">
         <v>199</v>
       </c>
-      <c r="L14" s="7"/>
+      <c r="L14" s="5"/>
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
     </row>
@@ -4095,7 +4114,7 @@
       <c r="K15">
         <v>188</v>
       </c>
-      <c r="L15" s="7"/>
+      <c r="L15" s="5"/>
       <c r="M15" s="5"/>
       <c r="N15" s="5"/>
     </row>
@@ -4133,7 +4152,7 @@
       <c r="K16">
         <v>200</v>
       </c>
-      <c r="L16" s="7"/>
+      <c r="L16" s="5"/>
       <c r="M16" s="5"/>
       <c r="N16" s="5"/>
     </row>
@@ -4171,7 +4190,7 @@
       <c r="K17" s="6">
         <v>200</v>
       </c>
-      <c r="L17" s="7"/>
+      <c r="L17" s="5"/>
       <c r="M17" s="5"/>
       <c r="N17" s="5"/>
     </row>
@@ -4209,7 +4228,7 @@
       <c r="K18" s="6">
         <v>197</v>
       </c>
-      <c r="L18" s="7"/>
+      <c r="L18" s="5"/>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
     </row>
@@ -4247,7 +4266,7 @@
       <c r="K19" s="6">
         <v>196</v>
       </c>
-      <c r="L19" s="7"/>
+      <c r="L19" s="5"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -4283,7 +4302,7 @@
       <c r="K20" s="6">
         <v>193</v>
       </c>
-      <c r="L20" s="7"/>
+      <c r="L20" s="5"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -4319,7 +4338,7 @@
       <c r="K21" s="6">
         <v>194</v>
       </c>
-      <c r="L21" s="7"/>
+      <c r="L21" s="5"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
@@ -4355,7 +4374,7 @@
       <c r="K22" s="6">
         <v>192</v>
       </c>
-      <c r="L22" s="7"/>
+      <c r="L22" s="5"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
@@ -4391,6 +4410,7 @@
       <c r="K23" s="6">
         <v>185</v>
       </c>
+      <c r="L23" s="5"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
@@ -4426,6 +4446,7 @@
       <c r="K24" s="6">
         <v>193</v>
       </c>
+      <c r="L24" s="5"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
@@ -4461,6 +4482,7 @@
       <c r="K25" s="6">
         <v>195</v>
       </c>
+      <c r="L25" s="5"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
@@ -4496,6 +4518,7 @@
       <c r="K26" s="6">
         <v>195</v>
       </c>
+      <c r="L26" s="5"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
@@ -4531,6 +4554,7 @@
       <c r="K27" s="6">
         <v>191</v>
       </c>
+      <c r="L27" s="5"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
@@ -4566,6 +4590,7 @@
       <c r="K28" s="6">
         <v>187</v>
       </c>
+      <c r="L28" s="5"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
@@ -4601,6 +4626,7 @@
       <c r="K29" s="6">
         <v>186</v>
       </c>
+      <c r="L29" s="5"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
@@ -4636,6 +4662,7 @@
       <c r="K30" s="6">
         <v>181</v>
       </c>
+      <c r="L30" s="5"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
@@ -4671,6 +4698,7 @@
       <c r="K31" s="6">
         <v>175</v>
       </c>
+      <c r="L31" s="5"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
@@ -4706,8 +4734,9 @@
       <c r="K32" s="6">
         <v>154</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L32" s="5"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43954.4375</v>
       </c>
@@ -4741,8 +4770,9 @@
       <c r="K33" s="6">
         <v>174</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L33" s="5"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43955.4375</v>
       </c>
@@ -4776,8 +4806,9 @@
       <c r="K34" s="6">
         <v>175</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L34" s="5"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>43956.4375</v>
       </c>
@@ -4811,8 +4842,9 @@
       <c r="K35" s="6">
         <v>166</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L35" s="5"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>43957.4375</v>
       </c>
@@ -4846,8 +4878,9 @@
       <c r="K36" s="6">
         <v>174</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L36" s="5"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>43958.4375</v>
       </c>
@@ -4881,8 +4914,9 @@
       <c r="K37" s="6">
         <v>155</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L37" s="5"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>43959.4375</v>
       </c>
@@ -4916,8 +4950,9 @@
       <c r="K38" s="6">
         <v>166</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L38" s="5"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>43960.4375</v>
       </c>
@@ -4951,8 +4986,9 @@
       <c r="K39" s="6">
         <v>158</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L39" s="5"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>43961.4375</v>
       </c>
@@ -4986,8 +5022,9 @@
       <c r="K40" s="6">
         <v>140</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L40" s="5"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>43962.4375</v>
       </c>
@@ -5021,44 +5058,86 @@
       <c r="K41" s="6">
         <v>147</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C42" s="3"/>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L41" s="5"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>43963.4375</v>
+      </c>
+      <c r="B42" s="6">
+        <v>8776</v>
+      </c>
+      <c r="C42" s="6">
+        <v>11971</v>
+      </c>
+      <c r="D42" s="6">
+        <v>552</v>
+      </c>
+      <c r="E42" s="6">
+        <v>4952</v>
+      </c>
+      <c r="F42" s="6">
+        <v>6392</v>
+      </c>
+      <c r="G42" s="6">
+        <v>4489</v>
+      </c>
+      <c r="H42" s="6">
+        <v>4508</v>
+      </c>
+      <c r="I42" s="6">
+        <v>1025</v>
+      </c>
+      <c r="J42" s="6">
+        <v>192</v>
+      </c>
+      <c r="K42" s="6">
+        <v>146</v>
+      </c>
+      <c r="L42" s="5"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C44" s="3"/>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C46" s="3"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C47" s="3"/>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C49" s="3"/>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C50" s="3"/>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C51" s="3"/>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C52" s="3"/>
-      <c r="F52" s="3"/>
-    </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C54" s="3"/>
-      <c r="E54" s="3"/>
-    </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C55" s="3"/>
-    </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C56" s="3"/>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D44" s="3"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D47" s="3"/>
+    </row>
+    <row r="49" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D50" s="3"/>
+    </row>
+    <row r="52" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D55" s="3"/>
+    </row>
+    <row r="57" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D58" s="3"/>
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D59" s="3"/>
+    </row>
+    <row r="61" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D61" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-13 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35B4FBE-1D32-E642-8FB0-FFD8BC187D46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15126B71-420C-714B-B2FD-AD9C82554AE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -1152,11 +1152,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I98"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C100" sqref="C100:F120"/>
+      <selection pane="bottomLeft" activeCell="C103" sqref="C103:F120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3544,6 +3544,36 @@
         <v>470732</v>
       </c>
     </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>43964.4375</v>
+      </c>
+      <c r="B99" s="6">
+        <v>436212</v>
+      </c>
+      <c r="C99" s="6">
+        <v>13395</v>
+      </c>
+      <c r="D99" s="6">
+        <v>21236</v>
+      </c>
+      <c r="E99" s="6">
+        <v>15845</v>
+      </c>
+      <c r="F99" s="6">
+        <v>1765</v>
+      </c>
+      <c r="G99" s="6">
+        <v>488453</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C100" s="6"/>
+      <c r="D100" s="3"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D102" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3551,11 +3581,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5097,47 +5127,74 @@
       <c r="L42" s="5"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C43" s="3"/>
+      <c r="A43" s="1">
+        <v>43964.4375</v>
+      </c>
+      <c r="B43" s="6">
+        <v>8923</v>
+      </c>
+      <c r="C43" s="6">
+        <v>12155</v>
+      </c>
+      <c r="D43" s="6">
+        <v>571</v>
+      </c>
+      <c r="E43" s="6">
+        <v>5045</v>
+      </c>
+      <c r="F43" s="6">
+        <v>6481</v>
+      </c>
+      <c r="G43" s="6">
+        <v>4544</v>
+      </c>
+      <c r="H43" s="6">
+        <v>4581</v>
+      </c>
+      <c r="I43" s="6">
+        <v>1018</v>
+      </c>
+      <c r="J43" s="6">
+        <v>189</v>
+      </c>
+      <c r="K43" s="6">
+        <v>144</v>
+      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D44" s="3"/>
+      <c r="C44" s="3"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D46" s="3"/>
+      <c r="C46" s="3"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D47" s="3"/>
-    </row>
-    <row r="49" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D49" s="3"/>
-    </row>
-    <row r="50" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D50" s="3"/>
-    </row>
-    <row r="52" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D52" s="3"/>
-    </row>
-    <row r="53" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D53" s="3"/>
-    </row>
-    <row r="54" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D54" s="3"/>
-    </row>
-    <row r="55" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D55" s="3"/>
-    </row>
-    <row r="57" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D57" s="3"/>
-    </row>
-    <row r="58" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D58" s="3"/>
+      <c r="C47" s="3"/>
+    </row>
+    <row r="49" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C50" s="3"/>
+    </row>
+    <row r="51" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C52" s="3"/>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C54" s="3"/>
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C56" s="3"/>
+    </row>
+    <row r="58" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C58" s="3"/>
       <c r="F58" s="3"/>
-    </row>
-    <row r="59" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D59" s="3"/>
-    </row>
-    <row r="61" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D61" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-14 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15126B71-420C-714B-B2FD-AD9C82554AE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF121F42-6F24-C24A-8A09-96A00A7F9C3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -1152,11 +1152,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I118"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C103" sqref="C103:F120"/>
+      <selection pane="bottomLeft" activeCell="B105" sqref="B105:D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3568,11 +3568,51 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C100" s="6"/>
-      <c r="D100" s="3"/>
+      <c r="A100" s="1">
+        <v>43965.4375</v>
+      </c>
+      <c r="B100" s="6">
+        <v>452991</v>
+      </c>
+      <c r="C100" s="6">
+        <v>17578</v>
+      </c>
+      <c r="D100" s="6">
+        <v>21494</v>
+      </c>
+      <c r="E100" s="6">
+        <v>16204</v>
+      </c>
+      <c r="F100" s="6">
+        <v>1798</v>
+      </c>
+      <c r="G100" s="6">
+        <v>510065</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C101" s="3"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D102" s="3"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C103" s="3"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C104" s="3"/>
+    </row>
+    <row r="114" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E114" s="3"/>
+    </row>
+    <row r="115" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C115" s="3"/>
+    </row>
+    <row r="116" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C116" s="3"/>
+    </row>
+    <row r="118" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C118" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3584,8 +3624,8 @@
   <dimension ref="A1:N58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I48" sqref="I48"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5162,7 +5202,42 @@
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C44" s="3"/>
+      <c r="A44" s="1">
+        <v>43965.4375</v>
+      </c>
+      <c r="B44" s="6">
+        <v>9037</v>
+      </c>
+      <c r="C44" s="6">
+        <v>12297</v>
+      </c>
+      <c r="D44" s="6">
+        <v>592</v>
+      </c>
+      <c r="E44" s="6">
+        <v>5118</v>
+      </c>
+      <c r="F44" s="6">
+        <v>6548</v>
+      </c>
+      <c r="G44" s="6">
+        <v>4589</v>
+      </c>
+      <c r="H44" s="6">
+        <v>4632</v>
+      </c>
+      <c r="I44" s="6">
+        <v>1026</v>
+      </c>
+      <c r="J44" s="6">
+        <v>184</v>
+      </c>
+      <c r="K44" s="6">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B45" s="6"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C46" s="3"/>

</xml_diff>

<commit_message>
excel update 2020-05-15 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF121F42-6F24-C24A-8A09-96A00A7F9C3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05AC26D-BE54-754A-9DA5-09096127A9AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -1152,11 +1152,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I118"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B105" sqref="B105:D114"/>
+      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C107" sqref="C107:F123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3591,7 +3591,27 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C101" s="3"/>
+      <c r="A101" s="1">
+        <v>43966.4375</v>
+      </c>
+      <c r="B101" s="6">
+        <v>470453</v>
+      </c>
+      <c r="C101" s="6">
+        <v>14373</v>
+      </c>
+      <c r="D101" s="6">
+        <v>21922</v>
+      </c>
+      <c r="E101" s="6">
+        <v>16641</v>
+      </c>
+      <c r="F101" s="6">
+        <v>1825</v>
+      </c>
+      <c r="G101" s="6">
+        <v>525214</v>
+      </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D102" s="3"/>
@@ -3601,18 +3621,10 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C104" s="3"/>
-    </row>
-    <row r="114" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="E114" s="3"/>
-    </row>
-    <row r="115" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C115" s="3"/>
-    </row>
-    <row r="116" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C116" s="3"/>
-    </row>
-    <row r="118" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C118" s="3"/>
+      <c r="D104" s="3"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D105" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3625,7 +3637,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F53" sqref="F53"/>
+      <selection pane="bottomLeft" activeCell="I49" sqref="I49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5237,39 +5249,78 @@
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B45" s="6"/>
+      <c r="A45" s="1">
+        <v>43966.4375</v>
+      </c>
+      <c r="B45" s="6">
+        <v>9225</v>
+      </c>
+      <c r="C45" s="6">
+        <v>12533</v>
+      </c>
+      <c r="D45" s="6">
+        <v>601</v>
+      </c>
+      <c r="E45" s="6">
+        <v>5251</v>
+      </c>
+      <c r="F45" s="6">
+        <v>6693</v>
+      </c>
+      <c r="G45" s="6">
+        <v>4659</v>
+      </c>
+      <c r="H45" s="6">
+        <v>4702</v>
+      </c>
+      <c r="I45" s="6">
+        <v>986</v>
+      </c>
+      <c r="J45" s="6">
+        <v>179</v>
+      </c>
+      <c r="K45" s="6">
+        <v>135</v>
+      </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C46" s="3"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C47" s="3"/>
-    </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C49" s="3"/>
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D48" s="3"/>
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
     </row>
     <row r="51" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
     </row>
     <row r="52" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D53" s="3"/>
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C54" s="3"/>
       <c r="E54" s="3"/>
     </row>
     <row r="55" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C55" s="3"/>
+      <c r="D55" s="3"/>
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D57" s="3"/>
     </row>
     <row r="58" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C58" s="3"/>
-      <c r="F58" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-16 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05AC26D-BE54-754A-9DA5-09096127A9AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060847E1-3F1D-F74A-A89F-AAC9D14ABAD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -446,11 +446,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1152,11 +1151,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C107" sqref="C107:F123"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E159" sqref="E159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1238,7 +1237,7 @@
       <c r="G3">
         <v>313</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -1262,7 +1261,7 @@
       <c r="G4">
         <v>340</v>
       </c>
-      <c r="H4" s="6"/>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -1286,7 +1285,7 @@
       <c r="G5">
         <v>364</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -1310,7 +1309,7 @@
       <c r="G6">
         <v>364</v>
       </c>
-      <c r="H6" s="6"/>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -1334,7 +1333,7 @@
       <c r="G7">
         <v>364</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -1358,7 +1357,7 @@
       <c r="G8">
         <v>402</v>
       </c>
-      <c r="H8" s="6"/>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -1382,7 +1381,7 @@
       <c r="G9">
         <v>421</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -1406,7 +1405,7 @@
       <c r="G10">
         <v>456</v>
       </c>
-      <c r="H10" s="6"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -1430,7 +1429,7 @@
       <c r="G11">
         <v>479</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -1454,7 +1453,7 @@
       <c r="G12">
         <v>498</v>
       </c>
-      <c r="H12" s="6"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -1478,7 +1477,7 @@
       <c r="G13">
         <v>498</v>
       </c>
-      <c r="H13" s="6"/>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -1502,7 +1501,7 @@
       <c r="G14">
         <v>498</v>
       </c>
-      <c r="H14" s="6"/>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -1526,7 +1525,7 @@
       <c r="G15">
         <v>553</v>
       </c>
-      <c r="H15" s="6"/>
+      <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -1550,7 +1549,7 @@
       <c r="G16">
         <v>593</v>
       </c>
-      <c r="H16" s="6"/>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -1574,7 +1573,7 @@
       <c r="G17">
         <v>629</v>
       </c>
-      <c r="H17" s="6"/>
+      <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -1598,7 +1597,7 @@
       <c r="G18">
         <v>699</v>
       </c>
-      <c r="H18" s="6"/>
+      <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -1622,7 +1621,7 @@
       <c r="G19">
         <v>699</v>
       </c>
-      <c r="H19" s="6"/>
+      <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -1646,7 +1645,7 @@
       <c r="G20">
         <v>768</v>
       </c>
-      <c r="H20" s="6"/>
+      <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -1670,7 +1669,7 @@
       <c r="G21">
         <v>768</v>
       </c>
-      <c r="H21" s="6"/>
+      <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
@@ -1694,7 +1693,7 @@
       <c r="G22">
         <v>1005</v>
       </c>
-      <c r="H22" s="6"/>
+      <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
@@ -1718,7 +1717,7 @@
       <c r="G23">
         <v>1126</v>
       </c>
-      <c r="H23" s="6"/>
+      <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
@@ -1742,7 +1741,7 @@
       <c r="G24">
         <v>1338</v>
       </c>
-      <c r="H24" s="6"/>
+      <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
@@ -1766,7 +1765,7 @@
       <c r="G25">
         <v>1566</v>
       </c>
-      <c r="H25" s="6"/>
+      <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
@@ -1790,7 +1789,7 @@
       <c r="G26">
         <v>1763</v>
       </c>
-      <c r="H26" s="6"/>
+      <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
@@ -1814,7 +1813,7 @@
       <c r="G27">
         <v>1982</v>
       </c>
-      <c r="H27" s="6"/>
+      <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
@@ -1838,7 +1837,7 @@
       <c r="G28">
         <v>1982</v>
       </c>
-      <c r="H28" s="6"/>
+      <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
@@ -1862,7 +1861,7 @@
       <c r="G29">
         <v>2403</v>
       </c>
-      <c r="H29" s="6"/>
+      <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
@@ -1886,7 +1885,7 @@
       <c r="G30">
         <v>2747</v>
       </c>
-      <c r="H30" s="6"/>
+      <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
@@ -1910,7 +1909,7 @@
       <c r="G31">
         <v>2747</v>
       </c>
-      <c r="H31" s="6"/>
+      <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
@@ -1934,7 +1933,7 @@
       <c r="G32">
         <v>3395</v>
       </c>
-      <c r="H32" s="6"/>
+      <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
@@ -1958,7 +1957,7 @@
       <c r="G33">
         <v>4185</v>
       </c>
-      <c r="H33" s="6"/>
+      <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
@@ -1982,7 +1981,7 @@
       <c r="G34">
         <v>5129</v>
       </c>
-      <c r="H34" s="6"/>
+      <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
@@ -2006,7 +2005,7 @@
       <c r="G35">
         <v>6648</v>
       </c>
-      <c r="H35" s="6"/>
+      <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
@@ -2030,7 +2029,7 @@
       <c r="G36">
         <v>8465</v>
       </c>
-      <c r="H36" s="6"/>
+      <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
@@ -2054,7 +2053,7 @@
       <c r="G37">
         <v>10178</v>
       </c>
-      <c r="H37" s="6"/>
+      <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
@@ -2078,7 +2077,7 @@
       <c r="G38">
         <v>11171</v>
       </c>
-      <c r="H38" s="6"/>
+      <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
@@ -2102,7 +2101,7 @@
       <c r="G39">
         <v>16650</v>
       </c>
-      <c r="H39" s="6"/>
+      <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
@@ -2126,7 +2125,7 @@
       <c r="G40">
         <v>16650</v>
       </c>
-      <c r="H40" s="6"/>
+      <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
@@ -2150,7 +2149,7 @@
       <c r="G41">
         <v>23384</v>
       </c>
-      <c r="H41" s="6"/>
+      <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
@@ -2174,7 +2173,7 @@
       <c r="G42">
         <v>23384</v>
       </c>
-      <c r="H42" s="6"/>
+      <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
@@ -2198,7 +2197,7 @@
       <c r="G43">
         <v>26420</v>
       </c>
-      <c r="H43" s="6"/>
+      <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
@@ -2222,7 +2221,7 @@
       <c r="G44">
         <v>28506</v>
       </c>
-      <c r="H44" s="6"/>
+      <c r="H44" s="5"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
@@ -2246,7 +2245,7 @@
       <c r="G45">
         <v>32457</v>
       </c>
-      <c r="H45" s="6"/>
+      <c r="H45" s="5"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
@@ -2270,7 +2269,7 @@
       <c r="G46">
         <v>35635</v>
       </c>
-      <c r="H46" s="6"/>
+      <c r="H46" s="5"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
@@ -2294,7 +2293,7 @@
       <c r="G47">
         <v>35635</v>
       </c>
-      <c r="H47" s="6"/>
+      <c r="H47" s="5"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
@@ -2318,7 +2317,7 @@
       <c r="G48">
         <v>38550</v>
       </c>
-      <c r="H48" s="6"/>
+      <c r="H48" s="5"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
@@ -2342,7 +2341,7 @@
       <c r="G49">
         <v>38550</v>
       </c>
-      <c r="H49" s="6"/>
+      <c r="H49" s="5"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
@@ -2366,7 +2365,7 @@
       <c r="G50">
         <v>41032</v>
       </c>
-      <c r="H50" s="6"/>
+      <c r="H50" s="5"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
@@ -2390,7 +2389,7 @@
       <c r="G51">
         <v>43072</v>
       </c>
-      <c r="H51" s="6"/>
+      <c r="H51" s="5"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
@@ -2414,7 +2413,7 @@
       <c r="G52">
         <v>43072</v>
       </c>
-      <c r="H52" s="6"/>
+      <c r="H52" s="5"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
@@ -2438,7 +2437,7 @@
       <c r="G53">
         <v>49186</v>
       </c>
-      <c r="H53" s="6"/>
+      <c r="H53" s="5"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
@@ -2462,7 +2461,7 @@
       <c r="G54">
         <v>49186</v>
       </c>
-      <c r="H54" s="6"/>
+      <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
@@ -2486,7 +2485,7 @@
       <c r="G55">
         <v>54112</v>
       </c>
-      <c r="H55" s="6"/>
+      <c r="H55" s="5"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
@@ -2511,7 +2510,7 @@
         <f>51629+C53</f>
         <v>58832</v>
       </c>
-      <c r="H56" s="6"/>
+      <c r="H56" s="5"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
@@ -2535,8 +2534,8 @@
       <c r="G57">
         <v>61009</v>
       </c>
-      <c r="H57" s="6"/>
-      <c r="I57" s="6"/>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
@@ -2560,8 +2559,8 @@
       <c r="G58">
         <v>64785</v>
       </c>
-      <c r="H58" s="6"/>
-      <c r="I58" s="6"/>
+      <c r="H58" s="5"/>
+      <c r="I58" s="5"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
@@ -2585,8 +2584,8 @@
       <c r="G59">
         <v>67998</v>
       </c>
-      <c r="H59" s="6"/>
-      <c r="I59" s="6"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
@@ -2610,8 +2609,8 @@
       <c r="G60">
         <v>72674</v>
       </c>
-      <c r="H60" s="6"/>
-      <c r="I60" s="6"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
@@ -2635,8 +2634,8 @@
       <c r="G61">
         <v>76027</v>
       </c>
-      <c r="H61" s="6"/>
-      <c r="I61" s="6"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
@@ -2660,8 +2659,8 @@
       <c r="G62">
         <v>79125</v>
       </c>
-      <c r="H62" s="6"/>
-      <c r="I62" s="6"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
@@ -2685,8 +2684,8 @@
       <c r="G63">
         <v>82055</v>
       </c>
-      <c r="H63" s="6"/>
-      <c r="I63" s="6"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
@@ -2710,8 +2709,8 @@
       <c r="G64">
         <v>85703</v>
       </c>
-      <c r="H64" s="6"/>
-      <c r="I64" s="6"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
@@ -2735,8 +2734,8 @@
       <c r="G65">
         <v>89906</v>
       </c>
-      <c r="H65" s="6"/>
-      <c r="I65" s="6"/>
+      <c r="H65" s="5"/>
+      <c r="I65" s="5"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
@@ -2760,8 +2759,8 @@
       <c r="G66">
         <v>94271</v>
       </c>
-      <c r="H66" s="6"/>
-      <c r="I66" s="6"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
@@ -2785,8 +2784,8 @@
       <c r="G67">
         <v>97838</v>
       </c>
-      <c r="H67" s="6"/>
-      <c r="I67" s="6"/>
+      <c r="H67" s="5"/>
+      <c r="I67" s="5"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
@@ -2810,8 +2809,8 @@
       <c r="G68">
         <v>104784</v>
       </c>
-      <c r="H68" s="6"/>
-      <c r="I68" s="6"/>
+      <c r="H68" s="5"/>
+      <c r="I68" s="5"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
@@ -2835,8 +2834,8 @@
       <c r="G69">
         <v>109764</v>
       </c>
-      <c r="H69" s="6"/>
-      <c r="I69" s="6"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
@@ -2860,8 +2859,8 @@
       <c r="G70">
         <v>115189</v>
       </c>
-      <c r="H70" s="6"/>
-      <c r="I70" s="6"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
@@ -2885,8 +2884,8 @@
       <c r="G71">
         <v>123521</v>
       </c>
-      <c r="H71" s="6"/>
-      <c r="I71" s="6"/>
+      <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
@@ -2910,108 +2909,108 @@
       <c r="G72">
         <v>132416</v>
       </c>
-      <c r="H72" s="6"/>
-      <c r="I72" s="6"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="5"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>43938.4375</v>
       </c>
-      <c r="B73" s="6">
+      <c r="B73" s="5">
         <v>122433</v>
       </c>
-      <c r="C73" s="6">
+      <c r="C73" s="5">
         <v>5993</v>
       </c>
-      <c r="D73" s="6">
+      <c r="D73" s="5">
         <v>9525</v>
       </c>
-      <c r="E73" s="6">
+      <c r="E73" s="5">
         <v>4556</v>
       </c>
-      <c r="F73" s="6">
+      <c r="F73" s="5">
         <v>478</v>
       </c>
-      <c r="G73" s="6">
+      <c r="G73" s="5">
         <v>142985</v>
       </c>
-      <c r="H73" s="6"/>
-      <c r="I73" s="6"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="5"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>43939.4375</v>
       </c>
-      <c r="B74" s="6">
+      <c r="B74" s="5">
         <v>131055</v>
       </c>
-      <c r="C74" s="6">
+      <c r="C74" s="5">
         <v>6833</v>
       </c>
-      <c r="D74" s="6">
+      <c r="D74" s="5">
         <v>10010</v>
       </c>
-      <c r="E74" s="6">
+      <c r="E74" s="5">
         <v>4875</v>
       </c>
-      <c r="F74" s="6">
+      <c r="F74" s="5">
         <v>514</v>
       </c>
-      <c r="G74" s="6">
+      <c r="G74" s="5">
         <v>153287</v>
       </c>
-      <c r="H74" s="6"/>
-      <c r="I74" s="6"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>43940.4375</v>
       </c>
-      <c r="B75" s="6">
+      <c r="B75" s="5">
         <v>139757</v>
       </c>
-      <c r="C75" s="6">
+      <c r="C75" s="5">
         <v>5736</v>
       </c>
-      <c r="D75" s="6">
+      <c r="D75" s="5">
         <v>10578</v>
       </c>
-      <c r="E75" s="6">
+      <c r="E75" s="5">
         <v>5209</v>
       </c>
-      <c r="F75" s="6">
+      <c r="F75" s="5">
         <v>553</v>
       </c>
-      <c r="G75" s="6">
+      <c r="G75" s="5">
         <v>161833</v>
       </c>
-      <c r="H75" s="6"/>
-      <c r="I75" s="6"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>43941.4375</v>
       </c>
-      <c r="B76" s="6">
+      <c r="B76" s="5">
         <v>147557</v>
       </c>
-      <c r="C76" s="6">
+      <c r="C76" s="5">
         <v>3799</v>
       </c>
-      <c r="D76" s="6">
+      <c r="D76" s="5">
         <v>11184</v>
       </c>
-      <c r="E76" s="6">
+      <c r="E76" s="5">
         <v>5515</v>
       </c>
-      <c r="F76" s="6">
+      <c r="F76" s="5">
         <v>584</v>
       </c>
-      <c r="G76" s="6">
+      <c r="G76" s="5">
         <v>168639</v>
       </c>
-      <c r="H76" s="6"/>
-      <c r="I76" s="6"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
@@ -3020,366 +3019,366 @@
       <c r="B77">
         <v>156007</v>
       </c>
-      <c r="C77" s="6">
+      <c r="C77" s="5">
         <v>5546</v>
       </c>
-      <c r="D77" s="6">
+      <c r="D77" s="5">
         <v>11735</v>
       </c>
-      <c r="E77" s="6">
+      <c r="E77" s="5">
         <v>5806</v>
       </c>
-      <c r="F77" s="6">
+      <c r="F77" s="5">
         <v>622</v>
       </c>
       <c r="G77">
         <v>179716</v>
       </c>
-      <c r="H77" s="6"/>
-      <c r="I77" s="6"/>
+      <c r="H77" s="5"/>
+      <c r="I77" s="5"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>43943.4375</v>
       </c>
-      <c r="B78" s="6">
+      <c r="B78" s="5">
         <v>165406</v>
       </c>
-      <c r="C78" s="6">
+      <c r="C78" s="5">
         <v>6845</v>
       </c>
-      <c r="D78" s="6">
+      <c r="D78" s="5">
         <v>12245</v>
       </c>
-      <c r="E78" s="6">
+      <c r="E78" s="5">
         <v>6221</v>
       </c>
-      <c r="F78" s="6">
+      <c r="F78" s="5">
         <v>659</v>
       </c>
-      <c r="G78" s="6">
+      <c r="G78" s="5">
         <v>191376</v>
       </c>
-      <c r="H78" s="6"/>
-      <c r="I78" s="6"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="5"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>43944.4375</v>
       </c>
-      <c r="B79" s="6">
+      <c r="B79" s="5">
         <v>174473</v>
       </c>
-      <c r="C79" s="6">
+      <c r="C79" s="5">
         <v>6757</v>
       </c>
-      <c r="D79" s="6">
+      <c r="D79" s="5">
         <v>12879</v>
       </c>
-      <c r="E79" s="6">
+      <c r="E79" s="5">
         <v>6680</v>
       </c>
-      <c r="F79" s="6">
+      <c r="F79" s="5">
         <v>713</v>
       </c>
-      <c r="G79" s="6">
+      <c r="G79" s="5">
         <v>201502</v>
       </c>
-      <c r="H79" s="6"/>
-      <c r="I79" s="6"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="5"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>43945.4375</v>
       </c>
-      <c r="B80" s="6">
+      <c r="B80" s="5">
         <v>185671</v>
       </c>
-      <c r="C80" s="6">
+      <c r="C80" s="5">
         <v>5414</v>
       </c>
-      <c r="D80" s="6">
+      <c r="D80" s="5">
         <v>13519</v>
       </c>
-      <c r="E80" s="6">
+      <c r="E80" s="5">
         <v>7087</v>
       </c>
-      <c r="F80" s="6">
+      <c r="F80" s="5">
         <v>763</v>
       </c>
-      <c r="G80" s="6">
+      <c r="G80" s="5">
         <v>212454</v>
       </c>
-      <c r="H80" s="6"/>
-      <c r="I80" s="6"/>
+      <c r="H80" s="5"/>
+      <c r="I80" s="5"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>43946.4375</v>
       </c>
-      <c r="B81" s="6">
+      <c r="B81" s="5">
         <v>195303</v>
       </c>
-      <c r="C81" s="6">
+      <c r="C81" s="5">
         <v>8171</v>
       </c>
-      <c r="D81" s="6">
+      <c r="D81" s="5">
         <v>13995</v>
       </c>
-      <c r="E81" s="6">
+      <c r="E81" s="5">
         <v>7509</v>
       </c>
-      <c r="F81" s="6">
+      <c r="F81" s="5">
         <v>811</v>
       </c>
-      <c r="G81" s="6">
+      <c r="G81" s="5">
         <v>225789</v>
       </c>
-      <c r="H81" s="6"/>
-      <c r="I81" s="6"/>
+      <c r="H81" s="5"/>
+      <c r="I81" s="5"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>43947.4375</v>
       </c>
-      <c r="B82" s="6">
+      <c r="B82" s="5">
         <v>206371</v>
       </c>
-      <c r="C82" s="6">
+      <c r="C82" s="5">
         <v>7417</v>
       </c>
-      <c r="D82" s="6">
+      <c r="D82" s="5">
         <v>14432</v>
       </c>
-      <c r="E82" s="6">
+      <c r="E82" s="5">
         <v>8000</v>
       </c>
-      <c r="F82" s="6">
+      <c r="F82" s="5">
         <v>835</v>
       </c>
-      <c r="G82" s="6">
+      <c r="G82" s="5">
         <v>237055</v>
       </c>
-      <c r="H82" s="6"/>
-      <c r="I82" s="6"/>
+      <c r="H82" s="5"/>
+      <c r="I82" s="5"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>43948.4375</v>
       </c>
-      <c r="B83" s="6">
+      <c r="B83" s="5">
         <v>217915</v>
       </c>
-      <c r="C83" s="6">
+      <c r="C83" s="5">
         <v>5001</v>
       </c>
-      <c r="D83" s="6">
+      <c r="D83" s="5">
         <v>14856</v>
       </c>
-      <c r="E83" s="6">
+      <c r="E83" s="5">
         <v>8525</v>
       </c>
-      <c r="F83" s="6">
+      <c r="F83" s="5">
         <v>892</v>
       </c>
-      <c r="G83" s="6">
+      <c r="G83" s="5">
         <v>247189</v>
       </c>
-      <c r="H83" s="6"/>
-      <c r="I83" s="6"/>
+      <c r="H83" s="5"/>
+      <c r="I83" s="5"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>43949.4375</v>
       </c>
-      <c r="B84" s="6">
+      <c r="B84" s="5">
         <v>227744</v>
       </c>
-      <c r="C84" s="6">
+      <c r="C84" s="5">
         <v>6282</v>
       </c>
-      <c r="D84" s="6">
+      <c r="D84" s="5">
         <v>15381</v>
       </c>
-      <c r="E84" s="6">
+      <c r="E84" s="5">
         <v>8964</v>
       </c>
-      <c r="F84" s="6">
+      <c r="F84" s="5">
         <v>951</v>
       </c>
-      <c r="G84" s="6">
+      <c r="G84" s="5">
         <v>259322</v>
       </c>
-      <c r="H84" s="6"/>
-      <c r="I84" s="6"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="5"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>43950.4375</v>
       </c>
-      <c r="B85" s="6">
+      <c r="B85" s="5">
         <v>238258</v>
       </c>
-      <c r="C85" s="6">
+      <c r="C85" s="5">
         <v>9530</v>
       </c>
-      <c r="D85" s="6">
+      <c r="D85" s="5">
         <v>15728</v>
       </c>
-      <c r="E85" s="6">
+      <c r="E85" s="5">
         <v>9612</v>
       </c>
-      <c r="F85" s="6">
+      <c r="F85" s="5">
         <v>996</v>
       </c>
-      <c r="G85" s="6">
+      <c r="G85" s="5">
         <v>274124</v>
       </c>
-      <c r="H85" s="6"/>
-      <c r="I85" s="6"/>
+      <c r="H85" s="5"/>
+      <c r="I85" s="5"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>43951.4375</v>
       </c>
-      <c r="B86" s="6">
+      <c r="B86" s="5">
         <v>250048</v>
       </c>
-      <c r="C86" s="6">
+      <c r="C86" s="5">
         <v>11859</v>
       </c>
-      <c r="D86" s="6">
+      <c r="D86" s="5">
         <v>16187</v>
       </c>
-      <c r="E86" s="6">
+      <c r="E86" s="5">
         <v>10205</v>
       </c>
-      <c r="F86" s="6">
+      <c r="F86" s="5">
         <v>1082</v>
       </c>
-      <c r="G86" s="6">
+      <c r="G86" s="5">
         <v>289381</v>
       </c>
-      <c r="H86" s="6"/>
-      <c r="I86" s="6"/>
+      <c r="H86" s="5"/>
+      <c r="I86" s="5"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>43952.4375</v>
       </c>
-      <c r="B87" s="6">
+      <c r="B87" s="5">
         <v>265500</v>
       </c>
-      <c r="C87" s="6">
+      <c r="C87" s="5">
         <v>11975</v>
       </c>
-      <c r="D87" s="6">
+      <c r="D87" s="5">
         <v>16608</v>
       </c>
-      <c r="E87" s="6">
+      <c r="E87" s="5">
         <v>10825</v>
       </c>
-      <c r="F87" s="6">
+      <c r="F87" s="5">
         <v>1121</v>
       </c>
-      <c r="G87" s="6">
+      <c r="G87" s="5">
         <v>306029</v>
       </c>
-      <c r="H87" s="6"/>
-      <c r="I87" s="6"/>
+      <c r="H87" s="5"/>
+      <c r="I87" s="5"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>43953.4375</v>
       </c>
-      <c r="B88" s="6">
+      <c r="B88" s="5">
         <v>280674</v>
       </c>
-      <c r="C88" s="6">
+      <c r="C88" s="5">
         <v>12829</v>
       </c>
-      <c r="D88" s="6">
+      <c r="D88" s="5">
         <v>17119</v>
       </c>
-      <c r="E88" s="6">
+      <c r="E88" s="5">
         <v>11390</v>
       </c>
-      <c r="F88" s="6">
+      <c r="F88" s="5">
         <v>1176</v>
       </c>
-      <c r="G88" s="6">
+      <c r="G88" s="5">
         <v>323188</v>
       </c>
-      <c r="H88" s="6"/>
+      <c r="H88" s="5"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>43954.4375</v>
       </c>
-      <c r="B89" s="6">
+      <c r="B89" s="5">
         <v>296731</v>
       </c>
-      <c r="C89" s="6">
+      <c r="C89" s="5">
         <v>9785</v>
       </c>
-      <c r="D89" s="6">
+      <c r="D89" s="5">
         <v>17553</v>
       </c>
-      <c r="E89" s="6">
+      <c r="E89" s="5">
         <v>12005</v>
       </c>
-      <c r="F89" s="6">
+      <c r="F89" s="5">
         <v>1216</v>
       </c>
-      <c r="G89" s="6">
+      <c r="G89" s="5">
         <v>337290</v>
       </c>
-      <c r="H89" s="6"/>
+      <c r="H89" s="5"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>43955.4375</v>
       </c>
-      <c r="B90" s="6">
+      <c r="B90" s="5">
         <v>310332</v>
       </c>
-      <c r="C90" s="6">
+      <c r="C90" s="5">
         <v>6265</v>
       </c>
-      <c r="D90" s="6">
+      <c r="D90" s="5">
         <v>17923</v>
       </c>
-      <c r="E90" s="6">
+      <c r="E90" s="5">
         <v>12505</v>
       </c>
-      <c r="F90" s="6">
+      <c r="F90" s="5">
         <v>1300</v>
       </c>
-      <c r="G90" s="6">
+      <c r="G90" s="5">
         <v>348325</v>
       </c>
-      <c r="H90" s="6"/>
+      <c r="H90" s="5"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>43956.4375</v>
       </c>
-      <c r="B91" s="6">
+      <c r="B91" s="5">
         <v>320264</v>
       </c>
-      <c r="C91" s="6">
+      <c r="C91" s="5">
         <v>6023</v>
       </c>
-      <c r="D91" s="6">
+      <c r="D91" s="5">
         <v>18310</v>
       </c>
-      <c r="E91" s="6">
+      <c r="E91" s="5">
         <v>12779</v>
       </c>
-      <c r="F91" s="6">
+      <c r="F91" s="5">
         <v>1361</v>
       </c>
-      <c r="G91" s="6">
+      <c r="G91" s="5">
         <v>358737</v>
       </c>
     </row>
@@ -3387,22 +3386,22 @@
       <c r="A92" s="1">
         <v>43957.4375</v>
       </c>
-      <c r="B92" s="6">
+      <c r="B92" s="5">
         <v>332302</v>
       </c>
-      <c r="C92" s="6">
+      <c r="C92" s="5">
         <v>8790</v>
       </c>
-      <c r="D92" s="6">
+      <c r="D92" s="5">
         <v>18722</v>
       </c>
-      <c r="E92" s="6">
+      <c r="E92" s="5">
         <v>13222</v>
       </c>
-      <c r="F92" s="6">
+      <c r="F92" s="5">
         <v>1429</v>
       </c>
-      <c r="G92" s="6">
+      <c r="G92" s="5">
         <v>374465</v>
       </c>
     </row>
@@ -3410,22 +3409,22 @@
       <c r="A93" s="1">
         <v>43958.4375</v>
       </c>
-      <c r="B93" s="6">
+      <c r="B93" s="5">
         <v>346687</v>
       </c>
-      <c r="C93" s="6">
+      <c r="C93" s="5">
         <v>13012</v>
       </c>
-      <c r="D93" s="6">
+      <c r="D93" s="5">
         <v>19121</v>
       </c>
-      <c r="E93" s="6">
+      <c r="E93" s="5">
         <v>13569</v>
       </c>
-      <c r="F93" s="6">
+      <c r="F93" s="5">
         <v>1477</v>
       </c>
-      <c r="G93" s="6">
+      <c r="G93" s="5">
         <v>393866</v>
       </c>
     </row>
@@ -3433,22 +3432,22 @@
       <c r="A94" s="1">
         <v>43959.4375</v>
       </c>
-      <c r="B94" s="6">
+      <c r="B94" s="5">
         <v>362021</v>
       </c>
-      <c r="C94" s="6">
+      <c r="C94" s="5">
         <v>14641</v>
       </c>
-      <c r="D94" s="6">
+      <c r="D94" s="5">
         <v>19598</v>
       </c>
-      <c r="E94" s="6">
+      <c r="E94" s="5">
         <v>13990</v>
       </c>
-      <c r="F94" s="6">
+      <c r="F94" s="5">
         <v>1540</v>
       </c>
-      <c r="G94" s="6">
+      <c r="G94" s="5">
         <v>411790</v>
       </c>
     </row>
@@ -3456,22 +3455,22 @@
       <c r="A95" s="1">
         <v>43960.4375</v>
       </c>
-      <c r="B95" s="6">
+      <c r="B95" s="5">
         <v>380450</v>
       </c>
-      <c r="C95" s="6">
+      <c r="C95" s="5">
         <v>15307</v>
       </c>
-      <c r="D95" s="6">
+      <c r="D95" s="5">
         <v>19944</v>
       </c>
-      <c r="E95" s="6">
+      <c r="E95" s="5">
         <v>14383</v>
       </c>
-      <c r="F95" s="6">
+      <c r="F95" s="5">
         <v>1599</v>
       </c>
-      <c r="G95" s="6">
+      <c r="G95" s="5">
         <v>431683</v>
       </c>
     </row>
@@ -3479,22 +3478,22 @@
       <c r="A96" s="1">
         <v>43961.4375</v>
       </c>
-      <c r="B96" s="6">
+      <c r="B96" s="5">
         <v>397350</v>
       </c>
-      <c r="C96" s="6">
+      <c r="C96" s="5">
         <v>14816</v>
       </c>
-      <c r="D96" s="6">
+      <c r="D96" s="5">
         <v>20238</v>
       </c>
-      <c r="E96" s="6">
+      <c r="E96" s="5">
         <v>14772</v>
       </c>
-      <c r="F96" s="6">
+      <c r="F96" s="5">
         <v>1634</v>
       </c>
-      <c r="G96" s="6">
+      <c r="G96" s="5">
         <v>448810</v>
       </c>
     </row>
@@ -3502,22 +3501,22 @@
       <c r="A97" s="1">
         <v>43962.4375</v>
       </c>
-      <c r="B97" s="6">
+      <c r="B97" s="5">
         <v>410618</v>
       </c>
-      <c r="C97" s="6">
+      <c r="C97" s="5">
         <v>9018</v>
       </c>
-      <c r="D97" s="6">
+      <c r="D97" s="5">
         <v>20546</v>
       </c>
-      <c r="E97" s="6">
+      <c r="E97" s="5">
         <v>15131</v>
       </c>
-      <c r="F97" s="6">
+      <c r="F97" s="5">
         <v>1669</v>
       </c>
-      <c r="G97" s="6">
+      <c r="G97" s="5">
         <v>456982</v>
       </c>
     </row>
@@ -3525,22 +3524,22 @@
       <c r="A98" s="1">
         <v>43963.4375</v>
       </c>
-      <c r="B98" s="6">
+      <c r="B98" s="5">
         <v>421898</v>
       </c>
-      <c r="C98" s="6">
+      <c r="C98" s="5">
         <v>10811</v>
       </c>
-      <c r="D98" s="6">
+      <c r="D98" s="5">
         <v>20907</v>
       </c>
-      <c r="E98" s="6">
+      <c r="E98" s="5">
         <v>15391</v>
       </c>
-      <c r="F98" s="6">
+      <c r="F98" s="5">
         <v>1725</v>
       </c>
-      <c r="G98" s="6">
+      <c r="G98" s="5">
         <v>470732</v>
       </c>
     </row>
@@ -3548,22 +3547,22 @@
       <c r="A99" s="1">
         <v>43964.4375</v>
       </c>
-      <c r="B99" s="6">
+      <c r="B99" s="5">
         <v>436212</v>
       </c>
-      <c r="C99" s="6">
+      <c r="C99" s="5">
         <v>13395</v>
       </c>
-      <c r="D99" s="6">
+      <c r="D99" s="5">
         <v>21236</v>
       </c>
-      <c r="E99" s="6">
+      <c r="E99" s="5">
         <v>15845</v>
       </c>
-      <c r="F99" s="6">
+      <c r="F99" s="5">
         <v>1765</v>
       </c>
-      <c r="G99" s="6">
+      <c r="G99" s="5">
         <v>488453</v>
       </c>
     </row>
@@ -3571,22 +3570,22 @@
       <c r="A100" s="1">
         <v>43965.4375</v>
       </c>
-      <c r="B100" s="6">
+      <c r="B100" s="5">
         <v>452991</v>
       </c>
-      <c r="C100" s="6">
+      <c r="C100" s="5">
         <v>17578</v>
       </c>
-      <c r="D100" s="6">
+      <c r="D100" s="5">
         <v>21494</v>
       </c>
-      <c r="E100" s="6">
+      <c r="E100" s="5">
         <v>16204</v>
       </c>
-      <c r="F100" s="6">
+      <c r="F100" s="5">
         <v>1798</v>
       </c>
-      <c r="G100" s="6">
+      <c r="G100" s="5">
         <v>510065</v>
       </c>
     </row>
@@ -3594,37 +3593,47 @@
       <c r="A101" s="1">
         <v>43966.4375</v>
       </c>
-      <c r="B101" s="6">
+      <c r="B101" s="5">
         <v>470453</v>
       </c>
-      <c r="C101" s="6">
+      <c r="C101" s="5">
         <v>14373</v>
       </c>
-      <c r="D101" s="6">
+      <c r="D101" s="5">
         <v>21922</v>
       </c>
-      <c r="E101" s="6">
+      <c r="E101" s="5">
         <v>16641</v>
       </c>
-      <c r="F101" s="6">
+      <c r="F101" s="5">
         <v>1825</v>
       </c>
-      <c r="G101" s="6">
+      <c r="G101" s="5">
         <v>525214</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D102" s="3"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C103" s="3"/>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C104" s="3"/>
-      <c r="D104" s="3"/>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D105" s="3"/>
+      <c r="A102" s="1">
+        <v>43967.4375</v>
+      </c>
+      <c r="B102" s="5">
+        <v>487418</v>
+      </c>
+      <c r="C102" s="5">
+        <v>10565</v>
+      </c>
+      <c r="D102" s="5">
+        <v>22313</v>
+      </c>
+      <c r="E102" s="5">
+        <v>17020</v>
+      </c>
+      <c r="F102" s="5">
+        <v>1858</v>
+      </c>
+      <c r="G102" s="5">
+        <v>539174</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3633,11 +3642,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N58"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I49" sqref="I49"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A47" sqref="A47:K65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3646,7 +3655,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
@@ -3740,9 +3749,9 @@
       <c r="K3">
         <v>140</v>
       </c>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -3778,9 +3787,9 @@
       <c r="K4">
         <v>152</v>
       </c>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -3816,9 +3825,9 @@
       <c r="K5">
         <v>154</v>
       </c>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -3854,9 +3863,9 @@
       <c r="K6">
         <v>160</v>
       </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -3892,9 +3901,9 @@
       <c r="K7">
         <v>187</v>
       </c>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -3930,9 +3939,9 @@
       <c r="K8">
         <v>195</v>
       </c>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -3968,9 +3977,9 @@
       <c r="K9">
         <v>214</v>
       </c>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -4006,9 +4015,9 @@
       <c r="K10">
         <v>217</v>
       </c>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -4044,9 +4053,9 @@
       <c r="K11">
         <v>215</v>
       </c>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -4082,9 +4091,9 @@
       <c r="K12">
         <v>196</v>
       </c>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -4120,9 +4129,9 @@
       <c r="K13">
         <v>203</v>
       </c>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -4158,9 +4167,9 @@
       <c r="K14">
         <v>199</v>
       </c>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -4196,9 +4205,9 @@
       <c r="K15">
         <v>188</v>
       </c>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -4234,982 +4243,982 @@
       <c r="K16">
         <v>200</v>
       </c>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43938.4375</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="5">
         <v>4074</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>5380</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>210</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>2164</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <v>3067</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <v>2214</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <v>1864</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="5">
         <v>829</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J17" s="5">
         <v>245</v>
       </c>
-      <c r="K17" s="6">
+      <c r="K17" s="5">
         <v>200</v>
       </c>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43939.4375</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <v>4277</v>
       </c>
-      <c r="C18" s="6">
+      <c r="C18" s="5">
         <v>5658</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <v>223</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>2269</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <v>3201</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="5">
         <v>2313</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="5">
         <v>1996</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="5">
         <v>828</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J18" s="5">
         <v>250</v>
       </c>
-      <c r="K18" s="6">
+      <c r="K18" s="5">
         <v>197</v>
       </c>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43940.4375</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <v>4495</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <v>5996</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <v>235</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="5">
         <v>2408</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="5">
         <v>3354</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="5">
         <v>2437</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="5">
         <v>2135</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="5">
         <v>809</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="5">
         <v>247</v>
       </c>
-      <c r="K19" s="6">
+      <c r="K19" s="5">
         <v>196</v>
       </c>
-      <c r="L19" s="5"/>
+      <c r="L19" s="4"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43941.4375</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <v>4728</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>6354</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <v>248</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>2525</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="5">
         <v>3502</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="5">
         <v>2580</v>
       </c>
-      <c r="H20" s="6">
+      <c r="H20" s="5">
         <v>2312</v>
       </c>
-      <c r="I20" s="6">
+      <c r="I20" s="5">
         <v>802</v>
       </c>
-      <c r="J20" s="6">
+      <c r="J20" s="5">
         <v>247</v>
       </c>
-      <c r="K20" s="6">
+      <c r="K20" s="5">
         <v>193</v>
       </c>
-      <c r="L20" s="5"/>
+      <c r="L20" s="4"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43942.4375</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <v>4955</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>6663</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <v>260</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="5">
         <v>2657</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="5">
         <v>3665</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="5">
         <v>2687</v>
       </c>
-      <c r="H21" s="6">
+      <c r="H21" s="5">
         <v>2457</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="5">
         <v>859</v>
       </c>
-      <c r="J21" s="6">
+      <c r="J21" s="5">
         <v>250</v>
       </c>
-      <c r="K21" s="6">
+      <c r="K21" s="5">
         <v>194</v>
       </c>
-      <c r="L21" s="5"/>
+      <c r="L21" s="4"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43943.4375</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <v>5169</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>6952</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <v>270</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="5">
         <v>2781</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="5">
         <v>3798</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="5">
         <v>2778</v>
       </c>
-      <c r="H22" s="6">
+      <c r="H22" s="5">
         <v>2609</v>
       </c>
-      <c r="I22" s="6">
+      <c r="I22" s="5">
         <v>878</v>
       </c>
-      <c r="J22" s="6">
+      <c r="J22" s="5">
         <v>243</v>
       </c>
-      <c r="K22" s="6">
+      <c r="K22" s="5">
         <v>192</v>
       </c>
-      <c r="L22" s="5"/>
+      <c r="L22" s="4"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43944.4375</v>
       </c>
-      <c r="B23" s="6">
+      <c r="B23" s="5">
         <v>5408</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="5">
         <v>7342</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <v>284</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="5">
         <v>2914</v>
       </c>
-      <c r="F23" s="6">
+      <c r="F23" s="5">
         <v>3945</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="5">
         <v>2909</v>
       </c>
-      <c r="H23" s="6">
+      <c r="H23" s="5">
         <v>2816</v>
       </c>
-      <c r="I23" s="6">
+      <c r="I23" s="5">
         <v>887</v>
       </c>
-      <c r="J23" s="6">
+      <c r="J23" s="5">
         <v>233</v>
       </c>
-      <c r="K23" s="6">
+      <c r="K23" s="5">
         <v>185</v>
       </c>
-      <c r="L23" s="5"/>
+      <c r="L23" s="4"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43945.4375</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <v>5640</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="5">
         <v>7737</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <v>292</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="5">
         <v>3052</v>
       </c>
-      <c r="F24" s="6">
+      <c r="F24" s="5">
         <v>4108</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="5">
         <v>3029</v>
       </c>
-      <c r="H24" s="6">
+      <c r="H24" s="5">
         <v>3029</v>
       </c>
-      <c r="I24" s="6">
+      <c r="I24" s="5">
         <v>910</v>
       </c>
-      <c r="J24" s="6">
+      <c r="J24" s="5">
         <v>243</v>
       </c>
-      <c r="K24" s="6">
+      <c r="K24" s="5">
         <v>193</v>
       </c>
-      <c r="L24" s="5"/>
+      <c r="L24" s="4"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43946.4375</v>
       </c>
-      <c r="B25" s="6">
+      <c r="B25" s="5">
         <v>5827</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5">
         <v>8030</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <v>309</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="5">
         <v>3179</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="5">
         <v>4276</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="5">
         <v>3108</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="5">
         <v>3114</v>
       </c>
-      <c r="I25" s="6">
+      <c r="I25" s="5">
         <v>925</v>
       </c>
-      <c r="J25" s="6">
+      <c r="J25" s="5">
         <v>245</v>
       </c>
-      <c r="K25" s="6">
+      <c r="K25" s="5">
         <v>195</v>
       </c>
-      <c r="L25" s="5"/>
+      <c r="L25" s="4"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43947.4375</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="5">
         <v>6005</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="5">
         <v>8290</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="5">
         <v>320</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="5">
         <v>3292</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="5">
         <v>4391</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="5">
         <v>3207</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H26" s="5">
         <v>3213</v>
       </c>
-      <c r="I26" s="6">
+      <c r="I26" s="5">
         <v>938</v>
       </c>
-      <c r="J26" s="6">
+      <c r="J26" s="5">
         <v>252</v>
       </c>
-      <c r="K26" s="6">
+      <c r="K26" s="5">
         <v>195</v>
       </c>
-      <c r="L26" s="5"/>
+      <c r="L26" s="4"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43948.4375</v>
       </c>
-      <c r="B27" s="6">
+      <c r="B27" s="5">
         <v>6168</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="5">
         <v>8548</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <v>326</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="5">
         <v>3398</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="5">
         <v>4504</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="5">
         <v>3302</v>
       </c>
-      <c r="H27" s="6">
+      <c r="H27" s="5">
         <v>3318</v>
       </c>
-      <c r="I27" s="6">
+      <c r="I27" s="5">
         <v>945</v>
       </c>
-      <c r="J27" s="6">
+      <c r="J27" s="5">
         <v>241</v>
       </c>
-      <c r="K27" s="6">
+      <c r="K27" s="5">
         <v>191</v>
       </c>
-      <c r="L27" s="5"/>
+      <c r="L27" s="4"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43949.4375</v>
       </c>
-      <c r="B28" s="6">
+      <c r="B28" s="5">
         <v>6392</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="5">
         <v>8848</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="5">
         <v>346</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="5">
         <v>3521</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F28" s="5">
         <v>4644</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G28" s="5">
         <v>3420</v>
       </c>
-      <c r="H28" s="6">
+      <c r="H28" s="5">
         <v>3443</v>
       </c>
-      <c r="I28" s="6">
+      <c r="I28" s="5">
         <v>957</v>
       </c>
-      <c r="J28" s="6">
+      <c r="J28" s="5">
         <v>239</v>
       </c>
-      <c r="K28" s="6">
+      <c r="K28" s="5">
         <v>187</v>
       </c>
-      <c r="L28" s="5"/>
+      <c r="L28" s="4"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43950.4375</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="5">
         <v>6546</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="5">
         <v>9041</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="5">
         <v>363</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="5">
         <v>3583</v>
       </c>
-      <c r="F29" s="6">
+      <c r="F29" s="5">
         <v>4725</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="5">
         <v>3486</v>
       </c>
-      <c r="H29" s="6">
+      <c r="H29" s="5">
         <v>3564</v>
       </c>
-      <c r="I29" s="6">
+      <c r="I29" s="5">
         <v>977</v>
       </c>
-      <c r="J29" s="6">
+      <c r="J29" s="5">
         <v>235</v>
       </c>
-      <c r="K29" s="6">
+      <c r="K29" s="5">
         <v>186</v>
       </c>
-      <c r="L29" s="5"/>
+      <c r="L29" s="4"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43951.4375</v>
       </c>
-      <c r="B30" s="6">
+      <c r="B30" s="5">
         <v>6754</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="5">
         <v>9280</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="5">
         <v>371</v>
       </c>
-      <c r="E30" s="6">
+      <c r="E30" s="5">
         <v>3693</v>
       </c>
-      <c r="F30" s="6">
+      <c r="F30" s="5">
         <v>4871</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G30" s="5">
         <v>3581</v>
       </c>
-      <c r="H30" s="6">
+      <c r="H30" s="5">
         <v>3664</v>
       </c>
-      <c r="I30" s="6">
+      <c r="I30" s="5">
         <v>999</v>
       </c>
-      <c r="J30" s="6">
+      <c r="J30" s="5">
         <v>233</v>
       </c>
-      <c r="K30" s="6">
+      <c r="K30" s="5">
         <v>181</v>
       </c>
-      <c r="L30" s="5"/>
+      <c r="L30" s="4"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>43952.4375</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="5">
         <v>6917</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="5">
         <v>9538</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <v>384</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="5">
         <v>3786</v>
       </c>
-      <c r="F31" s="6">
+      <c r="F31" s="5">
         <v>5004</v>
       </c>
-      <c r="G31" s="6">
+      <c r="G31" s="5">
         <v>3673</v>
       </c>
-      <c r="H31" s="6">
+      <c r="H31" s="5">
         <v>3753</v>
       </c>
-      <c r="I31" s="6">
+      <c r="I31" s="5">
         <v>1017</v>
       </c>
-      <c r="J31" s="6">
+      <c r="J31" s="5">
         <v>225</v>
       </c>
-      <c r="K31" s="6">
+      <c r="K31" s="5">
         <v>175</v>
       </c>
-      <c r="L31" s="5"/>
+      <c r="L31" s="4"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>43953.4375</v>
       </c>
-      <c r="B32" s="6">
+      <c r="B32" s="5">
         <v>7113</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="5">
         <v>9845</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="5">
         <v>405</v>
       </c>
-      <c r="E32" s="6">
+      <c r="E32" s="5">
         <v>3918</v>
       </c>
-      <c r="F32" s="6">
+      <c r="F32" s="5">
         <v>5169</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G32" s="5">
         <v>3776</v>
       </c>
-      <c r="H32" s="6">
+      <c r="H32" s="5">
         <v>3842</v>
       </c>
-      <c r="I32" s="6">
+      <c r="I32" s="5">
         <v>977</v>
       </c>
-      <c r="J32" s="6">
+      <c r="J32" s="5">
         <v>221</v>
       </c>
-      <c r="K32" s="6">
+      <c r="K32" s="5">
         <v>154</v>
       </c>
-      <c r="L32" s="5"/>
+      <c r="L32" s="4"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43954.4375</v>
       </c>
-      <c r="B33" s="6">
+      <c r="B33" s="5">
         <v>7284</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="5">
         <v>10112</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="5">
         <v>416</v>
       </c>
-      <c r="E33" s="6">
+      <c r="E33" s="5">
         <v>4041</v>
       </c>
-      <c r="F33" s="6">
+      <c r="F33" s="5">
         <v>5290</v>
       </c>
-      <c r="G33" s="6">
+      <c r="G33" s="5">
         <v>3865</v>
       </c>
-      <c r="H33" s="6">
+      <c r="H33" s="5">
         <v>3932</v>
       </c>
-      <c r="I33" s="6">
+      <c r="I33" s="5">
         <v>1010</v>
       </c>
-      <c r="J33" s="6">
+      <c r="J33" s="5">
         <v>232</v>
       </c>
-      <c r="K33" s="6">
+      <c r="K33" s="5">
         <v>174</v>
       </c>
-      <c r="L33" s="5"/>
+      <c r="L33" s="4"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43955.4375</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="5">
         <v>7453</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="5">
         <v>10312</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="5">
         <v>431</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="5">
         <v>4156</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34" s="5">
         <v>5403</v>
       </c>
-      <c r="G34" s="6">
+      <c r="G34" s="5">
         <v>3939</v>
       </c>
-      <c r="H34" s="6">
+      <c r="H34" s="5">
         <v>3984</v>
       </c>
-      <c r="I34" s="6">
+      <c r="I34" s="5">
         <v>984</v>
       </c>
-      <c r="J34" s="6">
+      <c r="J34" s="5">
         <v>225</v>
       </c>
-      <c r="K34" s="6">
+      <c r="K34" s="5">
         <v>175</v>
       </c>
-      <c r="L34" s="5"/>
+      <c r="L34" s="4"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>43956.4375</v>
       </c>
-      <c r="B35" s="6">
+      <c r="B35" s="5">
         <v>7629</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="5">
         <v>10521</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="5">
         <v>451</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E35" s="5">
         <v>4257</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F35" s="5">
         <v>5528</v>
       </c>
-      <c r="G35" s="6">
+      <c r="G35" s="5">
         <v>4012</v>
       </c>
-      <c r="H35" s="6">
+      <c r="H35" s="5">
         <v>4051</v>
       </c>
-      <c r="I35" s="6">
+      <c r="I35" s="5">
         <v>1043</v>
       </c>
-      <c r="J35" s="6">
+      <c r="J35" s="5">
         <v>223</v>
       </c>
-      <c r="K35" s="6">
+      <c r="K35" s="5">
         <v>166</v>
       </c>
-      <c r="L35" s="5"/>
+      <c r="L35" s="4"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>43957.4375</v>
       </c>
-      <c r="B36" s="6">
+      <c r="B36" s="5">
         <v>7824</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="5">
         <v>10732</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="5">
         <v>473</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="5">
         <v>4379</v>
       </c>
-      <c r="F36" s="6">
+      <c r="F36" s="5">
         <v>5652</v>
       </c>
-      <c r="G36" s="6">
+      <c r="G36" s="5">
         <v>4089</v>
       </c>
-      <c r="H36" s="6">
+      <c r="H36" s="5">
         <v>4116</v>
       </c>
-      <c r="I36" s="6">
+      <c r="I36" s="5">
         <v>1032</v>
       </c>
-      <c r="J36" s="6">
+      <c r="J36" s="5">
         <v>219</v>
       </c>
-      <c r="K36" s="6">
+      <c r="K36" s="5">
         <v>174</v>
       </c>
-      <c r="L36" s="5"/>
+      <c r="L36" s="4"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>43958.4375</v>
       </c>
-      <c r="B37" s="6">
+      <c r="B37" s="5">
         <v>8004</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37" s="5">
         <v>10954</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="5">
         <v>485</v>
       </c>
-      <c r="E37" s="6">
+      <c r="E37" s="5">
         <v>4478</v>
       </c>
-      <c r="F37" s="6">
+      <c r="F37" s="5">
         <v>5788</v>
       </c>
-      <c r="G37" s="6">
+      <c r="G37" s="5">
         <v>4176</v>
       </c>
-      <c r="H37" s="6">
+      <c r="H37" s="5">
         <v>4182</v>
       </c>
-      <c r="I37" s="6">
+      <c r="I37" s="5">
         <v>1033</v>
       </c>
-      <c r="J37" s="6">
+      <c r="J37" s="5">
         <v>220</v>
       </c>
-      <c r="K37" s="6">
+      <c r="K37" s="5">
         <v>155</v>
       </c>
-      <c r="L37" s="5"/>
+      <c r="L37" s="4"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>43959.4375</v>
       </c>
-      <c r="B38" s="6">
+      <c r="B38" s="5">
         <v>8213</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C38" s="5">
         <v>11222</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="5">
         <v>504</v>
       </c>
-      <c r="E38" s="6">
+      <c r="E38" s="5">
         <v>4602</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F38" s="5">
         <v>5972</v>
       </c>
-      <c r="G38" s="6">
+      <c r="G38" s="5">
         <v>4254</v>
       </c>
-      <c r="H38" s="6">
+      <c r="H38" s="5">
         <v>4254</v>
       </c>
-      <c r="I38" s="6">
+      <c r="I38" s="5">
         <v>1028</v>
       </c>
-      <c r="J38" s="6">
+      <c r="J38" s="5">
         <v>213</v>
       </c>
-      <c r="K38" s="6">
+      <c r="K38" s="5">
         <v>166</v>
       </c>
-      <c r="L38" s="5"/>
+      <c r="L38" s="4"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>43960.4375</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="5">
         <v>8382</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="5">
         <v>11407</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="5">
         <v>516</v>
       </c>
-      <c r="E39" s="6">
+      <c r="E39" s="5">
         <v>4692</v>
       </c>
-      <c r="F39" s="6">
+      <c r="F39" s="5">
         <v>6079</v>
       </c>
-      <c r="G39" s="6">
+      <c r="G39" s="5">
         <v>4310</v>
       </c>
-      <c r="H39" s="6">
+      <c r="H39" s="5">
         <v>4333</v>
       </c>
-      <c r="I39" s="6">
+      <c r="I39" s="5">
         <v>1016</v>
       </c>
-      <c r="J39" s="6">
+      <c r="J39" s="5">
         <v>203</v>
       </c>
-      <c r="K39" s="6">
+      <c r="K39" s="5">
         <v>158</v>
       </c>
-      <c r="L39" s="5"/>
+      <c r="L39" s="4"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>43961.4375</v>
       </c>
-      <c r="B40" s="6">
+      <c r="B40" s="5">
         <v>8494</v>
       </c>
-      <c r="C40" s="6">
+      <c r="C40" s="5">
         <v>11582</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="5">
         <v>524</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E40" s="5">
         <v>4762</v>
       </c>
-      <c r="F40" s="6">
+      <c r="F40" s="5">
         <v>6187</v>
       </c>
-      <c r="G40" s="6">
+      <c r="G40" s="5">
         <v>4364</v>
       </c>
-      <c r="H40" s="6">
+      <c r="H40" s="5">
         <v>4390</v>
       </c>
-      <c r="I40" s="6">
+      <c r="I40" s="5">
         <v>961</v>
       </c>
-      <c r="J40" s="6">
+      <c r="J40" s="5">
         <v>195</v>
       </c>
-      <c r="K40" s="6">
+      <c r="K40" s="5">
         <v>140</v>
       </c>
-      <c r="L40" s="5"/>
+      <c r="L40" s="4"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>43962.4375</v>
       </c>
-      <c r="B41" s="6">
+      <c r="B41" s="5">
         <v>8615</v>
       </c>
-      <c r="C41" s="6">
+      <c r="C41" s="5">
         <v>11768</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41" s="5">
         <v>538</v>
       </c>
-      <c r="E41" s="6">
+      <c r="E41" s="5">
         <v>4857</v>
       </c>
-      <c r="F41" s="6">
+      <c r="F41" s="5">
         <v>6287</v>
       </c>
-      <c r="G41" s="6">
+      <c r="G41" s="5">
         <v>4411</v>
       </c>
-      <c r="H41" s="6">
+      <c r="H41" s="5">
         <v>4439</v>
       </c>
-      <c r="I41" s="6">
+      <c r="I41" s="5">
         <v>1027</v>
       </c>
-      <c r="J41" s="6">
+      <c r="J41" s="5">
         <v>194</v>
       </c>
-      <c r="K41" s="6">
+      <c r="K41" s="5">
         <v>147</v>
       </c>
-      <c r="L41" s="5"/>
+      <c r="L41" s="4"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>43963.4375</v>
       </c>
-      <c r="B42" s="6">
+      <c r="B42" s="5">
         <v>8776</v>
       </c>
-      <c r="C42" s="6">
+      <c r="C42" s="5">
         <v>11971</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42" s="5">
         <v>552</v>
       </c>
-      <c r="E42" s="6">
+      <c r="E42" s="5">
         <v>4952</v>
       </c>
-      <c r="F42" s="6">
+      <c r="F42" s="5">
         <v>6392</v>
       </c>
-      <c r="G42" s="6">
+      <c r="G42" s="5">
         <v>4489</v>
       </c>
-      <c r="H42" s="6">
+      <c r="H42" s="5">
         <v>4508</v>
       </c>
-      <c r="I42" s="6">
+      <c r="I42" s="5">
         <v>1025</v>
       </c>
-      <c r="J42" s="6">
+      <c r="J42" s="5">
         <v>192</v>
       </c>
-      <c r="K42" s="6">
+      <c r="K42" s="5">
         <v>146</v>
       </c>
-      <c r="L42" s="5"/>
+      <c r="L42" s="4"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>43964.4375</v>
       </c>
-      <c r="B43" s="6">
+      <c r="B43" s="5">
         <v>8923</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C43" s="5">
         <v>12155</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="5">
         <v>571</v>
       </c>
-      <c r="E43" s="6">
+      <c r="E43" s="5">
         <v>5045</v>
       </c>
-      <c r="F43" s="6">
+      <c r="F43" s="5">
         <v>6481</v>
       </c>
-      <c r="G43" s="6">
+      <c r="G43" s="5">
         <v>4544</v>
       </c>
-      <c r="H43" s="6">
+      <c r="H43" s="5">
         <v>4581</v>
       </c>
-      <c r="I43" s="6">
+      <c r="I43" s="5">
         <v>1018</v>
       </c>
-      <c r="J43" s="6">
+      <c r="J43" s="5">
         <v>189</v>
       </c>
-      <c r="K43" s="6">
+      <c r="K43" s="5">
         <v>144</v>
       </c>
     </row>
@@ -5217,34 +5226,34 @@
       <c r="A44" s="1">
         <v>43965.4375</v>
       </c>
-      <c r="B44" s="6">
+      <c r="B44" s="5">
         <v>9037</v>
       </c>
-      <c r="C44" s="6">
+      <c r="C44" s="5">
         <v>12297</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="5">
         <v>592</v>
       </c>
-      <c r="E44" s="6">
+      <c r="E44" s="5">
         <v>5118</v>
       </c>
-      <c r="F44" s="6">
+      <c r="F44" s="5">
         <v>6548</v>
       </c>
-      <c r="G44" s="6">
+      <c r="G44" s="5">
         <v>4589</v>
       </c>
-      <c r="H44" s="6">
+      <c r="H44" s="5">
         <v>4632</v>
       </c>
-      <c r="I44" s="6">
+      <c r="I44" s="5">
         <v>1026</v>
       </c>
-      <c r="J44" s="6">
+      <c r="J44" s="5">
         <v>184</v>
       </c>
-      <c r="K44" s="6">
+      <c r="K44" s="5">
         <v>141</v>
       </c>
     </row>
@@ -5252,75 +5261,71 @@
       <c r="A45" s="1">
         <v>43966.4375</v>
       </c>
-      <c r="B45" s="6">
+      <c r="B45" s="5">
         <v>9225</v>
       </c>
-      <c r="C45" s="6">
+      <c r="C45" s="5">
         <v>12533</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="5">
         <v>601</v>
       </c>
-      <c r="E45" s="6">
+      <c r="E45" s="5">
         <v>5251</v>
       </c>
-      <c r="F45" s="6">
+      <c r="F45" s="5">
         <v>6693</v>
       </c>
-      <c r="G45" s="6">
+      <c r="G45" s="5">
         <v>4659</v>
       </c>
-      <c r="H45" s="6">
+      <c r="H45" s="5">
         <v>4702</v>
       </c>
-      <c r="I45" s="6">
+      <c r="I45" s="5">
         <v>986</v>
       </c>
-      <c r="J45" s="6">
+      <c r="J45" s="5">
         <v>179</v>
       </c>
-      <c r="K45" s="6">
+      <c r="K45" s="5">
         <v>135</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C46" s="3"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D47" s="3"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D48" s="3"/>
-    </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D50" s="3"/>
-    </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D51" s="3"/>
-    </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D52" s="3"/>
-    </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D53" s="3"/>
-    </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="E54" s="3"/>
-    </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-    </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="F56" s="3"/>
-    </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D57" s="3"/>
-    </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C58" s="3"/>
+      <c r="A46" s="1">
+        <v>43967.4375</v>
+      </c>
+      <c r="B46" s="5">
+        <v>9406</v>
+      </c>
+      <c r="C46" s="5">
+        <v>12738</v>
+      </c>
+      <c r="D46" s="5">
+        <v>621</v>
+      </c>
+      <c r="E46" s="5">
+        <v>5365</v>
+      </c>
+      <c r="F46" s="5">
+        <v>6825</v>
+      </c>
+      <c r="G46" s="5">
+        <v>4732</v>
+      </c>
+      <c r="H46" s="5">
+        <v>4757</v>
+      </c>
+      <c r="I46" s="5">
+        <v>975</v>
+      </c>
+      <c r="J46" s="5">
+        <v>180</v>
+      </c>
+      <c r="K46" s="5">
+        <v>135</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-17 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060847E1-3F1D-F74A-A89F-AAC9D14ABAD6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801887AF-1451-AB4B-ACF2-A91026A72E1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -446,13 +446,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1151,11 +1152,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I102"/>
+  <dimension ref="A1:I106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E159" sqref="E159"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C107" sqref="C107:F127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3635,6 +3636,35 @@
         <v>539174</v>
       </c>
     </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>43968.4375</v>
+      </c>
+      <c r="B103" s="5">
+        <v>502932</v>
+      </c>
+      <c r="C103" s="5">
+        <v>4414</v>
+      </c>
+      <c r="D103" s="5">
+        <v>22653</v>
+      </c>
+      <c r="E103" s="5">
+        <v>17360</v>
+      </c>
+      <c r="F103" s="5">
+        <v>1881</v>
+      </c>
+      <c r="G103" s="5">
+        <v>549240</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D104" s="6"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D106" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3642,11 +3672,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A47" sqref="A47:K65"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5325,6 +5355,41 @@
       </c>
       <c r="K46" s="5">
         <v>135</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>43968.4375</v>
+      </c>
+      <c r="B47" s="5">
+        <v>9560</v>
+      </c>
+      <c r="C47" s="5">
+        <v>12925</v>
+      </c>
+      <c r="D47" s="5">
+        <v>632</v>
+      </c>
+      <c r="E47" s="5">
+        <v>5451</v>
+      </c>
+      <c r="F47" s="5">
+        <v>6926</v>
+      </c>
+      <c r="G47" s="5">
+        <v>4802</v>
+      </c>
+      <c r="H47" s="5">
+        <v>4830</v>
+      </c>
+      <c r="I47" s="5">
+        <v>934</v>
+      </c>
+      <c r="J47" s="5">
+        <v>171</v>
+      </c>
+      <c r="K47" s="5">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel update 2020-05-18 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801887AF-1451-AB4B-ACF2-A91026A72E1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBA8EED-446F-AD4B-8ED4-E844B2C461F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -1152,11 +1152,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I106"/>
+  <dimension ref="A1:I104"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C107" sqref="C107:F127"/>
+      <selection pane="bottomLeft" activeCell="C105" sqref="C105:F127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3660,10 +3660,27 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D104" s="6"/>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D106" s="6"/>
+      <c r="A104" s="1">
+        <v>43969.4375</v>
+      </c>
+      <c r="B104" s="5">
+        <v>511482</v>
+      </c>
+      <c r="C104" s="5">
+        <v>2189</v>
+      </c>
+      <c r="D104" s="5">
+        <v>22957</v>
+      </c>
+      <c r="E104" s="5">
+        <v>17638</v>
+      </c>
+      <c r="F104" s="5">
+        <v>1904</v>
+      </c>
+      <c r="G104" s="5">
+        <v>563136</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3672,11 +3689,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N47"/>
+  <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5391,6 +5408,88 @@
       <c r="K47" s="5">
         <v>129</v>
       </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>43969.4375</v>
+      </c>
+      <c r="B48" s="5">
+        <v>9721</v>
+      </c>
+      <c r="C48" s="5">
+        <v>13066</v>
+      </c>
+      <c r="D48" s="5">
+        <v>644</v>
+      </c>
+      <c r="E48" s="5">
+        <v>5567</v>
+      </c>
+      <c r="F48" s="5">
+        <v>7020</v>
+      </c>
+      <c r="G48" s="5">
+        <v>4842</v>
+      </c>
+      <c r="H48" s="5">
+        <v>4869</v>
+      </c>
+      <c r="I48" s="5">
+        <v>972</v>
+      </c>
+      <c r="J48" s="5">
+        <v>174</v>
+      </c>
+      <c r="K48" s="5">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="49" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+      <c r="K49" s="5"/>
+    </row>
+    <row r="50" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+    </row>
+    <row r="51" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D51" s="6"/>
+    </row>
+    <row r="53" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D53" s="6"/>
+    </row>
+    <row r="54" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D54" s="6"/>
+    </row>
+    <row r="56" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D56" s="6"/>
+    </row>
+    <row r="57" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D57" s="6"/>
+    </row>
+    <row r="59" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D59" s="6"/>
+    </row>
+    <row r="60" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D60" s="6"/>
+    </row>
+    <row r="61" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D61" s="6"/>
+    </row>
+    <row r="62" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D62" s="6"/>
+    </row>
+    <row r="64" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D64" s="6"/>
+    </row>
+    <row r="65" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D65" s="6"/>
+      <c r="F65" s="6"/>
+    </row>
+    <row r="66" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D66" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-19 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBA8EED-446F-AD4B-8ED4-E844B2C461F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BE0B87-2E42-3B44-B116-C762E2682175}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -402,7 +402,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -420,6 +420,27 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF222222"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF222222"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -442,11 +463,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -454,8 +476,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -839,6 +865,57 @@
             <a:rPr lang="en-CA" sz="1400" b="0" baseline="0"/>
             <a:t>	- Total number of patients approved for COVID-19 testing to date = Total Tested + Currently under investigation</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" baseline="0"/>
+            <a:t>- </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1400" b="1"/>
+            <a:t>Schema change in data as of 2020/05/19</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-CA" sz="1400" b="1" baseline="0"/>
+            <a:t> added sub-fields for LTC into main report</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
           <a:endParaRPr lang="en-US" sz="1400" baseline="0"/>
         </a:p>
         <a:p>
@@ -1152,11 +1229,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I104"/>
+  <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C105" sqref="C105:F127"/>
+      <selection pane="bottomLeft" activeCell="G112" sqref="G112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3682,6 +3759,89 @@
         <v>563136</v>
       </c>
     </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <v>43970.4375</v>
+      </c>
+      <c r="B105" s="5">
+        <v>516593</v>
+      </c>
+      <c r="C105" s="5">
+        <v>2294</v>
+      </c>
+      <c r="D105" s="5">
+        <v>23384</v>
+      </c>
+      <c r="E105" s="5">
+        <v>17898</v>
+      </c>
+      <c r="F105" s="5">
+        <v>1919</v>
+      </c>
+      <c r="G105" s="5">
+        <v>562088</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+      <c r="E106" s="5"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+      <c r="E107" s="5"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C108" s="5"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="5"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C109" s="5"/>
+      <c r="D109" s="5"/>
+      <c r="E109" s="5"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C110" s="5"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="5"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C111" s="5"/>
+      <c r="D111" s="5"/>
+      <c r="E111" s="5"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C112" s="5"/>
+      <c r="D112" s="6"/>
+      <c r="E112" s="5"/>
+    </row>
+    <row r="113" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C113" s="5"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="5"/>
+    </row>
+    <row r="114" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C114" s="5"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="5"/>
+    </row>
+    <row r="115" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C115" s="5"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="5"/>
+    </row>
+    <row r="116" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C116" s="5"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="5"/>
+    </row>
+    <row r="117" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C117" s="5"/>
+      <c r="D117" s="5"/>
+      <c r="E117" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3691,9 +3851,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J51" sqref="J51"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5444,44 +5604,112 @@
         <v>133</v>
       </c>
     </row>
-    <row r="49" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-    </row>
-    <row r="50" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>43970.4375</v>
+      </c>
+      <c r="B49" s="5">
+        <v>9919</v>
+      </c>
+      <c r="C49" s="5">
+        <v>13294</v>
+      </c>
+      <c r="D49" s="5">
+        <v>668</v>
+      </c>
+      <c r="E49" s="5">
+        <v>5707</v>
+      </c>
+      <c r="F49" s="5">
+        <v>7155</v>
+      </c>
+      <c r="G49" s="5">
+        <v>4923</v>
+      </c>
+      <c r="H49" s="5">
+        <v>4916</v>
+      </c>
+      <c r="I49" s="5">
+        <v>987</v>
+      </c>
+      <c r="J49" s="5">
+        <v>167</v>
+      </c>
+      <c r="K49" s="5">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
     </row>
-    <row r="51" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D51" s="6"/>
-    </row>
-    <row r="53" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D53" s="6"/>
-    </row>
-    <row r="54" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D54" s="6"/>
-    </row>
-    <row r="56" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D56" s="6"/>
-    </row>
-    <row r="57" spans="4:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C52" s="5"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="5"/>
+    </row>
+    <row r="53" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="C53" s="5"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7"/>
+    </row>
+    <row r="54" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="C54" s="5"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+    </row>
+    <row r="55" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="C55" s="5"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+    </row>
+    <row r="56" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="C56" s="5"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C57" s="5"/>
       <c r="D57" s="6"/>
-    </row>
-    <row r="59" spans="4:11" x14ac:dyDescent="0.2">
-      <c r="D59" s="6"/>
-    </row>
-    <row r="60" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="E57" s="5"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C58" s="5"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="5"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C60" s="5"/>
       <c r="D60" s="6"/>
-    </row>
-    <row r="61" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="E60" s="5"/>
+      <c r="F60" s="6"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C61" s="5"/>
       <c r="D61" s="6"/>
-    </row>
-    <row r="62" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="E61" s="5"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C62" s="5"/>
       <c r="D62" s="6"/>
-    </row>
-    <row r="64" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="E62" s="5"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D64" s="6"/>
     </row>
     <row r="65" spans="4:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
excel update 2020-05-20 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BE0B87-2E42-3B44-B116-C762E2682175}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3C2F3C-E2FA-C648-96A4-64786ED85913}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="35320" yWindow="460" windowWidth="33600" windowHeight="20000" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -402,7 +402,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -420,27 +420,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF222222"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FF222222"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -463,12 +442,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -476,12 +454,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1229,11 +1203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I117"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G112" sqref="G112"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C109" sqref="C109:G131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3783,64 +3757,37 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C106" s="5"/>
-      <c r="D106" s="5"/>
-      <c r="E106" s="5"/>
+      <c r="A106" s="1">
+        <v>43971.4375</v>
+      </c>
+      <c r="B106" s="5">
+        <v>523250</v>
+      </c>
+      <c r="C106" s="5">
+        <v>4444</v>
+      </c>
+      <c r="D106" s="5">
+        <v>23774</v>
+      </c>
+      <c r="E106" s="5">
+        <v>18190</v>
+      </c>
+      <c r="F106" s="5">
+        <v>1962</v>
+      </c>
+      <c r="G106" s="5">
+        <v>571620</v>
+      </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C107" s="5"/>
-      <c r="D107" s="5"/>
+      <c r="D107" s="6"/>
       <c r="E107" s="5"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C108" s="5"/>
       <c r="D108" s="6"/>
       <c r="E108" s="5"/>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C109" s="5"/>
-      <c r="D109" s="5"/>
-      <c r="E109" s="5"/>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C110" s="5"/>
-      <c r="D110" s="6"/>
-      <c r="E110" s="5"/>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C111" s="5"/>
-      <c r="D111" s="5"/>
-      <c r="E111" s="5"/>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C112" s="5"/>
-      <c r="D112" s="6"/>
-      <c r="E112" s="5"/>
-    </row>
-    <row r="113" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C113" s="5"/>
-      <c r="D113" s="5"/>
-      <c r="E113" s="5"/>
-    </row>
-    <row r="114" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C114" s="5"/>
-      <c r="D114" s="6"/>
-      <c r="E114" s="5"/>
-    </row>
-    <row r="115" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C115" s="5"/>
-      <c r="D115" s="6"/>
-      <c r="E115" s="5"/>
-    </row>
-    <row r="116" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C116" s="5"/>
-      <c r="D116" s="6"/>
-      <c r="E116" s="5"/>
-    </row>
-    <row r="117" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C117" s="5"/>
-      <c r="D117" s="5"/>
-      <c r="E117" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3849,11 +3796,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N66"/>
+  <dimension ref="A1:N68"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
+      <selection pane="bottomLeft" activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5640,84 +5587,106 @@
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-      <c r="K50" s="5"/>
+      <c r="A50" s="1">
+        <v>43971.4375</v>
+      </c>
+      <c r="B50" s="5">
+        <v>10095</v>
+      </c>
+      <c r="C50" s="5">
+        <v>13507</v>
+      </c>
+      <c r="D50" s="5">
+        <v>686</v>
+      </c>
+      <c r="E50" s="5">
+        <v>5840</v>
+      </c>
+      <c r="F50" s="5">
+        <v>7258</v>
+      </c>
+      <c r="G50" s="5">
+        <v>4997</v>
+      </c>
+      <c r="H50" s="5">
+        <v>4981</v>
+      </c>
+      <c r="I50" s="5">
+        <v>991</v>
+      </c>
+      <c r="J50" s="5">
+        <v>160</v>
+      </c>
+      <c r="K50" s="5">
+        <v>120</v>
+      </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C51" s="5"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="6"/>
       <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C52" s="5"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="5"/>
-    </row>
-    <row r="53" spans="1:11" ht="20" x14ac:dyDescent="0.2">
+      <c r="B52" s="5"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="5"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B53" s="5"/>
       <c r="C53" s="5"/>
-      <c r="D53" s="9"/>
-      <c r="E53" s="7"/>
-      <c r="F53" s="7"/>
-    </row>
-    <row r="54" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="C54" s="5"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="7"/>
-      <c r="F54" s="7"/>
-    </row>
-    <row r="55" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="C55" s="5"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-    </row>
-    <row r="56" spans="1:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="C56" s="5"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="7"/>
-      <c r="F56" s="7"/>
+      <c r="D53" s="5"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B54" s="5"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="5"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B55" s="5"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B56" s="5"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="5"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C57" s="5"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="5"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="5"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C58" s="5"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="5"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="5"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C59" s="5"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="6"/>
       <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C60" s="5"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="6"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C61" s="5"/>
-      <c r="D61" s="6"/>
-      <c r="E61" s="5"/>
+      <c r="C61" s="6"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C62" s="5"/>
-      <c r="D62" s="6"/>
-      <c r="E62" s="5"/>
+      <c r="C62" s="6"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C63" s="6"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D64" s="6"/>
-    </row>
-    <row r="65" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D65" s="6"/>
-      <c r="F65" s="6"/>
-    </row>
-    <row r="66" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D66" s="6"/>
+      <c r="C64" s="6"/>
+    </row>
+    <row r="66" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C66" s="6"/>
+      <c r="E66" s="6"/>
+    </row>
+    <row r="67" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C67" s="6"/>
+    </row>
+    <row r="68" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C68" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-21 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F3C2F3C-E2FA-C648-96A4-64786ED85913}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E186DD-61E7-634C-9147-1955589B4BD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35320" yWindow="460" windowWidth="33600" windowHeight="20000" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="35320" yWindow="460" windowWidth="33600" windowHeight="20000" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -1203,11 +1203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I108"/>
+  <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C109" sqref="C109:G131"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3780,14 +3780,27 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C107" s="5"/>
-      <c r="D107" s="6"/>
-      <c r="E107" s="5"/>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C108" s="5"/>
-      <c r="D108" s="6"/>
-      <c r="E108" s="5"/>
+      <c r="A107" s="1">
+        <v>43972.4375</v>
+      </c>
+      <c r="B107" s="5">
+        <v>532993</v>
+      </c>
+      <c r="C107" s="5">
+        <v>5051</v>
+      </c>
+      <c r="D107" s="5">
+        <v>24187</v>
+      </c>
+      <c r="E107" s="5">
+        <v>18509</v>
+      </c>
+      <c r="F107" s="5">
+        <v>1993</v>
+      </c>
+      <c r="G107" s="5">
+        <v>582733</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3796,11 +3809,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N68"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E59" sqref="E59"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5622,71 +5635,72 @@
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B51" s="5"/>
-      <c r="C51" s="6"/>
-      <c r="D51" s="5"/>
+      <c r="A51" s="1">
+        <v>43972.4375</v>
+      </c>
+      <c r="B51" s="5">
+        <v>10279</v>
+      </c>
+      <c r="C51" s="5">
+        <v>13735</v>
+      </c>
+      <c r="D51" s="5">
+        <v>713</v>
+      </c>
+      <c r="E51" s="5">
+        <v>5951</v>
+      </c>
+      <c r="F51" s="5">
+        <v>7355</v>
+      </c>
+      <c r="G51" s="5">
+        <v>5075</v>
+      </c>
+      <c r="H51" s="5">
+        <v>5080</v>
+      </c>
+      <c r="I51" s="5">
+        <v>984</v>
+      </c>
+      <c r="J51" s="5">
+        <v>155</v>
+      </c>
+      <c r="K51" s="5">
+        <v>117</v>
+      </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B52" s="5"/>
-      <c r="C52" s="6"/>
-      <c r="D52" s="5"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="5"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B54" s="5"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="5"/>
+      <c r="D54" s="6"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B55" s="5"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="5"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B56" s="5"/>
-      <c r="C56" s="6"/>
-      <c r="D56" s="5"/>
+      <c r="D55" s="6"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B57" s="5"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="5"/>
+      <c r="D57" s="6"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B58" s="5"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="5"/>
+      <c r="D58" s="6"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B59" s="5"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="5"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C61" s="6"/>
+      <c r="D59" s="6"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D60" s="6"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="F63" s="6"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C64" s="6"/>
-    </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C66" s="6"/>
-      <c r="E66" s="6"/>
-    </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C67" s="6"/>
-    </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C68" s="6"/>
+      <c r="D64" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-22 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E186DD-61E7-634C-9147-1955589B4BD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5581CDE2-43AA-4248-8243-E5B5A2378B09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35320" yWindow="460" windowWidth="33600" windowHeight="20000" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="35320" yWindow="460" windowWidth="33600" windowHeight="20000" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -1203,11 +1203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I107"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C113" sqref="C113"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A109" sqref="A109:G134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3802,6 +3802,29 @@
         <v>582733</v>
       </c>
     </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <v>43973.4375</v>
+      </c>
+      <c r="B108" s="5">
+        <v>543542</v>
+      </c>
+      <c r="C108" s="5">
+        <v>5516</v>
+      </c>
+      <c r="D108" s="5">
+        <v>24628</v>
+      </c>
+      <c r="E108" s="5">
+        <v>18767</v>
+      </c>
+      <c r="F108" s="5">
+        <v>2021</v>
+      </c>
+      <c r="G108" s="5">
+        <v>600234</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3809,11 +3832,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N64"/>
+  <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I57" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5670,37 +5693,79 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C52" s="5"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="5"/>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D54" s="6"/>
+      <c r="A52" s="1">
+        <v>43973.4375</v>
+      </c>
+      <c r="B52" s="5">
+        <v>10506</v>
+      </c>
+      <c r="C52" s="5">
+        <v>13935</v>
+      </c>
+      <c r="D52" s="5">
+        <v>742</v>
+      </c>
+      <c r="E52" s="5">
+        <v>6099</v>
+      </c>
+      <c r="F52" s="5">
+        <v>7496</v>
+      </c>
+      <c r="G52" s="5">
+        <v>5143</v>
+      </c>
+      <c r="H52" s="5">
+        <v>5132</v>
+      </c>
+      <c r="I52" s="5">
+        <v>961</v>
+      </c>
+      <c r="J52" s="5">
+        <v>153</v>
+      </c>
+      <c r="K52" s="5">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E53" s="6"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D55" s="6"/>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D57" s="6"/>
+      <c r="E55" s="6"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D59" s="6"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D60" s="6"/>
+      <c r="E59" s="6"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D63" s="6"/>
-      <c r="F63" s="6"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D64" s="6"/>
+      <c r="E63" s="6"/>
+    </row>
+    <row r="65" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E65" s="6"/>
+    </row>
+    <row r="66" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E66" s="6"/>
+    </row>
+    <row r="67" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E67" s="6"/>
+    </row>
+    <row r="68" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E68" s="6"/>
+    </row>
+    <row r="70" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E70" s="6"/>
+    </row>
+    <row r="71" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E71" s="6"/>
+      <c r="G71" s="6"/>
+    </row>
+    <row r="72" spans="5:7" x14ac:dyDescent="0.2">
+      <c r="E72" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-24 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA79F00-DE76-E344-92EB-A4D6CAABABD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A536D241-D7AD-D340-8DCD-C405778A9441}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -1203,11 +1203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:I117"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D111" sqref="D111"/>
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C119" sqref="C119:F135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3849,49 +3849,46 @@
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B110" s="5"/>
-      <c r="C110" s="5"/>
-      <c r="D110" s="5"/>
-      <c r="E110" s="5"/>
-      <c r="F110" s="5"/>
-      <c r="G110" s="5"/>
+      <c r="A110" s="1">
+        <v>43975.4375</v>
+      </c>
+      <c r="B110" s="5">
+        <v>564319</v>
+      </c>
+      <c r="C110" s="5">
+        <v>3216</v>
+      </c>
+      <c r="D110" s="5">
+        <v>25500</v>
+      </c>
+      <c r="E110" s="5">
+        <v>19477</v>
+      </c>
+      <c r="F110" s="5">
+        <v>2073</v>
+      </c>
+      <c r="G110" s="5">
+        <v>614585</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D111" s="6"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C112" s="6"/>
     </row>
-    <row r="115" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="113" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D113" s="6"/>
+    </row>
+    <row r="115" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C115" s="6"/>
     </row>
-    <row r="116" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="116" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C116" s="6"/>
-    </row>
-    <row r="119" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C119" s="6"/>
-    </row>
-    <row r="120" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C120" s="6"/>
-    </row>
-    <row r="122" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C122" s="6"/>
-    </row>
-    <row r="123" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C123" s="6"/>
-    </row>
-    <row r="124" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C124" s="6"/>
-    </row>
-    <row r="125" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C125" s="6"/>
-    </row>
-    <row r="127" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C127" s="6"/>
-      <c r="E127" s="6"/>
-    </row>
-    <row r="128" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C128" s="6"/>
-    </row>
-    <row r="129" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C129" s="6"/>
+      <c r="D116" s="6"/>
+    </row>
+    <row r="117" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D117" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3903,8 +3900,8 @@
   <dimension ref="A1:N72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5830,41 +5827,89 @@
         <v>119</v>
       </c>
     </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>43975.4375</v>
+      </c>
+      <c r="B54" s="5">
+        <v>10923</v>
+      </c>
+      <c r="C54" s="5">
+        <v>14357</v>
+      </c>
+      <c r="D54" s="5">
+        <v>820</v>
+      </c>
+      <c r="E54" s="5">
+        <v>6400</v>
+      </c>
+      <c r="F54" s="5">
+        <v>7768</v>
+      </c>
+      <c r="G54" s="5">
+        <v>5263</v>
+      </c>
+      <c r="H54" s="5">
+        <v>5233</v>
+      </c>
+      <c r="I54" s="5">
+        <v>878</v>
+      </c>
+      <c r="J54" s="5">
+        <v>148</v>
+      </c>
+      <c r="K54" s="5">
+        <v>104</v>
+      </c>
+    </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E55" s="6"/>
+      <c r="C55" s="6"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D57" s="6"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E58" s="6"/>
+      <c r="C58" s="6"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E62" s="6"/>
+      <c r="D62" s="6"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C63" s="6"/>
       <c r="E63" s="6"/>
     </row>
-    <row r="65" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E65" s="6"/>
-    </row>
-    <row r="66" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E66" s="6"/>
-    </row>
-    <row r="67" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E67" s="6"/>
-    </row>
-    <row r="68" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E68" s="6"/>
-    </row>
-    <row r="70" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E70" s="6"/>
-    </row>
-    <row r="71" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E71" s="6"/>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+    </row>
+    <row r="65" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="F65" s="6"/>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D66" s="6"/>
+    </row>
+    <row r="71" spans="3:7" x14ac:dyDescent="0.2">
       <c r="G71" s="6"/>
     </row>
-    <row r="72" spans="5:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:7" x14ac:dyDescent="0.2">
       <c r="E72" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel update 2020-05-25 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A536D241-D7AD-D340-8DCD-C405778A9441}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769BD70D-1645-B545-8BEC-489CD14690BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -1203,11 +1203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I117"/>
+  <dimension ref="A1:I131"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C119" sqref="C119:F135"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F117" sqref="F117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3872,23 +3872,87 @@
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D111" s="6"/>
+      <c r="A111" s="1">
+        <v>43976.4375</v>
+      </c>
+      <c r="B111" s="5">
+        <v>571835</v>
+      </c>
+      <c r="C111" s="5">
+        <v>3883</v>
+      </c>
+      <c r="D111" s="5">
+        <v>25904</v>
+      </c>
+      <c r="E111" s="5">
+        <v>19698</v>
+      </c>
+      <c r="F111" s="5">
+        <v>2102</v>
+      </c>
+      <c r="G111" s="5">
+        <v>623422</v>
+      </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C112" s="6"/>
-    </row>
-    <row r="113" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="D113" s="6"/>
-    </row>
-    <row r="115" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="B112" s="5"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="5"/>
+      <c r="E112" s="5"/>
+      <c r="F112" s="5"/>
+      <c r="G112" s="5"/>
+    </row>
+    <row r="113" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B113" s="5"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="5"/>
+      <c r="E113" s="5"/>
+      <c r="F113" s="5"/>
+      <c r="G113" s="5"/>
+    </row>
+    <row r="114" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D114" s="6"/>
+    </row>
+    <row r="115" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C115" s="6"/>
     </row>
-    <row r="116" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.2">
       <c r="C116" s="6"/>
       <c r="D116" s="6"/>
     </row>
-    <row r="117" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D117" s="6"/>
+    </row>
+    <row r="118" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D118" s="6"/>
+    </row>
+    <row r="121" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D121" s="6"/>
+    </row>
+    <row r="122" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D122" s="6"/>
+    </row>
+    <row r="124" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D124" s="6"/>
+    </row>
+    <row r="125" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D125" s="6"/>
+    </row>
+    <row r="126" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D126" s="6"/>
+    </row>
+    <row r="127" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D127" s="6"/>
+    </row>
+    <row r="129" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D129" s="6"/>
+      <c r="F129" s="6"/>
+    </row>
+    <row r="130" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D130" s="6"/>
+    </row>
+    <row r="131" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D131" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3899,9 +3963,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
   <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H56" sqref="H56"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5863,36 +5927,79 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C55" s="6"/>
+      <c r="A55" s="1">
+        <v>43976.4375</v>
+      </c>
+      <c r="B55" s="5">
+        <v>11149</v>
+      </c>
+      <c r="C55" s="5">
+        <v>14526</v>
+      </c>
+      <c r="D55" s="5">
+        <v>845</v>
+      </c>
+      <c r="E55" s="5">
+        <v>6565</v>
+      </c>
+      <c r="F55" s="5">
+        <v>7906</v>
+      </c>
+      <c r="G55" s="5">
+        <v>5313</v>
+      </c>
+      <c r="H55" s="5">
+        <v>5260</v>
+      </c>
+      <c r="I55" s="5">
+        <v>859</v>
+      </c>
+      <c r="J55" s="5">
+        <v>148</v>
+      </c>
+      <c r="K55" s="5">
+        <v>114</v>
+      </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C57" s="5"/>
       <c r="D57" s="6"/>
+      <c r="E57" s="5"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C58" s="6"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="5"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C60" s="6"/>
+      <c r="C60" s="5"/>
       <c r="D60" s="6"/>
+      <c r="E60" s="5"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C61" s="6"/>
+      <c r="C61" s="5"/>
       <c r="D61" s="6"/>
+      <c r="E61" s="5"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C62" s="5"/>
       <c r="D62" s="6"/>
+      <c r="E62" s="5"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C63" s="6"/>
-      <c r="E63" s="6"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="5"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C64" s="6"/>

</xml_diff>

<commit_message>
excel update 2020-05-26 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{769BD70D-1645-B545-8BEC-489CD14690BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCAD2B6-9061-2344-940B-568E40A8DCD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -1203,11 +1203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I131"/>
+  <dimension ref="A1:I129"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F117" sqref="F117"/>
+      <selection pane="bottomLeft" activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3895,17 +3895,32 @@
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B112" s="5"/>
-      <c r="C112" s="5"/>
-      <c r="D112" s="5"/>
-      <c r="E112" s="5"/>
-      <c r="F112" s="5"/>
-      <c r="G112" s="5"/>
+      <c r="A112" s="1">
+        <v>43977.4375</v>
+      </c>
+      <c r="B112" s="5">
+        <v>581142</v>
+      </c>
+      <c r="C112" s="5">
+        <v>6961</v>
+      </c>
+      <c r="D112" s="5">
+        <v>26191</v>
+      </c>
+      <c r="E112" s="5">
+        <v>19958</v>
+      </c>
+      <c r="F112" s="5">
+        <v>2123</v>
+      </c>
+      <c r="G112" s="5">
+        <v>636375</v>
+      </c>
     </row>
     <row r="113" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
-      <c r="D113" s="5"/>
+      <c r="D113" s="6"/>
       <c r="E113" s="5"/>
       <c r="F113" s="5"/>
       <c r="G113" s="5"/>
@@ -3914,45 +3929,20 @@
       <c r="D114" s="6"/>
     </row>
     <row r="115" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
     </row>
     <row r="116" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C116" s="6"/>
       <c r="D116" s="6"/>
     </row>
     <row r="117" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D117" s="6"/>
+      <c r="E117" s="6"/>
     </row>
     <row r="118" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D118" s="6"/>
     </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D121" s="6"/>
-    </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D122" s="6"/>
-    </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D124" s="6"/>
-    </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D125" s="6"/>
-    </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D126" s="6"/>
-    </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D127" s="6"/>
-    </row>
-    <row r="129" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D129" s="6"/>
+    <row r="129" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F129" s="6"/>
-    </row>
-    <row r="130" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D130" s="6"/>
-    </row>
-    <row r="131" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D131" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3964,8 +3954,8 @@
   <dimension ref="A1:N72"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I59" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4106,9 +4096,6 @@
       <c r="K4">
         <v>152</v>
       </c>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -4144,9 +4131,6 @@
       <c r="K5">
         <v>154</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -4182,9 +4166,6 @@
       <c r="K6">
         <v>160</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -4220,9 +4201,6 @@
       <c r="K7">
         <v>187</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -4258,9 +4236,6 @@
       <c r="K8">
         <v>195</v>
       </c>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -4296,9 +4271,6 @@
       <c r="K9">
         <v>214</v>
       </c>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -4334,9 +4306,6 @@
       <c r="K10">
         <v>217</v>
       </c>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -4372,9 +4341,6 @@
       <c r="K11">
         <v>215</v>
       </c>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -4410,9 +4376,6 @@
       <c r="K12">
         <v>196</v>
       </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -4448,9 +4411,6 @@
       <c r="K13">
         <v>203</v>
       </c>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -4486,9 +4446,6 @@
       <c r="K14">
         <v>199</v>
       </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -4524,9 +4481,6 @@
       <c r="K15">
         <v>188</v>
       </c>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -4562,11 +4516,8 @@
       <c r="K16">
         <v>200</v>
       </c>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43938.4375</v>
       </c>
@@ -4600,11 +4551,8 @@
       <c r="K17" s="5">
         <v>200</v>
       </c>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43939.4375</v>
       </c>
@@ -4638,11 +4586,8 @@
       <c r="K18" s="5">
         <v>197</v>
       </c>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43940.4375</v>
       </c>
@@ -4676,9 +4621,8 @@
       <c r="K19" s="5">
         <v>196</v>
       </c>
-      <c r="L19" s="4"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43941.4375</v>
       </c>
@@ -4712,9 +4656,8 @@
       <c r="K20" s="5">
         <v>193</v>
       </c>
-      <c r="L20" s="4"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43942.4375</v>
       </c>
@@ -4748,9 +4691,8 @@
       <c r="K21" s="5">
         <v>194</v>
       </c>
-      <c r="L21" s="4"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43943.4375</v>
       </c>
@@ -4784,9 +4726,8 @@
       <c r="K22" s="5">
         <v>192</v>
       </c>
-      <c r="L22" s="4"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43944.4375</v>
       </c>
@@ -4820,9 +4761,8 @@
       <c r="K23" s="5">
         <v>185</v>
       </c>
-      <c r="L23" s="4"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43945.4375</v>
       </c>
@@ -4856,9 +4796,8 @@
       <c r="K24" s="5">
         <v>193</v>
       </c>
-      <c r="L24" s="4"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43946.4375</v>
       </c>
@@ -4892,9 +4831,8 @@
       <c r="K25" s="5">
         <v>195</v>
       </c>
-      <c r="L25" s="4"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43947.4375</v>
       </c>
@@ -4928,9 +4866,8 @@
       <c r="K26" s="5">
         <v>195</v>
       </c>
-      <c r="L26" s="4"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43948.4375</v>
       </c>
@@ -4964,9 +4901,8 @@
       <c r="K27" s="5">
         <v>191</v>
       </c>
-      <c r="L27" s="4"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43949.4375</v>
       </c>
@@ -5000,9 +4936,8 @@
       <c r="K28" s="5">
         <v>187</v>
       </c>
-      <c r="L28" s="4"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43950.4375</v>
       </c>
@@ -5036,9 +4971,8 @@
       <c r="K29" s="5">
         <v>186</v>
       </c>
-      <c r="L29" s="4"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43951.4375</v>
       </c>
@@ -5072,9 +5006,8 @@
       <c r="K30" s="5">
         <v>181</v>
       </c>
-      <c r="L30" s="4"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>43952.4375</v>
       </c>
@@ -5108,9 +5041,8 @@
       <c r="K31" s="5">
         <v>175</v>
       </c>
-      <c r="L31" s="4"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>43953.4375</v>
       </c>
@@ -5144,9 +5076,8 @@
       <c r="K32" s="5">
         <v>154</v>
       </c>
-      <c r="L32" s="4"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43954.4375</v>
       </c>
@@ -5180,9 +5111,8 @@
       <c r="K33" s="5">
         <v>174</v>
       </c>
-      <c r="L33" s="4"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43955.4375</v>
       </c>
@@ -5216,9 +5146,8 @@
       <c r="K34" s="5">
         <v>175</v>
       </c>
-      <c r="L34" s="4"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>43956.4375</v>
       </c>
@@ -5252,9 +5181,8 @@
       <c r="K35" s="5">
         <v>166</v>
       </c>
-      <c r="L35" s="4"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>43957.4375</v>
       </c>
@@ -5288,9 +5216,8 @@
       <c r="K36" s="5">
         <v>174</v>
       </c>
-      <c r="L36" s="4"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>43958.4375</v>
       </c>
@@ -5324,9 +5251,8 @@
       <c r="K37" s="5">
         <v>155</v>
       </c>
-      <c r="L37" s="4"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>43959.4375</v>
       </c>
@@ -5360,9 +5286,8 @@
       <c r="K38" s="5">
         <v>166</v>
       </c>
-      <c r="L38" s="4"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>43960.4375</v>
       </c>
@@ -5396,9 +5321,8 @@
       <c r="K39" s="5">
         <v>158</v>
       </c>
-      <c r="L39" s="4"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>43961.4375</v>
       </c>
@@ -5432,9 +5356,8 @@
       <c r="K40" s="5">
         <v>140</v>
       </c>
-      <c r="L40" s="4"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>43962.4375</v>
       </c>
@@ -5468,9 +5391,8 @@
       <c r="K41" s="5">
         <v>147</v>
       </c>
-      <c r="L41" s="4"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>43963.4375</v>
       </c>
@@ -5504,9 +5426,8 @@
       <c r="K42" s="5">
         <v>146</v>
       </c>
-      <c r="L42" s="4"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>43964.4375</v>
       </c>
@@ -5541,7 +5462,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43965.4375</v>
       </c>
@@ -5576,7 +5497,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43966.4375</v>
       </c>
@@ -5611,7 +5532,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>43967.4375</v>
       </c>
@@ -5646,7 +5567,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>43968.4375</v>
       </c>
@@ -5681,7 +5602,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>43969.4375</v>
       </c>
@@ -5962,44 +5883,48 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
+      <c r="A56" s="1">
+        <v>43977.4375</v>
+      </c>
+      <c r="B56" s="5">
+        <v>11286</v>
+      </c>
+      <c r="C56" s="5">
+        <v>14679</v>
+      </c>
+      <c r="D56" s="5">
+        <v>866</v>
+      </c>
+      <c r="E56" s="5">
+        <v>6651</v>
+      </c>
+      <c r="F56" s="5">
+        <v>8002</v>
+      </c>
+      <c r="G56" s="5">
+        <v>5371</v>
+      </c>
+      <c r="H56" s="5">
+        <v>5285</v>
+      </c>
+      <c r="I56" s="5">
+        <v>848</v>
+      </c>
+      <c r="J56" s="5">
+        <v>143</v>
+      </c>
+      <c r="K56" s="5">
+        <v>113</v>
+      </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C57" s="5"/>
       <c r="D57" s="6"/>
-      <c r="E57" s="5"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C58" s="5"/>
       <c r="D58" s="6"/>
-      <c r="E58" s="5"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C60" s="5"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="5"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C61" s="5"/>
-      <c r="D61" s="6"/>
-      <c r="E61" s="5"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C62" s="5"/>
-      <c r="D62" s="6"/>
-      <c r="E62" s="5"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C63" s="5"/>
       <c r="D63" s="6"/>
-      <c r="E63" s="5"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C64" s="6"/>

</xml_diff>

<commit_message>
excel update 2020-05-27 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DCAD2B6-9061-2344-940B-568E40A8DCD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE41A801-9440-B04F-9FEF-25C51506D550}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -1203,11 +1203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I129"/>
+  <dimension ref="A1:I114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A116" sqref="A116"/>
+      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G117" sqref="G117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3917,32 +3917,33 @@
         <v>636375</v>
       </c>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B113" s="5"/>
-      <c r="C113" s="5"/>
-      <c r="D113" s="6"/>
-      <c r="E113" s="5"/>
-      <c r="F113" s="5"/>
-      <c r="G113" s="5"/>
-    </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
+        <v>43978.4375</v>
+      </c>
+      <c r="B113" s="5">
+        <v>595537</v>
+      </c>
+      <c r="C113" s="5">
+        <v>11817</v>
+      </c>
+      <c r="D113" s="5">
+        <v>26483</v>
+      </c>
+      <c r="E113" s="5">
+        <v>20372</v>
+      </c>
+      <c r="F113" s="5">
+        <v>2155</v>
+      </c>
+      <c r="G113" s="5">
+        <v>656364</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C114" s="5"/>
       <c r="D114" s="6"/>
-    </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D115" s="6"/>
-    </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D116" s="6"/>
-    </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D117" s="6"/>
-      <c r="E117" s="6"/>
-    </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D118" s="6"/>
-    </row>
-    <row r="129" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F129" s="6"/>
+      <c r="E114" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3951,11 +3952,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N72"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I59" sqref="I59"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5918,31 +5919,60 @@
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D57" s="6"/>
+      <c r="A57" s="1">
+        <v>43978.4375</v>
+      </c>
+      <c r="B57" s="5">
+        <v>11433</v>
+      </c>
+      <c r="C57" s="5">
+        <v>14827</v>
+      </c>
+      <c r="D57" s="5">
+        <v>888</v>
+      </c>
+      <c r="E57" s="5">
+        <v>6737</v>
+      </c>
+      <c r="F57" s="5">
+        <v>8101</v>
+      </c>
+      <c r="G57" s="5">
+        <v>5421</v>
+      </c>
+      <c r="H57" s="5">
+        <v>5321</v>
+      </c>
+      <c r="I57" s="5">
+        <v>847</v>
+      </c>
+      <c r="J57" s="5">
+        <v>150</v>
+      </c>
+      <c r="K57" s="5">
+        <v>117</v>
+      </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D58" s="6"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D63" s="6"/>
+      <c r="G63" s="6"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C64" s="6"/>
-      <c r="D64" s="6"/>
-    </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C65" s="6"/>
-      <c r="D65" s="6"/>
-      <c r="F65" s="6"/>
-    </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="D66" s="6"/>
-    </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="G71" s="6"/>
-    </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E72" s="6"/>
+      <c r="E64" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-28 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE41A801-9440-B04F-9FEF-25C51506D550}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46EC981-7C21-8543-97B0-29160F9AF9B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -1203,11 +1203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I114"/>
+  <dimension ref="A1:I124"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G117" sqref="G117"/>
+      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3941,9 +3941,77 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C114" s="5"/>
-      <c r="D114" s="6"/>
-      <c r="E114" s="5"/>
+      <c r="A114" s="1">
+        <v>43979.4375</v>
+      </c>
+      <c r="B114" s="5">
+        <v>612434</v>
+      </c>
+      <c r="C114" s="5">
+        <v>11868</v>
+      </c>
+      <c r="D114" s="5">
+        <v>26866</v>
+      </c>
+      <c r="E114" s="5">
+        <v>20673</v>
+      </c>
+      <c r="F114" s="5">
+        <v>2189</v>
+      </c>
+      <c r="G114" s="5">
+        <v>674030</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C115" s="5"/>
+      <c r="D115" s="5"/>
+      <c r="E115" s="5"/>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C116" s="5"/>
+      <c r="D116" s="5"/>
+      <c r="E116" s="5"/>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C117" s="5"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="5"/>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C118" s="5"/>
+      <c r="D118" s="5"/>
+      <c r="E118" s="5"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C119" s="5"/>
+      <c r="D119" s="6"/>
+      <c r="E119" s="5"/>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C120" s="5"/>
+      <c r="D120" s="6"/>
+      <c r="E120" s="5"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C121" s="5"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="5"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C122" s="5"/>
+      <c r="D122" s="6"/>
+      <c r="E122" s="5"/>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C123" s="5"/>
+      <c r="D123" s="6"/>
+      <c r="E123" s="5"/>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C124" s="5"/>
+      <c r="D124" s="5"/>
+      <c r="E124" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3952,11 +4020,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N64"/>
+  <dimension ref="A1:N58"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J61" sqref="J61"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5954,25 +6022,39 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="G63" s="6"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="E64" s="6"/>
+      <c r="A58" s="1">
+        <v>43979.4375</v>
+      </c>
+      <c r="B58" s="5">
+        <v>11637</v>
+      </c>
+      <c r="C58" s="5">
+        <v>15005</v>
+      </c>
+      <c r="D58" s="5">
+        <v>922</v>
+      </c>
+      <c r="E58" s="5">
+        <v>6870</v>
+      </c>
+      <c r="F58" s="5">
+        <v>8208</v>
+      </c>
+      <c r="G58" s="5">
+        <v>5493</v>
+      </c>
+      <c r="H58" s="5">
+        <v>5359</v>
+      </c>
+      <c r="I58" s="5">
+        <v>833</v>
+      </c>
+      <c r="J58" s="5">
+        <v>137</v>
+      </c>
+      <c r="K58" s="5">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-29 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C46EC981-7C21-8543-97B0-29160F9AF9B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78569DFE-C37A-F149-B96C-E28B441B8305}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -1203,11 +1203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I124"/>
+  <dimension ref="A1:I121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A88" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A115" sqref="A115"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G107" sqref="G107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1266,6 +1266,10 @@
       <c r="G2">
         <v>285</v>
       </c>
+      <c r="H2" s="5">
+        <f>D2/SUM(B2,D2:F2)</f>
+        <v>1.1278195488721804E-2</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -1289,7 +1293,10 @@
       <c r="G3">
         <v>313</v>
       </c>
-      <c r="H3" s="5"/>
+      <c r="H3" s="5">
+        <f t="shared" ref="H3:H66" si="0">D3/SUM(B3,D3:F3)</f>
+        <v>6.5789473684210523E-3</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -1313,7 +1320,10 @@
       <c r="G4">
         <v>340</v>
       </c>
-      <c r="H4" s="5"/>
+      <c r="H4" s="5">
+        <f t="shared" si="0"/>
+        <v>6.1538461538461538E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -1337,7 +1347,10 @@
       <c r="G5">
         <v>364</v>
       </c>
-      <c r="H5" s="5"/>
+      <c r="H5" s="5">
+        <f t="shared" si="0"/>
+        <v>5.6179775280898875E-3</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -1361,7 +1374,10 @@
       <c r="G6">
         <v>364</v>
       </c>
-      <c r="H6" s="5"/>
+      <c r="H6" s="5">
+        <f t="shared" si="0"/>
+        <v>5.6179775280898875E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -1385,7 +1401,10 @@
       <c r="G7">
         <v>364</v>
       </c>
-      <c r="H7" s="5"/>
+      <c r="H7" s="5">
+        <f t="shared" si="0"/>
+        <v>5.6179775280898875E-3</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -1409,7 +1428,10 @@
       <c r="G8">
         <v>402</v>
       </c>
-      <c r="H8" s="5"/>
+      <c r="H8" s="5">
+        <f t="shared" si="0"/>
+        <v>4.9751243781094526E-3</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -1433,7 +1455,10 @@
       <c r="G9">
         <v>421</v>
       </c>
-      <c r="H9" s="5"/>
+      <c r="H9" s="5">
+        <f t="shared" si="0"/>
+        <v>4.7505938242280287E-3</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -1457,7 +1482,10 @@
       <c r="G10">
         <v>456</v>
       </c>
-      <c r="H10" s="5"/>
+      <c r="H10" s="5">
+        <f t="shared" si="0"/>
+        <v>4.5558086560364463E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -1481,7 +1509,10 @@
       <c r="G11">
         <v>479</v>
       </c>
-      <c r="H11" s="5"/>
+      <c r="H11" s="5">
+        <f t="shared" si="0"/>
+        <v>2.1505376344086021E-3</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -1505,7 +1536,10 @@
       <c r="G12">
         <v>498</v>
       </c>
-      <c r="H12" s="5"/>
+      <c r="H12" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -1529,7 +1563,10 @@
       <c r="G13">
         <v>498</v>
       </c>
-      <c r="H13" s="5"/>
+      <c r="H13" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -1553,7 +1590,10 @@
       <c r="G14">
         <v>498</v>
       </c>
-      <c r="H14" s="5"/>
+      <c r="H14" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -1577,7 +1617,10 @@
       <c r="G15">
         <v>553</v>
       </c>
-      <c r="H15" s="5"/>
+      <c r="H15" s="5">
+        <f t="shared" si="0"/>
+        <v>1.838235294117647E-3</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -1601,7 +1644,10 @@
       <c r="G16">
         <v>593</v>
       </c>
-      <c r="H16" s="5"/>
+      <c r="H16" s="5">
+        <f t="shared" si="0"/>
+        <v>1.7482517482517483E-3</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -1625,7 +1671,10 @@
       <c r="G17">
         <v>629</v>
       </c>
-      <c r="H17" s="5"/>
+      <c r="H17" s="5">
+        <f t="shared" si="0"/>
+        <v>3.2520325203252032E-3</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -1649,7 +1698,10 @@
       <c r="G18">
         <v>699</v>
       </c>
-      <c r="H18" s="5"/>
+      <c r="H18" s="5">
+        <f t="shared" si="0"/>
+        <v>4.4247787610619468E-3</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -1673,7 +1725,10 @@
       <c r="G19">
         <v>699</v>
       </c>
-      <c r="H19" s="5"/>
+      <c r="H19" s="5">
+        <f t="shared" si="0"/>
+        <v>4.4247787610619468E-3</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -1697,7 +1752,10 @@
       <c r="G20">
         <v>768</v>
       </c>
-      <c r="H20" s="5"/>
+      <c r="H20" s="5">
+        <f t="shared" si="0"/>
+        <v>5.3619302949061663E-3</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -1721,7 +1779,10 @@
       <c r="G21">
         <v>768</v>
       </c>
-      <c r="H21" s="5"/>
+      <c r="H21" s="5">
+        <f t="shared" si="0"/>
+        <v>5.3619302949061663E-3</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
@@ -1745,7 +1806,10 @@
       <c r="G22">
         <v>1005</v>
       </c>
-      <c r="H22" s="5"/>
+      <c r="H22" s="5">
+        <f t="shared" si="0"/>
+        <v>1.5105740181268883E-2</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
@@ -1769,7 +1833,10 @@
       <c r="G23">
         <v>1126</v>
       </c>
-      <c r="H23" s="5"/>
+      <c r="H23" s="5">
+        <f t="shared" si="0"/>
+        <v>1.572617946345976E-2</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
@@ -1793,7 +1860,10 @@
       <c r="G24">
         <v>1338</v>
       </c>
-      <c r="H24" s="5"/>
+      <c r="H24" s="5">
+        <f t="shared" si="0"/>
+        <v>1.3754045307443365E-2</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
@@ -1817,7 +1887,10 @@
       <c r="G25">
         <v>1566</v>
       </c>
-      <c r="H25" s="5"/>
+      <c r="H25" s="5">
+        <f t="shared" si="0"/>
+        <v>1.2096774193548387E-2</v>
+      </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
@@ -1841,7 +1914,10 @@
       <c r="G26">
         <v>1763</v>
       </c>
-      <c r="H26" s="5"/>
+      <c r="H26" s="5">
+        <f t="shared" si="0"/>
+        <v>1.3010053222945003E-2</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
@@ -1865,7 +1941,10 @@
       <c r="G27">
         <v>1982</v>
       </c>
-      <c r="H27" s="5"/>
+      <c r="H27" s="5">
+        <f t="shared" si="0"/>
+        <v>1.2332990750256937E-2</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
@@ -1889,7 +1968,10 @@
       <c r="G28">
         <v>1982</v>
       </c>
-      <c r="H28" s="5"/>
+      <c r="H28" s="5">
+        <f t="shared" si="0"/>
+        <v>1.2332990750256937E-2</v>
+      </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
@@ -1913,7 +1995,10 @@
       <c r="G29">
         <v>2403</v>
       </c>
-      <c r="H29" s="5"/>
+      <c r="H29" s="5">
+        <f t="shared" si="0"/>
+        <v>1.25997480050399E-2</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
@@ -1937,7 +2022,10 @@
       <c r="G30">
         <v>2747</v>
       </c>
-      <c r="H30" s="5"/>
+      <c r="H30" s="5">
+        <f t="shared" si="0"/>
+        <v>1.1764705882352941E-2</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
@@ -1961,7 +2049,10 @@
       <c r="G31">
         <v>2747</v>
       </c>
-      <c r="H31" s="5"/>
+      <c r="H31" s="5">
+        <f t="shared" si="0"/>
+        <v>1.1764705882352941E-2</v>
+      </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
@@ -1985,7 +2076,10 @@
       <c r="G32">
         <v>3395</v>
       </c>
-      <c r="H32" s="5"/>
+      <c r="H32" s="5">
+        <f t="shared" si="0"/>
+        <v>1.2627986348122866E-2</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
@@ -2009,7 +2103,10 @@
       <c r="G33">
         <v>4185</v>
       </c>
-      <c r="H33" s="5"/>
+      <c r="H33" s="5">
+        <f t="shared" si="0"/>
+        <v>1.4798574952041656E-2</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
@@ -2033,7 +2130,10 @@
       <c r="G34">
         <v>5129</v>
       </c>
-      <c r="H34" s="5"/>
+      <c r="H34" s="5">
+        <f t="shared" si="0"/>
+        <v>1.6267311497032314E-2</v>
+      </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
@@ -2057,7 +2157,10 @@
       <c r="G35">
         <v>6648</v>
       </c>
-      <c r="H35" s="5"/>
+      <c r="H35" s="5">
+        <f t="shared" si="0"/>
+        <v>1.7165878437554738E-2</v>
+      </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
@@ -2081,7 +2184,10 @@
       <c r="G36">
         <v>8465</v>
       </c>
-      <c r="H36" s="5"/>
+      <c r="H36" s="5">
+        <f t="shared" si="0"/>
+        <v>1.9583158483704014E-2</v>
+      </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
@@ -2105,7 +2211,10 @@
       <c r="G37">
         <v>10178</v>
       </c>
-      <c r="H37" s="5"/>
+      <c r="H37" s="5">
+        <f t="shared" si="0"/>
+        <v>1.9905103575975004E-2</v>
+      </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
@@ -2129,7 +2238,10 @@
       <c r="G38">
         <v>11171</v>
       </c>
-      <c r="H38" s="5"/>
+      <c r="H38" s="5">
+        <f t="shared" si="0"/>
+        <v>1.9054560599750105E-2</v>
+      </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
@@ -2153,7 +2265,10 @@
       <c r="G39">
         <v>16650</v>
       </c>
-      <c r="H39" s="5"/>
+      <c r="H39" s="5">
+        <f t="shared" si="0"/>
+        <v>1.979807540621549E-2</v>
+      </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
@@ -2177,7 +2292,10 @@
       <c r="G40">
         <v>16650</v>
       </c>
-      <c r="H40" s="5"/>
+      <c r="H40" s="5">
+        <f t="shared" si="0"/>
+        <v>1.9796513920656202E-2</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
@@ -2201,7 +2319,10 @@
       <c r="G41">
         <v>23384</v>
       </c>
-      <c r="H41" s="5"/>
+      <c r="H41" s="5">
+        <f t="shared" si="0"/>
+        <v>2.2855373180551253E-2</v>
+      </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
@@ -2225,7 +2346,10 @@
       <c r="G42">
         <v>23384</v>
       </c>
-      <c r="H42" s="5"/>
+      <c r="H42" s="5">
+        <f t="shared" si="0"/>
+        <v>2.2793434499845153E-2</v>
+      </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
@@ -2249,7 +2373,10 @@
       <c r="G43">
         <v>26420</v>
       </c>
-      <c r="H43" s="5"/>
+      <c r="H43" s="5">
+        <f t="shared" si="0"/>
+        <v>2.2814109308378093E-2</v>
+      </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
@@ -2273,7 +2400,10 @@
       <c r="G44">
         <v>28506</v>
       </c>
-      <c r="H44" s="5"/>
+      <c r="H44" s="5">
+        <f t="shared" si="0"/>
+        <v>2.4341679526108814E-2</v>
+      </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
@@ -2297,7 +2427,10 @@
       <c r="G45">
         <v>32457</v>
       </c>
-      <c r="H45" s="5"/>
+      <c r="H45" s="5">
+        <f t="shared" si="0"/>
+        <v>2.5599785551534648E-2</v>
+      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
@@ -2321,7 +2454,10 @@
       <c r="G46">
         <v>35635</v>
       </c>
-      <c r="H46" s="5"/>
+      <c r="H46" s="5">
+        <f t="shared" si="0"/>
+        <v>2.6684164479440071E-2</v>
+      </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
@@ -2345,7 +2481,10 @@
       <c r="G47">
         <v>35635</v>
       </c>
-      <c r="H47" s="5"/>
+      <c r="H47" s="5">
+        <f t="shared" si="0"/>
+        <v>2.6525093454227312E-2</v>
+      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
@@ -2369,7 +2508,10 @@
       <c r="G48">
         <v>38550</v>
       </c>
-      <c r="H48" s="5"/>
+      <c r="H48" s="5">
+        <f t="shared" si="0"/>
+        <v>3.0342577487765091E-2</v>
+      </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
@@ -2393,7 +2535,10 @@
       <c r="G49">
         <v>38550</v>
       </c>
-      <c r="H49" s="5"/>
+      <c r="H49" s="5">
+        <f t="shared" si="0"/>
+        <v>3.0270074315751315E-2</v>
+      </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
@@ -2417,7 +2562,10 @@
       <c r="G50">
         <v>41032</v>
       </c>
-      <c r="H50" s="5"/>
+      <c r="H50" s="5">
+        <f t="shared" si="0"/>
+        <v>3.1233850129198968E-2</v>
+      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
@@ -2441,7 +2589,10 @@
       <c r="G51">
         <v>43072</v>
       </c>
-      <c r="H51" s="5"/>
+      <c r="H51" s="5">
+        <f t="shared" si="0"/>
+        <v>3.2515123313168914E-2</v>
+      </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
@@ -2465,7 +2616,10 @@
       <c r="G52">
         <v>43072</v>
       </c>
-      <c r="H52" s="5"/>
+      <c r="H52" s="5">
+        <f t="shared" si="0"/>
+        <v>3.2486040018613306E-2</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
@@ -2489,7 +2643,10 @@
       <c r="G53">
         <v>49186</v>
       </c>
-      <c r="H53" s="5"/>
+      <c r="H53" s="5">
+        <f t="shared" si="0"/>
+        <v>3.1582708110039298E-2</v>
+      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
@@ -2513,7 +2670,10 @@
       <c r="G54">
         <v>49186</v>
       </c>
-      <c r="H54" s="5"/>
+      <c r="H54" s="5">
+        <f t="shared" si="0"/>
+        <v>3.15350720495415E-2</v>
+      </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
@@ -2537,7 +2697,10 @@
       <c r="G55">
         <v>54112</v>
       </c>
-      <c r="H55" s="5"/>
+      <c r="H55" s="5">
+        <f t="shared" si="0"/>
+        <v>3.5203565753905201E-2</v>
+      </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
@@ -2562,7 +2725,10 @@
         <f>51629+C53</f>
         <v>58832</v>
       </c>
-      <c r="H56" s="5"/>
+      <c r="H56" s="5">
+        <f t="shared" si="0"/>
+        <v>3.8477346119972597E-2</v>
+      </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
@@ -2586,7 +2752,10 @@
       <c r="G57">
         <v>61009</v>
       </c>
-      <c r="H57" s="5"/>
+      <c r="H57" s="5">
+        <f t="shared" si="0"/>
+        <v>4.133116770916128E-2</v>
+      </c>
       <c r="I57" s="5"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
@@ -2611,7 +2780,10 @@
       <c r="G58">
         <v>64785</v>
       </c>
-      <c r="H58" s="5"/>
+      <c r="H58" s="5">
+        <f t="shared" si="0"/>
+        <v>4.4522021902348045E-2</v>
+      </c>
       <c r="I58" s="5"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -2636,7 +2808,10 @@
       <c r="G59">
         <v>67998</v>
       </c>
-      <c r="H59" s="5"/>
+      <c r="H59" s="5">
+        <f t="shared" si="0"/>
+        <v>4.8761853399847198E-2</v>
+      </c>
       <c r="I59" s="5"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
@@ -2661,7 +2836,10 @@
       <c r="G60">
         <v>72674</v>
       </c>
-      <c r="H60" s="5"/>
+      <c r="H60" s="5">
+        <f t="shared" si="0"/>
+        <v>5.0884521573355011E-2</v>
+      </c>
       <c r="I60" s="5"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
@@ -2686,7 +2864,10 @@
       <c r="G61">
         <v>76027</v>
       </c>
-      <c r="H61" s="5"/>
+      <c r="H61" s="5">
+        <f t="shared" si="0"/>
+        <v>5.3806998374330409E-2</v>
+      </c>
       <c r="I61" s="5"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
@@ -2711,7 +2892,10 @@
       <c r="G62">
         <v>79125</v>
       </c>
-      <c r="H62" s="5"/>
+      <c r="H62" s="5">
+        <f t="shared" si="0"/>
+        <v>5.4938388625592416E-2</v>
+      </c>
       <c r="I62" s="5"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
@@ -2736,7 +2920,10 @@
       <c r="G63">
         <v>82055</v>
       </c>
-      <c r="H63" s="5"/>
+      <c r="H63" s="5">
+        <f t="shared" si="0"/>
+        <v>5.8084656604886681E-2</v>
+      </c>
       <c r="I63" s="5"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
@@ -2761,7 +2948,10 @@
       <c r="G64">
         <v>85703</v>
       </c>
-      <c r="H64" s="5"/>
+      <c r="H64" s="5">
+        <f t="shared" si="0"/>
+        <v>6.2363329038663845E-2</v>
+      </c>
       <c r="I64" s="5"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
@@ -2786,7 +2976,10 @@
       <c r="G65">
         <v>89906</v>
       </c>
-      <c r="H65" s="5"/>
+      <c r="H65" s="5">
+        <f t="shared" si="0"/>
+        <v>6.4928183273580006E-2</v>
+      </c>
       <c r="I65" s="5"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
@@ -2811,7 +3004,10 @@
       <c r="G66">
         <v>94271</v>
       </c>
-      <c r="H66" s="5"/>
+      <c r="H66" s="5">
+        <f t="shared" si="0"/>
+        <v>6.7301155676410609E-2</v>
+      </c>
       <c r="I66" s="5"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
@@ -2836,7 +3032,10 @@
       <c r="G67">
         <v>97838</v>
       </c>
-      <c r="H67" s="5"/>
+      <c r="H67" s="5">
+        <f t="shared" ref="H67:H115" si="1">D67/SUM(B67,D67:F67)</f>
+        <v>6.9019216993179061E-2</v>
+      </c>
       <c r="I67" s="5"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
@@ -2861,7 +3060,10 @@
       <c r="G68">
         <v>104784</v>
       </c>
-      <c r="H68" s="5"/>
+      <c r="H68" s="5">
+        <f t="shared" si="1"/>
+        <v>6.832743663064024E-2</v>
+      </c>
       <c r="I68" s="5"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
@@ -2886,7 +3088,10 @@
       <c r="G69">
         <v>109764</v>
       </c>
-      <c r="H69" s="5"/>
+      <c r="H69" s="5">
+        <f t="shared" si="1"/>
+        <v>6.9019680310449971E-2</v>
+      </c>
       <c r="I69" s="5"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
@@ -2911,7 +3116,10 @@
       <c r="G70">
         <v>115189</v>
       </c>
-      <c r="H70" s="5"/>
+      <c r="H70" s="5">
+        <f t="shared" si="1"/>
+        <v>7.0329495410410142E-2</v>
+      </c>
       <c r="I70" s="5"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
@@ -2936,7 +3144,10 @@
       <c r="G71">
         <v>123521</v>
       </c>
-      <c r="H71" s="5"/>
+      <c r="H71" s="5">
+        <f t="shared" si="1"/>
+        <v>6.8385132892382669E-2</v>
+      </c>
       <c r="I71" s="5"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
@@ -2961,7 +3172,10 @@
       <c r="G72">
         <v>132416</v>
       </c>
-      <c r="H72" s="5"/>
+      <c r="H72" s="5">
+        <f t="shared" si="1"/>
+        <v>6.9956984378537465E-2</v>
+      </c>
       <c r="I72" s="5"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
@@ -2986,7 +3200,10 @@
       <c r="G73" s="5">
         <v>142985</v>
       </c>
-      <c r="H73" s="5"/>
+      <c r="H73" s="5">
+        <f t="shared" si="1"/>
+        <v>6.9529607568325158E-2</v>
+      </c>
       <c r="I73" s="5"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
@@ -3011,7 +3228,10 @@
       <c r="G74" s="5">
         <v>153287</v>
       </c>
-      <c r="H74" s="5"/>
+      <c r="H74" s="5">
+        <f t="shared" si="1"/>
+        <v>6.8349106203995799E-2</v>
+      </c>
       <c r="I74" s="5"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -3036,7 +3256,10 @@
       <c r="G75" s="5">
         <v>161833</v>
       </c>
-      <c r="H75" s="5"/>
+      <c r="H75" s="5">
+        <f t="shared" si="1"/>
+        <v>6.7765556032466992E-2</v>
+      </c>
       <c r="I75" s="5"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -3061,7 +3284,10 @@
       <c r="G76" s="5">
         <v>168639</v>
       </c>
-      <c r="H76" s="5"/>
+      <c r="H76" s="5">
+        <f t="shared" si="1"/>
+        <v>6.7847609803445771E-2</v>
+      </c>
       <c r="I76" s="5"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -3086,7 +3312,10 @@
       <c r="G77">
         <v>179716</v>
       </c>
-      <c r="H77" s="5"/>
+      <c r="H77" s="5">
+        <f t="shared" si="1"/>
+        <v>6.737670092438422E-2</v>
+      </c>
       <c r="I77" s="5"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
@@ -3111,7 +3340,10 @@
       <c r="G78" s="5">
         <v>191376</v>
       </c>
-      <c r="H78" s="5"/>
+      <c r="H78" s="5">
+        <f t="shared" si="1"/>
+        <v>6.6357414201407894E-2</v>
+      </c>
       <c r="I78" s="5"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
@@ -3136,7 +3368,10 @@
       <c r="G79" s="5">
         <v>201502</v>
       </c>
-      <c r="H79" s="5"/>
+      <c r="H79" s="5">
+        <f t="shared" si="1"/>
+        <v>6.6132634984210126E-2</v>
+      </c>
       <c r="I79" s="5"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
@@ -3161,7 +3396,10 @@
       <c r="G80" s="5">
         <v>212454</v>
       </c>
-      <c r="H80" s="5"/>
+      <c r="H80" s="5">
+        <f t="shared" si="1"/>
+        <v>6.5296561051004634E-2</v>
+      </c>
       <c r="I80" s="5"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
@@ -3186,7 +3424,10 @@
       <c r="G81" s="5">
         <v>225789</v>
       </c>
-      <c r="H81" s="5"/>
+      <c r="H81" s="5">
+        <f t="shared" si="1"/>
+        <v>6.4309937597073777E-2</v>
+      </c>
       <c r="I81" s="5"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
@@ -3211,7 +3452,10 @@
       <c r="G82" s="5">
         <v>237055</v>
       </c>
-      <c r="H82" s="5"/>
+      <c r="H82" s="5">
+        <f t="shared" si="1"/>
+        <v>6.2846741392975025E-2</v>
+      </c>
       <c r="I82" s="5"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
@@ -3236,7 +3480,10 @@
       <c r="G83" s="5">
         <v>247189</v>
       </c>
-      <c r="H83" s="5"/>
+      <c r="H83" s="5">
+        <f t="shared" si="1"/>
+        <v>6.1340776586783823E-2</v>
+      </c>
       <c r="I83" s="5"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
@@ -3261,7 +3508,10 @@
       <c r="G84" s="5">
         <v>259322</v>
       </c>
-      <c r="H84" s="5"/>
+      <c r="H84" s="5">
+        <f t="shared" si="1"/>
+        <v>6.0784856149225422E-2</v>
+      </c>
       <c r="I84" s="5"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
@@ -3286,7 +3536,10 @@
       <c r="G85" s="5">
         <v>274124</v>
       </c>
-      <c r="H85" s="5"/>
+      <c r="H85" s="5">
+        <f t="shared" si="1"/>
+        <v>5.9442013046403168E-2</v>
+      </c>
       <c r="I85" s="5"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
@@ -3311,7 +3564,10 @@
       <c r="G86" s="5">
         <v>289381</v>
       </c>
-      <c r="H86" s="5"/>
+      <c r="H86" s="5">
+        <f t="shared" si="1"/>
+        <v>5.8326907416348973E-2</v>
+      </c>
       <c r="I86" s="5"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
@@ -3336,7 +3592,10 @@
       <c r="G87" s="5">
         <v>306029</v>
       </c>
-      <c r="H87" s="5"/>
+      <c r="H87" s="5">
+        <f t="shared" si="1"/>
+        <v>5.6479422146952597E-2</v>
+      </c>
       <c r="I87" s="5"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
@@ -3361,7 +3620,10 @@
       <c r="G88" s="5">
         <v>323188</v>
       </c>
-      <c r="H88" s="5"/>
+      <c r="H88" s="5">
+        <f t="shared" si="1"/>
+        <v>5.5158703308104483E-2</v>
+      </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
@@ -3385,7 +3647,10 @@
       <c r="G89" s="5">
         <v>337290</v>
       </c>
-      <c r="H89" s="5"/>
+      <c r="H89" s="5">
+        <f t="shared" si="1"/>
+        <v>5.3596128303384678E-2</v>
+      </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
@@ -3409,7 +3674,10 @@
       <c r="G90" s="5">
         <v>348325</v>
       </c>
-      <c r="H90" s="5"/>
+      <c r="H90" s="5">
+        <f t="shared" si="1"/>
+        <v>5.2397240250248493E-2</v>
+      </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
@@ -3433,6 +3701,10 @@
       <c r="G91" s="5">
         <v>358737</v>
       </c>
+      <c r="H91" s="5">
+        <f t="shared" si="1"/>
+        <v>5.1911747194610933E-2</v>
+      </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
@@ -3456,6 +3728,10 @@
       <c r="G92" s="5">
         <v>374465</v>
       </c>
+      <c r="H92" s="5">
+        <f t="shared" si="1"/>
+        <v>5.1198468585492582E-2</v>
+      </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
@@ -3479,6 +3755,10 @@
       <c r="G93" s="5">
         <v>393866</v>
       </c>
+      <c r="H93" s="5">
+        <f t="shared" si="1"/>
+        <v>5.0205590593770839E-2</v>
+      </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
@@ -3502,6 +3782,10 @@
       <c r="G94" s="5">
         <v>411790</v>
       </c>
+      <c r="H94" s="5">
+        <f t="shared" si="1"/>
+        <v>4.9346718737803698E-2</v>
+      </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
@@ -3525,6 +3809,10 @@
       <c r="G95" s="5">
         <v>431683</v>
       </c>
+      <c r="H95" s="5">
+        <f t="shared" si="1"/>
+        <v>4.7899014352412242E-2</v>
+      </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
@@ -3548,8 +3836,12 @@
       <c r="G96" s="5">
         <v>448810</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H96" s="5">
+        <f t="shared" si="1"/>
+        <v>4.6631981087296138E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>43962.4375</v>
       </c>
@@ -3571,8 +3863,12 @@
       <c r="G97" s="5">
         <v>456982</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H97" s="5">
+        <f t="shared" si="1"/>
+        <v>4.5865292746738576E-2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>43963.4375</v>
       </c>
@@ -3594,8 +3890,12 @@
       <c r="G98" s="5">
         <v>470732</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H98" s="5">
+        <f t="shared" si="1"/>
+        <v>4.5457806884225772E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>43964.4375</v>
       </c>
@@ -3617,8 +3917,12 @@
       <c r="G99" s="5">
         <v>488453</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H99" s="5">
+        <f t="shared" si="1"/>
+        <v>4.470191008255834E-2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>43965.4375</v>
       </c>
@@ -3640,8 +3944,12 @@
       <c r="G100" s="5">
         <v>510065</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H100" s="5">
+        <f t="shared" si="1"/>
+        <v>4.3643791612773535E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>43966.4375</v>
       </c>
@@ -3663,8 +3971,12 @@
       <c r="G101" s="5">
         <v>525214</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H101" s="5">
+        <f t="shared" si="1"/>
+        <v>4.2913548442666115E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>43967.4375</v>
       </c>
@@ -3686,8 +3998,12 @@
       <c r="G102" s="5">
         <v>539174</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H102" s="5">
+        <f t="shared" si="1"/>
+        <v>4.2210783395666737E-2</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>43968.4375</v>
       </c>
@@ -3709,8 +4025,12 @@
       <c r="G103" s="5">
         <v>549240</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H103" s="5">
+        <f t="shared" si="1"/>
+        <v>4.1578412190313975E-2</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>43969.4375</v>
       </c>
@@ -3732,8 +4052,12 @@
       <c r="G104" s="5">
         <v>563136</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H104" s="5">
+        <f t="shared" si="1"/>
+        <v>4.1440049387975401E-2</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>43970.4375</v>
       </c>
@@ -3755,8 +4079,12 @@
       <c r="G105" s="5">
         <v>562088</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H105" s="5">
+        <f t="shared" si="1"/>
+        <v>4.1772509173017218E-2</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>43971.4375</v>
       </c>
@@ -3778,8 +4106,12 @@
       <c r="G106" s="5">
         <v>571620</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H106" s="5">
+        <f t="shared" si="1"/>
+        <v>4.1916442162573876E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>43972.4375</v>
       </c>
@@ -3801,8 +4133,12 @@
       <c r="G107" s="5">
         <v>582733</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H107" s="5">
+        <f t="shared" si="1"/>
+        <v>4.1869055985819185E-2</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>43973.4375</v>
       </c>
@@ -3824,8 +4160,12 @@
       <c r="G108" s="5">
         <v>600234</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H108" s="5">
+        <f t="shared" si="1"/>
+        <v>4.1816224586473057E-2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>43974.4375</v>
       </c>
@@ -3847,8 +4187,12 @@
       <c r="G109" s="5">
         <v>605857</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H109" s="5">
+        <f t="shared" si="1"/>
+        <v>4.1734307133833123E-2</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>43975.4375</v>
       </c>
@@ -3870,8 +4214,12 @@
       <c r="G110" s="5">
         <v>614585</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H110" s="5">
+        <f t="shared" si="1"/>
+        <v>4.1709671246006913E-2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>43976.4375</v>
       </c>
@@ -3893,8 +4241,12 @@
       <c r="G111" s="5">
         <v>623422</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H111" s="5">
+        <f t="shared" si="1"/>
+        <v>4.1811734208823011E-2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>43977.4375</v>
       </c>
@@ -3916,8 +4268,12 @@
       <c r="G112" s="5">
         <v>636375</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H112" s="5">
+        <f t="shared" si="1"/>
+        <v>4.1611721378933424E-2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>43978.4375</v>
       </c>
@@ -3939,8 +4295,12 @@
       <c r="G113" s="5">
         <v>656364</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H113" s="5">
+        <f t="shared" si="1"/>
+        <v>4.1087771721844954E-2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>43979.4375</v>
       </c>
@@ -3962,56 +4322,72 @@
       <c r="G114" s="5">
         <v>674030</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C115" s="5"/>
-      <c r="D115" s="5"/>
-      <c r="E115" s="5"/>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H114" s="5">
+        <f t="shared" si="1"/>
+        <v>4.0573152793425174E-2</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
+        <v>43980.4375</v>
+      </c>
+      <c r="B115" s="5">
+        <v>630264</v>
+      </c>
+      <c r="C115" s="5">
+        <v>13351</v>
+      </c>
+      <c r="D115" s="5">
+        <v>27210</v>
+      </c>
+      <c r="E115" s="5">
+        <v>20983</v>
+      </c>
+      <c r="F115" s="5">
+        <v>2230</v>
+      </c>
+      <c r="G115" s="5">
+        <v>694038</v>
+      </c>
+      <c r="H115" s="5">
+        <f t="shared" si="1"/>
+        <v>3.9974320061937428E-2</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C116" s="5"/>
       <c r="D116" s="5"/>
       <c r="E116" s="5"/>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B117" s="5"/>
       <c r="C117" s="5"/>
       <c r="D117" s="6"/>
       <c r="E117" s="5"/>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B118" s="5"/>
       <c r="C118" s="5"/>
       <c r="D118" s="5"/>
       <c r="E118" s="5"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C119" s="5"/>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B119" s="5"/>
+      <c r="C119" s="6"/>
       <c r="D119" s="6"/>
       <c r="E119" s="5"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B120" s="5"/>
       <c r="C120" s="5"/>
       <c r="D120" s="6"/>
       <c r="E120" s="5"/>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C121" s="5"/>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B121" s="5"/>
+      <c r="C121" s="6"/>
       <c r="D121" s="6"/>
       <c r="E121" s="5"/>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C122" s="5"/>
-      <c r="D122" s="6"/>
-      <c r="E122" s="5"/>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C123" s="5"/>
-      <c r="D123" s="6"/>
-      <c r="E123" s="5"/>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C124" s="5"/>
-      <c r="D124" s="5"/>
-      <c r="E124" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4020,11 +4396,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N58"/>
+  <dimension ref="A1:N69"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E59" sqref="E59"/>
+      <selection pane="bottomLeft" activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6055,6 +6431,92 @@
       <c r="K58" s="5">
         <v>94</v>
       </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>43980.4375</v>
+      </c>
+      <c r="B59" s="5">
+        <v>11818</v>
+      </c>
+      <c r="C59" s="5">
+        <v>15162</v>
+      </c>
+      <c r="D59" s="5">
+        <v>948</v>
+      </c>
+      <c r="E59" s="5">
+        <v>6992</v>
+      </c>
+      <c r="F59" s="5">
+        <v>8310</v>
+      </c>
+      <c r="G59" s="5">
+        <v>5551</v>
+      </c>
+      <c r="H59" s="5">
+        <v>5394</v>
+      </c>
+      <c r="I59" s="5">
+        <v>826</v>
+      </c>
+      <c r="J59" s="5">
+        <v>129</v>
+      </c>
+      <c r="K59" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="5"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C62" s="5"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="6"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C63" s="5"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="5"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C64" s="5"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="5"/>
+    </row>
+    <row r="65" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C65" s="5"/>
+      <c r="D65" s="5"/>
+      <c r="E65" s="5"/>
+    </row>
+    <row r="66" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+      <c r="E66" s="5"/>
+    </row>
+    <row r="67" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+      <c r="E67" s="5"/>
+    </row>
+    <row r="68" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+    </row>
+    <row r="69" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-30 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78569DFE-C37A-F149-B96C-E28B441B8305}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D33E06-9D21-7D42-A324-F0C8C76B9DE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -1203,11 +1203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I121"/>
+  <dimension ref="A1:I116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G107" sqref="G107"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A117" sqref="A117:G144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1266,10 +1266,7 @@
       <c r="G2">
         <v>285</v>
       </c>
-      <c r="H2" s="5">
-        <f>D2/SUM(B2,D2:F2)</f>
-        <v>1.1278195488721804E-2</v>
-      </c>
+      <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
@@ -1293,10 +1290,7 @@
       <c r="G3">
         <v>313</v>
       </c>
-      <c r="H3" s="5">
-        <f t="shared" ref="H3:H66" si="0">D3/SUM(B3,D3:F3)</f>
-        <v>6.5789473684210523E-3</v>
-      </c>
+      <c r="H3" s="5"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -1320,10 +1314,7 @@
       <c r="G4">
         <v>340</v>
       </c>
-      <c r="H4" s="5">
-        <f t="shared" si="0"/>
-        <v>6.1538461538461538E-3</v>
-      </c>
+      <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -1347,10 +1338,7 @@
       <c r="G5">
         <v>364</v>
       </c>
-      <c r="H5" s="5">
-        <f t="shared" si="0"/>
-        <v>5.6179775280898875E-3</v>
-      </c>
+      <c r="H5" s="5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -1374,10 +1362,7 @@
       <c r="G6">
         <v>364</v>
       </c>
-      <c r="H6" s="5">
-        <f t="shared" si="0"/>
-        <v>5.6179775280898875E-3</v>
-      </c>
+      <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -1401,10 +1386,7 @@
       <c r="G7">
         <v>364</v>
       </c>
-      <c r="H7" s="5">
-        <f t="shared" si="0"/>
-        <v>5.6179775280898875E-3</v>
-      </c>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -1428,10 +1410,7 @@
       <c r="G8">
         <v>402</v>
       </c>
-      <c r="H8" s="5">
-        <f t="shared" si="0"/>
-        <v>4.9751243781094526E-3</v>
-      </c>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -1455,10 +1434,7 @@
       <c r="G9">
         <v>421</v>
       </c>
-      <c r="H9" s="5">
-        <f t="shared" si="0"/>
-        <v>4.7505938242280287E-3</v>
-      </c>
+      <c r="H9" s="5"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -1482,10 +1458,7 @@
       <c r="G10">
         <v>456</v>
       </c>
-      <c r="H10" s="5">
-        <f t="shared" si="0"/>
-        <v>4.5558086560364463E-3</v>
-      </c>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -1509,10 +1482,7 @@
       <c r="G11">
         <v>479</v>
       </c>
-      <c r="H11" s="5">
-        <f t="shared" si="0"/>
-        <v>2.1505376344086021E-3</v>
-      </c>
+      <c r="H11" s="5"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -1536,10 +1506,7 @@
       <c r="G12">
         <v>498</v>
       </c>
-      <c r="H12" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -1563,10 +1530,7 @@
       <c r="G13">
         <v>498</v>
       </c>
-      <c r="H13" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -1590,10 +1554,7 @@
       <c r="G14">
         <v>498</v>
       </c>
-      <c r="H14" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -1617,10 +1578,7 @@
       <c r="G15">
         <v>553</v>
       </c>
-      <c r="H15" s="5">
-        <f t="shared" si="0"/>
-        <v>1.838235294117647E-3</v>
-      </c>
+      <c r="H15" s="5"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -1644,10 +1602,7 @@
       <c r="G16">
         <v>593</v>
       </c>
-      <c r="H16" s="5">
-        <f t="shared" si="0"/>
-        <v>1.7482517482517483E-3</v>
-      </c>
+      <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
@@ -1671,10 +1626,7 @@
       <c r="G17">
         <v>629</v>
       </c>
-      <c r="H17" s="5">
-        <f t="shared" si="0"/>
-        <v>3.2520325203252032E-3</v>
-      </c>
+      <c r="H17" s="5"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
@@ -1698,10 +1650,7 @@
       <c r="G18">
         <v>699</v>
       </c>
-      <c r="H18" s="5">
-        <f t="shared" si="0"/>
-        <v>4.4247787610619468E-3</v>
-      </c>
+      <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
@@ -1725,10 +1674,7 @@
       <c r="G19">
         <v>699</v>
       </c>
-      <c r="H19" s="5">
-        <f t="shared" si="0"/>
-        <v>4.4247787610619468E-3</v>
-      </c>
+      <c r="H19" s="5"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
@@ -1752,10 +1698,7 @@
       <c r="G20">
         <v>768</v>
       </c>
-      <c r="H20" s="5">
-        <f t="shared" si="0"/>
-        <v>5.3619302949061663E-3</v>
-      </c>
+      <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
@@ -1779,10 +1722,7 @@
       <c r="G21">
         <v>768</v>
       </c>
-      <c r="H21" s="5">
-        <f t="shared" si="0"/>
-        <v>5.3619302949061663E-3</v>
-      </c>
+      <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
@@ -1806,10 +1746,7 @@
       <c r="G22">
         <v>1005</v>
       </c>
-      <c r="H22" s="5">
-        <f t="shared" si="0"/>
-        <v>1.5105740181268883E-2</v>
-      </c>
+      <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
@@ -1833,10 +1770,7 @@
       <c r="G23">
         <v>1126</v>
       </c>
-      <c r="H23" s="5">
-        <f t="shared" si="0"/>
-        <v>1.572617946345976E-2</v>
-      </c>
+      <c r="H23" s="5"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
@@ -1860,10 +1794,7 @@
       <c r="G24">
         <v>1338</v>
       </c>
-      <c r="H24" s="5">
-        <f t="shared" si="0"/>
-        <v>1.3754045307443365E-2</v>
-      </c>
+      <c r="H24" s="5"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
@@ -1887,10 +1818,7 @@
       <c r="G25">
         <v>1566</v>
       </c>
-      <c r="H25" s="5">
-        <f t="shared" si="0"/>
-        <v>1.2096774193548387E-2</v>
-      </c>
+      <c r="H25" s="5"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
@@ -1914,10 +1842,7 @@
       <c r="G26">
         <v>1763</v>
       </c>
-      <c r="H26" s="5">
-        <f t="shared" si="0"/>
-        <v>1.3010053222945003E-2</v>
-      </c>
+      <c r="H26" s="5"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
@@ -1941,10 +1866,7 @@
       <c r="G27">
         <v>1982</v>
       </c>
-      <c r="H27" s="5">
-        <f t="shared" si="0"/>
-        <v>1.2332990750256937E-2</v>
-      </c>
+      <c r="H27" s="5"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
@@ -1968,10 +1890,7 @@
       <c r="G28">
         <v>1982</v>
       </c>
-      <c r="H28" s="5">
-        <f t="shared" si="0"/>
-        <v>1.2332990750256937E-2</v>
-      </c>
+      <c r="H28" s="5"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
@@ -1995,10 +1914,7 @@
       <c r="G29">
         <v>2403</v>
       </c>
-      <c r="H29" s="5">
-        <f t="shared" si="0"/>
-        <v>1.25997480050399E-2</v>
-      </c>
+      <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
@@ -2022,10 +1938,7 @@
       <c r="G30">
         <v>2747</v>
       </c>
-      <c r="H30" s="5">
-        <f t="shared" si="0"/>
-        <v>1.1764705882352941E-2</v>
-      </c>
+      <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
@@ -2049,10 +1962,7 @@
       <c r="G31">
         <v>2747</v>
       </c>
-      <c r="H31" s="5">
-        <f t="shared" si="0"/>
-        <v>1.1764705882352941E-2</v>
-      </c>
+      <c r="H31" s="5"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
@@ -2076,10 +1986,7 @@
       <c r="G32">
         <v>3395</v>
       </c>
-      <c r="H32" s="5">
-        <f t="shared" si="0"/>
-        <v>1.2627986348122866E-2</v>
-      </c>
+      <c r="H32" s="5"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
@@ -2103,10 +2010,7 @@
       <c r="G33">
         <v>4185</v>
       </c>
-      <c r="H33" s="5">
-        <f t="shared" si="0"/>
-        <v>1.4798574952041656E-2</v>
-      </c>
+      <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
@@ -2130,10 +2034,7 @@
       <c r="G34">
         <v>5129</v>
       </c>
-      <c r="H34" s="5">
-        <f t="shared" si="0"/>
-        <v>1.6267311497032314E-2</v>
-      </c>
+      <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
@@ -2157,10 +2058,7 @@
       <c r="G35">
         <v>6648</v>
       </c>
-      <c r="H35" s="5">
-        <f t="shared" si="0"/>
-        <v>1.7165878437554738E-2</v>
-      </c>
+      <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
@@ -2184,10 +2082,7 @@
       <c r="G36">
         <v>8465</v>
       </c>
-      <c r="H36" s="5">
-        <f t="shared" si="0"/>
-        <v>1.9583158483704014E-2</v>
-      </c>
+      <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
@@ -2211,10 +2106,7 @@
       <c r="G37">
         <v>10178</v>
       </c>
-      <c r="H37" s="5">
-        <f t="shared" si="0"/>
-        <v>1.9905103575975004E-2</v>
-      </c>
+      <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
@@ -2238,10 +2130,7 @@
       <c r="G38">
         <v>11171</v>
       </c>
-      <c r="H38" s="5">
-        <f t="shared" si="0"/>
-        <v>1.9054560599750105E-2</v>
-      </c>
+      <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
@@ -2265,10 +2154,7 @@
       <c r="G39">
         <v>16650</v>
       </c>
-      <c r="H39" s="5">
-        <f t="shared" si="0"/>
-        <v>1.979807540621549E-2</v>
-      </c>
+      <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
@@ -2292,10 +2178,7 @@
       <c r="G40">
         <v>16650</v>
       </c>
-      <c r="H40" s="5">
-        <f t="shared" si="0"/>
-        <v>1.9796513920656202E-2</v>
-      </c>
+      <c r="H40" s="5"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
@@ -2319,10 +2202,7 @@
       <c r="G41">
         <v>23384</v>
       </c>
-      <c r="H41" s="5">
-        <f t="shared" si="0"/>
-        <v>2.2855373180551253E-2</v>
-      </c>
+      <c r="H41" s="5"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
@@ -2346,10 +2226,7 @@
       <c r="G42">
         <v>23384</v>
       </c>
-      <c r="H42" s="5">
-        <f t="shared" si="0"/>
-        <v>2.2793434499845153E-2</v>
-      </c>
+      <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
@@ -2373,10 +2250,7 @@
       <c r="G43">
         <v>26420</v>
       </c>
-      <c r="H43" s="5">
-        <f t="shared" si="0"/>
-        <v>2.2814109308378093E-2</v>
-      </c>
+      <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
@@ -2400,10 +2274,7 @@
       <c r="G44">
         <v>28506</v>
       </c>
-      <c r="H44" s="5">
-        <f t="shared" si="0"/>
-        <v>2.4341679526108814E-2</v>
-      </c>
+      <c r="H44" s="5"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
@@ -2427,10 +2298,7 @@
       <c r="G45">
         <v>32457</v>
       </c>
-      <c r="H45" s="5">
-        <f t="shared" si="0"/>
-        <v>2.5599785551534648E-2</v>
-      </c>
+      <c r="H45" s="5"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
@@ -2454,10 +2322,7 @@
       <c r="G46">
         <v>35635</v>
       </c>
-      <c r="H46" s="5">
-        <f t="shared" si="0"/>
-        <v>2.6684164479440071E-2</v>
-      </c>
+      <c r="H46" s="5"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
@@ -2481,10 +2346,7 @@
       <c r="G47">
         <v>35635</v>
       </c>
-      <c r="H47" s="5">
-        <f t="shared" si="0"/>
-        <v>2.6525093454227312E-2</v>
-      </c>
+      <c r="H47" s="5"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
@@ -2508,10 +2370,7 @@
       <c r="G48">
         <v>38550</v>
       </c>
-      <c r="H48" s="5">
-        <f t="shared" si="0"/>
-        <v>3.0342577487765091E-2</v>
-      </c>
+      <c r="H48" s="5"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
@@ -2535,10 +2394,7 @@
       <c r="G49">
         <v>38550</v>
       </c>
-      <c r="H49" s="5">
-        <f t="shared" si="0"/>
-        <v>3.0270074315751315E-2</v>
-      </c>
+      <c r="H49" s="5"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
@@ -2562,10 +2418,7 @@
       <c r="G50">
         <v>41032</v>
       </c>
-      <c r="H50" s="5">
-        <f t="shared" si="0"/>
-        <v>3.1233850129198968E-2</v>
-      </c>
+      <c r="H50" s="5"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
@@ -2589,10 +2442,7 @@
       <c r="G51">
         <v>43072</v>
       </c>
-      <c r="H51" s="5">
-        <f t="shared" si="0"/>
-        <v>3.2515123313168914E-2</v>
-      </c>
+      <c r="H51" s="5"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
@@ -2616,10 +2466,7 @@
       <c r="G52">
         <v>43072</v>
       </c>
-      <c r="H52" s="5">
-        <f t="shared" si="0"/>
-        <v>3.2486040018613306E-2</v>
-      </c>
+      <c r="H52" s="5"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
@@ -2643,10 +2490,7 @@
       <c r="G53">
         <v>49186</v>
       </c>
-      <c r="H53" s="5">
-        <f t="shared" si="0"/>
-        <v>3.1582708110039298E-2</v>
-      </c>
+      <c r="H53" s="5"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
@@ -2670,10 +2514,7 @@
       <c r="G54">
         <v>49186</v>
       </c>
-      <c r="H54" s="5">
-        <f t="shared" si="0"/>
-        <v>3.15350720495415E-2</v>
-      </c>
+      <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
@@ -2697,10 +2538,7 @@
       <c r="G55">
         <v>54112</v>
       </c>
-      <c r="H55" s="5">
-        <f t="shared" si="0"/>
-        <v>3.5203565753905201E-2</v>
-      </c>
+      <c r="H55" s="5"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
@@ -2725,10 +2563,7 @@
         <f>51629+C53</f>
         <v>58832</v>
       </c>
-      <c r="H56" s="5">
-        <f t="shared" si="0"/>
-        <v>3.8477346119972597E-2</v>
-      </c>
+      <c r="H56" s="5"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
@@ -2752,10 +2587,7 @@
       <c r="G57">
         <v>61009</v>
       </c>
-      <c r="H57" s="5">
-        <f t="shared" si="0"/>
-        <v>4.133116770916128E-2</v>
-      </c>
+      <c r="H57" s="5"/>
       <c r="I57" s="5"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
@@ -2780,10 +2612,7 @@
       <c r="G58">
         <v>64785</v>
       </c>
-      <c r="H58" s="5">
-        <f t="shared" si="0"/>
-        <v>4.4522021902348045E-2</v>
-      </c>
+      <c r="H58" s="5"/>
       <c r="I58" s="5"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -2808,10 +2637,7 @@
       <c r="G59">
         <v>67998</v>
       </c>
-      <c r="H59" s="5">
-        <f t="shared" si="0"/>
-        <v>4.8761853399847198E-2</v>
-      </c>
+      <c r="H59" s="5"/>
       <c r="I59" s="5"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
@@ -2836,10 +2662,7 @@
       <c r="G60">
         <v>72674</v>
       </c>
-      <c r="H60" s="5">
-        <f t="shared" si="0"/>
-        <v>5.0884521573355011E-2</v>
-      </c>
+      <c r="H60" s="5"/>
       <c r="I60" s="5"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
@@ -2864,10 +2687,7 @@
       <c r="G61">
         <v>76027</v>
       </c>
-      <c r="H61" s="5">
-        <f t="shared" si="0"/>
-        <v>5.3806998374330409E-2</v>
-      </c>
+      <c r="H61" s="5"/>
       <c r="I61" s="5"/>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
@@ -2892,10 +2712,7 @@
       <c r="G62">
         <v>79125</v>
       </c>
-      <c r="H62" s="5">
-        <f t="shared" si="0"/>
-        <v>5.4938388625592416E-2</v>
-      </c>
+      <c r="H62" s="5"/>
       <c r="I62" s="5"/>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
@@ -2920,10 +2737,7 @@
       <c r="G63">
         <v>82055</v>
       </c>
-      <c r="H63" s="5">
-        <f t="shared" si="0"/>
-        <v>5.8084656604886681E-2</v>
-      </c>
+      <c r="H63" s="5"/>
       <c r="I63" s="5"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
@@ -2948,10 +2762,7 @@
       <c r="G64">
         <v>85703</v>
       </c>
-      <c r="H64" s="5">
-        <f t="shared" si="0"/>
-        <v>6.2363329038663845E-2</v>
-      </c>
+      <c r="H64" s="5"/>
       <c r="I64" s="5"/>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.2">
@@ -2976,10 +2787,7 @@
       <c r="G65">
         <v>89906</v>
       </c>
-      <c r="H65" s="5">
-        <f t="shared" si="0"/>
-        <v>6.4928183273580006E-2</v>
-      </c>
+      <c r="H65" s="5"/>
       <c r="I65" s="5"/>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.2">
@@ -3004,10 +2812,7 @@
       <c r="G66">
         <v>94271</v>
       </c>
-      <c r="H66" s="5">
-        <f t="shared" si="0"/>
-        <v>6.7301155676410609E-2</v>
-      </c>
+      <c r="H66" s="5"/>
       <c r="I66" s="5"/>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.2">
@@ -3032,10 +2837,7 @@
       <c r="G67">
         <v>97838</v>
       </c>
-      <c r="H67" s="5">
-        <f t="shared" ref="H67:H115" si="1">D67/SUM(B67,D67:F67)</f>
-        <v>6.9019216993179061E-2</v>
-      </c>
+      <c r="H67" s="5"/>
       <c r="I67" s="5"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.2">
@@ -3060,10 +2862,7 @@
       <c r="G68">
         <v>104784</v>
       </c>
-      <c r="H68" s="5">
-        <f t="shared" si="1"/>
-        <v>6.832743663064024E-2</v>
-      </c>
+      <c r="H68" s="5"/>
       <c r="I68" s="5"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.2">
@@ -3088,10 +2887,7 @@
       <c r="G69">
         <v>109764</v>
       </c>
-      <c r="H69" s="5">
-        <f t="shared" si="1"/>
-        <v>6.9019680310449971E-2</v>
-      </c>
+      <c r="H69" s="5"/>
       <c r="I69" s="5"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.2">
@@ -3116,10 +2912,7 @@
       <c r="G70">
         <v>115189</v>
       </c>
-      <c r="H70" s="5">
-        <f t="shared" si="1"/>
-        <v>7.0329495410410142E-2</v>
-      </c>
+      <c r="H70" s="5"/>
       <c r="I70" s="5"/>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.2">
@@ -3144,10 +2937,7 @@
       <c r="G71">
         <v>123521</v>
       </c>
-      <c r="H71" s="5">
-        <f t="shared" si="1"/>
-        <v>6.8385132892382669E-2</v>
-      </c>
+      <c r="H71" s="5"/>
       <c r="I71" s="5"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.2">
@@ -3172,10 +2962,7 @@
       <c r="G72">
         <v>132416</v>
       </c>
-      <c r="H72" s="5">
-        <f t="shared" si="1"/>
-        <v>6.9956984378537465E-2</v>
-      </c>
+      <c r="H72" s="5"/>
       <c r="I72" s="5"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.2">
@@ -3200,10 +2987,7 @@
       <c r="G73" s="5">
         <v>142985</v>
       </c>
-      <c r="H73" s="5">
-        <f t="shared" si="1"/>
-        <v>6.9529607568325158E-2</v>
-      </c>
+      <c r="H73" s="5"/>
       <c r="I73" s="5"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.2">
@@ -3228,10 +3012,7 @@
       <c r="G74" s="5">
         <v>153287</v>
       </c>
-      <c r="H74" s="5">
-        <f t="shared" si="1"/>
-        <v>6.8349106203995799E-2</v>
-      </c>
+      <c r="H74" s="5"/>
       <c r="I74" s="5"/>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.2">
@@ -3256,10 +3037,7 @@
       <c r="G75" s="5">
         <v>161833</v>
       </c>
-      <c r="H75" s="5">
-        <f t="shared" si="1"/>
-        <v>6.7765556032466992E-2</v>
-      </c>
+      <c r="H75" s="5"/>
       <c r="I75" s="5"/>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.2">
@@ -3284,10 +3062,7 @@
       <c r="G76" s="5">
         <v>168639</v>
       </c>
-      <c r="H76" s="5">
-        <f t="shared" si="1"/>
-        <v>6.7847609803445771E-2</v>
-      </c>
+      <c r="H76" s="5"/>
       <c r="I76" s="5"/>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.2">
@@ -3312,10 +3087,7 @@
       <c r="G77">
         <v>179716</v>
       </c>
-      <c r="H77" s="5">
-        <f t="shared" si="1"/>
-        <v>6.737670092438422E-2</v>
-      </c>
+      <c r="H77" s="5"/>
       <c r="I77" s="5"/>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.2">
@@ -3340,10 +3112,7 @@
       <c r="G78" s="5">
         <v>191376</v>
       </c>
-      <c r="H78" s="5">
-        <f t="shared" si="1"/>
-        <v>6.6357414201407894E-2</v>
-      </c>
+      <c r="H78" s="5"/>
       <c r="I78" s="5"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.2">
@@ -3368,10 +3137,7 @@
       <c r="G79" s="5">
         <v>201502</v>
       </c>
-      <c r="H79" s="5">
-        <f t="shared" si="1"/>
-        <v>6.6132634984210126E-2</v>
-      </c>
+      <c r="H79" s="5"/>
       <c r="I79" s="5"/>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.2">
@@ -3396,10 +3162,7 @@
       <c r="G80" s="5">
         <v>212454</v>
       </c>
-      <c r="H80" s="5">
-        <f t="shared" si="1"/>
-        <v>6.5296561051004634E-2</v>
-      </c>
+      <c r="H80" s="5"/>
       <c r="I80" s="5"/>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.2">
@@ -3424,10 +3187,7 @@
       <c r="G81" s="5">
         <v>225789</v>
       </c>
-      <c r="H81" s="5">
-        <f t="shared" si="1"/>
-        <v>6.4309937597073777E-2</v>
-      </c>
+      <c r="H81" s="5"/>
       <c r="I81" s="5"/>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.2">
@@ -3452,10 +3212,7 @@
       <c r="G82" s="5">
         <v>237055</v>
       </c>
-      <c r="H82" s="5">
-        <f t="shared" si="1"/>
-        <v>6.2846741392975025E-2</v>
-      </c>
+      <c r="H82" s="5"/>
       <c r="I82" s="5"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.2">
@@ -3480,10 +3237,7 @@
       <c r="G83" s="5">
         <v>247189</v>
       </c>
-      <c r="H83" s="5">
-        <f t="shared" si="1"/>
-        <v>6.1340776586783823E-2</v>
-      </c>
+      <c r="H83" s="5"/>
       <c r="I83" s="5"/>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.2">
@@ -3508,10 +3262,7 @@
       <c r="G84" s="5">
         <v>259322</v>
       </c>
-      <c r="H84" s="5">
-        <f t="shared" si="1"/>
-        <v>6.0784856149225422E-2</v>
-      </c>
+      <c r="H84" s="5"/>
       <c r="I84" s="5"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.2">
@@ -3536,10 +3287,7 @@
       <c r="G85" s="5">
         <v>274124</v>
       </c>
-      <c r="H85" s="5">
-        <f t="shared" si="1"/>
-        <v>5.9442013046403168E-2</v>
-      </c>
+      <c r="H85" s="5"/>
       <c r="I85" s="5"/>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.2">
@@ -3564,10 +3312,7 @@
       <c r="G86" s="5">
         <v>289381</v>
       </c>
-      <c r="H86" s="5">
-        <f t="shared" si="1"/>
-        <v>5.8326907416348973E-2</v>
-      </c>
+      <c r="H86" s="5"/>
       <c r="I86" s="5"/>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.2">
@@ -3592,10 +3337,7 @@
       <c r="G87" s="5">
         <v>306029</v>
       </c>
-      <c r="H87" s="5">
-        <f t="shared" si="1"/>
-        <v>5.6479422146952597E-2</v>
-      </c>
+      <c r="H87" s="5"/>
       <c r="I87" s="5"/>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.2">
@@ -3620,10 +3362,7 @@
       <c r="G88" s="5">
         <v>323188</v>
       </c>
-      <c r="H88" s="5">
-        <f t="shared" si="1"/>
-        <v>5.5158703308104483E-2</v>
-      </c>
+      <c r="H88" s="5"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
@@ -3647,10 +3386,7 @@
       <c r="G89" s="5">
         <v>337290</v>
       </c>
-      <c r="H89" s="5">
-        <f t="shared" si="1"/>
-        <v>5.3596128303384678E-2</v>
-      </c>
+      <c r="H89" s="5"/>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
@@ -3674,10 +3410,7 @@
       <c r="G90" s="5">
         <v>348325</v>
       </c>
-      <c r="H90" s="5">
-        <f t="shared" si="1"/>
-        <v>5.2397240250248493E-2</v>
-      </c>
+      <c r="H90" s="5"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
@@ -3701,10 +3434,7 @@
       <c r="G91" s="5">
         <v>358737</v>
       </c>
-      <c r="H91" s="5">
-        <f t="shared" si="1"/>
-        <v>5.1911747194610933E-2</v>
-      </c>
+      <c r="H91" s="5"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
@@ -3728,10 +3458,7 @@
       <c r="G92" s="5">
         <v>374465</v>
       </c>
-      <c r="H92" s="5">
-        <f t="shared" si="1"/>
-        <v>5.1198468585492582E-2</v>
-      </c>
+      <c r="H92" s="5"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
@@ -3755,10 +3482,7 @@
       <c r="G93" s="5">
         <v>393866</v>
       </c>
-      <c r="H93" s="5">
-        <f t="shared" si="1"/>
-        <v>5.0205590593770839E-2</v>
-      </c>
+      <c r="H93" s="5"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
@@ -3782,10 +3506,7 @@
       <c r="G94" s="5">
         <v>411790</v>
       </c>
-      <c r="H94" s="5">
-        <f t="shared" si="1"/>
-        <v>4.9346718737803698E-2</v>
-      </c>
+      <c r="H94" s="5"/>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
@@ -3809,10 +3530,7 @@
       <c r="G95" s="5">
         <v>431683</v>
       </c>
-      <c r="H95" s="5">
-        <f t="shared" si="1"/>
-        <v>4.7899014352412242E-2</v>
-      </c>
+      <c r="H95" s="5"/>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
@@ -3836,10 +3554,7 @@
       <c r="G96" s="5">
         <v>448810</v>
       </c>
-      <c r="H96" s="5">
-        <f t="shared" si="1"/>
-        <v>4.6631981087296138E-2</v>
-      </c>
+      <c r="H96" s="5"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
@@ -3863,10 +3578,7 @@
       <c r="G97" s="5">
         <v>456982</v>
       </c>
-      <c r="H97" s="5">
-        <f t="shared" si="1"/>
-        <v>4.5865292746738576E-2</v>
-      </c>
+      <c r="H97" s="5"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
@@ -3890,10 +3602,7 @@
       <c r="G98" s="5">
         <v>470732</v>
       </c>
-      <c r="H98" s="5">
-        <f t="shared" si="1"/>
-        <v>4.5457806884225772E-2</v>
-      </c>
+      <c r="H98" s="5"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
@@ -3917,10 +3626,7 @@
       <c r="G99" s="5">
         <v>488453</v>
       </c>
-      <c r="H99" s="5">
-        <f t="shared" si="1"/>
-        <v>4.470191008255834E-2</v>
-      </c>
+      <c r="H99" s="5"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
@@ -3944,10 +3650,7 @@
       <c r="G100" s="5">
         <v>510065</v>
       </c>
-      <c r="H100" s="5">
-        <f t="shared" si="1"/>
-        <v>4.3643791612773535E-2</v>
-      </c>
+      <c r="H100" s="5"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
@@ -3971,10 +3674,7 @@
       <c r="G101" s="5">
         <v>525214</v>
       </c>
-      <c r="H101" s="5">
-        <f t="shared" si="1"/>
-        <v>4.2913548442666115E-2</v>
-      </c>
+      <c r="H101" s="5"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
@@ -3998,10 +3698,7 @@
       <c r="G102" s="5">
         <v>539174</v>
       </c>
-      <c r="H102" s="5">
-        <f t="shared" si="1"/>
-        <v>4.2210783395666737E-2</v>
-      </c>
+      <c r="H102" s="5"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
@@ -4025,10 +3722,7 @@
       <c r="G103" s="5">
         <v>549240</v>
       </c>
-      <c r="H103" s="5">
-        <f t="shared" si="1"/>
-        <v>4.1578412190313975E-2</v>
-      </c>
+      <c r="H103" s="5"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
@@ -4052,10 +3746,7 @@
       <c r="G104" s="5">
         <v>563136</v>
       </c>
-      <c r="H104" s="5">
-        <f t="shared" si="1"/>
-        <v>4.1440049387975401E-2</v>
-      </c>
+      <c r="H104" s="5"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
@@ -4079,10 +3770,7 @@
       <c r="G105" s="5">
         <v>562088</v>
       </c>
-      <c r="H105" s="5">
-        <f t="shared" si="1"/>
-        <v>4.1772509173017218E-2</v>
-      </c>
+      <c r="H105" s="5"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
@@ -4106,10 +3794,7 @@
       <c r="G106" s="5">
         <v>571620</v>
       </c>
-      <c r="H106" s="5">
-        <f t="shared" si="1"/>
-        <v>4.1916442162573876E-2</v>
-      </c>
+      <c r="H106" s="5"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
@@ -4133,10 +3818,7 @@
       <c r="G107" s="5">
         <v>582733</v>
       </c>
-      <c r="H107" s="5">
-        <f t="shared" si="1"/>
-        <v>4.1869055985819185E-2</v>
-      </c>
+      <c r="H107" s="5"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
@@ -4160,10 +3842,7 @@
       <c r="G108" s="5">
         <v>600234</v>
       </c>
-      <c r="H108" s="5">
-        <f t="shared" si="1"/>
-        <v>4.1816224586473057E-2</v>
-      </c>
+      <c r="H108" s="5"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
@@ -4187,10 +3866,7 @@
       <c r="G109" s="5">
         <v>605857</v>
       </c>
-      <c r="H109" s="5">
-        <f t="shared" si="1"/>
-        <v>4.1734307133833123E-2</v>
-      </c>
+      <c r="H109" s="5"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
@@ -4214,10 +3890,7 @@
       <c r="G110" s="5">
         <v>614585</v>
       </c>
-      <c r="H110" s="5">
-        <f t="shared" si="1"/>
-        <v>4.1709671246006913E-2</v>
-      </c>
+      <c r="H110" s="5"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
@@ -4241,10 +3914,7 @@
       <c r="G111" s="5">
         <v>623422</v>
       </c>
-      <c r="H111" s="5">
-        <f t="shared" si="1"/>
-        <v>4.1811734208823011E-2</v>
-      </c>
+      <c r="H111" s="5"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
@@ -4268,10 +3938,7 @@
       <c r="G112" s="5">
         <v>636375</v>
       </c>
-      <c r="H112" s="5">
-        <f t="shared" si="1"/>
-        <v>4.1611721378933424E-2</v>
-      </c>
+      <c r="H112" s="5"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
@@ -4295,10 +3962,7 @@
       <c r="G113" s="5">
         <v>656364</v>
       </c>
-      <c r="H113" s="5">
-        <f t="shared" si="1"/>
-        <v>4.1087771721844954E-2</v>
-      </c>
+      <c r="H113" s="5"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
@@ -4322,10 +3986,7 @@
       <c r="G114" s="5">
         <v>674030</v>
       </c>
-      <c r="H114" s="5">
-        <f t="shared" si="1"/>
-        <v>4.0573152793425174E-2</v>
-      </c>
+      <c r="H114" s="5"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
@@ -4349,45 +4010,30 @@
       <c r="G115" s="5">
         <v>694038</v>
       </c>
-      <c r="H115" s="5">
-        <f t="shared" si="1"/>
-        <v>3.9974320061937428E-2</v>
-      </c>
+      <c r="H115" s="5"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C116" s="5"/>
-      <c r="D116" s="5"/>
-      <c r="E116" s="5"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B117" s="5"/>
-      <c r="C117" s="5"/>
-      <c r="D117" s="6"/>
-      <c r="E117" s="5"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B118" s="5"/>
-      <c r="C118" s="5"/>
-      <c r="D118" s="5"/>
-      <c r="E118" s="5"/>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B119" s="5"/>
-      <c r="C119" s="6"/>
-      <c r="D119" s="6"/>
-      <c r="E119" s="5"/>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B120" s="5"/>
-      <c r="C120" s="5"/>
-      <c r="D120" s="6"/>
-      <c r="E120" s="5"/>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B121" s="5"/>
-      <c r="C121" s="6"/>
-      <c r="D121" s="6"/>
-      <c r="E121" s="5"/>
+      <c r="A116" s="1">
+        <v>43981.4375</v>
+      </c>
+      <c r="B116" s="5">
+        <v>650194</v>
+      </c>
+      <c r="C116" s="5">
+        <v>12760</v>
+      </c>
+      <c r="D116" s="5">
+        <v>27533</v>
+      </c>
+      <c r="E116" s="5">
+        <v>21353</v>
+      </c>
+      <c r="F116" s="5">
+        <v>2247</v>
+      </c>
+      <c r="G116" s="5">
+        <v>714087</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4396,11 +4042,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N69"/>
+  <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N49" sqref="N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6467,56 +6113,119 @@
         <v>100</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
+    <row r="60" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>43981.4375</v>
+      </c>
+      <c r="B60" s="5">
+        <v>12001</v>
+      </c>
+      <c r="C60" s="5">
+        <v>15302</v>
+      </c>
+      <c r="D60" s="5">
+        <v>977</v>
+      </c>
+      <c r="E60" s="5">
+        <v>7113</v>
+      </c>
+      <c r="F60" s="5">
+        <v>8417</v>
+      </c>
+      <c r="G60" s="5">
+        <v>5594</v>
+      </c>
+      <c r="H60" s="5">
+        <v>5414</v>
+      </c>
+      <c r="I60" s="5">
+        <v>801</v>
+      </c>
+      <c r="J60" s="5">
+        <v>121</v>
+      </c>
+      <c r="K60" s="5">
+        <v>84</v>
+      </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C61" s="5"/>
       <c r="D61" s="5"/>
       <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C62" s="5"/>
-      <c r="D62" s="6"/>
+      <c r="D62" s="5"/>
       <c r="E62" s="5"/>
-      <c r="F62" s="6"/>
+      <c r="F62" s="5"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C63" s="5"/>
-      <c r="D63" s="6"/>
-      <c r="E63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C64" s="5"/>
-      <c r="D64" s="6"/>
-      <c r="E64" s="5"/>
-    </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D64" s="5"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="5"/>
+    </row>
+    <row r="65" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
-    </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="F65" s="5"/>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C66" s="5"/>
       <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-    </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E66" s="6"/>
+      <c r="F66" s="5"/>
+    </row>
+    <row r="67" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C67" s="5"/>
       <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-    </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E67" s="6"/>
+      <c r="F67" s="5"/>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-    </row>
-    <row r="69" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E68" s="6"/>
+      <c r="F68" s="5"/>
+    </row>
+    <row r="69" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="5"/>
+    </row>
+    <row r="70" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+    </row>
+    <row r="71" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D71" s="5"/>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+    </row>
+    <row r="72" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D72" s="5"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="6"/>
+    </row>
+    <row r="73" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D73" s="5"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="5"/>
+    </row>
+    <row r="74" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="D74" s="5"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-05-31 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D33E06-9D21-7D42-A324-F0C8C76B9DE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05ECC9EE-75DE-EE46-BB16-8197DC5D217C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="20000" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -1203,11 +1203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I116"/>
+  <dimension ref="A1:I117"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A115" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A117" sqref="A117:G144"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D129" sqref="D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4035,6 +4035,29 @@
         <v>714087</v>
       </c>
     </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A117" s="1">
+        <v>43982.4375</v>
+      </c>
+      <c r="B117" s="5">
+        <v>666406</v>
+      </c>
+      <c r="C117" s="5">
+        <v>9647</v>
+      </c>
+      <c r="D117" s="5">
+        <v>27859</v>
+      </c>
+      <c r="E117" s="5">
+        <v>21810</v>
+      </c>
+      <c r="F117" s="5">
+        <v>2266</v>
+      </c>
+      <c r="G117" s="5">
+        <v>727988</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4044,9 +4067,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
   <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N49" sqref="N49"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6149,9 +6172,39 @@
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
+      <c r="A61" s="1">
+        <v>43982.4375</v>
+      </c>
+      <c r="B61" s="5">
+        <v>12163</v>
+      </c>
+      <c r="C61" s="5">
+        <v>15461</v>
+      </c>
+      <c r="D61" s="5">
+        <v>989</v>
+      </c>
+      <c r="E61" s="5">
+        <v>7244</v>
+      </c>
+      <c r="F61" s="5">
+        <v>8521</v>
+      </c>
+      <c r="G61" s="5">
+        <v>5644</v>
+      </c>
+      <c r="H61" s="5">
+        <v>5443</v>
+      </c>
+      <c r="I61" s="5">
+        <v>781</v>
+      </c>
+      <c r="J61" s="5">
+        <v>118</v>
+      </c>
+      <c r="K61" s="5">
+        <v>90</v>
+      </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C62" s="5"/>
@@ -6166,63 +6219,69 @@
       <c r="F63" s="5"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C64" s="5"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
       <c r="D64" s="5"/>
       <c r="E64" s="6"/>
       <c r="F64" s="5"/>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C65" s="5"/>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C66" s="5"/>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B66" s="3"/>
+      <c r="C66" s="3"/>
       <c r="D66" s="5"/>
       <c r="E66" s="6"/>
       <c r="F66" s="5"/>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C67" s="5"/>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B67" s="3"/>
+      <c r="C67" s="3"/>
       <c r="D67" s="5"/>
       <c r="E67" s="6"/>
       <c r="F67" s="5"/>
     </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C68" s="5"/>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
       <c r="D68" s="5"/>
       <c r="E68" s="6"/>
       <c r="F68" s="5"/>
     </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C69" s="5"/>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B69" s="3"/>
+      <c r="C69" s="3"/>
       <c r="D69" s="5"/>
       <c r="E69" s="6"/>
       <c r="F69" s="5"/>
     </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D70" s="5"/>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
     </row>
-    <row r="71" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D71" s="5"/>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
     </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D72" s="5"/>
       <c r="E72" s="6"/>
       <c r="F72" s="5"/>
       <c r="G72" s="6"/>
     </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D73" s="5"/>
       <c r="E73" s="6"/>
       <c r="F73" s="5"/>
     </row>
-    <row r="74" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D74" s="5"/>
       <c r="E74" s="6"/>
       <c r="F74" s="5"/>

</xml_diff>

<commit_message>
excel update 2020-06-01 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05ECC9EE-75DE-EE46-BB16-8197DC5D217C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6EF9EC-9BCA-574A-962E-D7AB9D98D748}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -402,7 +402,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -420,6 +420,33 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -442,11 +469,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -454,8 +482,14 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1203,11 +1237,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I117"/>
+  <dimension ref="A1:J140"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A95" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D129" sqref="D129"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A118" sqref="A118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1221,7 +1255,7 @@
     <col min="7" max="7" width="54.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1244,7 +1278,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43872.645833333336</v>
       </c>
@@ -1268,7 +1302,7 @@
       </c>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43873.645833333336</v>
       </c>
@@ -1292,7 +1326,7 @@
       </c>
       <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43874.645833333336</v>
       </c>
@@ -1315,8 +1349,10 @@
         <v>340</v>
       </c>
       <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43875.645833333336</v>
       </c>
@@ -1339,8 +1375,10 @@
         <v>364</v>
       </c>
       <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43875.645833333336</v>
       </c>
@@ -1363,8 +1401,10 @@
         <v>364</v>
       </c>
       <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43875.645833333336</v>
       </c>
@@ -1387,8 +1427,10 @@
         <v>364</v>
       </c>
       <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43878.645833333336</v>
       </c>
@@ -1411,8 +1453,10 @@
         <v>402</v>
       </c>
       <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43879.645833333336</v>
       </c>
@@ -1435,8 +1479,10 @@
         <v>421</v>
       </c>
       <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43880.645833333336</v>
       </c>
@@ -1459,8 +1505,10 @@
         <v>456</v>
       </c>
       <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43881.645833333336</v>
       </c>
@@ -1483,8 +1531,10 @@
         <v>479</v>
       </c>
       <c r="H11" s="5"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43882.645833333336</v>
       </c>
@@ -1507,8 +1557,10 @@
         <v>498</v>
       </c>
       <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43882.645833333336</v>
       </c>
@@ -1531,8 +1583,10 @@
         <v>498</v>
       </c>
       <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43882.645833333336</v>
       </c>
@@ -1555,8 +1609,10 @@
         <v>498</v>
       </c>
       <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43885.645833333336</v>
       </c>
@@ -1579,8 +1635,10 @@
         <v>553</v>
       </c>
       <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43886.645833333336</v>
       </c>
@@ -1603,8 +1661,10 @@
         <v>593</v>
       </c>
       <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43887.645833333336</v>
       </c>
@@ -1627,8 +1687,10 @@
         <v>629</v>
       </c>
       <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43888.645833333336</v>
       </c>
@@ -1651,8 +1713,10 @@
         <v>699</v>
       </c>
       <c r="H18" s="5"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43888.645833333336</v>
       </c>
@@ -1675,8 +1739,10 @@
         <v>699</v>
       </c>
       <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43889.645833333336</v>
       </c>
@@ -1699,8 +1765,10 @@
         <v>768</v>
       </c>
       <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43889.645833333336</v>
       </c>
@@ -1723,8 +1791,10 @@
         <v>768</v>
       </c>
       <c r="H21" s="5"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43892.645833333336</v>
       </c>
@@ -1747,8 +1817,10 @@
         <v>1005</v>
       </c>
       <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43893.645833333336</v>
       </c>
@@ -1771,8 +1843,10 @@
         <v>1126</v>
       </c>
       <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43894.645833333336</v>
       </c>
@@ -1795,8 +1869,10 @@
         <v>1338</v>
       </c>
       <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43895.645833333336</v>
       </c>
@@ -1819,8 +1895,10 @@
         <v>1566</v>
       </c>
       <c r="H25" s="5"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43896.645833333336</v>
       </c>
@@ -1843,8 +1921,10 @@
         <v>1763</v>
       </c>
       <c r="H26" s="5"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43897.604166666664</v>
       </c>
@@ -1867,8 +1947,10 @@
         <v>1982</v>
       </c>
       <c r="H27" s="5"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43897.645833333336</v>
       </c>
@@ -1891,8 +1973,10 @@
         <v>1982</v>
       </c>
       <c r="H28" s="5"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43899.604166666664</v>
       </c>
@@ -1915,8 +1999,10 @@
         <v>2403</v>
       </c>
       <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43900.604166666664</v>
       </c>
@@ -1939,8 +2025,10 @@
         <v>2747</v>
       </c>
       <c r="H30" s="5"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>43900.604166666664</v>
       </c>
@@ -1963,8 +2051,10 @@
         <v>2747</v>
       </c>
       <c r="H31" s="5"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>43901.604166666664</v>
       </c>
@@ -1987,8 +2077,10 @@
         <v>3395</v>
       </c>
       <c r="H32" s="5"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43902.604166666664</v>
       </c>
@@ -2011,8 +2103,10 @@
         <v>4185</v>
       </c>
       <c r="H33" s="5"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43903.604166666664</v>
       </c>
@@ -2035,8 +2129,10 @@
         <v>5129</v>
       </c>
       <c r="H34" s="5"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>43904.895833333336</v>
       </c>
@@ -2059,8 +2155,10 @@
         <v>6648</v>
       </c>
       <c r="H35" s="5"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>43905.895833333336</v>
       </c>
@@ -2083,8 +2181,10 @@
         <v>8465</v>
       </c>
       <c r="H36" s="5"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>43906.895833333336</v>
       </c>
@@ -2107,8 +2207,10 @@
         <v>10178</v>
       </c>
       <c r="H37" s="5"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>43907.895833333336</v>
       </c>
@@ -2131,8 +2233,10 @@
         <v>11171</v>
       </c>
       <c r="H38" s="5"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>43909.604166666664</v>
       </c>
@@ -2155,8 +2259,10 @@
         <v>16650</v>
       </c>
       <c r="H39" s="5"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>43909.895833333336</v>
       </c>
@@ -2179,8 +2285,10 @@
         <v>16650</v>
       </c>
       <c r="H40" s="5"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>43911.604166666664</v>
       </c>
@@ -2203,8 +2311,10 @@
         <v>23384</v>
       </c>
       <c r="H41" s="5"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>43911.895833333336</v>
       </c>
@@ -2227,8 +2337,10 @@
         <v>23384</v>
       </c>
       <c r="H42" s="5"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>43912.895833333336</v>
       </c>
@@ -2251,8 +2363,10 @@
         <v>26420</v>
       </c>
       <c r="H43" s="5"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43913.4375</v>
       </c>
@@ -2275,8 +2389,10 @@
         <v>28506</v>
       </c>
       <c r="H44" s="5"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43914.4375</v>
       </c>
@@ -2299,8 +2415,10 @@
         <v>32457</v>
       </c>
       <c r="H45" s="5"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>43915.4375</v>
       </c>
@@ -2323,8 +2441,10 @@
         <v>35635</v>
       </c>
       <c r="H46" s="5"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>43915.729166666664</v>
       </c>
@@ -2347,8 +2467,10 @@
         <v>35635</v>
       </c>
       <c r="H47" s="5"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>43916.4375</v>
       </c>
@@ -2371,8 +2493,10 @@
         <v>38550</v>
       </c>
       <c r="H48" s="5"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>43916.729166666664</v>
       </c>
@@ -2395,8 +2519,10 @@
         <v>38550</v>
       </c>
       <c r="H49" s="5"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>43917.4375</v>
       </c>
@@ -2419,8 +2545,10 @@
         <v>41032</v>
       </c>
       <c r="H50" s="5"/>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>43918.4375</v>
       </c>
@@ -2443,8 +2571,10 @@
         <v>43072</v>
       </c>
       <c r="H51" s="5"/>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>43918.729166666664</v>
       </c>
@@ -2467,8 +2597,10 @@
         <v>43072</v>
       </c>
       <c r="H52" s="5"/>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>43919.4375</v>
       </c>
@@ -2491,8 +2623,10 @@
         <v>49186</v>
       </c>
       <c r="H53" s="5"/>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>43919.729166666664</v>
       </c>
@@ -2515,8 +2649,10 @@
         <v>49186</v>
       </c>
       <c r="H54" s="5"/>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>43920.4375</v>
       </c>
@@ -2539,8 +2675,10 @@
         <v>54112</v>
       </c>
       <c r="H55" s="5"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>43921.4375</v>
       </c>
@@ -2564,8 +2702,10 @@
         <v>58832</v>
       </c>
       <c r="H56" s="5"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I56" s="5"/>
+      <c r="J56" s="5"/>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>43922.4375</v>
       </c>
@@ -2589,8 +2729,9 @@
       </c>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J57" s="5"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>43923.4375</v>
       </c>
@@ -2614,8 +2755,9 @@
       </c>
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J58" s="5"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>43924.4375</v>
       </c>
@@ -2639,8 +2781,9 @@
       </c>
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J59" s="5"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>43925.4375</v>
       </c>
@@ -2664,8 +2807,9 @@
       </c>
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J60" s="5"/>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>43926.4375</v>
       </c>
@@ -2689,8 +2833,9 @@
       </c>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J61" s="5"/>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>43927.4375</v>
       </c>
@@ -2714,8 +2859,9 @@
       </c>
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J62" s="5"/>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>43928.4375</v>
       </c>
@@ -2739,8 +2885,9 @@
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J63" s="5"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>43929.4375</v>
       </c>
@@ -2764,8 +2911,9 @@
       </c>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J64" s="5"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>43930.4375</v>
       </c>
@@ -2789,8 +2937,9 @@
       </c>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J65" s="5"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>43931.4375</v>
       </c>
@@ -2814,8 +2963,9 @@
       </c>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J66" s="5"/>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>43932.4375</v>
       </c>
@@ -2839,8 +2989,9 @@
       </c>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J67" s="5"/>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>43933.4375</v>
       </c>
@@ -2864,8 +3015,9 @@
       </c>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J68" s="5"/>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>43934.4375</v>
       </c>
@@ -2889,8 +3041,9 @@
       </c>
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J69" s="5"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>43935.4375</v>
       </c>
@@ -2914,8 +3067,9 @@
       </c>
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J70" s="5"/>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>43936.4375</v>
       </c>
@@ -2939,8 +3093,9 @@
       </c>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J71" s="5"/>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>43937.4375</v>
       </c>
@@ -2964,8 +3119,9 @@
       </c>
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J72" s="5"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>43938.4375</v>
       </c>
@@ -2989,8 +3145,9 @@
       </c>
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J73" s="5"/>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>43939.4375</v>
       </c>
@@ -3014,8 +3171,9 @@
       </c>
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J74" s="5"/>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>43940.4375</v>
       </c>
@@ -3039,8 +3197,9 @@
       </c>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J75" s="5"/>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>43941.4375</v>
       </c>
@@ -3064,8 +3223,9 @@
       </c>
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J76" s="5"/>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>43942.4375</v>
       </c>
@@ -3089,8 +3249,9 @@
       </c>
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J77" s="5"/>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>43943.4375</v>
       </c>
@@ -3114,8 +3275,9 @@
       </c>
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J78" s="5"/>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>43944.4375</v>
       </c>
@@ -3139,8 +3301,9 @@
       </c>
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J79" s="5"/>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>43945.4375</v>
       </c>
@@ -3164,8 +3327,9 @@
       </c>
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J80" s="5"/>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>43946.4375</v>
       </c>
@@ -3189,8 +3353,9 @@
       </c>
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J81" s="5"/>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>43947.4375</v>
       </c>
@@ -3214,8 +3379,9 @@
       </c>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J82" s="5"/>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>43948.4375</v>
       </c>
@@ -3239,8 +3405,9 @@
       </c>
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J83" s="5"/>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>43949.4375</v>
       </c>
@@ -3264,8 +3431,9 @@
       </c>
       <c r="H84" s="5"/>
       <c r="I84" s="5"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J84" s="5"/>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>43950.4375</v>
       </c>
@@ -3289,8 +3457,9 @@
       </c>
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J85" s="5"/>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>43951.4375</v>
       </c>
@@ -3314,8 +3483,9 @@
       </c>
       <c r="H86" s="5"/>
       <c r="I86" s="5"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J86" s="5"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>43952.4375</v>
       </c>
@@ -3339,8 +3509,9 @@
       </c>
       <c r="H87" s="5"/>
       <c r="I87" s="5"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J87" s="5"/>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>43953.4375</v>
       </c>
@@ -3363,8 +3534,10 @@
         <v>323188</v>
       </c>
       <c r="H88" s="5"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I88" s="5"/>
+      <c r="J88" s="5"/>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>43954.4375</v>
       </c>
@@ -3387,8 +3560,10 @@
         <v>337290</v>
       </c>
       <c r="H89" s="5"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I89" s="5"/>
+      <c r="J89" s="5"/>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>43955.4375</v>
       </c>
@@ -3411,8 +3586,10 @@
         <v>348325</v>
       </c>
       <c r="H90" s="5"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I90" s="5"/>
+      <c r="J90" s="5"/>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>43956.4375</v>
       </c>
@@ -3435,8 +3612,10 @@
         <v>358737</v>
       </c>
       <c r="H91" s="5"/>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I91" s="5"/>
+      <c r="J91" s="5"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>43957.4375</v>
       </c>
@@ -3459,8 +3638,10 @@
         <v>374465</v>
       </c>
       <c r="H92" s="5"/>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I92" s="5"/>
+      <c r="J92" s="5"/>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>43958.4375</v>
       </c>
@@ -3483,8 +3664,10 @@
         <v>393866</v>
       </c>
       <c r="H93" s="5"/>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I93" s="5"/>
+      <c r="J93" s="5"/>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>43959.4375</v>
       </c>
@@ -3507,8 +3690,10 @@
         <v>411790</v>
       </c>
       <c r="H94" s="5"/>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I94" s="5"/>
+      <c r="J94" s="5"/>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>43960.4375</v>
       </c>
@@ -3531,8 +3716,10 @@
         <v>431683</v>
       </c>
       <c r="H95" s="5"/>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I95" s="5"/>
+      <c r="J95" s="5"/>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>43961.4375</v>
       </c>
@@ -3555,8 +3742,10 @@
         <v>448810</v>
       </c>
       <c r="H96" s="5"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I96" s="5"/>
+      <c r="J96" s="5"/>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>43962.4375</v>
       </c>
@@ -3579,8 +3768,10 @@
         <v>456982</v>
       </c>
       <c r="H97" s="5"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I97" s="5"/>
+      <c r="J97" s="5"/>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>43963.4375</v>
       </c>
@@ -3603,8 +3794,10 @@
         <v>470732</v>
       </c>
       <c r="H98" s="5"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I98" s="5"/>
+      <c r="J98" s="5"/>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>43964.4375</v>
       </c>
@@ -3627,8 +3820,10 @@
         <v>488453</v>
       </c>
       <c r="H99" s="5"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I99" s="5"/>
+      <c r="J99" s="5"/>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>43965.4375</v>
       </c>
@@ -3651,8 +3846,10 @@
         <v>510065</v>
       </c>
       <c r="H100" s="5"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I100" s="5"/>
+      <c r="J100" s="5"/>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>43966.4375</v>
       </c>
@@ -3675,8 +3872,10 @@
         <v>525214</v>
       </c>
       <c r="H101" s="5"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I101" s="5"/>
+      <c r="J101" s="5"/>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>43967.4375</v>
       </c>
@@ -3699,8 +3898,10 @@
         <v>539174</v>
       </c>
       <c r="H102" s="5"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I102" s="5"/>
+      <c r="J102" s="5"/>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>43968.4375</v>
       </c>
@@ -3723,8 +3924,10 @@
         <v>549240</v>
       </c>
       <c r="H103" s="5"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I103" s="5"/>
+      <c r="J103" s="5"/>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>43969.4375</v>
       </c>
@@ -3747,8 +3950,10 @@
         <v>563136</v>
       </c>
       <c r="H104" s="5"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I104" s="5"/>
+      <c r="J104" s="5"/>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>43970.4375</v>
       </c>
@@ -3771,8 +3976,10 @@
         <v>562088</v>
       </c>
       <c r="H105" s="5"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I105" s="5"/>
+      <c r="J105" s="5"/>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>43971.4375</v>
       </c>
@@ -3795,8 +4002,10 @@
         <v>571620</v>
       </c>
       <c r="H106" s="5"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I106" s="5"/>
+      <c r="J106" s="5"/>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>43972.4375</v>
       </c>
@@ -3819,8 +4028,10 @@
         <v>582733</v>
       </c>
       <c r="H107" s="5"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I107" s="5"/>
+      <c r="J107" s="5"/>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>43973.4375</v>
       </c>
@@ -3843,8 +4054,10 @@
         <v>600234</v>
       </c>
       <c r="H108" s="5"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I108" s="5"/>
+      <c r="J108" s="5"/>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>43974.4375</v>
       </c>
@@ -3867,8 +4080,10 @@
         <v>605857</v>
       </c>
       <c r="H109" s="5"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I109" s="5"/>
+      <c r="J109" s="5"/>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>43975.4375</v>
       </c>
@@ -3891,8 +4106,10 @@
         <v>614585</v>
       </c>
       <c r="H110" s="5"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I110" s="5"/>
+      <c r="J110" s="5"/>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>43976.4375</v>
       </c>
@@ -3915,8 +4132,10 @@
         <v>623422</v>
       </c>
       <c r="H111" s="5"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I111" s="5"/>
+      <c r="J111" s="5"/>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>43977.4375</v>
       </c>
@@ -3939,8 +4158,10 @@
         <v>636375</v>
       </c>
       <c r="H112" s="5"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I112" s="5"/>
+      <c r="J112" s="5"/>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>43978.4375</v>
       </c>
@@ -3963,8 +4184,10 @@
         <v>656364</v>
       </c>
       <c r="H113" s="5"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I113" s="5"/>
+      <c r="J113" s="5"/>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>43979.4375</v>
       </c>
@@ -3987,8 +4210,10 @@
         <v>674030</v>
       </c>
       <c r="H114" s="5"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I114" s="5"/>
+      <c r="J114" s="5"/>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>43980.4375</v>
       </c>
@@ -4011,8 +4236,10 @@
         <v>694038</v>
       </c>
       <c r="H115" s="5"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I115" s="5"/>
+      <c r="J115" s="5"/>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>43981.4375</v>
       </c>
@@ -4034,8 +4261,11 @@
       <c r="G116" s="5">
         <v>714087</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H116" s="5"/>
+      <c r="I116" s="5"/>
+      <c r="J116" s="5"/>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>43982.4375</v>
       </c>
@@ -4057,6 +4287,101 @@
       <c r="G117" s="5">
         <v>727988</v>
       </c>
+      <c r="H117" s="5"/>
+      <c r="I117" s="5"/>
+      <c r="J117" s="5"/>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A118" s="1">
+        <v>43983.4375</v>
+      </c>
+      <c r="B118" s="5">
+        <v>680028</v>
+      </c>
+      <c r="C118" s="5">
+        <v>6427</v>
+      </c>
+      <c r="D118" s="5">
+        <v>28263</v>
+      </c>
+      <c r="E118" s="5">
+        <v>22153</v>
+      </c>
+      <c r="F118" s="5">
+        <v>2276</v>
+      </c>
+      <c r="G118" s="5">
+        <v>739147</v>
+      </c>
+      <c r="H118" s="5"/>
+      <c r="I118" s="5"/>
+      <c r="J118" s="5"/>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B119" s="5"/>
+      <c r="C119" s="6"/>
+      <c r="D119" s="5"/>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B120" s="5"/>
+      <c r="C120" s="5"/>
+      <c r="D120" s="5"/>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B121" s="5"/>
+      <c r="C121" s="6"/>
+      <c r="D121" s="5"/>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B122" s="5"/>
+      <c r="C122" s="6"/>
+      <c r="D122" s="5"/>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B123" s="5"/>
+      <c r="C123" s="6"/>
+      <c r="D123" s="5"/>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B124" s="5"/>
+      <c r="C124" s="6"/>
+      <c r="D124" s="5"/>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B125" s="5"/>
+      <c r="C125" s="6"/>
+      <c r="D125" s="5"/>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B126" s="5"/>
+      <c r="C126" s="5"/>
+      <c r="D126" s="5"/>
+    </row>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B136" s="5"/>
+      <c r="C136" s="5"/>
+      <c r="D136" s="5"/>
+    </row>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B137" s="5"/>
+      <c r="C137" s="5"/>
+      <c r="D137" s="5"/>
+    </row>
+    <row r="138" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B138" s="5"/>
+      <c r="C138" s="6"/>
+      <c r="D138" s="5"/>
+      <c r="E138" s="6"/>
+    </row>
+    <row r="139" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B139" s="5"/>
+      <c r="C139" s="6"/>
+      <c r="D139" s="5"/>
+    </row>
+    <row r="140" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B140" s="5"/>
+      <c r="C140" s="6"/>
+      <c r="D140" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4067,9 +4392,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
   <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4210,6 +4535,7 @@
       <c r="K4">
         <v>152</v>
       </c>
+      <c r="L4" s="4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -4245,6 +4571,7 @@
       <c r="K5">
         <v>154</v>
       </c>
+      <c r="L5" s="4"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -4280,6 +4607,7 @@
       <c r="K6">
         <v>160</v>
       </c>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -4315,6 +4643,7 @@
       <c r="K7">
         <v>187</v>
       </c>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -4350,6 +4679,7 @@
       <c r="K8">
         <v>195</v>
       </c>
+      <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
@@ -4385,6 +4715,7 @@
       <c r="K9">
         <v>214</v>
       </c>
+      <c r="L9" s="4"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
@@ -4420,6 +4751,7 @@
       <c r="K10">
         <v>217</v>
       </c>
+      <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
@@ -4455,6 +4787,7 @@
       <c r="K11">
         <v>215</v>
       </c>
+      <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
@@ -4490,6 +4823,7 @@
       <c r="K12">
         <v>196</v>
       </c>
+      <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
@@ -4525,6 +4859,7 @@
       <c r="K13">
         <v>203</v>
       </c>
+      <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
@@ -4560,6 +4895,7 @@
       <c r="K14">
         <v>199</v>
       </c>
+      <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
@@ -4595,6 +4931,7 @@
       <c r="K15">
         <v>188</v>
       </c>
+      <c r="L15" s="4"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
@@ -4630,8 +4967,9 @@
       <c r="K16">
         <v>200</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L16" s="4"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43938.4375</v>
       </c>
@@ -4665,8 +5003,9 @@
       <c r="K17" s="5">
         <v>200</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L17" s="4"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43939.4375</v>
       </c>
@@ -4700,8 +5039,9 @@
       <c r="K18" s="5">
         <v>197</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43940.4375</v>
       </c>
@@ -4735,8 +5075,9 @@
       <c r="K19" s="5">
         <v>196</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43941.4375</v>
       </c>
@@ -4770,8 +5111,9 @@
       <c r="K20" s="5">
         <v>193</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L20" s="4"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43942.4375</v>
       </c>
@@ -4805,8 +5147,9 @@
       <c r="K21" s="5">
         <v>194</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L21" s="4"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43943.4375</v>
       </c>
@@ -4840,8 +5183,9 @@
       <c r="K22" s="5">
         <v>192</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L22" s="4"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43944.4375</v>
       </c>
@@ -4875,8 +5219,9 @@
       <c r="K23" s="5">
         <v>185</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L23" s="4"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43945.4375</v>
       </c>
@@ -4910,8 +5255,9 @@
       <c r="K24" s="5">
         <v>193</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L24" s="4"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43946.4375</v>
       </c>
@@ -4945,8 +5291,9 @@
       <c r="K25" s="5">
         <v>195</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L25" s="4"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43947.4375</v>
       </c>
@@ -4980,8 +5327,9 @@
       <c r="K26" s="5">
         <v>195</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L26" s="4"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43948.4375</v>
       </c>
@@ -5015,8 +5363,9 @@
       <c r="K27" s="5">
         <v>191</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27" s="4"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43949.4375</v>
       </c>
@@ -5050,8 +5399,9 @@
       <c r="K28" s="5">
         <v>187</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L28" s="4"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43950.4375</v>
       </c>
@@ -5085,8 +5435,9 @@
       <c r="K29" s="5">
         <v>186</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L29" s="4"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43951.4375</v>
       </c>
@@ -5120,8 +5471,9 @@
       <c r="K30" s="5">
         <v>181</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L30" s="4"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>43952.4375</v>
       </c>
@@ -5155,8 +5507,9 @@
       <c r="K31" s="5">
         <v>175</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L31" s="4"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>43953.4375</v>
       </c>
@@ -5190,8 +5543,9 @@
       <c r="K32" s="5">
         <v>154</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L32" s="4"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43954.4375</v>
       </c>
@@ -5225,8 +5579,9 @@
       <c r="K33" s="5">
         <v>174</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L33" s="4"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43955.4375</v>
       </c>
@@ -5260,8 +5615,9 @@
       <c r="K34" s="5">
         <v>175</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L34" s="4"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>43956.4375</v>
       </c>
@@ -5295,8 +5651,9 @@
       <c r="K35" s="5">
         <v>166</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L35" s="4"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>43957.4375</v>
       </c>
@@ -5330,8 +5687,9 @@
       <c r="K36" s="5">
         <v>174</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L36" s="4"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>43958.4375</v>
       </c>
@@ -5365,8 +5723,9 @@
       <c r="K37" s="5">
         <v>155</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L37" s="4"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>43959.4375</v>
       </c>
@@ -5400,8 +5759,9 @@
       <c r="K38" s="5">
         <v>166</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L38" s="4"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>43960.4375</v>
       </c>
@@ -5435,8 +5795,9 @@
       <c r="K39" s="5">
         <v>158</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L39" s="4"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>43961.4375</v>
       </c>
@@ -5470,8 +5831,9 @@
       <c r="K40" s="5">
         <v>140</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L40" s="4"/>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>43962.4375</v>
       </c>
@@ -5505,8 +5867,9 @@
       <c r="K41" s="5">
         <v>147</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L41" s="4"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>43963.4375</v>
       </c>
@@ -5540,8 +5903,9 @@
       <c r="K42" s="5">
         <v>146</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L42" s="4"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>43964.4375</v>
       </c>
@@ -5575,8 +5939,9 @@
       <c r="K43" s="5">
         <v>144</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L43" s="4"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43965.4375</v>
       </c>
@@ -5610,8 +5975,9 @@
       <c r="K44" s="5">
         <v>141</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L44" s="4"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43966.4375</v>
       </c>
@@ -5645,8 +6011,9 @@
       <c r="K45" s="5">
         <v>135</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L45" s="4"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>43967.4375</v>
       </c>
@@ -5680,8 +6047,9 @@
       <c r="K46" s="5">
         <v>135</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L46" s="4"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>43968.4375</v>
       </c>
@@ -5715,8 +6083,9 @@
       <c r="K47" s="5">
         <v>129</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L47" s="4"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>43969.4375</v>
       </c>
@@ -5750,8 +6119,9 @@
       <c r="K48" s="5">
         <v>133</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L48" s="4"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>43970.4375</v>
       </c>
@@ -5785,8 +6155,9 @@
       <c r="K49" s="5">
         <v>123</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L49" s="4"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>43971.4375</v>
       </c>
@@ -5820,8 +6191,9 @@
       <c r="K50" s="5">
         <v>120</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L50" s="4"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>43972.4375</v>
       </c>
@@ -5855,8 +6227,9 @@
       <c r="K51" s="5">
         <v>117</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L51" s="4"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>43973.4375</v>
       </c>
@@ -5890,8 +6263,9 @@
       <c r="K52" s="5">
         <v>120</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L52" s="4"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>43974.4375</v>
       </c>
@@ -5925,8 +6299,9 @@
       <c r="K53" s="5">
         <v>119</v>
       </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L53" s="4"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>43975.4375</v>
       </c>
@@ -5960,8 +6335,9 @@
       <c r="K54" s="5">
         <v>104</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L54" s="4"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>43976.4375</v>
       </c>
@@ -5995,8 +6371,9 @@
       <c r="K55" s="5">
         <v>114</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L55" s="4"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>43977.4375</v>
       </c>
@@ -6030,8 +6407,9 @@
       <c r="K56" s="5">
         <v>113</v>
       </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L56" s="4"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>43978.4375</v>
       </c>
@@ -6065,8 +6443,9 @@
       <c r="K57" s="5">
         <v>117</v>
       </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L57" s="4"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>43979.4375</v>
       </c>
@@ -6100,8 +6479,9 @@
       <c r="K58" s="5">
         <v>94</v>
       </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L58" s="4"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>43980.4375</v>
       </c>
@@ -6135,8 +6515,9 @@
       <c r="K59" s="5">
         <v>100</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="L59" s="4"/>
+    </row>
+    <row r="60" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>43981.4375</v>
       </c>
@@ -6170,8 +6551,9 @@
       <c r="K60" s="5">
         <v>84</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L60" s="4"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>43982.4375</v>
       </c>
@@ -6205,88 +6587,143 @@
       <c r="K61" s="5">
         <v>90</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L61" s="4"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>43983.4375</v>
+      </c>
+      <c r="B62" s="5">
+        <v>12386</v>
+      </c>
+      <c r="C62" s="5">
+        <v>15638</v>
+      </c>
+      <c r="D62" s="5">
+        <v>1013</v>
+      </c>
+      <c r="E62" s="5">
+        <v>7406</v>
+      </c>
+      <c r="F62" s="5">
+        <v>8651</v>
+      </c>
+      <c r="G62" s="5">
+        <v>5705</v>
+      </c>
+      <c r="H62" s="5">
+        <v>5471</v>
+      </c>
+      <c r="I62" s="5">
+        <v>781</v>
+      </c>
+      <c r="J62" s="5">
+        <v>125</v>
+      </c>
+      <c r="K62" s="5">
+        <v>89</v>
+      </c>
+      <c r="L62" s="4"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B63" s="5"/>
       <c r="C63" s="5"/>
       <c r="D63" s="5"/>
-      <c r="E63" s="6"/>
+      <c r="E63" s="5"/>
       <c r="F63" s="5"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B64" s="3"/>
-      <c r="C64" s="3"/>
+      <c r="C64" s="5"/>
       <c r="D64" s="5"/>
-      <c r="E64" s="6"/>
+      <c r="E64" s="5"/>
       <c r="F64" s="5"/>
-    </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I64" s="11"/>
+      <c r="J64" s="11"/>
+      <c r="K64" s="11"/>
+    </row>
+    <row r="65" spans="2:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B65" s="3"/>
-      <c r="C65" s="3"/>
+      <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="5"/>
       <c r="F65" s="5"/>
-    </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I65" s="7"/>
+      <c r="J65" s="7"/>
+      <c r="K65" s="7"/>
+    </row>
+    <row r="66" spans="2:11" ht="23" x14ac:dyDescent="0.3">
       <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="6"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="5"/>
       <c r="F66" s="5"/>
-    </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I66" s="8"/>
+      <c r="J66" s="9"/>
+      <c r="K66" s="10"/>
+    </row>
+    <row r="67" spans="2:11" ht="23" x14ac:dyDescent="0.3">
       <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="6"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="5"/>
       <c r="F67" s="5"/>
-    </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I67" s="8"/>
+      <c r="J67" s="9"/>
+      <c r="K67" s="10"/>
+    </row>
+    <row r="68" spans="2:11" ht="23" x14ac:dyDescent="0.3">
       <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="6"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="5"/>
       <c r="F68" s="5"/>
-    </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="I68" s="8"/>
+      <c r="J68" s="9"/>
+      <c r="K68" s="10"/>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="6"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="5"/>
       <c r="F69" s="5"/>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D70" s="5"/>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C70" s="5"/>
+      <c r="D70" s="6"/>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D71" s="5"/>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C71" s="5"/>
+      <c r="D71" s="6"/>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="D72" s="5"/>
-      <c r="E72" s="6"/>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="C72" s="5"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="5"/>
       <c r="F72" s="5"/>
       <c r="G72" s="6"/>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D73" s="5"/>
       <c r="E73" s="6"/>
       <c r="F73" s="5"/>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D74" s="5"/>
       <c r="E74" s="6"/>
       <c r="F74" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I64:K64"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
excel update 2020-06-02 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6EF9EC-9BCA-574A-962E-D7AB9D98D748}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915FF2BE-824D-D241-BF37-60FDCCCF2018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -486,6 +486,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
@@ -1237,11 +1238,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:J140"/>
+  <dimension ref="A1:J138"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A118" sqref="A118"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B127" sqref="B127:D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4318,70 +4319,66 @@
       <c r="J118" s="5"/>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B119" s="5"/>
-      <c r="C119" s="6"/>
-      <c r="D119" s="5"/>
+      <c r="A119" s="1">
+        <v>43984.4375</v>
+      </c>
+      <c r="B119" s="11">
+        <v>694478</v>
+      </c>
+      <c r="C119" s="11">
+        <v>10622</v>
+      </c>
+      <c r="D119" s="11">
+        <v>28709</v>
+      </c>
+      <c r="E119" s="11">
+        <v>22484</v>
+      </c>
+      <c r="F119" s="11">
+        <v>2293</v>
+      </c>
+      <c r="G119" s="11">
+        <v>758586</v>
+      </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B120" s="5"/>
-      <c r="C120" s="5"/>
-      <c r="D120" s="5"/>
+      <c r="B120" s="11"/>
+      <c r="C120" s="11"/>
+      <c r="D120" s="11"/>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B121" s="5"/>
+      <c r="B121" s="11"/>
       <c r="C121" s="6"/>
-      <c r="D121" s="5"/>
+      <c r="D121" s="11"/>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B122" s="5"/>
+      <c r="B122" s="11"/>
       <c r="C122" s="6"/>
-      <c r="D122" s="5"/>
+      <c r="D122" s="11"/>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B123" s="5"/>
+      <c r="B123" s="11"/>
       <c r="C123" s="6"/>
-      <c r="D123" s="5"/>
+      <c r="D123" s="11"/>
+      <c r="E123" s="6"/>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B124" s="5"/>
+      <c r="B124" s="11"/>
       <c r="C124" s="6"/>
-      <c r="D124" s="5"/>
+      <c r="D124" s="11"/>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B125" s="5"/>
+      <c r="B125" s="11"/>
       <c r="C125" s="6"/>
-      <c r="D125" s="5"/>
+      <c r="D125" s="11"/>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B126" s="5"/>
-      <c r="C126" s="5"/>
-      <c r="D126" s="5"/>
-    </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B136" s="5"/>
-      <c r="C136" s="5"/>
-      <c r="D136" s="5"/>
-    </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B137" s="5"/>
-      <c r="C137" s="5"/>
-      <c r="D137" s="5"/>
-    </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B138" s="5"/>
-      <c r="C138" s="6"/>
-      <c r="D138" s="5"/>
+      <c r="B126" s="11"/>
+      <c r="C126" s="11"/>
+      <c r="D126" s="11"/>
+    </row>
+    <row r="138" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E138" s="6"/>
-    </row>
-    <row r="139" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B139" s="5"/>
-      <c r="C139" s="6"/>
-      <c r="D139" s="5"/>
-    </row>
-    <row r="140" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B140" s="5"/>
-      <c r="C140" s="6"/>
-      <c r="D140" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4390,11 +4387,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N74"/>
+  <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6626,13 +6623,39 @@
       <c r="L62" s="4"/>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
+      <c r="A63" s="1">
+        <v>43984.4375</v>
+      </c>
+      <c r="B63" s="11">
+        <v>12658</v>
+      </c>
+      <c r="C63" s="11">
+        <v>15811</v>
+      </c>
+      <c r="D63" s="11">
+        <v>1047</v>
+      </c>
+      <c r="E63" s="11">
+        <v>7601</v>
+      </c>
+      <c r="F63" s="11">
+        <v>8789</v>
+      </c>
+      <c r="G63" s="11">
+        <v>5766</v>
+      </c>
+      <c r="H63" s="11">
+        <v>5488</v>
+      </c>
+      <c r="I63" s="11">
+        <v>801</v>
+      </c>
+      <c r="J63" s="11">
+        <v>125</v>
+      </c>
+      <c r="K63" s="11">
+        <v>87</v>
+      </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B64" s="3"/>
@@ -6640,85 +6663,109 @@
       <c r="D64" s="5"/>
       <c r="E64" s="5"/>
       <c r="F64" s="5"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="11"/>
-      <c r="K64" s="11"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="12"/>
+      <c r="K64" s="12"/>
     </row>
     <row r="65" spans="2:11" ht="20" x14ac:dyDescent="0.2">
       <c r="B65" s="3"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
       <c r="I65" s="7"/>
       <c r="J65" s="7"/>
       <c r="K65" s="7"/>
     </row>
     <row r="66" spans="2:11" ht="23" x14ac:dyDescent="0.3">
       <c r="B66" s="3"/>
-      <c r="C66" s="5"/>
+      <c r="C66" s="11"/>
       <c r="D66" s="6"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
       <c r="I66" s="8"/>
       <c r="J66" s="9"/>
       <c r="K66" s="10"/>
     </row>
     <row r="67" spans="2:11" ht="23" x14ac:dyDescent="0.3">
       <c r="B67" s="3"/>
-      <c r="C67" s="5"/>
+      <c r="C67" s="11"/>
       <c r="D67" s="6"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
       <c r="I67" s="8"/>
       <c r="J67" s="9"/>
       <c r="K67" s="10"/>
     </row>
     <row r="68" spans="2:11" ht="23" x14ac:dyDescent="0.3">
       <c r="B68" s="3"/>
-      <c r="C68" s="5"/>
+      <c r="C68" s="11"/>
       <c r="D68" s="6"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11"/>
       <c r="I68" s="8"/>
       <c r="J68" s="9"/>
       <c r="K68" s="10"/>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B69" s="3"/>
-      <c r="C69" s="5"/>
+      <c r="C69" s="11"/>
       <c r="D69" s="6"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11"/>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C70" s="5"/>
+      <c r="C70" s="11"/>
       <c r="D70" s="6"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="11"/>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C71" s="5"/>
+      <c r="C71" s="11"/>
       <c r="D71" s="6"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C72" s="5"/>
+      <c r="C72" s="11"/>
       <c r="D72" s="6"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="5"/>
-      <c r="G72" s="6"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="11"/>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D73" s="5"/>
       <c r="E73" s="6"/>
-      <c r="F73" s="5"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="11"/>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.2">
       <c r="D74" s="5"/>
       <c r="E74" s="6"/>
-      <c r="F74" s="5"/>
+      <c r="F74" s="11"/>
+      <c r="G74" s="11"/>
+      <c r="H74" s="11"/>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="F75" s="11"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
excel update 2020-06-03 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915FF2BE-824D-D241-BF37-60FDCCCF2018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96C6146-0517-D946-9813-043C6B645313}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -1238,11 +1238,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:J138"/>
+  <dimension ref="A1:J120"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B127" sqref="B127:D137"/>
+      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A119" sqref="A119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4342,43 +4342,27 @@
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B120" s="11"/>
-      <c r="C120" s="11"/>
-      <c r="D120" s="11"/>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B121" s="11"/>
-      <c r="C121" s="6"/>
-      <c r="D121" s="11"/>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B122" s="11"/>
-      <c r="C122" s="6"/>
-      <c r="D122" s="11"/>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B123" s="11"/>
-      <c r="C123" s="6"/>
-      <c r="D123" s="11"/>
-      <c r="E123" s="6"/>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B124" s="11"/>
-      <c r="C124" s="6"/>
-      <c r="D124" s="11"/>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B125" s="11"/>
-      <c r="C125" s="6"/>
-      <c r="D125" s="11"/>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B126" s="11"/>
-      <c r="C126" s="11"/>
-      <c r="D126" s="11"/>
-    </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.2">
-      <c r="E138" s="6"/>
+      <c r="A120" s="1">
+        <v>43985.4375</v>
+      </c>
+      <c r="B120" s="12">
+        <v>711331</v>
+      </c>
+      <c r="C120" s="12">
+        <v>11636</v>
+      </c>
+      <c r="D120" s="12">
+        <v>29047</v>
+      </c>
+      <c r="E120" s="12">
+        <v>22811</v>
+      </c>
+      <c r="F120" s="12">
+        <v>2312</v>
+      </c>
+      <c r="G120" s="12">
+        <v>777137</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4390,8 +4374,8 @@
   <dimension ref="A1:N75"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A64" sqref="A64"/>
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6658,19 +6642,44 @@
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B64" s="3"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
-      <c r="I64" s="12"/>
-      <c r="J64" s="12"/>
-      <c r="K64" s="12"/>
+      <c r="A64" s="1">
+        <v>43985.4375</v>
+      </c>
+      <c r="B64" s="12">
+        <v>12851</v>
+      </c>
+      <c r="C64" s="12">
+        <v>15956</v>
+      </c>
+      <c r="D64" s="12">
+        <v>1068</v>
+      </c>
+      <c r="E64" s="12">
+        <v>7728</v>
+      </c>
+      <c r="F64" s="12">
+        <v>8912</v>
+      </c>
+      <c r="G64" s="12">
+        <v>5816</v>
+      </c>
+      <c r="H64" s="12">
+        <v>5506</v>
+      </c>
+      <c r="I64" s="12">
+        <v>791</v>
+      </c>
+      <c r="J64" s="12">
+        <v>127</v>
+      </c>
+      <c r="K64" s="12">
+        <v>92</v>
+      </c>
     </row>
     <row r="65" spans="2:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B65" s="3"/>
-      <c r="C65" s="11"/>
-      <c r="D65" s="11"/>
+      <c r="B65" s="12"/>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
       <c r="E65" s="11"/>
       <c r="F65" s="11"/>
       <c r="G65" s="11"/>
@@ -6680,9 +6689,9 @@
       <c r="K65" s="7"/>
     </row>
     <row r="66" spans="2:11" ht="23" x14ac:dyDescent="0.3">
-      <c r="B66" s="3"/>
-      <c r="C66" s="11"/>
-      <c r="D66" s="6"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="12"/>
       <c r="E66" s="11"/>
       <c r="F66" s="11"/>
       <c r="G66" s="11"/>
@@ -6692,9 +6701,9 @@
       <c r="K66" s="10"/>
     </row>
     <row r="67" spans="2:11" ht="23" x14ac:dyDescent="0.3">
-      <c r="B67" s="3"/>
-      <c r="C67" s="11"/>
-      <c r="D67" s="6"/>
+      <c r="B67" s="12"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="12"/>
       <c r="E67" s="11"/>
       <c r="F67" s="11"/>
       <c r="G67" s="11"/>
@@ -6704,9 +6713,9 @@
       <c r="K67" s="10"/>
     </row>
     <row r="68" spans="2:11" ht="23" x14ac:dyDescent="0.3">
-      <c r="B68" s="3"/>
-      <c r="C68" s="11"/>
-      <c r="D68" s="6"/>
+      <c r="B68" s="12"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="12"/>
       <c r="E68" s="11"/>
       <c r="F68" s="11"/>
       <c r="G68" s="11"/>
@@ -6716,33 +6725,36 @@
       <c r="K68" s="10"/>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B69" s="3"/>
-      <c r="C69" s="11"/>
-      <c r="D69" s="6"/>
+      <c r="B69" s="12"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="12"/>
       <c r="E69" s="11"/>
       <c r="F69" s="11"/>
       <c r="G69" s="11"/>
       <c r="H69" s="11"/>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C70" s="11"/>
-      <c r="D70" s="6"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="12"/>
       <c r="E70" s="11"/>
       <c r="F70" s="11"/>
       <c r="G70" s="11"/>
       <c r="H70" s="11"/>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C71" s="11"/>
-      <c r="D71" s="6"/>
+      <c r="B71" s="12"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="12"/>
       <c r="E71" s="11"/>
       <c r="F71" s="11"/>
       <c r="G71" s="11"/>
       <c r="H71" s="11"/>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="C72" s="11"/>
-      <c r="D72" s="6"/>
+      <c r="B72" s="12"/>
+      <c r="C72" s="6"/>
+      <c r="D72" s="12"/>
       <c r="E72" s="11"/>
       <c r="F72" s="11"/>
       <c r="G72" s="11"/>
@@ -6768,9 +6780,6 @@
       <c r="H75" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="I64:K64"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
excel update 2020-06-04 + 2020-06-05
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96C6146-0517-D946-9813-043C6B645313}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F34652-9044-8846-A14E-01BBB233606E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -402,7 +402,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -420,33 +420,6 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color rgb="FF222222"/>
-      <name val="Consolas"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF222222"/>
-      <name val="Consolas"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -469,28 +442,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -1238,11 +1204,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:J120"/>
+  <dimension ref="A1:J122"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A117" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A119" sqref="A119"/>
+      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C130" sqref="C130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4322,22 +4288,22 @@
       <c r="A119" s="1">
         <v>43984.4375</v>
       </c>
-      <c r="B119" s="11">
+      <c r="B119" s="6">
         <v>694478</v>
       </c>
-      <c r="C119" s="11">
+      <c r="C119" s="6">
         <v>10622</v>
       </c>
-      <c r="D119" s="11">
+      <c r="D119" s="6">
         <v>28709</v>
       </c>
-      <c r="E119" s="11">
+      <c r="E119" s="6">
         <v>22484</v>
       </c>
-      <c r="F119" s="11">
+      <c r="F119" s="6">
         <v>2293</v>
       </c>
-      <c r="G119" s="11">
+      <c r="G119" s="6">
         <v>758586</v>
       </c>
     </row>
@@ -4345,23 +4311,69 @@
       <c r="A120" s="1">
         <v>43985.4375</v>
       </c>
-      <c r="B120" s="12">
+      <c r="B120" s="7">
         <v>711331</v>
       </c>
-      <c r="C120" s="12">
+      <c r="C120" s="7">
         <v>11636</v>
       </c>
-      <c r="D120" s="12">
+      <c r="D120" s="7">
         <v>29047</v>
       </c>
-      <c r="E120" s="12">
+      <c r="E120" s="7">
         <v>22811</v>
       </c>
-      <c r="F120" s="12">
+      <c r="F120" s="7">
         <v>2312</v>
       </c>
-      <c r="G120" s="12">
+      <c r="G120" s="7">
         <v>777137</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A121" s="1">
+        <v>43986.4375</v>
+      </c>
+      <c r="B121" s="7">
+        <v>731355</v>
+      </c>
+      <c r="C121" s="7">
+        <v>12760</v>
+      </c>
+      <c r="D121" s="7">
+        <v>29403</v>
+      </c>
+      <c r="E121" s="7">
+        <v>23208</v>
+      </c>
+      <c r="F121" s="7">
+        <v>2357</v>
+      </c>
+      <c r="G121" s="7">
+        <v>799083</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A122" s="1">
+        <v>43987.4375</v>
+      </c>
+      <c r="B122" s="7">
+        <v>753351</v>
+      </c>
+      <c r="C122" s="7">
+        <v>12247</v>
+      </c>
+      <c r="D122" s="7">
+        <v>29747</v>
+      </c>
+      <c r="E122" s="7">
+        <v>23583</v>
+      </c>
+      <c r="F122" s="7">
+        <v>2372</v>
+      </c>
+      <c r="G122" s="7">
+        <v>821300</v>
       </c>
     </row>
   </sheetData>
@@ -4371,11 +4383,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N75"/>
+  <dimension ref="A1:N66"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A66" sqref="A66"/>
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B66" sqref="B66:K66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6610,34 +6622,34 @@
       <c r="A63" s="1">
         <v>43984.4375</v>
       </c>
-      <c r="B63" s="11">
+      <c r="B63" s="6">
         <v>12658</v>
       </c>
-      <c r="C63" s="11">
+      <c r="C63" s="6">
         <v>15811</v>
       </c>
-      <c r="D63" s="11">
+      <c r="D63" s="6">
         <v>1047</v>
       </c>
-      <c r="E63" s="11">
+      <c r="E63" s="6">
         <v>7601</v>
       </c>
-      <c r="F63" s="11">
+      <c r="F63" s="6">
         <v>8789</v>
       </c>
-      <c r="G63" s="11">
+      <c r="G63" s="6">
         <v>5766</v>
       </c>
-      <c r="H63" s="11">
+      <c r="H63" s="6">
         <v>5488</v>
       </c>
-      <c r="I63" s="11">
+      <c r="I63" s="6">
         <v>801</v>
       </c>
-      <c r="J63" s="11">
+      <c r="J63" s="6">
         <v>125</v>
       </c>
-      <c r="K63" s="11">
+      <c r="K63" s="6">
         <v>87</v>
       </c>
     </row>
@@ -6645,139 +6657,106 @@
       <c r="A64" s="1">
         <v>43985.4375</v>
       </c>
-      <c r="B64" s="12">
+      <c r="B64" s="7">
         <v>12851</v>
       </c>
-      <c r="C64" s="12">
+      <c r="C64" s="7">
         <v>15956</v>
       </c>
-      <c r="D64" s="12">
+      <c r="D64" s="7">
         <v>1068</v>
       </c>
-      <c r="E64" s="12">
+      <c r="E64" s="7">
         <v>7728</v>
       </c>
-      <c r="F64" s="12">
+      <c r="F64" s="7">
         <v>8912</v>
       </c>
-      <c r="G64" s="12">
+      <c r="G64" s="7">
         <v>5816</v>
       </c>
-      <c r="H64" s="12">
+      <c r="H64" s="7">
         <v>5506</v>
       </c>
-      <c r="I64" s="12">
+      <c r="I64" s="7">
         <v>791</v>
       </c>
-      <c r="J64" s="12">
+      <c r="J64" s="7">
         <v>127</v>
       </c>
-      <c r="K64" s="12">
+      <c r="K64" s="7">
         <v>92</v>
       </c>
     </row>
-    <row r="65" spans="2:11" ht="20" x14ac:dyDescent="0.2">
-      <c r="B65" s="12"/>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11"/>
-      <c r="I65" s="7"/>
-      <c r="J65" s="7"/>
-      <c r="K65" s="7"/>
-    </row>
-    <row r="66" spans="2:11" ht="23" x14ac:dyDescent="0.3">
-      <c r="B66" s="12"/>
-      <c r="C66" s="6"/>
-      <c r="D66" s="12"/>
-      <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
-      <c r="I66" s="8"/>
-      <c r="J66" s="9"/>
-      <c r="K66" s="10"/>
-    </row>
-    <row r="67" spans="2:11" ht="23" x14ac:dyDescent="0.3">
-      <c r="B67" s="12"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11"/>
-      <c r="I67" s="8"/>
-      <c r="J67" s="9"/>
-      <c r="K67" s="10"/>
-    </row>
-    <row r="68" spans="2:11" ht="23" x14ac:dyDescent="0.3">
-      <c r="B68" s="12"/>
-      <c r="C68" s="6"/>
-      <c r="D68" s="12"/>
-      <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
-      <c r="G68" s="11"/>
-      <c r="H68" s="11"/>
-      <c r="I68" s="8"/>
-      <c r="J68" s="9"/>
-      <c r="K68" s="10"/>
-    </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B69" s="12"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="12"/>
-      <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="11"/>
-    </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B70" s="12"/>
-      <c r="C70" s="6"/>
-      <c r="D70" s="12"/>
-      <c r="E70" s="11"/>
-      <c r="F70" s="11"/>
-      <c r="G70" s="11"/>
-      <c r="H70" s="11"/>
-    </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B71" s="12"/>
-      <c r="C71" s="6"/>
-      <c r="D71" s="12"/>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="11"/>
-      <c r="H71" s="11"/>
-    </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B72" s="12"/>
-      <c r="C72" s="6"/>
-      <c r="D72" s="12"/>
-      <c r="E72" s="11"/>
-      <c r="F72" s="11"/>
-      <c r="G72" s="11"/>
-      <c r="H72" s="11"/>
-    </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D73" s="5"/>
-      <c r="E73" s="6"/>
-      <c r="F73" s="11"/>
-      <c r="G73" s="11"/>
-      <c r="H73" s="11"/>
-    </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="D74" s="5"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="11"/>
-    </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="F75" s="11"/>
-      <c r="G75" s="11"/>
-      <c r="H75" s="11"/>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>43986.4375</v>
+      </c>
+      <c r="B65" s="7">
+        <v>13021</v>
+      </c>
+      <c r="C65" s="7">
+        <v>16139</v>
+      </c>
+      <c r="D65" s="7">
+        <v>1096</v>
+      </c>
+      <c r="E65" s="7">
+        <v>7841</v>
+      </c>
+      <c r="F65" s="7">
+        <v>9040</v>
+      </c>
+      <c r="G65" s="7">
+        <v>5871</v>
+      </c>
+      <c r="H65" s="7">
+        <v>5538</v>
+      </c>
+      <c r="I65" s="7">
+        <v>776</v>
+      </c>
+      <c r="J65" s="7">
+        <v>121</v>
+      </c>
+      <c r="K65" s="7">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>43987.4375</v>
+      </c>
+      <c r="B66" s="7">
+        <v>13197</v>
+      </c>
+      <c r="C66" s="7">
+        <v>16302</v>
+      </c>
+      <c r="D66" s="7">
+        <v>1123</v>
+      </c>
+      <c r="E66" s="7">
+        <v>7987</v>
+      </c>
+      <c r="F66" s="7">
+        <v>9151</v>
+      </c>
+      <c r="G66" s="7">
+        <v>5907</v>
+      </c>
+      <c r="H66" s="7">
+        <v>5563</v>
+      </c>
+      <c r="I66" s="7">
+        <v>749</v>
+      </c>
+      <c r="J66" s="7">
+        <v>118</v>
+      </c>
+      <c r="K66" s="7">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-06-06 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F34652-9044-8846-A14E-01BBB233606E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222D8F57-65FB-C948-BF34-DC183EC1C702}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -446,7 +446,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -455,6 +455,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1204,11 +1205,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:J122"/>
+  <dimension ref="A1:J144"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C130" sqref="C130"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C125" sqref="C125:D135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4376,6 +4377,71 @@
         <v>821300</v>
       </c>
     </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A123" s="1">
+        <v>43988.4375</v>
+      </c>
+      <c r="B123" s="7">
+        <v>775602</v>
+      </c>
+      <c r="C123" s="7">
+        <v>12384</v>
+      </c>
+      <c r="D123" s="7">
+        <v>30202</v>
+      </c>
+      <c r="E123" s="7">
+        <v>23947</v>
+      </c>
+      <c r="F123" s="7">
+        <v>2407</v>
+      </c>
+      <c r="G123" s="7">
+        <v>844542</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B124" s="7"/>
+      <c r="C124" s="7"/>
+      <c r="D124" s="7"/>
+    </row>
+    <row r="136" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C136" s="7"/>
+      <c r="D136" s="7"/>
+    </row>
+    <row r="137" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C137" s="7"/>
+      <c r="D137" s="8"/>
+      <c r="E137" s="8"/>
+    </row>
+    <row r="138" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C138" s="7"/>
+      <c r="D138" s="8"/>
+    </row>
+    <row r="139" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C139" s="7"/>
+      <c r="D139" s="8"/>
+    </row>
+    <row r="140" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C140" s="7"/>
+      <c r="D140" s="7"/>
+    </row>
+    <row r="141" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C141" s="7"/>
+      <c r="D141" s="7"/>
+    </row>
+    <row r="142" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C142" s="7"/>
+      <c r="D142" s="7"/>
+    </row>
+    <row r="143" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C143" s="7"/>
+      <c r="D143" s="7"/>
+    </row>
+    <row r="144" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C144" s="7"/>
+      <c r="D144" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4383,11 +4449,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N66"/>
+  <dimension ref="A1:N86"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B66" sqref="B66:K66"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6757,6 +6823,140 @@
       <c r="K66" s="7">
         <v>94</v>
       </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>43988.4375</v>
+      </c>
+      <c r="B67" s="7">
+        <v>13441</v>
+      </c>
+      <c r="C67" s="7">
+        <v>16514</v>
+      </c>
+      <c r="D67" s="7">
+        <v>1178</v>
+      </c>
+      <c r="E67" s="7">
+        <v>8153</v>
+      </c>
+      <c r="F67" s="7">
+        <v>9276</v>
+      </c>
+      <c r="G67" s="7">
+        <v>5989</v>
+      </c>
+      <c r="H67" s="7">
+        <v>5590</v>
+      </c>
+      <c r="I67" s="7">
+        <v>673</v>
+      </c>
+      <c r="J67" s="7">
+        <v>117</v>
+      </c>
+      <c r="K67" s="7">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C69" s="7"/>
+      <c r="D69" s="7"/>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C70" s="7"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C72" s="7"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="7"/>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C73" s="7"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
+      <c r="F73" s="7"/>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C74" s="7"/>
+      <c r="D74" s="8"/>
+      <c r="E74" s="8"/>
+      <c r="F74" s="7"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C75" s="7"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C76" s="7"/>
+      <c r="D76" s="8"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C77" s="7"/>
+      <c r="D77" s="8"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C78" s="7"/>
+      <c r="D78" s="8"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+    </row>
+    <row r="81" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+    </row>
+    <row r="82" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
+    </row>
+    <row r="83" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="8"/>
+    </row>
+    <row r="84" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="8"/>
+    </row>
+    <row r="85" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D85" s="7"/>
+      <c r="E85" s="8"/>
+      <c r="F85" s="8"/>
+    </row>
+    <row r="86" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-06-07 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222D8F57-65FB-C948-BF34-DC183EC1C702}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE04A7A0-A91F-F242-9A47-877730C0065F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -433,9 +433,18 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -446,7 +455,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -456,6 +465,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1205,11 +1215,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:J144"/>
+  <dimension ref="A1:I124"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C125" sqref="C125:D135"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1223,7 +1233,7 @@
     <col min="7" max="7" width="54.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1246,7 +1256,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43872.645833333336</v>
       </c>
@@ -1268,9 +1278,8 @@
       <c r="G2">
         <v>285</v>
       </c>
-      <c r="H2" s="5"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43873.645833333336</v>
       </c>
@@ -1292,9 +1301,8 @@
       <c r="G3">
         <v>313</v>
       </c>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43874.645833333336</v>
       </c>
@@ -1318,9 +1326,8 @@
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43875.645833333336</v>
       </c>
@@ -1344,9 +1351,8 @@
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43875.645833333336</v>
       </c>
@@ -1370,9 +1376,8 @@
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43875.645833333336</v>
       </c>
@@ -1396,9 +1401,8 @@
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43878.645833333336</v>
       </c>
@@ -1422,9 +1426,8 @@
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43879.645833333336</v>
       </c>
@@ -1448,9 +1451,8 @@
       </c>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43880.645833333336</v>
       </c>
@@ -1474,9 +1476,8 @@
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43881.645833333336</v>
       </c>
@@ -1500,9 +1501,8 @@
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>43882.645833333336</v>
       </c>
@@ -1526,9 +1526,8 @@
       </c>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43882.645833333336</v>
       </c>
@@ -1552,9 +1551,8 @@
       </c>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>43882.645833333336</v>
       </c>
@@ -1578,9 +1576,8 @@
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43885.645833333336</v>
       </c>
@@ -1604,9 +1601,8 @@
       </c>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>43886.645833333336</v>
       </c>
@@ -1630,9 +1626,8 @@
       </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43887.645833333336</v>
       </c>
@@ -1656,9 +1651,8 @@
       </c>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43888.645833333336</v>
       </c>
@@ -1682,9 +1676,8 @@
       </c>
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43888.645833333336</v>
       </c>
@@ -1708,9 +1701,8 @@
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>43889.645833333336</v>
       </c>
@@ -1734,9 +1726,8 @@
       </c>
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43889.645833333336</v>
       </c>
@@ -1760,9 +1751,8 @@
       </c>
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43892.645833333336</v>
       </c>
@@ -1786,9 +1776,8 @@
       </c>
       <c r="H22" s="5"/>
       <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43893.645833333336</v>
       </c>
@@ -1812,9 +1801,8 @@
       </c>
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43894.645833333336</v>
       </c>
@@ -1838,9 +1826,8 @@
       </c>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>43895.645833333336</v>
       </c>
@@ -1864,9 +1851,8 @@
       </c>
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>43896.645833333336</v>
       </c>
@@ -1890,9 +1876,8 @@
       </c>
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43897.604166666664</v>
       </c>
@@ -1916,9 +1901,8 @@
       </c>
       <c r="H27" s="5"/>
       <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43897.645833333336</v>
       </c>
@@ -1942,9 +1926,8 @@
       </c>
       <c r="H28" s="5"/>
       <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43899.604166666664</v>
       </c>
@@ -1968,9 +1951,8 @@
       </c>
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43900.604166666664</v>
       </c>
@@ -1994,9 +1976,8 @@
       </c>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>43900.604166666664</v>
       </c>
@@ -2020,9 +2001,8 @@
       </c>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>43901.604166666664</v>
       </c>
@@ -2046,9 +2026,8 @@
       </c>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43902.604166666664</v>
       </c>
@@ -2072,9 +2051,8 @@
       </c>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43903.604166666664</v>
       </c>
@@ -2098,9 +2076,8 @@
       </c>
       <c r="H34" s="5"/>
       <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>43904.895833333336</v>
       </c>
@@ -2124,9 +2101,8 @@
       </c>
       <c r="H35" s="5"/>
       <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>43905.895833333336</v>
       </c>
@@ -2150,9 +2126,8 @@
       </c>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>43906.895833333336</v>
       </c>
@@ -2176,9 +2151,8 @@
       </c>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>43907.895833333336</v>
       </c>
@@ -2202,9 +2176,8 @@
       </c>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>43909.604166666664</v>
       </c>
@@ -2228,9 +2201,8 @@
       </c>
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>43909.895833333336</v>
       </c>
@@ -2254,9 +2226,8 @@
       </c>
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>43911.604166666664</v>
       </c>
@@ -2280,9 +2251,8 @@
       </c>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>43911.895833333336</v>
       </c>
@@ -2306,9 +2276,8 @@
       </c>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>43912.895833333336</v>
       </c>
@@ -2332,9 +2301,8 @@
       </c>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43913.4375</v>
       </c>
@@ -2358,9 +2326,8 @@
       </c>
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43914.4375</v>
       </c>
@@ -2384,9 +2351,8 @@
       </c>
       <c r="H45" s="5"/>
       <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>43915.4375</v>
       </c>
@@ -2410,9 +2376,8 @@
       </c>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>43915.729166666664</v>
       </c>
@@ -2436,9 +2401,8 @@
       </c>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>43916.4375</v>
       </c>
@@ -2462,9 +2426,8 @@
       </c>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
-      <c r="J48" s="5"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>43916.729166666664</v>
       </c>
@@ -2488,9 +2451,8 @@
       </c>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>43917.4375</v>
       </c>
@@ -2514,9 +2476,8 @@
       </c>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>43918.4375</v>
       </c>
@@ -2540,9 +2501,8 @@
       </c>
       <c r="H51" s="5"/>
       <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>43918.729166666664</v>
       </c>
@@ -2566,9 +2526,8 @@
       </c>
       <c r="H52" s="5"/>
       <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>43919.4375</v>
       </c>
@@ -2592,9 +2551,8 @@
       </c>
       <c r="H53" s="5"/>
       <c r="I53" s="5"/>
-      <c r="J53" s="5"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>43919.729166666664</v>
       </c>
@@ -2618,9 +2576,8 @@
       </c>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
-      <c r="J54" s="5"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>43920.4375</v>
       </c>
@@ -2644,9 +2601,8 @@
       </c>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>43921.4375</v>
       </c>
@@ -2671,9 +2627,8 @@
       </c>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
-      <c r="J56" s="5"/>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>43922.4375</v>
       </c>
@@ -2697,9 +2652,8 @@
       </c>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
-      <c r="J57" s="5"/>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>43923.4375</v>
       </c>
@@ -2723,9 +2677,8 @@
       </c>
       <c r="H58" s="5"/>
       <c r="I58" s="5"/>
-      <c r="J58" s="5"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>43924.4375</v>
       </c>
@@ -2749,9 +2702,8 @@
       </c>
       <c r="H59" s="5"/>
       <c r="I59" s="5"/>
-      <c r="J59" s="5"/>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>43925.4375</v>
       </c>
@@ -2775,9 +2727,8 @@
       </c>
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
-      <c r="J60" s="5"/>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>43926.4375</v>
       </c>
@@ -2801,9 +2752,8 @@
       </c>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
-      <c r="J61" s="5"/>
-    </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>43927.4375</v>
       </c>
@@ -2827,9 +2777,8 @@
       </c>
       <c r="H62" s="5"/>
       <c r="I62" s="5"/>
-      <c r="J62" s="5"/>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>43928.4375</v>
       </c>
@@ -2853,9 +2802,8 @@
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>
-      <c r="J63" s="5"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>43929.4375</v>
       </c>
@@ -2879,9 +2827,8 @@
       </c>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
-      <c r="J64" s="5"/>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>43930.4375</v>
       </c>
@@ -2905,9 +2852,8 @@
       </c>
       <c r="H65" s="5"/>
       <c r="I65" s="5"/>
-      <c r="J65" s="5"/>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>43931.4375</v>
       </c>
@@ -2931,9 +2877,8 @@
       </c>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
-      <c r="J66" s="5"/>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>43932.4375</v>
       </c>
@@ -2957,9 +2902,8 @@
       </c>
       <c r="H67" s="5"/>
       <c r="I67" s="5"/>
-      <c r="J67" s="5"/>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>43933.4375</v>
       </c>
@@ -2983,9 +2927,8 @@
       </c>
       <c r="H68" s="5"/>
       <c r="I68" s="5"/>
-      <c r="J68" s="5"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>43934.4375</v>
       </c>
@@ -3009,9 +2952,8 @@
       </c>
       <c r="H69" s="5"/>
       <c r="I69" s="5"/>
-      <c r="J69" s="5"/>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>43935.4375</v>
       </c>
@@ -3035,9 +2977,8 @@
       </c>
       <c r="H70" s="5"/>
       <c r="I70" s="5"/>
-      <c r="J70" s="5"/>
-    </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>43936.4375</v>
       </c>
@@ -3061,9 +3002,8 @@
       </c>
       <c r="H71" s="5"/>
       <c r="I71" s="5"/>
-      <c r="J71" s="5"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>43937.4375</v>
       </c>
@@ -3087,9 +3027,8 @@
       </c>
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
-      <c r="J72" s="5"/>
-    </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>43938.4375</v>
       </c>
@@ -3113,9 +3052,8 @@
       </c>
       <c r="H73" s="5"/>
       <c r="I73" s="5"/>
-      <c r="J73" s="5"/>
-    </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>43939.4375</v>
       </c>
@@ -3139,9 +3077,8 @@
       </c>
       <c r="H74" s="5"/>
       <c r="I74" s="5"/>
-      <c r="J74" s="5"/>
-    </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>43940.4375</v>
       </c>
@@ -3165,9 +3102,8 @@
       </c>
       <c r="H75" s="5"/>
       <c r="I75" s="5"/>
-      <c r="J75" s="5"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>43941.4375</v>
       </c>
@@ -3191,9 +3127,8 @@
       </c>
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
-      <c r="J76" s="5"/>
-    </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>43942.4375</v>
       </c>
@@ -3217,9 +3152,8 @@
       </c>
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
-      <c r="J77" s="5"/>
-    </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>43943.4375</v>
       </c>
@@ -3243,9 +3177,8 @@
       </c>
       <c r="H78" s="5"/>
       <c r="I78" s="5"/>
-      <c r="J78" s="5"/>
-    </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>43944.4375</v>
       </c>
@@ -3269,9 +3202,8 @@
       </c>
       <c r="H79" s="5"/>
       <c r="I79" s="5"/>
-      <c r="J79" s="5"/>
-    </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>43945.4375</v>
       </c>
@@ -3295,9 +3227,8 @@
       </c>
       <c r="H80" s="5"/>
       <c r="I80" s="5"/>
-      <c r="J80" s="5"/>
-    </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>43946.4375</v>
       </c>
@@ -3321,9 +3252,8 @@
       </c>
       <c r="H81" s="5"/>
       <c r="I81" s="5"/>
-      <c r="J81" s="5"/>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>43947.4375</v>
       </c>
@@ -3347,9 +3277,8 @@
       </c>
       <c r="H82" s="5"/>
       <c r="I82" s="5"/>
-      <c r="J82" s="5"/>
-    </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>43948.4375</v>
       </c>
@@ -3373,9 +3302,8 @@
       </c>
       <c r="H83" s="5"/>
       <c r="I83" s="5"/>
-      <c r="J83" s="5"/>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>43949.4375</v>
       </c>
@@ -3399,9 +3327,8 @@
       </c>
       <c r="H84" s="5"/>
       <c r="I84" s="5"/>
-      <c r="J84" s="5"/>
-    </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>43950.4375</v>
       </c>
@@ -3425,9 +3352,8 @@
       </c>
       <c r="H85" s="5"/>
       <c r="I85" s="5"/>
-      <c r="J85" s="5"/>
-    </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>43951.4375</v>
       </c>
@@ -3451,9 +3377,8 @@
       </c>
       <c r="H86" s="5"/>
       <c r="I86" s="5"/>
-      <c r="J86" s="5"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>43952.4375</v>
       </c>
@@ -3477,9 +3402,8 @@
       </c>
       <c r="H87" s="5"/>
       <c r="I87" s="5"/>
-      <c r="J87" s="5"/>
-    </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>43953.4375</v>
       </c>
@@ -3503,9 +3427,8 @@
       </c>
       <c r="H88" s="5"/>
       <c r="I88" s="5"/>
-      <c r="J88" s="5"/>
-    </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>43954.4375</v>
       </c>
@@ -3529,9 +3452,8 @@
       </c>
       <c r="H89" s="5"/>
       <c r="I89" s="5"/>
-      <c r="J89" s="5"/>
-    </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>43955.4375</v>
       </c>
@@ -3555,9 +3477,8 @@
       </c>
       <c r="H90" s="5"/>
       <c r="I90" s="5"/>
-      <c r="J90" s="5"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>43956.4375</v>
       </c>
@@ -3581,9 +3502,8 @@
       </c>
       <c r="H91" s="5"/>
       <c r="I91" s="5"/>
-      <c r="J91" s="5"/>
-    </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>43957.4375</v>
       </c>
@@ -3607,9 +3527,8 @@
       </c>
       <c r="H92" s="5"/>
       <c r="I92" s="5"/>
-      <c r="J92" s="5"/>
-    </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>43958.4375</v>
       </c>
@@ -3633,9 +3552,8 @@
       </c>
       <c r="H93" s="5"/>
       <c r="I93" s="5"/>
-      <c r="J93" s="5"/>
-    </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>43959.4375</v>
       </c>
@@ -3659,9 +3577,8 @@
       </c>
       <c r="H94" s="5"/>
       <c r="I94" s="5"/>
-      <c r="J94" s="5"/>
-    </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>43960.4375</v>
       </c>
@@ -3685,9 +3602,8 @@
       </c>
       <c r="H95" s="5"/>
       <c r="I95" s="5"/>
-      <c r="J95" s="5"/>
-    </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>43961.4375</v>
       </c>
@@ -3711,9 +3627,8 @@
       </c>
       <c r="H96" s="5"/>
       <c r="I96" s="5"/>
-      <c r="J96" s="5"/>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>43962.4375</v>
       </c>
@@ -3737,9 +3652,8 @@
       </c>
       <c r="H97" s="5"/>
       <c r="I97" s="5"/>
-      <c r="J97" s="5"/>
-    </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>43963.4375</v>
       </c>
@@ -3763,9 +3677,8 @@
       </c>
       <c r="H98" s="5"/>
       <c r="I98" s="5"/>
-      <c r="J98" s="5"/>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>43964.4375</v>
       </c>
@@ -3789,9 +3702,8 @@
       </c>
       <c r="H99" s="5"/>
       <c r="I99" s="5"/>
-      <c r="J99" s="5"/>
-    </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>43965.4375</v>
       </c>
@@ -3815,9 +3727,8 @@
       </c>
       <c r="H100" s="5"/>
       <c r="I100" s="5"/>
-      <c r="J100" s="5"/>
-    </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>43966.4375</v>
       </c>
@@ -3841,9 +3752,8 @@
       </c>
       <c r="H101" s="5"/>
       <c r="I101" s="5"/>
-      <c r="J101" s="5"/>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>43967.4375</v>
       </c>
@@ -3867,9 +3777,8 @@
       </c>
       <c r="H102" s="5"/>
       <c r="I102" s="5"/>
-      <c r="J102" s="5"/>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>43968.4375</v>
       </c>
@@ -3893,9 +3802,8 @@
       </c>
       <c r="H103" s="5"/>
       <c r="I103" s="5"/>
-      <c r="J103" s="5"/>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>43969.4375</v>
       </c>
@@ -3919,9 +3827,8 @@
       </c>
       <c r="H104" s="5"/>
       <c r="I104" s="5"/>
-      <c r="J104" s="5"/>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>43970.4375</v>
       </c>
@@ -3945,9 +3852,8 @@
       </c>
       <c r="H105" s="5"/>
       <c r="I105" s="5"/>
-      <c r="J105" s="5"/>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>43971.4375</v>
       </c>
@@ -3971,9 +3877,8 @@
       </c>
       <c r="H106" s="5"/>
       <c r="I106" s="5"/>
-      <c r="J106" s="5"/>
-    </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>43972.4375</v>
       </c>
@@ -3997,9 +3902,8 @@
       </c>
       <c r="H107" s="5"/>
       <c r="I107" s="5"/>
-      <c r="J107" s="5"/>
-    </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>43973.4375</v>
       </c>
@@ -4023,9 +3927,8 @@
       </c>
       <c r="H108" s="5"/>
       <c r="I108" s="5"/>
-      <c r="J108" s="5"/>
-    </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>43974.4375</v>
       </c>
@@ -4049,9 +3952,8 @@
       </c>
       <c r="H109" s="5"/>
       <c r="I109" s="5"/>
-      <c r="J109" s="5"/>
-    </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>43975.4375</v>
       </c>
@@ -4075,9 +3977,8 @@
       </c>
       <c r="H110" s="5"/>
       <c r="I110" s="5"/>
-      <c r="J110" s="5"/>
-    </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>43976.4375</v>
       </c>
@@ -4101,9 +4002,8 @@
       </c>
       <c r="H111" s="5"/>
       <c r="I111" s="5"/>
-      <c r="J111" s="5"/>
-    </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>43977.4375</v>
       </c>
@@ -4127,9 +4027,8 @@
       </c>
       <c r="H112" s="5"/>
       <c r="I112" s="5"/>
-      <c r="J112" s="5"/>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>43978.4375</v>
       </c>
@@ -4153,9 +4052,8 @@
       </c>
       <c r="H113" s="5"/>
       <c r="I113" s="5"/>
-      <c r="J113" s="5"/>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>43979.4375</v>
       </c>
@@ -4179,9 +4077,8 @@
       </c>
       <c r="H114" s="5"/>
       <c r="I114" s="5"/>
-      <c r="J114" s="5"/>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>43980.4375</v>
       </c>
@@ -4205,9 +4102,8 @@
       </c>
       <c r="H115" s="5"/>
       <c r="I115" s="5"/>
-      <c r="J115" s="5"/>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>43981.4375</v>
       </c>
@@ -4231,9 +4127,8 @@
       </c>
       <c r="H116" s="5"/>
       <c r="I116" s="5"/>
-      <c r="J116" s="5"/>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>43982.4375</v>
       </c>
@@ -4257,9 +4152,8 @@
       </c>
       <c r="H117" s="5"/>
       <c r="I117" s="5"/>
-      <c r="J117" s="5"/>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>43983.4375</v>
       </c>
@@ -4283,9 +4177,8 @@
       </c>
       <c r="H118" s="5"/>
       <c r="I118" s="5"/>
-      <c r="J118" s="5"/>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>43984.4375</v>
       </c>
@@ -4308,7 +4201,7 @@
         <v>758586</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>43985.4375</v>
       </c>
@@ -4331,7 +4224,7 @@
         <v>777137</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>43986.4375</v>
       </c>
@@ -4354,7 +4247,7 @@
         <v>799083</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>43987.4375</v>
       </c>
@@ -4377,7 +4270,7 @@
         <v>821300</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>43988.4375</v>
       </c>
@@ -4400,47 +4293,28 @@
         <v>844542</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B124" s="7"/>
-      <c r="C124" s="7"/>
-      <c r="D124" s="7"/>
-    </row>
-    <row r="136" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C136" s="7"/>
-      <c r="D136" s="7"/>
-    </row>
-    <row r="137" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C137" s="7"/>
-      <c r="D137" s="8"/>
-      <c r="E137" s="8"/>
-    </row>
-    <row r="138" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C138" s="7"/>
-      <c r="D138" s="8"/>
-    </row>
-    <row r="139" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C139" s="7"/>
-      <c r="D139" s="8"/>
-    </row>
-    <row r="140" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C140" s="7"/>
-      <c r="D140" s="7"/>
-    </row>
-    <row r="141" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C141" s="7"/>
-      <c r="D141" s="7"/>
-    </row>
-    <row r="142" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C142" s="7"/>
-      <c r="D142" s="7"/>
-    </row>
-    <row r="143" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C143" s="7"/>
-      <c r="D143" s="7"/>
-    </row>
-    <row r="144" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C144" s="7"/>
-      <c r="D144" s="7"/>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A124" s="1">
+        <v>43989.4375</v>
+      </c>
+      <c r="B124" s="7">
+        <v>794237</v>
+      </c>
+      <c r="C124" s="7">
+        <v>6779</v>
+      </c>
+      <c r="D124" s="7">
+        <v>30617</v>
+      </c>
+      <c r="E124" s="7">
+        <v>24252</v>
+      </c>
+      <c r="F124" s="7">
+        <v>2426</v>
+      </c>
+      <c r="G124" s="7">
+        <v>858311</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4451,9 +4325,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
   <dimension ref="A1:N86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J70" sqref="J70"/>
+      <selection pane="bottomLeft" activeCell="I70" sqref="I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6859,71 +6733,120 @@
         <v>97</v>
       </c>
     </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>43989.418749999997</v>
+      </c>
+      <c r="B68" s="7">
+        <v>13662</v>
+      </c>
+      <c r="C68" s="7">
+        <v>16700</v>
+      </c>
+      <c r="D68" s="7">
+        <v>1226</v>
+      </c>
+      <c r="E68" s="7">
+        <v>8331</v>
+      </c>
+      <c r="F68" s="7">
+        <v>9398</v>
+      </c>
+      <c r="G68" s="7">
+        <v>6048</v>
+      </c>
+      <c r="H68" s="7">
+        <v>5599</v>
+      </c>
+      <c r="I68" s="7">
+        <v>635</v>
+      </c>
+      <c r="J68" s="7">
+        <v>117</v>
+      </c>
+      <c r="K68" s="7">
+        <v>92</v>
+      </c>
+    </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C69" s="7"/>
-      <c r="D69" s="7"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="8"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C70" s="7"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="8"/>
       <c r="D70" s="7"/>
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
+      <c r="I70" s="9"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C71" s="7"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="8"/>
       <c r="D71" s="7"/>
       <c r="E71" s="7"/>
       <c r="F71" s="7"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C72" s="7"/>
-      <c r="D72" s="8"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="7"/>
       <c r="E72" s="8"/>
       <c r="F72" s="7"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C73" s="7"/>
-      <c r="D73" s="8"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="7"/>
       <c r="E73" s="8"/>
       <c r="F73" s="7"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C74" s="7"/>
-      <c r="D74" s="8"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="7"/>
       <c r="E74" s="8"/>
       <c r="F74" s="7"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C75" s="7"/>
-      <c r="D75" s="8"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="7"/>
       <c r="E75" s="7"/>
       <c r="F75" s="7"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C76" s="7"/>
-      <c r="D76" s="8"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="7"/>
       <c r="E76" s="7"/>
       <c r="F76" s="7"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B77" s="7"/>
       <c r="C77" s="7"/>
-      <c r="D77" s="8"/>
+      <c r="D77" s="7"/>
       <c r="E77" s="7"/>
       <c r="F77" s="7"/>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B78" s="7"/>
       <c r="C78" s="7"/>
-      <c r="D78" s="8"/>
+      <c r="D78" s="7"/>
       <c r="E78" s="7"/>
       <c r="F78" s="7"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B79" s="7"/>
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="7"/>
       <c r="F79" s="7"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
       <c r="D80" s="7"/>
       <c r="E80" s="7"/>
       <c r="F80" s="7"/>

</xml_diff>

<commit_message>
excel update 2020-06-08 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE04A7A0-A91F-F242-9A47-877730C0065F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309C25F6-442A-2240-94B7-58C952A90C0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -1215,11 +1215,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I124"/>
+  <dimension ref="A1:I139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C129" sqref="C129"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C127" sqref="C127:E146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4316,6 +4316,40 @@
         <v>858311</v>
       </c>
     </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A125" s="1">
+        <v>43990.4375</v>
+      </c>
+      <c r="B125" s="7">
+        <v>809087</v>
+      </c>
+      <c r="C125" s="7">
+        <v>4811</v>
+      </c>
+      <c r="D125" s="7">
+        <v>30860</v>
+      </c>
+      <c r="E125" s="7">
+        <v>24492</v>
+      </c>
+      <c r="F125" s="7">
+        <v>2450</v>
+      </c>
+      <c r="G125" s="7">
+        <v>871700</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C126" s="7"/>
+      <c r="D126" s="7"/>
+      <c r="E126" s="7"/>
+    </row>
+    <row r="139" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F139" s="8" t="e">
+        <f>Demographics!#REF!+Demographics!#REF!</f>
+        <v>#REF!</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4323,11 +4357,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N86"/>
+  <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I70" sqref="I70"/>
+      <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6735,7 +6769,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <v>43989.418749999997</v>
+        <v>43989.4375</v>
       </c>
       <c r="B68" s="7">
         <v>13662</v>
@@ -6769,9 +6803,39 @@
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B69" s="7"/>
-      <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
+      <c r="A69" s="1">
+        <v>43990.4375</v>
+      </c>
+      <c r="B69" s="7">
+        <v>13793</v>
+      </c>
+      <c r="C69" s="7">
+        <v>16813</v>
+      </c>
+      <c r="D69" s="7">
+        <v>1243</v>
+      </c>
+      <c r="E69" s="7">
+        <v>8457</v>
+      </c>
+      <c r="F69" s="7">
+        <v>9472</v>
+      </c>
+      <c r="G69" s="7">
+        <v>6066</v>
+      </c>
+      <c r="H69" s="7">
+        <v>5609</v>
+      </c>
+      <c r="I69" s="7">
+        <v>603</v>
+      </c>
+      <c r="J69" s="7">
+        <v>118</v>
+      </c>
+      <c r="K69" s="7">
+        <v>81</v>
+      </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B70" s="7"/>
@@ -6783,103 +6847,32 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B71" s="7"/>
-      <c r="C71" s="8"/>
+      <c r="C71" s="7"/>
       <c r="D71" s="7"/>
-      <c r="E71" s="7"/>
-      <c r="F71" s="7"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="8"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B72" s="7"/>
-      <c r="C72" s="8"/>
+      <c r="C72" s="7"/>
       <c r="D72" s="7"/>
-      <c r="E72" s="8"/>
+      <c r="E72" s="7"/>
       <c r="F72" s="7"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B73" s="7"/>
-      <c r="C73" s="8"/>
+      <c r="C73" s="7"/>
       <c r="D73" s="7"/>
-      <c r="E73" s="8"/>
-      <c r="F73" s="7"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B74" s="7"/>
-      <c r="C74" s="8"/>
+      <c r="C74" s="7"/>
       <c r="D74" s="7"/>
-      <c r="E74" s="8"/>
-      <c r="F74" s="7"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B75" s="7"/>
-      <c r="C75" s="8"/>
+      <c r="C75" s="7"/>
       <c r="D75" s="7"/>
-      <c r="E75" s="7"/>
-      <c r="F75" s="7"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B76" s="7"/>
-      <c r="C76" s="8"/>
-      <c r="D76" s="7"/>
-      <c r="E76" s="7"/>
-      <c r="F76" s="7"/>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B77" s="7"/>
-      <c r="C77" s="7"/>
-      <c r="D77" s="7"/>
-      <c r="E77" s="7"/>
-      <c r="F77" s="7"/>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
-      <c r="D78" s="7"/>
-      <c r="E78" s="7"/>
-      <c r="F78" s="7"/>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
-      <c r="D79" s="7"/>
-      <c r="E79" s="7"/>
-      <c r="F79" s="7"/>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B80" s="7"/>
-      <c r="C80" s="7"/>
-      <c r="D80" s="7"/>
-      <c r="E80" s="7"/>
-      <c r="F80" s="7"/>
-    </row>
-    <row r="81" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D81" s="7"/>
-      <c r="E81" s="7"/>
-      <c r="F81" s="7"/>
-    </row>
-    <row r="82" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D82" s="7"/>
-      <c r="E82" s="7"/>
-      <c r="F82" s="7"/>
-    </row>
-    <row r="83" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D83" s="7"/>
-      <c r="E83" s="7"/>
-      <c r="F83" s="8"/>
-    </row>
-    <row r="84" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D84" s="7"/>
-      <c r="E84" s="7"/>
-      <c r="F84" s="8"/>
-    </row>
-    <row r="85" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D85" s="7"/>
-      <c r="E85" s="8"/>
-      <c r="F85" s="8"/>
-    </row>
-    <row r="86" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D86" s="7"/>
-      <c r="E86" s="7"/>
-      <c r="F86" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-06-09 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309C25F6-442A-2240-94B7-58C952A90C0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D31A7F-5689-5B4A-A635-2A39824E95A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -433,18 +433,9 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -455,7 +446,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -465,7 +456,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1215,11 +1205,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I139"/>
+  <dimension ref="A1:I128"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C127" sqref="C127:E146"/>
+      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B128" sqref="B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4340,15 +4330,35 @@
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C126" s="7"/>
-      <c r="D126" s="7"/>
-      <c r="E126" s="7"/>
-    </row>
-    <row r="139" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F139" s="8" t="e">
-        <f>Demographics!#REF!+Demographics!#REF!</f>
-        <v>#REF!</v>
-      </c>
+      <c r="A126" s="1">
+        <v>43991.4375</v>
+      </c>
+      <c r="B126" s="7">
+        <v>822015</v>
+      </c>
+      <c r="C126" s="7">
+        <v>11020</v>
+      </c>
+      <c r="D126" s="7">
+        <v>31090</v>
+      </c>
+      <c r="E126" s="7">
+        <v>24829</v>
+      </c>
+      <c r="F126" s="7">
+        <v>2464</v>
+      </c>
+      <c r="G126" s="7">
+        <v>891418</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="C127" s="7"/>
+      <c r="D127" s="7"/>
+      <c r="E127" s="7"/>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F128" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4357,11 +4367,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N75"/>
+  <dimension ref="A1:N88"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6838,12 +6848,39 @@
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B70" s="7"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="7"/>
-      <c r="E70" s="7"/>
-      <c r="F70" s="7"/>
-      <c r="I70" s="9"/>
+      <c r="A70" s="1">
+        <v>43991.4375</v>
+      </c>
+      <c r="B70" s="7">
+        <v>13917</v>
+      </c>
+      <c r="C70" s="7">
+        <v>16920</v>
+      </c>
+      <c r="D70" s="7">
+        <v>1257</v>
+      </c>
+      <c r="E70" s="7">
+        <v>8546</v>
+      </c>
+      <c r="F70" s="7">
+        <v>9546</v>
+      </c>
+      <c r="G70" s="7">
+        <v>6103</v>
+      </c>
+      <c r="H70" s="7">
+        <v>5625</v>
+      </c>
+      <c r="I70" s="7">
+        <v>600</v>
+      </c>
+      <c r="J70" s="7">
+        <v>116</v>
+      </c>
+      <c r="K70" s="7">
+        <v>88</v>
+      </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B71" s="7"/>
@@ -6854,25 +6891,90 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
+      <c r="C72" s="8"/>
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
       <c r="F72" s="7"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B73" s="7"/>
-      <c r="C73" s="7"/>
+      <c r="C73" s="8"/>
       <c r="D73" s="7"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
+      <c r="C74" s="8"/>
       <c r="D74" s="7"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
+      <c r="C75" s="8"/>
       <c r="D75" s="7"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B76" s="7"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="7"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B77" s="7"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="7"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B78" s="7"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="7"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B81" s="7"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="8"/>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B82" s="7"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="7"/>
+    </row>
+    <row r="83" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B83" s="7"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="7"/>
+    </row>
+    <row r="84" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+    </row>
+    <row r="85" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B85" s="7"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="7"/>
+    </row>
+    <row r="86" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B86" s="7"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="7"/>
+    </row>
+    <row r="87" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B87" s="7"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="7"/>
+    </row>
+    <row r="88" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B88" s="7"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-06-10 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D31A7F-5689-5B4A-A635-2A39824E95A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9A5DB9-1090-DE43-8133-7933412CCC4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -1205,11 +1205,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I128"/>
+  <dimension ref="A1:I138"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B128" sqref="B128"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A127" sqref="A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4353,12 +4353,74 @@
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C127" s="7"/>
-      <c r="D127" s="7"/>
-      <c r="E127" s="7"/>
+      <c r="A127" s="1">
+        <v>43992.4375</v>
+      </c>
+      <c r="B127" s="7">
+        <v>841143</v>
+      </c>
+      <c r="C127" s="7">
+        <v>13897</v>
+      </c>
+      <c r="D127" s="7">
+        <v>31341</v>
+      </c>
+      <c r="E127" s="7">
+        <v>25380</v>
+      </c>
+      <c r="F127" s="7">
+        <v>2475</v>
+      </c>
+      <c r="G127" s="7">
+        <v>914236</v>
+      </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B128" s="7"/>
+      <c r="C128" s="7"/>
+      <c r="D128" s="7"/>
       <c r="F128" s="8"/>
+    </row>
+    <row r="129" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C129" s="7"/>
+      <c r="D129" s="7"/>
+    </row>
+    <row r="130" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C130" s="7"/>
+      <c r="D130" s="7"/>
+    </row>
+    <row r="131" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C131" s="7"/>
+      <c r="D131" s="7"/>
+    </row>
+    <row r="132" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C132" s="7"/>
+      <c r="D132" s="8"/>
+      <c r="E132" s="8"/>
+    </row>
+    <row r="133" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C133" s="7"/>
+      <c r="D133" s="8"/>
+    </row>
+    <row r="134" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C134" s="7"/>
+      <c r="D134" s="8"/>
+    </row>
+    <row r="135" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C135" s="7"/>
+      <c r="D135" s="8"/>
+    </row>
+    <row r="136" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C136" s="7"/>
+      <c r="D136" s="8"/>
+    </row>
+    <row r="137" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C137" s="7"/>
+      <c r="D137" s="8"/>
+    </row>
+    <row r="138" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C138" s="7"/>
+      <c r="D138" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4369,9 +4431,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
   <dimension ref="A1:N88"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H70" sqref="H70"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6883,22 +6945,50 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B71" s="7"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="7"/>
-      <c r="E71" s="8"/>
-      <c r="F71" s="8"/>
+      <c r="A71" s="1">
+        <v>43992.4375</v>
+      </c>
+      <c r="B71" s="7">
+        <v>14060</v>
+      </c>
+      <c r="C71" s="7">
+        <v>17019</v>
+      </c>
+      <c r="D71" s="7">
+        <v>1280</v>
+      </c>
+      <c r="E71" s="7">
+        <v>8659</v>
+      </c>
+      <c r="F71" s="7">
+        <v>9606</v>
+      </c>
+      <c r="G71" s="7">
+        <v>6136</v>
+      </c>
+      <c r="H71" s="7">
+        <v>5647</v>
+      </c>
+      <c r="I71" s="7">
+        <v>580</v>
+      </c>
+      <c r="J71" s="7">
+        <v>118</v>
+      </c>
+      <c r="K71" s="7">
+        <v>86</v>
+      </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B72" s="7"/>
-      <c r="C72" s="8"/>
+      <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
       <c r="F72" s="7"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B73" s="7"/>
-      <c r="C73" s="8"/>
+      <c r="C73" s="7"/>
       <c r="D73" s="7"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
@@ -6928,27 +7018,27 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
+      <c r="C79" s="8"/>
       <c r="D79" s="7"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B80" s="7"/>
-      <c r="C80" s="7"/>
+      <c r="C80" s="8"/>
       <c r="D80" s="7"/>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B81" s="7"/>
-      <c r="C81" s="8"/>
+      <c r="C81" s="7"/>
       <c r="D81" s="8"/>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B82" s="7"/>
-      <c r="C82" s="8"/>
+      <c r="C82" s="7"/>
       <c r="D82" s="7"/>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B83" s="7"/>
-      <c r="C83" s="8"/>
+      <c r="C83" s="7"/>
       <c r="D83" s="7"/>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
excel update 2020-06-12 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1249664F-175E-D946-8047-0D9EC3F45653}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E3C093-7F0A-0B4D-9013-840BE049D4CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -1205,11 +1205,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I153"/>
+  <dimension ref="A1:I140"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F143" sqref="F143"/>
+      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C138" sqref="C138:D140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4398,81 +4398,79 @@
         <v>941039</v>
       </c>
     </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B129" s="7"/>
-      <c r="C129" s="7"/>
-      <c r="D129" s="7"/>
-    </row>
-    <row r="130" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A129" s="1">
+        <v>43994.4375</v>
+      </c>
+      <c r="B129" s="7">
+        <v>892604</v>
+      </c>
+      <c r="C129" s="7">
+        <v>18512</v>
+      </c>
+      <c r="D129" s="7">
+        <v>31726</v>
+      </c>
+      <c r="E129" s="7">
+        <v>26187</v>
+      </c>
+      <c r="F129" s="7">
+        <v>2498</v>
+      </c>
+      <c r="G129" s="7">
+        <v>971527</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B130" s="7"/>
       <c r="C130" s="7"/>
       <c r="D130" s="7"/>
     </row>
-    <row r="131" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B131" s="7"/>
       <c r="C131" s="7"/>
-      <c r="D131" s="8"/>
-    </row>
-    <row r="132" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D131" s="7"/>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B132" s="7"/>
       <c r="C132" s="7"/>
       <c r="D132" s="7"/>
       <c r="E132" s="8"/>
     </row>
-    <row r="133" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B133" s="7"/>
       <c r="C133" s="7"/>
       <c r="D133" s="8"/>
     </row>
-    <row r="134" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B134" s="7"/>
       <c r="C134" s="7"/>
-      <c r="D134" s="7"/>
-    </row>
-    <row r="135" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D134" s="8"/>
+      <c r="E134" s="8"/>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B135" s="7"/>
       <c r="C135" s="7"/>
       <c r="D135" s="8"/>
     </row>
-    <row r="136" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B136" s="7"/>
       <c r="C136" s="7"/>
-      <c r="D136" s="8"/>
-    </row>
-    <row r="137" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D136" s="7"/>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B137" s="7"/>
       <c r="C137" s="7"/>
-      <c r="D137" s="8"/>
-    </row>
-    <row r="138" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C138" s="7"/>
-      <c r="D138" s="8"/>
-    </row>
-    <row r="139" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C139" s="7"/>
-      <c r="D139" s="7"/>
-    </row>
-    <row r="140" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C140" s="7"/>
-      <c r="D140" s="7"/>
-    </row>
-    <row r="141" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C141" s="7"/>
-      <c r="D141" s="7"/>
-    </row>
-    <row r="149" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C149" s="7"/>
-      <c r="D149" s="7"/>
-    </row>
-    <row r="150" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C150" s="7"/>
-      <c r="D150" s="7"/>
-    </row>
-    <row r="151" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C151" s="7"/>
-      <c r="D151" s="8"/>
-      <c r="E151" s="8"/>
-    </row>
-    <row r="152" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C152" s="7"/>
-      <c r="D152" s="8"/>
-    </row>
-    <row r="153" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C153" s="7"/>
-      <c r="D153" s="8"/>
+      <c r="D137" s="7"/>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B138" s="7"/>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B139" s="7"/>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B140" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4481,11 +4479,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N72"/>
+  <dimension ref="A1:N81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C78" sqref="C78"/>
+      <selection pane="bottomLeft" activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7065,6 +7063,79 @@
       <c r="K72" s="7">
         <v>87</v>
       </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>43994.4375</v>
+      </c>
+      <c r="B73" s="7">
+        <v>14265</v>
+      </c>
+      <c r="C73" s="7">
+        <v>17203</v>
+      </c>
+      <c r="D73" s="7">
+        <v>1326</v>
+      </c>
+      <c r="E73" s="7">
+        <v>8783</v>
+      </c>
+      <c r="F73" s="7">
+        <v>9730</v>
+      </c>
+      <c r="G73" s="7">
+        <v>6204</v>
+      </c>
+      <c r="H73" s="7">
+        <v>5669</v>
+      </c>
+      <c r="I73" s="7">
+        <v>527</v>
+      </c>
+      <c r="J73" s="7">
+        <v>114</v>
+      </c>
+      <c r="K73" s="7">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C74" s="7"/>
+      <c r="D74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C75" s="7"/>
+      <c r="D75" s="8"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C76" s="7"/>
+      <c r="D76" s="8"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C77" s="7"/>
+      <c r="D77" s="8"/>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C78" s="7"/>
+      <c r="D78" s="8"/>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C79" s="7"/>
+      <c r="D79" s="8"/>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C80" s="7"/>
+      <c r="D80" s="8"/>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C81" s="7"/>
+      <c r="D81" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
excel update 2020-06-16 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68996E9-E6FD-2848-845E-0EE2C3C10624}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C159565-78DC-E64E-BA96-166A8FF828AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="460" windowWidth="33600" windowHeight="19400" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
   <sheets>
     <sheet name="Status" sheetId="1" r:id="rId1"/>
@@ -1212,11 +1212,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I132"/>
+  <dimension ref="A1:I133"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G134" sqref="G134"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G137" sqref="G137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4479,6 +4479,29 @@
         <v>1043758</v>
       </c>
     </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A133" s="1">
+        <v>43998.4375</v>
+      </c>
+      <c r="B133" s="7">
+        <v>984701</v>
+      </c>
+      <c r="C133" s="7">
+        <v>17920</v>
+      </c>
+      <c r="D133" s="7">
+        <v>32554</v>
+      </c>
+      <c r="E133" s="7">
+        <v>27431</v>
+      </c>
+      <c r="F133" s="7">
+        <v>2538</v>
+      </c>
+      <c r="G133" s="7">
+        <v>1065144</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4488,9 +4511,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
   <dimension ref="A1:N85"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G80" sqref="G80"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7194,54 +7217,59 @@
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B77" s="8"/>
-      <c r="C77" s="8"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="8"/>
-      <c r="F77" s="8"/>
-      <c r="G77" s="8"/>
-      <c r="H77" s="8"/>
+      <c r="A77" s="1">
+        <v>43998.4375</v>
+      </c>
+      <c r="B77" s="7">
+        <v>14710</v>
+      </c>
+      <c r="C77" s="7">
+        <v>17582</v>
+      </c>
+      <c r="D77" s="7">
+        <v>1422</v>
+      </c>
+      <c r="E77" s="7">
+        <v>9115</v>
+      </c>
+      <c r="F77" s="7">
+        <v>9974</v>
+      </c>
+      <c r="G77" s="7">
+        <v>6312</v>
+      </c>
+      <c r="H77" s="7">
+        <v>5718</v>
+      </c>
+      <c r="I77" s="7">
+        <v>413</v>
+      </c>
+      <c r="J77" s="7">
+        <v>98</v>
+      </c>
+      <c r="K77" s="7">
+        <v>70</v>
+      </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C79" s="8"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="8"/>
       <c r="F79" s="8"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C80" s="8"/>
-      <c r="D80" s="8"/>
-      <c r="E80" s="8"/>
       <c r="F80" s="8"/>
     </row>
-    <row r="81" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C81" s="8"/>
-      <c r="D81" s="8"/>
-      <c r="E81" s="8"/>
+    <row r="81" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F81" s="8"/>
     </row>
-    <row r="82" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C82" s="8"/>
-      <c r="D82" s="8"/>
-      <c r="E82" s="8"/>
+    <row r="82" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F82" s="8"/>
     </row>
-    <row r="83" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8"/>
+    <row r="83" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F83" s="8"/>
     </row>
-    <row r="84" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C84" s="8"/>
-      <c r="D84" s="8"/>
-      <c r="E84" s="8"/>
+    <row r="84" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F84" s="8"/>
     </row>
-    <row r="85" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C85" s="8"/>
-      <c r="D85" s="8"/>
-      <c r="E85" s="8"/>
+    <row r="85" spans="6:6" x14ac:dyDescent="0.2">
       <c r="F85" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel update 2020-06-17 10:30
</commit_message>
<xml_diff>
--- a/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
+++ b/excel/2019-novel-coronavirus-MOHLTC-updates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mylesharrison/Dropbox/everyday analytics/COVID/covid-ontario/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C159565-78DC-E64E-BA96-166A8FF828AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A81FB2-0C4C-5D43-9382-25B3AEF9BCD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19400" activeTab="1" xr2:uid="{F6EB6DDD-A4F4-3F43-81CA-DE177063DF70}"/>
   </bookViews>
@@ -402,7 +402,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -419,13 +419,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -453,7 +446,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -462,7 +455,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1212,11 +1204,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D436A8-25F8-DF4F-B5F7-C434CB655956}">
-  <dimension ref="A1:I133"/>
+  <dimension ref="A1:I134"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G137" sqref="G137"/>
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A134" sqref="A134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4502,6 +4494,29 @@
         <v>1065144</v>
       </c>
     </row>
+    <row r="134" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="1">
+        <v>43999.4375</v>
+      </c>
+      <c r="B134" s="7">
+        <v>1008351</v>
+      </c>
+      <c r="C134" s="7">
+        <v>21635</v>
+      </c>
+      <c r="D134" s="7">
+        <v>32744</v>
+      </c>
+      <c r="E134" s="7">
+        <v>27784</v>
+      </c>
+      <c r="F134" s="7">
+        <v>2550</v>
+      </c>
+      <c r="G134" s="7">
+        <v>1093064</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4509,11 +4524,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E12E741F-EC18-1F45-86FE-BCD79EE1B960}">
-  <dimension ref="A1:N85"/>
+  <dimension ref="A1:N81"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A76" sqref="A76"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7251,26 +7266,55 @@
         <v>70</v>
       </c>
     </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>43999.4375</v>
+      </c>
+      <c r="B78" s="7">
+        <v>14796</v>
+      </c>
+      <c r="C78" s="7">
+        <v>17677</v>
+      </c>
+      <c r="D78" s="7">
+        <v>1441</v>
+      </c>
+      <c r="E78" s="7">
+        <v>9196</v>
+      </c>
+      <c r="F78" s="7">
+        <v>10031</v>
+      </c>
+      <c r="G78" s="7">
+        <v>6334</v>
+      </c>
+      <c r="H78" s="7">
+        <v>5729</v>
+      </c>
+      <c r="I78" s="7">
+        <v>383</v>
+      </c>
+      <c r="J78" s="7">
+        <v>92</v>
+      </c>
+      <c r="K78" s="7">
+        <v>65</v>
+      </c>
+    </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F79" s="8"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="F80" s="8"/>
-    </row>
-    <row r="81" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F81" s="8"/>
-    </row>
-    <row r="82" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F82" s="8"/>
-    </row>
-    <row r="83" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F83" s="8"/>
-    </row>
-    <row r="84" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F84" s="8"/>
-    </row>
-    <row r="85" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F85" s="8"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="7"/>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>